<commit_message>
I updated the CertTest so that *hopefully* it will run on other people's machines. :) I added some extra files and updated FASTCertTestCases.xlsx.
I also needed to decrease the time step in the TLP (case 21) to get results comparable to FAST v7.02.00d-bjj

git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@380 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="2670" windowWidth="15180" windowHeight="8835" tabRatio="712"/>
+    <workbookView xWindow="5955" yWindow="2730" windowWidth="15180" windowHeight="8775" tabRatio="712"/>
   </bookViews>
   <sheets>
     <sheet name="TestMatrix" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2147" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="1081">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3278,6 +3278,18 @@
   </si>
   <si>
     <t>Test 22</t>
+  </si>
+  <si>
+    <t>checked</t>
+  </si>
+  <si>
+    <t>needs smaller time step to match platform heave and fairlead/anchor tensions</t>
+  </si>
+  <si>
+    <t>2-bladed CART</t>
+  </si>
+  <si>
+    <t>need to compile with changes for OC3 Hywind to check these results</t>
   </si>
 </sst>
 </file>
@@ -4198,7 +4210,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
@@ -4231,6 +4242,9 @@
     <xf numFmtId="164" fontId="0" fillId="10" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4294,7 +4308,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="9">
     <dxf>
       <font>
         <condense val="0"/>
@@ -4363,76 +4377,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -4751,10 +4695,10 @@
   <dimension ref="A1:BC48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="X24" sqref="X24"/>
+      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4885,7 +4829,7 @@
       <c r="G3" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="99" t="s">
+      <c r="H3" s="98" t="s">
         <v>1061</v>
       </c>
       <c r="I3" s="67" t="s">
@@ -4942,10 +4886,10 @@
       <c r="Z3" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="AA3" s="110" t="s">
+      <c r="AA3" s="109" t="s">
         <v>309</v>
       </c>
-      <c r="AB3" s="110" t="s">
+      <c r="AB3" s="109" t="s">
         <v>310</v>
       </c>
       <c r="AC3" s="85" t="s">
@@ -4963,7 +4907,7 @@
       <c r="AG3" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="AH3" s="104" t="s">
+      <c r="AH3" s="103" t="s">
         <v>1066</v>
       </c>
       <c r="AI3" s="86" t="s">
@@ -4990,7 +4934,7 @@
       <c r="AP3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="AQ3" s="100"/>
+      <c r="AQ3" s="99"/>
       <c r="AR3" s="75"/>
       <c r="AS3" s="75"/>
       <c r="AT3" s="76"/>
@@ -5149,7 +5093,7 @@
       <c r="AP4" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="AQ4" s="101"/>
+      <c r="AQ4" s="100"/>
       <c r="AR4" s="36"/>
       <c r="AS4" s="36"/>
       <c r="AT4" s="34"/>
@@ -5309,7 +5253,7 @@
       <c r="AP5" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ5" s="102"/>
+      <c r="AQ5" s="101"/>
       <c r="AR5" s="42"/>
       <c r="AS5" s="42"/>
       <c r="AT5" s="43"/>
@@ -5469,7 +5413,7 @@
       <c r="AP6" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ6" s="102"/>
+      <c r="AQ6" s="101"/>
       <c r="AR6" s="42"/>
       <c r="AS6" s="42"/>
       <c r="AT6" s="43"/>
@@ -5629,7 +5573,7 @@
       <c r="AP7" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ7" s="102"/>
+      <c r="AQ7" s="101"/>
       <c r="AR7" s="42"/>
       <c r="AS7" s="42"/>
       <c r="AT7" s="43"/>
@@ -5789,7 +5733,7 @@
       <c r="AP8" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ8" s="102"/>
+      <c r="AQ8" s="101"/>
       <c r="AR8" s="42"/>
       <c r="AS8" s="42"/>
       <c r="AT8" s="43"/>
@@ -5950,7 +5894,7 @@
       <c r="AP9" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ9" s="102"/>
+      <c r="AQ9" s="101"/>
       <c r="AR9" s="42"/>
       <c r="AS9" s="42"/>
       <c r="AT9" s="43"/>
@@ -6111,7 +6055,7 @@
       <c r="AP10" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ10" s="102"/>
+      <c r="AQ10" s="101"/>
       <c r="AR10" s="42"/>
       <c r="AS10" s="42"/>
       <c r="AT10" s="43"/>
@@ -6272,7 +6216,7 @@
       <c r="AP11" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ11" s="102"/>
+      <c r="AQ11" s="101"/>
       <c r="AR11" s="42"/>
       <c r="AS11" s="42"/>
       <c r="AT11" s="43"/>
@@ -6432,7 +6376,7 @@
       <c r="AP12" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AQ12" s="102"/>
+      <c r="AQ12" s="101"/>
       <c r="AR12" s="42"/>
       <c r="AS12" s="42"/>
       <c r="AT12" s="43"/>
@@ -6592,7 +6536,7 @@
       <c r="AP13" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AQ13" s="102"/>
+      <c r="AQ13" s="101"/>
       <c r="AR13" s="42"/>
       <c r="AS13" s="42"/>
       <c r="AT13" s="43"/>
@@ -6752,7 +6696,7 @@
       <c r="AP14" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ14" s="102"/>
+      <c r="AQ14" s="101"/>
       <c r="AR14" s="42"/>
       <c r="AS14" s="42"/>
       <c r="AT14" s="43"/>
@@ -6912,7 +6856,7 @@
       <c r="AP15" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ15" s="102"/>
+      <c r="AQ15" s="101"/>
       <c r="AR15" s="42"/>
       <c r="AS15" s="42"/>
       <c r="AT15" s="43"/>
@@ -7072,7 +7016,7 @@
       <c r="AP16" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ16" s="102"/>
+      <c r="AQ16" s="101"/>
       <c r="AR16" s="42"/>
       <c r="AS16" s="42"/>
       <c r="AT16" s="43"/>
@@ -7232,7 +7176,7 @@
       <c r="AP17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="AQ17" s="102"/>
+      <c r="AQ17" s="101"/>
       <c r="AR17" s="42"/>
       <c r="AS17" s="42"/>
       <c r="AT17" s="43"/>
@@ -7392,7 +7336,7 @@
       <c r="AP18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ18" s="102"/>
+      <c r="AQ18" s="101"/>
       <c r="AR18" s="42"/>
       <c r="AS18" s="42"/>
       <c r="AT18" s="43"/>
@@ -7552,7 +7496,7 @@
       <c r="AP19" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ19" s="102"/>
+      <c r="AQ19" s="101"/>
       <c r="AR19" s="42"/>
       <c r="AS19" s="42"/>
       <c r="AT19" s="43"/>
@@ -7712,7 +7656,7 @@
       <c r="AP20" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AQ20" s="102"/>
+      <c r="AQ20" s="101"/>
       <c r="AR20" s="42"/>
       <c r="AS20" s="42"/>
       <c r="AT20" s="43"/>
@@ -7765,7 +7709,9 @@
       <c r="G21" s="40" t="s">
         <v>1068</v>
       </c>
-      <c r="H21" s="37"/>
+      <c r="H21" s="110" t="s">
+        <v>1077</v>
+      </c>
       <c r="I21" s="41" t="s">
         <v>22</v>
       </c>
@@ -7868,7 +7814,7 @@
       <c r="AP21" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AQ21" s="102"/>
+      <c r="AQ21" s="101"/>
       <c r="AR21" s="42"/>
       <c r="AS21" s="42"/>
       <c r="AT21" s="43"/>
@@ -7904,7 +7850,9 @@
       <c r="G22" s="40" t="s">
         <v>1072</v>
       </c>
-      <c r="H22" s="37"/>
+      <c r="H22" s="110" t="s">
+        <v>1077</v>
+      </c>
       <c r="I22" s="41"/>
       <c r="J22" s="44"/>
       <c r="K22" s="25"/>
@@ -7941,7 +7889,7 @@
       <c r="AN22" s="42"/>
       <c r="AO22" s="42"/>
       <c r="AP22" s="43"/>
-      <c r="AQ22" s="102"/>
+      <c r="AQ22" s="101"/>
       <c r="AR22" s="42"/>
       <c r="AS22" s="42"/>
       <c r="AT22" s="43"/>
@@ -7977,7 +7925,9 @@
       <c r="G23" s="40" t="s">
         <v>1073</v>
       </c>
-      <c r="H23" s="37"/>
+      <c r="H23" s="110" t="s">
+        <v>1077</v>
+      </c>
       <c r="I23" s="41"/>
       <c r="J23" s="44"/>
       <c r="K23" s="25"/>
@@ -8014,7 +7964,7 @@
       <c r="AN23" s="42"/>
       <c r="AO23" s="42"/>
       <c r="AP23" s="43"/>
-      <c r="AQ23" s="102"/>
+      <c r="AQ23" s="101"/>
       <c r="AR23" s="42"/>
       <c r="AS23" s="42"/>
       <c r="AT23" s="43"/>
@@ -8050,7 +8000,9 @@
       <c r="G24" s="40" t="s">
         <v>1074</v>
       </c>
-      <c r="H24" s="37"/>
+      <c r="H24" s="110" t="s">
+        <v>1078</v>
+      </c>
       <c r="I24" s="41"/>
       <c r="J24" s="44"/>
       <c r="K24" s="25"/>
@@ -8087,7 +8039,7 @@
       <c r="AN24" s="42"/>
       <c r="AO24" s="42"/>
       <c r="AP24" s="43"/>
-      <c r="AQ24" s="102"/>
+      <c r="AQ24" s="101"/>
       <c r="AR24" s="42"/>
       <c r="AS24" s="42"/>
       <c r="AT24" s="43"/>
@@ -8123,7 +8075,9 @@
       <c r="G25" s="40" t="s">
         <v>1075</v>
       </c>
-      <c r="H25" s="37"/>
+      <c r="H25" s="110" t="s">
+        <v>1080</v>
+      </c>
       <c r="I25" s="41"/>
       <c r="J25" s="44"/>
       <c r="K25" s="25"/>
@@ -8160,7 +8114,7 @@
       <c r="AN25" s="42"/>
       <c r="AO25" s="42"/>
       <c r="AP25" s="43"/>
-      <c r="AQ25" s="102"/>
+      <c r="AQ25" s="101"/>
       <c r="AR25" s="42"/>
       <c r="AS25" s="42"/>
       <c r="AT25" s="43"/>
@@ -8189,8 +8143,12 @@
       </c>
       <c r="E26" s="25"/>
       <c r="F26" s="25"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="97"/>
+      <c r="G26" s="40" t="s">
+        <v>1079</v>
+      </c>
+      <c r="H26" s="41" t="s">
+        <v>22</v>
+      </c>
       <c r="I26" s="41" t="s">
         <v>22</v>
       </c>
@@ -8291,7 +8249,7 @@
       <c r="AP26" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AQ26" s="102"/>
+      <c r="AQ26" s="101"/>
       <c r="AR26" s="42"/>
       <c r="AS26" s="42"/>
       <c r="AT26" s="43"/>
@@ -8322,7 +8280,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="98"/>
+      <c r="H27" s="97"/>
       <c r="I27" s="5"/>
       <c r="J27" s="7"/>
       <c r="K27" s="4"/>
@@ -8357,7 +8315,7 @@
       <c r="AN27" s="8"/>
       <c r="AO27" s="8"/>
       <c r="AP27" s="6"/>
-      <c r="AQ27" s="103"/>
+      <c r="AQ27" s="102"/>
       <c r="AR27" s="8"/>
       <c r="AS27" s="8"/>
       <c r="AT27" s="6"/>
@@ -8512,62 +8470,62 @@
       <c r="G46" s="92"/>
       <c r="H46" s="92"/>
     </row>
-    <row r="48" spans="1:55" s="107" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="106"/>
-      <c r="B48" s="106"/>
-      <c r="C48" s="105" t="s">
+    <row r="48" spans="1:55" s="106" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="105"/>
+      <c r="B48" s="105"/>
+      <c r="C48" s="104" t="s">
         <v>1067</v>
       </c>
-      <c r="D48" s="106"/>
-      <c r="E48" s="106"/>
-      <c r="F48" s="106"/>
-      <c r="I48" s="106"/>
-      <c r="J48" s="106"/>
-      <c r="K48" s="106"/>
-      <c r="L48" s="106"/>
-      <c r="M48" s="106"/>
-      <c r="N48" s="106"/>
-      <c r="O48" s="106"/>
-      <c r="P48" s="106"/>
-      <c r="Q48" s="106"/>
-      <c r="R48" s="106"/>
-      <c r="S48" s="106"/>
-      <c r="T48" s="106"/>
-      <c r="U48" s="106"/>
-      <c r="V48" s="106"/>
-      <c r="W48" s="106"/>
-      <c r="X48" s="106"/>
-      <c r="Y48" s="106"/>
-      <c r="Z48" s="106"/>
-      <c r="AA48" s="106"/>
-      <c r="AB48" s="106"/>
-      <c r="AC48" s="106"/>
-      <c r="AD48" s="106"/>
-      <c r="AE48" s="106"/>
-      <c r="AF48" s="106"/>
-      <c r="AG48" s="106"/>
-      <c r="AH48" s="106"/>
-      <c r="AI48" s="106"/>
-      <c r="AJ48" s="106"/>
-      <c r="AK48" s="106"/>
-      <c r="AL48" s="106"/>
-      <c r="AM48" s="106"/>
-      <c r="AN48" s="106"/>
-      <c r="AO48" s="106"/>
-      <c r="AP48" s="106"/>
-      <c r="AQ48" s="106"/>
-      <c r="AR48" s="106"/>
-      <c r="AS48" s="106"/>
-      <c r="AT48" s="106"/>
-      <c r="AU48" s="106"/>
-      <c r="AV48" s="108"/>
-      <c r="AW48" s="109"/>
-      <c r="AX48" s="106"/>
-      <c r="AY48" s="106"/>
-      <c r="AZ48" s="108"/>
-      <c r="BA48" s="108"/>
-      <c r="BB48" s="108"/>
-      <c r="BC48" s="106"/>
+      <c r="D48" s="105"/>
+      <c r="E48" s="105"/>
+      <c r="F48" s="105"/>
+      <c r="I48" s="105"/>
+      <c r="J48" s="105"/>
+      <c r="K48" s="105"/>
+      <c r="L48" s="105"/>
+      <c r="M48" s="105"/>
+      <c r="N48" s="105"/>
+      <c r="O48" s="105"/>
+      <c r="P48" s="105"/>
+      <c r="Q48" s="105"/>
+      <c r="R48" s="105"/>
+      <c r="S48" s="105"/>
+      <c r="T48" s="105"/>
+      <c r="U48" s="105"/>
+      <c r="V48" s="105"/>
+      <c r="W48" s="105"/>
+      <c r="X48" s="105"/>
+      <c r="Y48" s="105"/>
+      <c r="Z48" s="105"/>
+      <c r="AA48" s="105"/>
+      <c r="AB48" s="105"/>
+      <c r="AC48" s="105"/>
+      <c r="AD48" s="105"/>
+      <c r="AE48" s="105"/>
+      <c r="AF48" s="105"/>
+      <c r="AG48" s="105"/>
+      <c r="AH48" s="105"/>
+      <c r="AI48" s="105"/>
+      <c r="AJ48" s="105"/>
+      <c r="AK48" s="105"/>
+      <c r="AL48" s="105"/>
+      <c r="AM48" s="105"/>
+      <c r="AN48" s="105"/>
+      <c r="AO48" s="105"/>
+      <c r="AP48" s="105"/>
+      <c r="AQ48" s="105"/>
+      <c r="AR48" s="105"/>
+      <c r="AS48" s="105"/>
+      <c r="AT48" s="105"/>
+      <c r="AU48" s="105"/>
+      <c r="AV48" s="107"/>
+      <c r="AW48" s="108"/>
+      <c r="AX48" s="105"/>
+      <c r="AY48" s="105"/>
+      <c r="AZ48" s="107"/>
+      <c r="BA48" s="107"/>
+      <c r="BB48" s="107"/>
+      <c r="BC48" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -8580,7 +8538,7 @@
     <mergeCell ref="AK2:AP2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="A4:B31 G4:H29 C4:F30 I4:BC31">
+  <conditionalFormatting sqref="A4:B31 C4:F30 I4:BC31 G4:H29">
     <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>

</xml_diff>

<commit_message>
+ renamed certtest 20,21,22  to 22,23,24 so Jason can add 2 more offshore tests and have them in order of increasing depth + updated HydroDyn input files so that it doesn't generate its own output files. + specified the units on UJacSclFact in the FAST input files + added code in matlab conversion script to convert the ServoDyn input switches that indicated the bladed dll would be used (if compiled for BladedDLLInterface) [not tested]
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@531 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -34,7 +34,7 @@
     <definedName name="_Toc46290868" localSheetId="1">Variables!$B$759</definedName>
     <definedName name="_Toc46290869" localSheetId="1">Variables!$B$770</definedName>
     <definedName name="_Toc46290870" localSheetId="1">Variables!$B$781</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">TestMatrix!$B$2:$AX$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">TestMatrix!$B$2:$AX$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Variables!$B$1:$P$855</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="1081">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="1080">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3259,12 +3259,6 @@
     <t>Test19</t>
   </si>
   <si>
-    <t>Test 20</t>
-  </si>
-  <si>
-    <t>Test 21</t>
-  </si>
-  <si>
     <t>Monopile RF</t>
   </si>
   <si>
@@ -3277,19 +3271,22 @@
     <t>Floating OC3 Hywind</t>
   </si>
   <si>
+    <t>2-bladed CART</t>
+  </si>
+  <si>
+    <t>Test 24</t>
+  </si>
+  <si>
+    <t>Test 23</t>
+  </si>
+  <si>
     <t>Test 22</t>
   </si>
   <si>
-    <t>checked</t>
-  </si>
-  <si>
-    <t>needs smaller time step to match platform heave and fairlead/anchor tensions</t>
-  </si>
-  <si>
-    <t>2-bladed CART</t>
-  </si>
-  <si>
-    <t>need to compile with changes for OC3 Hywind to check these results</t>
+    <t>Test20</t>
+  </si>
+  <si>
+    <t>Test21</t>
   </si>
 </sst>
 </file>
@@ -3320,7 +3317,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3378,6 +3375,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3940,7 +3943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4303,12 +4306,113 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -4692,13 +4796,13 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BC48"/>
+  <dimension ref="A1:BC50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5166,7 +5270,7 @@
       <c r="M5" s="25">
         <v>2</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="N5" s="130" t="s">
         <v>32</v>
       </c>
       <c r="O5" s="25" t="s">
@@ -5175,7 +5279,7 @@
       <c r="P5" s="25">
         <v>1</v>
       </c>
-      <c r="Q5" s="25" t="s">
+      <c r="Q5" s="130" t="s">
         <v>32</v>
       </c>
       <c r="R5" s="25" t="s">
@@ -5646,7 +5750,7 @@
       <c r="M8" s="25">
         <v>2</v>
       </c>
-      <c r="N8" s="25" t="s">
+      <c r="N8" s="130" t="s">
         <v>32</v>
       </c>
       <c r="O8" s="25" t="s">
@@ -5658,7 +5762,7 @@
       <c r="Q8" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="R8" s="25" t="s">
+      <c r="R8" s="130" t="s">
         <v>32</v>
       </c>
       <c r="S8" s="42" t="s">
@@ -5807,7 +5911,7 @@
       <c r="M9" s="25">
         <v>2</v>
       </c>
-      <c r="N9" s="25" t="s">
+      <c r="N9" s="130" t="s">
         <v>32</v>
       </c>
       <c r="O9" s="25" t="s">
@@ -5819,7 +5923,7 @@
       <c r="Q9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="R9" s="25" t="s">
+      <c r="R9" s="130" t="s">
         <v>32</v>
       </c>
       <c r="S9" s="42" t="s">
@@ -7709,9 +7813,7 @@
       <c r="G21" s="40" t="s">
         <v>1068</v>
       </c>
-      <c r="H21" s="110" t="s">
-        <v>1077</v>
-      </c>
+      <c r="H21" s="110"/>
       <c r="I21" s="41" t="s">
         <v>22</v>
       </c>
@@ -7728,7 +7830,7 @@
         <v>2</v>
       </c>
       <c r="N21" s="25" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="O21" s="25" t="s">
         <v>22</v>
@@ -7821,7 +7923,9 @@
       <c r="AU21" s="44"/>
       <c r="AV21" s="54"/>
       <c r="AW21" s="45"/>
-      <c r="AX21" s="43"/>
+      <c r="AX21" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="AY21" s="61"/>
       <c r="AZ21" s="62"/>
       <c r="BA21" s="64"/>
@@ -7848,15 +7952,17 @@
         <v>5000</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>1072</v>
-      </c>
-      <c r="H22" s="110" t="s">
-        <v>1077</v>
-      </c>
+        <v>1070</v>
+      </c>
+      <c r="H22" s="110"/>
       <c r="I22" s="41"/>
       <c r="J22" s="44"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
+      <c r="K22" s="25">
+        <v>5</v>
+      </c>
+      <c r="L22" s="25">
+        <v>5</v>
+      </c>
       <c r="M22" s="25"/>
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
@@ -7896,7 +8002,9 @@
       <c r="AU22" s="44"/>
       <c r="AV22" s="54"/>
       <c r="AW22" s="45"/>
-      <c r="AX22" s="43"/>
+      <c r="AX22" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="AY22" s="61"/>
       <c r="AZ22" s="62"/>
       <c r="BA22" s="64"/>
@@ -7908,7 +8016,7 @@
     <row r="23" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="87" t="s">
-        <v>1070</v>
+        <v>1078</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>1063</v>
@@ -7922,16 +8030,16 @@
       <c r="F23" s="25">
         <v>5000</v>
       </c>
-      <c r="G23" s="40" t="s">
-        <v>1073</v>
-      </c>
-      <c r="H23" s="110" t="s">
-        <v>1077</v>
-      </c>
+      <c r="G23" s="40"/>
+      <c r="H23" s="110"/>
       <c r="I23" s="41"/>
       <c r="J23" s="44"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
+      <c r="K23" s="25">
+        <v>5</v>
+      </c>
+      <c r="L23" s="25">
+        <v>5</v>
+      </c>
       <c r="M23" s="25"/>
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
@@ -7953,9 +8061,7 @@
       <c r="AE23" s="25"/>
       <c r="AF23" s="25"/>
       <c r="AG23" s="25"/>
-      <c r="AH23" s="25" t="s">
-        <v>28</v>
-      </c>
+      <c r="AH23" s="25"/>
       <c r="AI23" s="25"/>
       <c r="AJ23" s="43"/>
       <c r="AK23" s="44"/>
@@ -7975,15 +8081,13 @@
       <c r="AY23" s="61"/>
       <c r="AZ23" s="62"/>
       <c r="BA23" s="64"/>
-      <c r="BB23" s="64" t="s">
-        <v>1052</v>
-      </c>
+      <c r="BB23" s="64"/>
       <c r="BC23" s="43"/>
     </row>
     <row r="24" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="87" t="s">
-        <v>1071</v>
+        <v>1079</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>1063</v>
@@ -7997,16 +8101,16 @@
       <c r="F24" s="25">
         <v>5000</v>
       </c>
-      <c r="G24" s="40" t="s">
-        <v>1074</v>
-      </c>
-      <c r="H24" s="110" t="s">
-        <v>1078</v>
-      </c>
+      <c r="G24" s="40"/>
+      <c r="H24" s="110"/>
       <c r="I24" s="41"/>
       <c r="J24" s="44"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
+      <c r="K24" s="25">
+        <v>5</v>
+      </c>
+      <c r="L24" s="25">
+        <v>5</v>
+      </c>
       <c r="M24" s="25"/>
       <c r="N24" s="25"/>
       <c r="O24" s="25"/>
@@ -8028,9 +8132,7 @@
       <c r="AE24" s="25"/>
       <c r="AF24" s="25"/>
       <c r="AG24" s="25"/>
-      <c r="AH24" s="25" t="s">
-        <v>28</v>
-      </c>
+      <c r="AH24" s="25"/>
       <c r="AI24" s="25"/>
       <c r="AJ24" s="43"/>
       <c r="AK24" s="44"/>
@@ -8050,15 +8152,13 @@
       <c r="AY24" s="61"/>
       <c r="AZ24" s="62"/>
       <c r="BA24" s="64"/>
-      <c r="BB24" s="64" t="s">
-        <v>1052</v>
-      </c>
+      <c r="BB24" s="64"/>
       <c r="BC24" s="43"/>
     </row>
     <row r="25" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="87" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>1063</v>
@@ -8073,15 +8173,17 @@
         <v>5000</v>
       </c>
       <c r="G25" s="40" t="s">
-        <v>1075</v>
-      </c>
-      <c r="H25" s="110" t="s">
-        <v>1080</v>
-      </c>
+        <v>1071</v>
+      </c>
+      <c r="H25" s="110"/>
       <c r="I25" s="41"/>
       <c r="J25" s="44"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
+      <c r="K25" s="25">
+        <v>5</v>
+      </c>
+      <c r="L25" s="25">
+        <v>5</v>
+      </c>
       <c r="M25" s="25"/>
       <c r="N25" s="25"/>
       <c r="O25" s="25"/>
@@ -8121,7 +8223,9 @@
       <c r="AU25" s="44"/>
       <c r="AV25" s="54"/>
       <c r="AW25" s="45"/>
-      <c r="AX25" s="43"/>
+      <c r="AX25" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="AY25" s="61"/>
       <c r="AZ25" s="62"/>
       <c r="BA25" s="64"/>
@@ -8131,401 +8235,559 @@
       <c r="BC25" s="43"/>
     </row>
     <row r="26" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
-        <v>286</v>
-      </c>
-      <c r="B26" s="41"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="87" t="s">
+        <v>1076</v>
+      </c>
       <c r="C26" s="25" t="s">
-        <v>55</v>
+        <v>1063</v>
       </c>
       <c r="D26" s="25">
-        <v>2</v>
-      </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
+        <v>3</v>
+      </c>
+      <c r="E26" s="25">
+        <v>126</v>
+      </c>
+      <c r="F26" s="25">
+        <v>5000</v>
+      </c>
       <c r="G26" s="40" t="s">
-        <v>1079</v>
-      </c>
-      <c r="H26" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="J26" s="44">
-        <v>0</v>
-      </c>
+        <v>1072</v>
+      </c>
+      <c r="H26" s="110"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="44"/>
       <c r="K26" s="25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L26" s="25">
-        <v>0</v>
-      </c>
-      <c r="M26" s="25">
-        <v>1</v>
-      </c>
-      <c r="N26" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="O26" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="P26" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="R26" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="S26" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="T26" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="U26" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="42"/>
+      <c r="T26" s="42"/>
+      <c r="U26" s="41"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="25"/>
+      <c r="X26" s="25"/>
+      <c r="Y26" s="25"/>
+      <c r="Z26" s="25"/>
+      <c r="AA26" s="25"/>
+      <c r="AB26" s="25"/>
+      <c r="AC26" s="25"/>
+      <c r="AD26" s="25"/>
+      <c r="AE26" s="25"/>
+      <c r="AF26" s="25"/>
+      <c r="AG26" s="25"/>
+      <c r="AH26" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="V26" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="W26" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="X26" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y26" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z26" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA26" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB26" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC26" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD26" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE26" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF26" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG26" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH26" s="25"/>
-      <c r="AI26" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ26" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK26" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL26" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM26" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="AN26" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="AO26" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP26" s="43" t="s">
-        <v>32</v>
-      </c>
+      <c r="AI26" s="25"/>
+      <c r="AJ26" s="43"/>
+      <c r="AK26" s="44"/>
+      <c r="AL26" s="25"/>
+      <c r="AM26" s="42"/>
+      <c r="AN26" s="42"/>
+      <c r="AO26" s="42"/>
+      <c r="AP26" s="43"/>
       <c r="AQ26" s="101"/>
       <c r="AR26" s="42"/>
       <c r="AS26" s="42"/>
       <c r="AT26" s="43"/>
-      <c r="AU26" s="44" t="s">
+      <c r="AU26" s="44"/>
+      <c r="AV26" s="54"/>
+      <c r="AW26" s="45"/>
+      <c r="AX26" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AV26" s="48" t="s">
+      <c r="AY26" s="61"/>
+      <c r="AZ26" s="62"/>
+      <c r="BA26" s="64"/>
+      <c r="BB26" s="64" t="s">
+        <v>1052</v>
+      </c>
+      <c r="BC26" s="43"/>
+    </row>
+    <row r="27" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="27"/>
+      <c r="B27" s="87" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D27" s="25">
+        <v>3</v>
+      </c>
+      <c r="E27" s="25">
+        <v>126</v>
+      </c>
+      <c r="F27" s="25">
+        <v>5000</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H27" s="110"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="25">
+        <v>5</v>
+      </c>
+      <c r="L27" s="25">
+        <v>5</v>
+      </c>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="42"/>
+      <c r="T27" s="42"/>
+      <c r="U27" s="41"/>
+      <c r="V27" s="25"/>
+      <c r="W27" s="25"/>
+      <c r="X27" s="25"/>
+      <c r="Y27" s="25"/>
+      <c r="Z27" s="25"/>
+      <c r="AA27" s="25"/>
+      <c r="AB27" s="25"/>
+      <c r="AC27" s="25"/>
+      <c r="AD27" s="25"/>
+      <c r="AE27" s="25"/>
+      <c r="AF27" s="25"/>
+      <c r="AG27" s="25"/>
+      <c r="AH27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI27" s="25"/>
+      <c r="AJ27" s="43"/>
+      <c r="AK27" s="44"/>
+      <c r="AL27" s="25"/>
+      <c r="AM27" s="42"/>
+      <c r="AN27" s="42"/>
+      <c r="AO27" s="42"/>
+      <c r="AP27" s="43"/>
+      <c r="AQ27" s="101"/>
+      <c r="AR27" s="42"/>
+      <c r="AS27" s="42"/>
+      <c r="AT27" s="43"/>
+      <c r="AU27" s="44"/>
+      <c r="AV27" s="54"/>
+      <c r="AW27" s="45"/>
+      <c r="AX27" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AY27" s="61"/>
+      <c r="AZ27" s="62"/>
+      <c r="BA27" s="64"/>
+      <c r="BB27" s="64" t="s">
+        <v>1052</v>
+      </c>
+      <c r="BC27" s="43"/>
+    </row>
+    <row r="28" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="B28" s="41"/>
+      <c r="C28" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="25">
+        <v>2</v>
+      </c>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="40" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H28" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="44">
+        <v>0</v>
+      </c>
+      <c r="K28" s="25">
+        <v>0</v>
+      </c>
+      <c r="L28" s="25">
+        <v>0</v>
+      </c>
+      <c r="M28" s="25">
+        <v>1</v>
+      </c>
+      <c r="N28" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="O28" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="P28" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="R28" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="S28" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="T28" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="U28" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="V28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="W28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="X28" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA28" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB28" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH28" s="25"/>
+      <c r="AI28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ28" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK28" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL28" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM28" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN28" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO28" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP28" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ28" s="101"/>
+      <c r="AR28" s="42"/>
+      <c r="AS28" s="42"/>
+      <c r="AT28" s="43"/>
+      <c r="AU28" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV28" s="48" t="s">
         <v>287</v>
       </c>
-      <c r="AW26" s="45">
+      <c r="AW28" s="45">
         <v>0.2</v>
       </c>
-      <c r="AX26" s="43" t="s">
+      <c r="AX28" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AY26" s="44"/>
-      <c r="AZ26" s="48"/>
-      <c r="BA26" s="65"/>
-      <c r="BB26" s="65"/>
-      <c r="BC26" s="43" t="s">
+      <c r="AY28" s="44"/>
+      <c r="AZ28" s="48"/>
+      <c r="BA28" s="65"/>
+      <c r="BB28" s="65"/>
+      <c r="BC28" s="43" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="27" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="97"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="5"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
-      <c r="AA27" s="4"/>
-      <c r="AB27" s="4"/>
-      <c r="AC27" s="4"/>
-      <c r="AD27" s="4"/>
-      <c r="AE27" s="4"/>
-      <c r="AF27" s="4"/>
-      <c r="AG27" s="4"/>
-      <c r="AH27" s="4"/>
-      <c r="AI27" s="4"/>
-      <c r="AJ27" s="6"/>
-      <c r="AK27" s="7"/>
-      <c r="AL27" s="4"/>
-      <c r="AM27" s="8"/>
-      <c r="AN27" s="8"/>
-      <c r="AO27" s="8"/>
-      <c r="AP27" s="6"/>
-      <c r="AQ27" s="102"/>
-      <c r="AR27" s="8"/>
-      <c r="AS27" s="8"/>
-      <c r="AT27" s="6"/>
-      <c r="AU27" s="7"/>
-      <c r="AV27" s="49"/>
-      <c r="AW27" s="10"/>
-      <c r="AX27" s="6"/>
-      <c r="AY27" s="7"/>
-      <c r="AZ27" s="49"/>
-      <c r="BA27" s="66"/>
-      <c r="BB27" s="66"/>
-      <c r="BC27" s="6"/>
-    </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="B29" s="50" t="s">
+    <row r="29" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="97"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="4"/>
+      <c r="AF29" s="4"/>
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="4"/>
+      <c r="AI29" s="4"/>
+      <c r="AJ29" s="6"/>
+      <c r="AK29" s="7"/>
+      <c r="AL29" s="4"/>
+      <c r="AM29" s="8"/>
+      <c r="AN29" s="8"/>
+      <c r="AO29" s="8"/>
+      <c r="AP29" s="6"/>
+      <c r="AQ29" s="102"/>
+      <c r="AR29" s="8"/>
+      <c r="AS29" s="8"/>
+      <c r="AT29" s="6"/>
+      <c r="AU29" s="7"/>
+      <c r="AV29" s="49"/>
+      <c r="AW29" s="10"/>
+      <c r="AX29" s="6"/>
+      <c r="AY29" s="7"/>
+      <c r="AZ29" s="49"/>
+      <c r="BA29" s="66"/>
+      <c r="BB29" s="66"/>
+      <c r="BC29" s="6"/>
+    </row>
+    <row r="31" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B31" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-    </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="B30" s="50"/>
-      <c r="C30" s="11" t="s">
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+    </row>
+    <row r="32" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B32" s="50"/>
+      <c r="C32" s="11" t="s">
         <v>307</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-    </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="B31" s="12"/>
-      <c r="C31" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-    </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="B32" s="12"/>
-      <c r="C32" s="11" t="s">
-        <v>308</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B33" s="12"/>
-      <c r="C33" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-    </row>
-    <row r="34" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="C33" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B34" s="12"/>
       <c r="C34" s="11" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
-      <c r="T34" s="11"/>
-    </row>
-    <row r="35" spans="1:55" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B35" s="12"/>
       <c r="C35" s="11" t="s">
-        <v>295</v>
+        <v>50</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
     </row>
-    <row r="36" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B36" s="12"/>
       <c r="C36" s="11" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
-    </row>
-    <row r="37" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="T36" s="11"/>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C37" s="11" t="s">
-        <v>343</v>
+        <v>295</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C38" s="11" t="s">
-        <v>339</v>
+        <v>300</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
     </row>
-    <row r="39" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C39" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
     </row>
-    <row r="40" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C40" s="11" t="s">
-        <v>443</v>
+        <v>339</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
     </row>
-    <row r="41" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C41" s="11" t="s">
-        <v>444</v>
+        <v>342</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
     </row>
-    <row r="42" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C42" s="11" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
     </row>
-    <row r="43" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="C43" s="12" t="s">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C43" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C44" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C45" s="12" t="s">
         <v>668</v>
       </c>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-    </row>
-    <row r="44" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-    </row>
-    <row r="46" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="B46" s="90" t="s">
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B48" s="90" t="s">
         <v>1054</v>
       </c>
-      <c r="C46" s="91"/>
-      <c r="D46" s="91"/>
-      <c r="E46" s="91"/>
-      <c r="F46" s="91"/>
-      <c r="G46" s="92"/>
-      <c r="H46" s="92"/>
-    </row>
-    <row r="48" spans="1:55" s="106" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="105"/>
-      <c r="B48" s="105"/>
-      <c r="C48" s="104" t="s">
+      <c r="C48" s="91"/>
+      <c r="D48" s="91"/>
+      <c r="E48" s="91"/>
+      <c r="F48" s="91"/>
+      <c r="G48" s="92"/>
+      <c r="H48" s="92"/>
+    </row>
+    <row r="50" spans="1:55" s="106" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="105"/>
+      <c r="B50" s="105"/>
+      <c r="C50" s="104" t="s">
         <v>1067</v>
       </c>
-      <c r="D48" s="105"/>
-      <c r="E48" s="105"/>
-      <c r="F48" s="105"/>
-      <c r="I48" s="105"/>
-      <c r="J48" s="105"/>
-      <c r="K48" s="105"/>
-      <c r="L48" s="105"/>
-      <c r="M48" s="105"/>
-      <c r="N48" s="105"/>
-      <c r="O48" s="105"/>
-      <c r="P48" s="105"/>
-      <c r="Q48" s="105"/>
-      <c r="R48" s="105"/>
-      <c r="S48" s="105"/>
-      <c r="T48" s="105"/>
-      <c r="U48" s="105"/>
-      <c r="V48" s="105"/>
-      <c r="W48" s="105"/>
-      <c r="X48" s="105"/>
-      <c r="Y48" s="105"/>
-      <c r="Z48" s="105"/>
-      <c r="AA48" s="105"/>
-      <c r="AB48" s="105"/>
-      <c r="AC48" s="105"/>
-      <c r="AD48" s="105"/>
-      <c r="AE48" s="105"/>
-      <c r="AF48" s="105"/>
-      <c r="AG48" s="105"/>
-      <c r="AH48" s="105"/>
-      <c r="AI48" s="105"/>
-      <c r="AJ48" s="105"/>
-      <c r="AK48" s="105"/>
-      <c r="AL48" s="105"/>
-      <c r="AM48" s="105"/>
-      <c r="AN48" s="105"/>
-      <c r="AO48" s="105"/>
-      <c r="AP48" s="105"/>
-      <c r="AQ48" s="105"/>
-      <c r="AR48" s="105"/>
-      <c r="AS48" s="105"/>
-      <c r="AT48" s="105"/>
-      <c r="AU48" s="105"/>
-      <c r="AV48" s="107"/>
-      <c r="AW48" s="108"/>
-      <c r="AX48" s="105"/>
-      <c r="AY48" s="105"/>
-      <c r="AZ48" s="107"/>
-      <c r="BA48" s="107"/>
-      <c r="BB48" s="107"/>
-      <c r="BC48" s="105"/>
+      <c r="D50" s="105"/>
+      <c r="E50" s="105"/>
+      <c r="F50" s="105"/>
+      <c r="I50" s="105"/>
+      <c r="J50" s="105"/>
+      <c r="K50" s="105"/>
+      <c r="L50" s="105"/>
+      <c r="M50" s="105"/>
+      <c r="N50" s="105"/>
+      <c r="O50" s="105"/>
+      <c r="P50" s="105"/>
+      <c r="Q50" s="105"/>
+      <c r="R50" s="105"/>
+      <c r="S50" s="105"/>
+      <c r="T50" s="105"/>
+      <c r="U50" s="105"/>
+      <c r="V50" s="105"/>
+      <c r="W50" s="105"/>
+      <c r="X50" s="105"/>
+      <c r="Y50" s="105"/>
+      <c r="Z50" s="105"/>
+      <c r="AA50" s="105"/>
+      <c r="AB50" s="105"/>
+      <c r="AC50" s="105"/>
+      <c r="AD50" s="105"/>
+      <c r="AE50" s="105"/>
+      <c r="AF50" s="105"/>
+      <c r="AG50" s="105"/>
+      <c r="AH50" s="105"/>
+      <c r="AI50" s="105"/>
+      <c r="AJ50" s="105"/>
+      <c r="AK50" s="105"/>
+      <c r="AL50" s="105"/>
+      <c r="AM50" s="105"/>
+      <c r="AN50" s="105"/>
+      <c r="AO50" s="105"/>
+      <c r="AP50" s="105"/>
+      <c r="AQ50" s="105"/>
+      <c r="AR50" s="105"/>
+      <c r="AS50" s="105"/>
+      <c r="AT50" s="105"/>
+      <c r="AU50" s="105"/>
+      <c r="AV50" s="107"/>
+      <c r="AW50" s="108"/>
+      <c r="AX50" s="105"/>
+      <c r="AY50" s="105"/>
+      <c r="AZ50" s="107"/>
+      <c r="BA50" s="107"/>
+      <c r="BB50" s="107"/>
+      <c r="BC50" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -8538,11 +8800,11 @@
     <mergeCell ref="AK2:AP2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="A4:B31 C4:F30 I4:BC31 G4:H29">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="A4:B33 G4:H31 C4:F32 I4:BC33">
+    <cfRule type="expression" dxfId="22" priority="9" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="10" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39988,31 +40250,31 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="C782:C787 C844:C855 C789:C842">
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="1" stopIfTrue="1">
       <formula>$A782=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="2" stopIfTrue="1">
       <formula>$A782=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B336:C353 B764:C769 B301:C303 B4:C10 B297:C299 B38:C49 B25:C36 B496:C528 B12:C23 B844:B855 B315:C326 B530:C539 B541:C550 B728:C743 B745:C748 B750:C758 B332:C334 B771:C780 B328:C330 B760:C760 B762:C762 B305:C313 B355:C358 B782:B787 B552:C561 B51:C131 B133:C213 B215:C295 B360:C494 B563:C616 B673:C726 B618:C671 B789:B842">
-    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="3" stopIfTrue="1">
       <formula>$A4=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="4" stopIfTrue="1">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2 D2:Z2">
-    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A10 A12:A23 A25:A36 A38:A49 A297:A299 A301:A303 A305:A313 A315:A326 A328:A330 A332:A334 A336:A353 A355:A358 A496:A528 A530:A539 A541:A550 A552:A561 A745:A748 A750:A758 A760 A762 A764:A769 A771:A780 A782:A787 A844:A855 A51:A131 A133:A213 A215:A295 A360:A494 A563:A616 A673:A726 A618:A671 A728:A743 A789:A842">
-    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
+ Updated certtest/TstFiles. Had to modify my IVF optimization settings because of strange behavior in Release mode (test 7 gave NaNs in the output after 25.3 s though it ran to completion). Will need to figure that out... + updated labels in map input files + modified compile_fast to run on other people's machines (registry had issues with my personal paths) + made some improvements in certtest.bat + fixed typo in FAST input files + added check that TeetCDm wasn't allowed in ED + updated warning text about BladedDLLInterface in SrvD
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@535 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="1080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2159" uniqueCount="1080">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -4249,6 +4249,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4306,113 +4309,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <condense val="0"/>
@@ -4799,7 +4701,7 @@
   <dimension ref="A1:BC50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight"/>
@@ -4842,74 +4744,74 @@
   <sheetData>
     <row r="1" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="117" t="s">
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="118" t="s">
         <v>1065</v>
       </c>
-      <c r="J2" s="118"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="126"/>
-      <c r="O2" s="126"/>
-      <c r="P2" s="126"/>
-      <c r="Q2" s="126"/>
-      <c r="R2" s="126"/>
-      <c r="S2" s="126"/>
-      <c r="T2" s="127"/>
-      <c r="U2" s="120" t="s">
+      <c r="J2" s="119"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="127"/>
+      <c r="M2" s="127"/>
+      <c r="N2" s="127"/>
+      <c r="O2" s="127"/>
+      <c r="P2" s="127"/>
+      <c r="Q2" s="127"/>
+      <c r="R2" s="127"/>
+      <c r="S2" s="127"/>
+      <c r="T2" s="128"/>
+      <c r="U2" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="121"/>
-      <c r="W2" s="121"/>
-      <c r="X2" s="121"/>
-      <c r="Y2" s="121"/>
-      <c r="Z2" s="121"/>
-      <c r="AA2" s="121"/>
-      <c r="AB2" s="121"/>
-      <c r="AC2" s="121"/>
-      <c r="AD2" s="121"/>
-      <c r="AE2" s="121"/>
-      <c r="AF2" s="121"/>
-      <c r="AG2" s="121"/>
-      <c r="AH2" s="121"/>
-      <c r="AI2" s="121"/>
-      <c r="AJ2" s="122"/>
-      <c r="AK2" s="114" t="s">
+      <c r="V2" s="122"/>
+      <c r="W2" s="122"/>
+      <c r="X2" s="122"/>
+      <c r="Y2" s="122"/>
+      <c r="Z2" s="122"/>
+      <c r="AA2" s="122"/>
+      <c r="AB2" s="122"/>
+      <c r="AC2" s="122"/>
+      <c r="AD2" s="122"/>
+      <c r="AE2" s="122"/>
+      <c r="AF2" s="122"/>
+      <c r="AG2" s="122"/>
+      <c r="AH2" s="122"/>
+      <c r="AI2" s="122"/>
+      <c r="AJ2" s="123"/>
+      <c r="AK2" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="128"/>
-      <c r="AM2" s="128"/>
-      <c r="AN2" s="128"/>
-      <c r="AO2" s="128"/>
-      <c r="AP2" s="129"/>
-      <c r="AQ2" s="114" t="s">
+      <c r="AL2" s="129"/>
+      <c r="AM2" s="129"/>
+      <c r="AN2" s="129"/>
+      <c r="AO2" s="129"/>
+      <c r="AP2" s="130"/>
+      <c r="AQ2" s="115" t="s">
         <v>1064</v>
       </c>
-      <c r="AR2" s="115"/>
-      <c r="AS2" s="115"/>
-      <c r="AT2" s="116"/>
-      <c r="AU2" s="123" t="s">
+      <c r="AR2" s="116"/>
+      <c r="AS2" s="116"/>
+      <c r="AT2" s="117"/>
+      <c r="AU2" s="124" t="s">
         <v>18</v>
       </c>
-      <c r="AV2" s="124"/>
-      <c r="AW2" s="124"/>
-      <c r="AX2" s="125"/>
-      <c r="AY2" s="117" t="s">
+      <c r="AV2" s="125"/>
+      <c r="AW2" s="125"/>
+      <c r="AX2" s="126"/>
+      <c r="AY2" s="118" t="s">
         <v>1049</v>
       </c>
-      <c r="AZ2" s="118"/>
-      <c r="BA2" s="118"/>
-      <c r="BB2" s="118"/>
-      <c r="BC2" s="119"/>
+      <c r="AZ2" s="119"/>
+      <c r="BA2" s="119"/>
+      <c r="BB2" s="119"/>
+      <c r="BC2" s="120"/>
     </row>
     <row r="3" spans="1:55" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -5270,7 +5172,7 @@
       <c r="M5" s="25">
         <v>2</v>
       </c>
-      <c r="N5" s="130" t="s">
+      <c r="N5" s="111" t="s">
         <v>32</v>
       </c>
       <c r="O5" s="25" t="s">
@@ -5279,7 +5181,7 @@
       <c r="P5" s="25">
         <v>1</v>
       </c>
-      <c r="Q5" s="130" t="s">
+      <c r="Q5" s="111" t="s">
         <v>32</v>
       </c>
       <c r="R5" s="25" t="s">
@@ -5750,7 +5652,7 @@
       <c r="M8" s="25">
         <v>2</v>
       </c>
-      <c r="N8" s="130" t="s">
+      <c r="N8" s="111" t="s">
         <v>32</v>
       </c>
       <c r="O8" s="25" t="s">
@@ -5762,7 +5664,7 @@
       <c r="Q8" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="R8" s="130" t="s">
+      <c r="R8" s="111" t="s">
         <v>32</v>
       </c>
       <c r="S8" s="42" t="s">
@@ -5911,7 +5813,7 @@
       <c r="M9" s="25">
         <v>2</v>
       </c>
-      <c r="N9" s="130" t="s">
+      <c r="N9" s="111" t="s">
         <v>32</v>
       </c>
       <c r="O9" s="25" t="s">
@@ -5923,7 +5825,7 @@
       <c r="Q9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="R9" s="130" t="s">
+      <c r="R9" s="111" t="s">
         <v>32</v>
       </c>
       <c r="S9" s="42" t="s">
@@ -7813,7 +7715,9 @@
       <c r="G21" s="40" t="s">
         <v>1068</v>
       </c>
-      <c r="H21" s="110"/>
+      <c r="H21" s="110" t="s">
+        <v>22</v>
+      </c>
       <c r="I21" s="41" t="s">
         <v>22</v>
       </c>
@@ -8801,10 +8705,10 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A4:B33 G4:H31 C4:F32 I4:BC33">
-    <cfRule type="expression" dxfId="22" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40250,31 +40154,31 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="C782:C787 C844:C855 C789:C842">
-    <cfRule type="expression" dxfId="20" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>$A782=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
       <formula>$A782=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B336:C353 B764:C769 B301:C303 B4:C10 B297:C299 B38:C49 B25:C36 B496:C528 B12:C23 B844:B855 B315:C326 B530:C539 B541:C550 B728:C743 B745:C748 B750:C758 B332:C334 B771:C780 B328:C330 B760:C760 B762:C762 B305:C313 B355:C358 B782:B787 B552:C561 B51:C131 B133:C213 B215:C295 B360:C494 B563:C616 B673:C726 B618:C671 B789:B842">
-    <cfRule type="expression" dxfId="18" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>$A4=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2 D2:Z2">
-    <cfRule type="cellIs" dxfId="16" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A10 A12:A23 A25:A36 A38:A49 A297:A299 A301:A303 A305:A313 A315:A326 A328:A330 A332:A334 A336:A353 A355:A358 A496:A528 A530:A539 A541:A550 A552:A561 A745:A748 A750:A758 A760 A762 A764:A769 A771:A780 A782:A787 A844:A855 A51:A131 A133:A213 A215:A295 A360:A494 A563:A616 A673:A726 A618:A671 A728:A743 A789:A842">
-    <cfRule type="cellIs" dxfId="15" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
- I renamed several of the CertTest files     + 5MW tower files are now called {configuration}_ElastDyn_Tower.ipt);     + I removed the "Floating" from "Floating_OC3Hywind" - I added test 21 (OC4 Jacket) to SVN, but it needs some work (doesn't run properly, yet) + I modified the output format for Crunch stats on a couple of tests.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@575 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2159" uniqueCount="1080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2160" uniqueCount="1081">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3287,6 +3287,9 @@
   </si>
   <si>
     <t>Test21</t>
+  </si>
+  <si>
+    <t>OC4 Jacket</t>
   </si>
 </sst>
 </file>
@@ -4704,7 +4707,7 @@
       <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8005,7 +8008,9 @@
       <c r="F24" s="25">
         <v>5000</v>
       </c>
-      <c r="G24" s="40"/>
+      <c r="G24" s="40" t="s">
+        <v>1080</v>
+      </c>
       <c r="H24" s="110"/>
       <c r="I24" s="41"/>
       <c r="J24" s="44"/>

</xml_diff>

<commit_message>
+ updated input files with "default" time steps + removed unnecessary input files (with this new option) + moved all the adams input files into a separate folder (we can't use them now anyway) + updated the v8.3 results for test18, using the corrected AD tower input file (it had NTwrR set incorrectly)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@626 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="2730" windowWidth="15180" windowHeight="8775" tabRatio="712"/>
+    <workbookView xWindow="5955" yWindow="2790" windowWidth="15180" windowHeight="8715" tabRatio="712"/>
   </bookViews>
   <sheets>
     <sheet name="TestMatrix" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,16 @@
     <definedName name="_Toc46290868" localSheetId="1">Variables!$B$759</definedName>
     <definedName name="_Toc46290869" localSheetId="1">Variables!$B$770</definedName>
     <definedName name="_Toc46290870" localSheetId="1">Variables!$B$781</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">TestMatrix!$B$2:$AX$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">TestMatrix!$B$2:$AX$36</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Variables!$B$1:$P$855</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2160" uniqueCount="1081">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="1084">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3268,9 +3269,6 @@
     <t>Floating TLP</t>
   </si>
   <si>
-    <t>Floating OC3 Hywind</t>
-  </si>
-  <si>
     <t>2-bladed CART</t>
   </si>
   <si>
@@ -3290,6 +3288,18 @@
   </si>
   <si>
     <t>OC4 Jacket</t>
+  </si>
+  <si>
+    <t>OC3 Hywind (floating)</t>
+  </si>
+  <si>
+    <t>Semi</t>
+  </si>
+  <si>
+    <t>Tripod</t>
+  </si>
+  <si>
+    <t>Test 25</t>
   </si>
 </sst>
 </file>
@@ -3946,7 +3956,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4255,6 +4265,9 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4317,7 +4330,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
     <dxf>
       <font>
         <condense val="0"/>
@@ -4386,6 +4399,20 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -4701,13 +4728,13 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BC50"/>
+  <dimension ref="A1:BC51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4747,74 +4774,74 @@
   <sheetData>
     <row r="1" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="118" t="s">
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="119" t="s">
         <v>1065</v>
       </c>
-      <c r="J2" s="119"/>
-      <c r="K2" s="127"/>
-      <c r="L2" s="127"/>
-      <c r="M2" s="127"/>
-      <c r="N2" s="127"/>
-      <c r="O2" s="127"/>
-      <c r="P2" s="127"/>
-      <c r="Q2" s="127"/>
-      <c r="R2" s="127"/>
-      <c r="S2" s="127"/>
-      <c r="T2" s="128"/>
-      <c r="U2" s="121" t="s">
+      <c r="J2" s="120"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="128"/>
+      <c r="N2" s="128"/>
+      <c r="O2" s="128"/>
+      <c r="P2" s="128"/>
+      <c r="Q2" s="128"/>
+      <c r="R2" s="128"/>
+      <c r="S2" s="128"/>
+      <c r="T2" s="129"/>
+      <c r="U2" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="122"/>
-      <c r="W2" s="122"/>
-      <c r="X2" s="122"/>
-      <c r="Y2" s="122"/>
-      <c r="Z2" s="122"/>
-      <c r="AA2" s="122"/>
-      <c r="AB2" s="122"/>
-      <c r="AC2" s="122"/>
-      <c r="AD2" s="122"/>
-      <c r="AE2" s="122"/>
-      <c r="AF2" s="122"/>
-      <c r="AG2" s="122"/>
-      <c r="AH2" s="122"/>
-      <c r="AI2" s="122"/>
-      <c r="AJ2" s="123"/>
-      <c r="AK2" s="115" t="s">
+      <c r="V2" s="123"/>
+      <c r="W2" s="123"/>
+      <c r="X2" s="123"/>
+      <c r="Y2" s="123"/>
+      <c r="Z2" s="123"/>
+      <c r="AA2" s="123"/>
+      <c r="AB2" s="123"/>
+      <c r="AC2" s="123"/>
+      <c r="AD2" s="123"/>
+      <c r="AE2" s="123"/>
+      <c r="AF2" s="123"/>
+      <c r="AG2" s="123"/>
+      <c r="AH2" s="123"/>
+      <c r="AI2" s="123"/>
+      <c r="AJ2" s="124"/>
+      <c r="AK2" s="116" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="129"/>
-      <c r="AM2" s="129"/>
-      <c r="AN2" s="129"/>
-      <c r="AO2" s="129"/>
-      <c r="AP2" s="130"/>
-      <c r="AQ2" s="115" t="s">
+      <c r="AL2" s="130"/>
+      <c r="AM2" s="130"/>
+      <c r="AN2" s="130"/>
+      <c r="AO2" s="130"/>
+      <c r="AP2" s="131"/>
+      <c r="AQ2" s="116" t="s">
         <v>1064</v>
       </c>
-      <c r="AR2" s="116"/>
-      <c r="AS2" s="116"/>
-      <c r="AT2" s="117"/>
-      <c r="AU2" s="124" t="s">
+      <c r="AR2" s="117"/>
+      <c r="AS2" s="117"/>
+      <c r="AT2" s="118"/>
+      <c r="AU2" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="AV2" s="125"/>
-      <c r="AW2" s="125"/>
-      <c r="AX2" s="126"/>
-      <c r="AY2" s="118" t="s">
+      <c r="AV2" s="126"/>
+      <c r="AW2" s="126"/>
+      <c r="AX2" s="127"/>
+      <c r="AY2" s="119" t="s">
         <v>1049</v>
       </c>
-      <c r="AZ2" s="119"/>
-      <c r="BA2" s="119"/>
-      <c r="BB2" s="119"/>
-      <c r="BC2" s="120"/>
+      <c r="AZ2" s="120"/>
+      <c r="BA2" s="120"/>
+      <c r="BB2" s="120"/>
+      <c r="BC2" s="121"/>
     </row>
     <row r="3" spans="1:55" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -7080,7 +7107,7 @@
       <c r="G17" s="40" t="s">
         <v>503</v>
       </c>
-      <c r="H17" s="44" t="s">
+      <c r="H17" s="112" t="s">
         <v>22</v>
       </c>
       <c r="I17" s="41" t="s">
@@ -7923,7 +7950,7 @@
     <row r="23" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="87" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>1063</v>
@@ -7937,7 +7964,9 @@
       <c r="F23" s="25">
         <v>5000</v>
       </c>
-      <c r="G23" s="40"/>
+      <c r="G23" s="40" t="s">
+        <v>1082</v>
+      </c>
       <c r="H23" s="110"/>
       <c r="I23" s="41"/>
       <c r="J23" s="44"/>
@@ -7994,7 +8023,7 @@
     <row r="24" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="87" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>1063</v>
@@ -8009,7 +8038,7 @@
         <v>5000</v>
       </c>
       <c r="G24" s="40" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H24" s="110"/>
       <c r="I24" s="41"/>
@@ -8067,7 +8096,7 @@
     <row r="25" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="87" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>1063</v>
@@ -8146,7 +8175,7 @@
     <row r="26" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="87" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C26" s="25" t="s">
         <v>1063</v>
@@ -8225,7 +8254,7 @@
     <row r="27" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="87" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>1063</v>
@@ -8240,7 +8269,7 @@
         <v>5000</v>
       </c>
       <c r="G27" s="40" t="s">
-        <v>1073</v>
+        <v>1080</v>
       </c>
       <c r="H27" s="110"/>
       <c r="I27" s="41"/>
@@ -8302,244 +8331,314 @@
       <c r="BC27" s="43"/>
     </row>
     <row r="28" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
-        <v>286</v>
-      </c>
-      <c r="B28" s="41"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="87" t="s">
+        <v>1083</v>
+      </c>
       <c r="C28" s="25" t="s">
-        <v>55</v>
+        <v>1063</v>
       </c>
       <c r="D28" s="25">
-        <v>2</v>
-      </c>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
+        <v>3</v>
+      </c>
+      <c r="E28" s="25">
+        <v>126</v>
+      </c>
+      <c r="F28" s="25">
+        <v>5000</v>
+      </c>
       <c r="G28" s="40" t="s">
-        <v>1074</v>
-      </c>
-      <c r="H28" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28" s="44">
-        <v>0</v>
-      </c>
+        <v>1081</v>
+      </c>
+      <c r="H28" s="110"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="44"/>
       <c r="K28" s="25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L28" s="25">
-        <v>0</v>
-      </c>
-      <c r="M28" s="25">
-        <v>1</v>
-      </c>
-      <c r="N28" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="O28" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="P28" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="R28" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="S28" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="T28" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="U28" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="25"/>
+      <c r="S28" s="42"/>
+      <c r="T28" s="42"/>
+      <c r="U28" s="41"/>
+      <c r="V28" s="25"/>
+      <c r="W28" s="25"/>
+      <c r="X28" s="25"/>
+      <c r="Y28" s="25"/>
+      <c r="Z28" s="25"/>
+      <c r="AA28" s="25"/>
+      <c r="AB28" s="25"/>
+      <c r="AC28" s="25"/>
+      <c r="AD28" s="25"/>
+      <c r="AE28" s="25"/>
+      <c r="AF28" s="25"/>
+      <c r="AG28" s="25"/>
+      <c r="AH28" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="V28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="W28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="X28" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA28" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB28" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH28" s="25"/>
-      <c r="AI28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ28" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK28" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL28" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM28" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="AN28" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="AO28" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP28" s="43" t="s">
-        <v>32</v>
-      </c>
+      <c r="AI28" s="25"/>
+      <c r="AJ28" s="43"/>
+      <c r="AK28" s="44"/>
+      <c r="AL28" s="25"/>
+      <c r="AM28" s="42"/>
+      <c r="AN28" s="42"/>
+      <c r="AO28" s="42"/>
+      <c r="AP28" s="43"/>
       <c r="AQ28" s="101"/>
       <c r="AR28" s="42"/>
       <c r="AS28" s="42"/>
       <c r="AT28" s="43"/>
-      <c r="AU28" s="44" t="s">
+      <c r="AU28" s="44"/>
+      <c r="AV28" s="54"/>
+      <c r="AW28" s="45"/>
+      <c r="AX28" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AV28" s="48" t="s">
+      <c r="AY28" s="61"/>
+      <c r="AZ28" s="62"/>
+      <c r="BA28" s="64"/>
+      <c r="BB28" s="64" t="s">
+        <v>1052</v>
+      </c>
+      <c r="BC28" s="43"/>
+    </row>
+    <row r="29" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="B29" s="41"/>
+      <c r="C29" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="25">
+        <v>2</v>
+      </c>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="40" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H29" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="44">
+        <v>0</v>
+      </c>
+      <c r="K29" s="25">
+        <v>0</v>
+      </c>
+      <c r="L29" s="25">
+        <v>0</v>
+      </c>
+      <c r="M29" s="25">
+        <v>1</v>
+      </c>
+      <c r="N29" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="O29" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="P29" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="R29" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="S29" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="T29" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="U29" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="V29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="W29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="X29" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA29" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB29" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH29" s="25"/>
+      <c r="AI29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ29" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK29" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL29" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM29" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN29" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO29" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP29" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ29" s="101"/>
+      <c r="AR29" s="42"/>
+      <c r="AS29" s="42"/>
+      <c r="AT29" s="43"/>
+      <c r="AU29" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV29" s="48" t="s">
         <v>287</v>
       </c>
-      <c r="AW28" s="45">
+      <c r="AW29" s="45">
         <v>0.2</v>
       </c>
-      <c r="AX28" s="43" t="s">
+      <c r="AX29" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AY28" s="44"/>
-      <c r="AZ28" s="48"/>
-      <c r="BA28" s="65"/>
-      <c r="BB28" s="65"/>
-      <c r="BC28" s="43" t="s">
+      <c r="AY29" s="44"/>
+      <c r="AZ29" s="48"/>
+      <c r="BA29" s="65"/>
+      <c r="BB29" s="65"/>
+      <c r="BC29" s="43" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="29" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="5"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="97"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="5"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
-      <c r="AA29" s="4"/>
-      <c r="AB29" s="4"/>
-      <c r="AC29" s="4"/>
-      <c r="AD29" s="4"/>
-      <c r="AE29" s="4"/>
-      <c r="AF29" s="4"/>
-      <c r="AG29" s="4"/>
-      <c r="AH29" s="4"/>
-      <c r="AI29" s="4"/>
-      <c r="AJ29" s="6"/>
-      <c r="AK29" s="7"/>
-      <c r="AL29" s="4"/>
-      <c r="AM29" s="8"/>
-      <c r="AN29" s="8"/>
-      <c r="AO29" s="8"/>
-      <c r="AP29" s="6"/>
-      <c r="AQ29" s="102"/>
-      <c r="AR29" s="8"/>
-      <c r="AS29" s="8"/>
-      <c r="AT29" s="6"/>
-      <c r="AU29" s="7"/>
-      <c r="AV29" s="49"/>
-      <c r="AW29" s="10"/>
-      <c r="AX29" s="6"/>
-      <c r="AY29" s="7"/>
-      <c r="AZ29" s="49"/>
-      <c r="BA29" s="66"/>
-      <c r="BB29" s="66"/>
-      <c r="BC29" s="6"/>
-    </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="B31" s="50" t="s">
+    <row r="30" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="97"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="4"/>
+      <c r="AE30" s="4"/>
+      <c r="AF30" s="4"/>
+      <c r="AG30" s="4"/>
+      <c r="AH30" s="4"/>
+      <c r="AI30" s="4"/>
+      <c r="AJ30" s="6"/>
+      <c r="AK30" s="7"/>
+      <c r="AL30" s="4"/>
+      <c r="AM30" s="8"/>
+      <c r="AN30" s="8"/>
+      <c r="AO30" s="8"/>
+      <c r="AP30" s="6"/>
+      <c r="AQ30" s="102"/>
+      <c r="AR30" s="8"/>
+      <c r="AS30" s="8"/>
+      <c r="AT30" s="6"/>
+      <c r="AU30" s="7"/>
+      <c r="AV30" s="49"/>
+      <c r="AW30" s="10"/>
+      <c r="AX30" s="6"/>
+      <c r="AY30" s="7"/>
+      <c r="AZ30" s="49"/>
+      <c r="BA30" s="66"/>
+      <c r="BB30" s="66"/>
+      <c r="BC30" s="6"/>
+    </row>
+    <row r="32" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B32" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-    </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="B32" s="50"/>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B33" s="50"/>
+      <c r="C33" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-    </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B33" s="12"/>
-      <c r="C33" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B34" s="12"/>
-      <c r="C34" s="11" t="s">
-        <v>308</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
+      <c r="C34" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B35" s="12"/>
       <c r="C35" s="11" t="s">
-        <v>50</v>
+        <v>308</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
@@ -8548,24 +8647,25 @@
     <row r="36" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B36" s="12"/>
       <c r="C36" s="11" t="s">
-        <v>294</v>
+        <v>50</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
-      <c r="T36" s="11"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B37" s="12"/>
       <c r="C37" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
+      <c r="T37" s="11"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C38" s="11" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
@@ -8573,7 +8673,7 @@
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C39" s="11" t="s">
-        <v>343</v>
+        <v>300</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
@@ -8581,7 +8681,7 @@
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C40" s="11" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
@@ -8589,7 +8689,7 @@
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C41" s="11" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
@@ -8597,7 +8697,7 @@
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C42" s="11" t="s">
-        <v>443</v>
+        <v>342</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
@@ -8605,7 +8705,7 @@
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C43" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
@@ -8613,90 +8713,98 @@
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C44" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C46" s="12" t="s">
         <v>668</v>
       </c>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-    </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.2">
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
     </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B48" s="90" t="s">
+    <row r="47" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+    </row>
+    <row r="49" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B49" s="90" t="s">
         <v>1054</v>
       </c>
-      <c r="C48" s="91"/>
-      <c r="D48" s="91"/>
-      <c r="E48" s="91"/>
-      <c r="F48" s="91"/>
-      <c r="G48" s="92"/>
-      <c r="H48" s="92"/>
-    </row>
-    <row r="50" spans="1:55" s="106" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="105"/>
-      <c r="B50" s="105"/>
-      <c r="C50" s="104" t="s">
+      <c r="C49" s="91"/>
+      <c r="D49" s="91"/>
+      <c r="E49" s="91"/>
+      <c r="F49" s="91"/>
+      <c r="G49" s="92"/>
+      <c r="H49" s="92"/>
+    </row>
+    <row r="51" spans="1:55" s="106" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="105"/>
+      <c r="B51" s="105"/>
+      <c r="C51" s="104" t="s">
         <v>1067</v>
       </c>
-      <c r="D50" s="105"/>
-      <c r="E50" s="105"/>
-      <c r="F50" s="105"/>
-      <c r="I50" s="105"/>
-      <c r="J50" s="105"/>
-      <c r="K50" s="105"/>
-      <c r="L50" s="105"/>
-      <c r="M50" s="105"/>
-      <c r="N50" s="105"/>
-      <c r="O50" s="105"/>
-      <c r="P50" s="105"/>
-      <c r="Q50" s="105"/>
-      <c r="R50" s="105"/>
-      <c r="S50" s="105"/>
-      <c r="T50" s="105"/>
-      <c r="U50" s="105"/>
-      <c r="V50" s="105"/>
-      <c r="W50" s="105"/>
-      <c r="X50" s="105"/>
-      <c r="Y50" s="105"/>
-      <c r="Z50" s="105"/>
-      <c r="AA50" s="105"/>
-      <c r="AB50" s="105"/>
-      <c r="AC50" s="105"/>
-      <c r="AD50" s="105"/>
-      <c r="AE50" s="105"/>
-      <c r="AF50" s="105"/>
-      <c r="AG50" s="105"/>
-      <c r="AH50" s="105"/>
-      <c r="AI50" s="105"/>
-      <c r="AJ50" s="105"/>
-      <c r="AK50" s="105"/>
-      <c r="AL50" s="105"/>
-      <c r="AM50" s="105"/>
-      <c r="AN50" s="105"/>
-      <c r="AO50" s="105"/>
-      <c r="AP50" s="105"/>
-      <c r="AQ50" s="105"/>
-      <c r="AR50" s="105"/>
-      <c r="AS50" s="105"/>
-      <c r="AT50" s="105"/>
-      <c r="AU50" s="105"/>
-      <c r="AV50" s="107"/>
-      <c r="AW50" s="108"/>
-      <c r="AX50" s="105"/>
-      <c r="AY50" s="105"/>
-      <c r="AZ50" s="107"/>
-      <c r="BA50" s="107"/>
-      <c r="BB50" s="107"/>
-      <c r="BC50" s="105"/>
+      <c r="D51" s="105"/>
+      <c r="E51" s="105"/>
+      <c r="F51" s="105"/>
+      <c r="I51" s="105"/>
+      <c r="J51" s="105"/>
+      <c r="K51" s="105"/>
+      <c r="L51" s="105"/>
+      <c r="M51" s="105"/>
+      <c r="N51" s="105"/>
+      <c r="O51" s="105"/>
+      <c r="P51" s="105"/>
+      <c r="Q51" s="105"/>
+      <c r="R51" s="105"/>
+      <c r="S51" s="105"/>
+      <c r="T51" s="105"/>
+      <c r="U51" s="105"/>
+      <c r="V51" s="105"/>
+      <c r="W51" s="105"/>
+      <c r="X51" s="105"/>
+      <c r="Y51" s="105"/>
+      <c r="Z51" s="105"/>
+      <c r="AA51" s="105"/>
+      <c r="AB51" s="105"/>
+      <c r="AC51" s="105"/>
+      <c r="AD51" s="105"/>
+      <c r="AE51" s="105"/>
+      <c r="AF51" s="105"/>
+      <c r="AG51" s="105"/>
+      <c r="AH51" s="105"/>
+      <c r="AI51" s="105"/>
+      <c r="AJ51" s="105"/>
+      <c r="AK51" s="105"/>
+      <c r="AL51" s="105"/>
+      <c r="AM51" s="105"/>
+      <c r="AN51" s="105"/>
+      <c r="AO51" s="105"/>
+      <c r="AP51" s="105"/>
+      <c r="AQ51" s="105"/>
+      <c r="AR51" s="105"/>
+      <c r="AS51" s="105"/>
+      <c r="AT51" s="105"/>
+      <c r="AU51" s="105"/>
+      <c r="AV51" s="107"/>
+      <c r="AW51" s="108"/>
+      <c r="AX51" s="105"/>
+      <c r="AY51" s="105"/>
+      <c r="AZ51" s="107"/>
+      <c r="BA51" s="107"/>
+      <c r="BB51" s="107"/>
+      <c r="BC51" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -8709,12 +8817,20 @@
     <mergeCell ref="AK2:AP2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="A4:B33 G4:H31 C4:F32 I4:BC33">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="A4:BC27 I29:BC34 C29:F33 G29:H32 A29:B34">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
       <formula>$A4="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:BC28">
+    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+      <formula>$A28="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+      <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
+ added HydroData for OC4 DeepCwind Semi + renamed "Floating_TLP" input files to "MIT_NREL_TLP". Also modified description where it was mentioned elsewhere. + copied/renamed "NRELOffshrBsline5MW_AeroDyn.ipt" file to "NRELOffshrBsline5MW_ITIBarge4_AeroDyn.dat","NRELOffshrBsline5MW_MIT_NREL_TLP_AeroDyn.dat", and "NRELOffshrBsline5MW_OC3Hywind_AeroDyn.dat" to allow easy changes to aerodyn properties (so we can test different combinations of things with the different certtests. Currently they are all the same AeroDyn input file.
+ ALSO, previous commit removed line_tension output from MAP for tests 22-23 so that there aren't so many output channels.

git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@735 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -3253,9 +3253,6 @@
     <t>ITI Barge</t>
   </si>
   <si>
-    <t>Floating TLP</t>
-  </si>
-  <si>
     <t>Test 24</t>
   </si>
   <si>
@@ -3274,9 +3271,6 @@
     <t>OC4 Jacket</t>
   </si>
   <si>
-    <t>Semi</t>
-  </si>
-  <si>
     <t>Test 25</t>
   </si>
   <si>
@@ -3293,6 +3287,12 @@
   </si>
   <si>
     <t>Feature not (yet) in FAST v8</t>
+  </si>
+  <si>
+    <t>OC4 DeepCwind Semi</t>
+  </si>
+  <si>
+    <t>MIT-NREL TLP</t>
   </si>
 </sst>
 </file>
@@ -3949,7 +3949,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4243,9 +4243,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4253,6 +4250,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4310,124 +4335,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <condense val="0"/>
@@ -4496,6 +4409,48 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -4831,7 +4786,7 @@
       <pane xSplit="7" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AJ22" sqref="AJ22:AJ28"/>
+      <selection pane="bottomRight" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4871,74 +4826,74 @@
   <sheetData>
     <row r="1" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="117" t="s">
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="126" t="s">
         <v>1063</v>
       </c>
-      <c r="J2" s="118"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="126"/>
-      <c r="O2" s="126"/>
-      <c r="P2" s="126"/>
-      <c r="Q2" s="126"/>
-      <c r="R2" s="126"/>
-      <c r="S2" s="126"/>
-      <c r="T2" s="127"/>
-      <c r="U2" s="120" t="s">
+      <c r="J2" s="127"/>
+      <c r="K2" s="135"/>
+      <c r="L2" s="135"/>
+      <c r="M2" s="135"/>
+      <c r="N2" s="135"/>
+      <c r="O2" s="135"/>
+      <c r="P2" s="135"/>
+      <c r="Q2" s="135"/>
+      <c r="R2" s="135"/>
+      <c r="S2" s="135"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="121"/>
-      <c r="W2" s="121"/>
-      <c r="X2" s="121"/>
-      <c r="Y2" s="121"/>
-      <c r="Z2" s="121"/>
-      <c r="AA2" s="121"/>
-      <c r="AB2" s="121"/>
-      <c r="AC2" s="121"/>
-      <c r="AD2" s="121"/>
-      <c r="AE2" s="121"/>
-      <c r="AF2" s="121"/>
-      <c r="AG2" s="121"/>
-      <c r="AH2" s="121"/>
-      <c r="AI2" s="121"/>
-      <c r="AJ2" s="122"/>
-      <c r="AK2" s="114" t="s">
+      <c r="V2" s="130"/>
+      <c r="W2" s="130"/>
+      <c r="X2" s="130"/>
+      <c r="Y2" s="130"/>
+      <c r="Z2" s="130"/>
+      <c r="AA2" s="130"/>
+      <c r="AB2" s="130"/>
+      <c r="AC2" s="130"/>
+      <c r="AD2" s="130"/>
+      <c r="AE2" s="130"/>
+      <c r="AF2" s="130"/>
+      <c r="AG2" s="130"/>
+      <c r="AH2" s="130"/>
+      <c r="AI2" s="130"/>
+      <c r="AJ2" s="131"/>
+      <c r="AK2" s="123" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="128"/>
-      <c r="AM2" s="128"/>
-      <c r="AN2" s="128"/>
-      <c r="AO2" s="128"/>
-      <c r="AP2" s="129"/>
-      <c r="AQ2" s="114" t="s">
+      <c r="AL2" s="137"/>
+      <c r="AM2" s="137"/>
+      <c r="AN2" s="137"/>
+      <c r="AO2" s="137"/>
+      <c r="AP2" s="138"/>
+      <c r="AQ2" s="123" t="s">
         <v>1062</v>
       </c>
-      <c r="AR2" s="115"/>
-      <c r="AS2" s="115"/>
-      <c r="AT2" s="116"/>
-      <c r="AU2" s="123" t="s">
+      <c r="AR2" s="124"/>
+      <c r="AS2" s="124"/>
+      <c r="AT2" s="125"/>
+      <c r="AU2" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="AV2" s="124"/>
-      <c r="AW2" s="124"/>
-      <c r="AX2" s="125"/>
-      <c r="AY2" s="117" t="s">
+      <c r="AV2" s="133"/>
+      <c r="AW2" s="133"/>
+      <c r="AX2" s="134"/>
+      <c r="AY2" s="126" t="s">
         <v>1047</v>
       </c>
-      <c r="AZ2" s="118"/>
-      <c r="BA2" s="118"/>
-      <c r="BB2" s="118"/>
-      <c r="BC2" s="119"/>
+      <c r="AZ2" s="127"/>
+      <c r="BA2" s="127"/>
+      <c r="BB2" s="127"/>
+      <c r="BC2" s="128"/>
     </row>
     <row r="3" spans="1:55" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -5019,10 +4974,10 @@
       <c r="Z3" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="AA3" s="107" t="s">
+      <c r="AA3" s="83" t="s">
         <v>307</v>
       </c>
-      <c r="AB3" s="107" t="s">
+      <c r="AB3" s="83" t="s">
         <v>308</v>
       </c>
       <c r="AC3" s="83" t="s">
@@ -5121,10 +5076,10 @@
       <c r="G4" s="28" t="s">
         <v>497</v>
       </c>
-      <c r="H4" s="132" t="s">
+      <c r="H4" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="130" t="s">
+      <c r="I4" s="110" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="36">
@@ -5178,10 +5133,10 @@
       <c r="Z4" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="AA4" s="137" t="s">
+      <c r="AA4" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="AB4" s="137" t="s">
+      <c r="AB4" s="117" t="s">
         <v>29</v>
       </c>
       <c r="AC4" s="32" t="s">
@@ -5205,7 +5160,7 @@
       <c r="AI4" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="AJ4" s="138" t="s">
+      <c r="AJ4" s="118" t="s">
         <v>29</v>
       </c>
       <c r="AK4" s="34" t="s">
@@ -5281,10 +5236,10 @@
       <c r="G5" s="39" t="s">
         <v>498</v>
       </c>
-      <c r="H5" s="109" t="s">
+      <c r="H5" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="131" t="s">
+      <c r="I5" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="43">
@@ -5299,7 +5254,7 @@
       <c r="M5" s="25">
         <v>2</v>
       </c>
-      <c r="N5" s="108" t="s">
+      <c r="N5" s="107" t="s">
         <v>32</v>
       </c>
       <c r="O5" s="25" t="s">
@@ -5308,7 +5263,7 @@
       <c r="P5" s="25">
         <v>1</v>
       </c>
-      <c r="Q5" s="108" t="s">
+      <c r="Q5" s="107" t="s">
         <v>32</v>
       </c>
       <c r="R5" s="25" t="s">
@@ -5338,10 +5293,10 @@
       <c r="Z5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AA5" s="108" t="s">
+      <c r="AA5" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB5" s="108" t="s">
+      <c r="AB5" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC5" s="25" t="s">
@@ -5365,7 +5320,7 @@
       <c r="AI5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ5" s="139" t="s">
+      <c r="AJ5" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK5" s="43" t="s">
@@ -5441,10 +5396,10 @@
       <c r="G6" s="39" t="s">
         <v>491</v>
       </c>
-      <c r="H6" s="132" t="s">
+      <c r="H6" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="131" t="s">
+      <c r="I6" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="43">
@@ -5498,10 +5453,10 @@
       <c r="Z6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AA6" s="108" t="s">
+      <c r="AA6" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB6" s="108" t="s">
+      <c r="AB6" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC6" s="25" t="s">
@@ -5525,7 +5480,7 @@
       <c r="AI6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ6" s="139" t="s">
+      <c r="AJ6" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK6" s="43" t="s">
@@ -5601,10 +5556,10 @@
       <c r="G7" s="39" t="s">
         <v>492</v>
       </c>
-      <c r="H7" s="132" t="s">
+      <c r="H7" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="131" t="s">
+      <c r="I7" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="43">
@@ -5658,10 +5613,10 @@
       <c r="Z7" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AA7" s="108" t="s">
+      <c r="AA7" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB7" s="108" t="s">
+      <c r="AB7" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC7" s="25" t="s">
@@ -5685,7 +5640,7 @@
       <c r="AI7" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ7" s="139" t="s">
+      <c r="AJ7" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK7" s="43" t="s">
@@ -5761,10 +5716,10 @@
       <c r="G8" s="39" t="s">
         <v>499</v>
       </c>
-      <c r="H8" s="132" t="s">
+      <c r="H8" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="131" t="s">
+      <c r="I8" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="43">
@@ -5779,7 +5734,7 @@
       <c r="M8" s="25">
         <v>2</v>
       </c>
-      <c r="N8" s="108" t="s">
+      <c r="N8" s="107" t="s">
         <v>32</v>
       </c>
       <c r="O8" s="25" t="s">
@@ -5791,7 +5746,7 @@
       <c r="Q8" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="R8" s="108" t="s">
+      <c r="R8" s="107" t="s">
         <v>32</v>
       </c>
       <c r="S8" s="41" t="s">
@@ -5818,10 +5773,10 @@
       <c r="Z8" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AA8" s="108" t="s">
+      <c r="AA8" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB8" s="108" t="s">
+      <c r="AB8" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC8" s="25" t="s">
@@ -5845,7 +5800,7 @@
       <c r="AI8" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ8" s="139" t="s">
+      <c r="AJ8" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK8" s="43" t="s">
@@ -5922,10 +5877,10 @@
       <c r="G9" s="39" t="s">
         <v>499</v>
       </c>
-      <c r="H9" s="132" t="s">
+      <c r="H9" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="131" t="s">
+      <c r="I9" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="43">
@@ -5940,7 +5895,7 @@
       <c r="M9" s="25">
         <v>2</v>
       </c>
-      <c r="N9" s="108" t="s">
+      <c r="N9" s="107" t="s">
         <v>32</v>
       </c>
       <c r="O9" s="25" t="s">
@@ -5952,7 +5907,7 @@
       <c r="Q9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="R9" s="108" t="s">
+      <c r="R9" s="107" t="s">
         <v>32</v>
       </c>
       <c r="S9" s="41" t="s">
@@ -5979,10 +5934,10 @@
       <c r="Z9" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AA9" s="108" t="s">
+      <c r="AA9" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB9" s="108" t="s">
+      <c r="AB9" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC9" s="25" t="s">
@@ -6006,7 +5961,7 @@
       <c r="AI9" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ9" s="139" t="s">
+      <c r="AJ9" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK9" s="43" t="s">
@@ -6083,10 +6038,10 @@
       <c r="G10" s="39" t="s">
         <v>492</v>
       </c>
-      <c r="H10" s="132" t="s">
+      <c r="H10" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="131" t="s">
+      <c r="I10" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J10" s="43">
@@ -6140,10 +6095,10 @@
       <c r="Z10" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AA10" s="108" t="s">
+      <c r="AA10" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB10" s="108" t="s">
+      <c r="AB10" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC10" s="25" t="s">
@@ -6167,7 +6122,7 @@
       <c r="AI10" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ10" s="139" t="s">
+      <c r="AJ10" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK10" s="43" t="s">
@@ -6244,10 +6199,10 @@
       <c r="G11" s="28" t="s">
         <v>497</v>
       </c>
-      <c r="H11" s="132" t="s">
+      <c r="H11" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="131" t="s">
+      <c r="I11" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J11" s="43">
@@ -6301,10 +6256,10 @@
       <c r="Z11" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AA11" s="108" t="s">
+      <c r="AA11" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB11" s="108" t="s">
+      <c r="AB11" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC11" s="25" t="s">
@@ -6328,7 +6283,7 @@
       <c r="AI11" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ11" s="139" t="s">
+      <c r="AJ11" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK11" s="43" t="s">
@@ -6404,10 +6359,10 @@
       <c r="G12" s="39" t="s">
         <v>493</v>
       </c>
-      <c r="H12" s="132" t="s">
+      <c r="H12" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="131" t="s">
+      <c r="I12" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J12" s="43">
@@ -6461,10 +6416,10 @@
       <c r="Z12" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AA12" s="108" t="s">
+      <c r="AA12" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB12" s="108" t="s">
+      <c r="AB12" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC12" s="25" t="s">
@@ -6488,7 +6443,7 @@
       <c r="AI12" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ12" s="139" t="s">
+      <c r="AJ12" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK12" s="43" t="s">
@@ -6564,10 +6519,10 @@
       <c r="G13" s="39" t="s">
         <v>496</v>
       </c>
-      <c r="H13" s="132" t="s">
+      <c r="H13" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="131" t="s">
+      <c r="I13" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J13" s="43">
@@ -6621,10 +6576,10 @@
       <c r="Z13" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AA13" s="108" t="s">
+      <c r="AA13" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB13" s="108" t="s">
+      <c r="AB13" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC13" s="25" t="s">
@@ -6648,7 +6603,7 @@
       <c r="AI13" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ13" s="139" t="s">
+      <c r="AJ13" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK13" s="43" t="s">
@@ -6724,10 +6679,10 @@
       <c r="G14" s="39" t="s">
         <v>500</v>
       </c>
-      <c r="H14" s="132" t="s">
+      <c r="H14" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="131" t="s">
+      <c r="I14" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="43">
@@ -6781,10 +6736,10 @@
       <c r="Z14" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AA14" s="108" t="s">
+      <c r="AA14" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB14" s="108" t="s">
+      <c r="AB14" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC14" s="25" t="s">
@@ -6808,7 +6763,7 @@
       <c r="AI14" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ14" s="139" t="s">
+      <c r="AJ14" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK14" s="43" t="s">
@@ -6884,10 +6839,10 @@
       <c r="G15" s="39" t="s">
         <v>494</v>
       </c>
-      <c r="H15" s="132" t="s">
+      <c r="H15" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="131" t="s">
+      <c r="I15" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="43">
@@ -6941,10 +6896,10 @@
       <c r="Z15" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AA15" s="108" t="s">
+      <c r="AA15" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB15" s="108" t="s">
+      <c r="AB15" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC15" s="25" t="s">
@@ -6968,7 +6923,7 @@
       <c r="AI15" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ15" s="139" t="s">
+      <c r="AJ15" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK15" s="43" t="s">
@@ -7044,10 +6999,10 @@
       <c r="G16" s="39" t="s">
         <v>495</v>
       </c>
-      <c r="H16" s="132" t="s">
+      <c r="H16" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="131" t="s">
+      <c r="I16" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J16" s="43">
@@ -7101,10 +7056,10 @@
       <c r="Z16" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AA16" s="108" t="s">
+      <c r="AA16" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB16" s="108" t="s">
+      <c r="AB16" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC16" s="25" t="s">
@@ -7128,7 +7083,7 @@
       <c r="AI16" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ16" s="139" t="s">
+      <c r="AJ16" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK16" s="43" t="s">
@@ -7201,13 +7156,13 @@
       <c r="F17" s="25">
         <v>1500</v>
       </c>
-      <c r="G17" s="110" t="s">
+      <c r="G17" s="109" t="s">
         <v>501</v>
       </c>
-      <c r="H17" s="109" t="s">
+      <c r="H17" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="131" t="s">
+      <c r="I17" s="111" t="s">
         <v>32</v>
       </c>
       <c r="J17" s="43">
@@ -7261,10 +7216,10 @@
       <c r="Z17" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AA17" s="108" t="s">
+      <c r="AA17" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB17" s="108" t="s">
+      <c r="AB17" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC17" s="25" t="s">
@@ -7288,7 +7243,7 @@
       <c r="AI17" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AJ17" s="139" t="s">
+      <c r="AJ17" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK17" s="43" t="s">
@@ -7364,10 +7319,10 @@
       <c r="G18" s="39" t="s">
         <v>502</v>
       </c>
-      <c r="H18" s="132" t="s">
+      <c r="H18" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="131" t="s">
+      <c r="I18" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J18" s="43">
@@ -7421,10 +7376,10 @@
       <c r="Z18" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AA18" s="108" t="s">
+      <c r="AA18" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB18" s="108" t="s">
+      <c r="AB18" s="107" t="s">
         <v>28</v>
       </c>
       <c r="AC18" s="25" t="s">
@@ -7448,7 +7403,7 @@
       <c r="AI18" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ18" s="139" t="s">
+      <c r="AJ18" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK18" s="43" t="s">
@@ -7524,10 +7479,10 @@
       <c r="G19" s="39" t="s">
         <v>503</v>
       </c>
-      <c r="H19" s="132" t="s">
+      <c r="H19" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="131" t="s">
+      <c r="I19" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J19" s="43">
@@ -7581,10 +7536,10 @@
       <c r="Z19" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AA19" s="108" t="s">
+      <c r="AA19" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB19" s="108" t="s">
+      <c r="AB19" s="107" t="s">
         <v>28</v>
       </c>
       <c r="AC19" s="25" t="s">
@@ -7608,7 +7563,7 @@
       <c r="AI19" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ19" s="139" t="s">
+      <c r="AJ19" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK19" s="43" t="s">
@@ -7684,10 +7639,10 @@
       <c r="G20" s="39" t="s">
         <v>504</v>
       </c>
-      <c r="H20" s="132" t="s">
+      <c r="H20" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="131" t="s">
+      <c r="I20" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J20" s="43">
@@ -7741,10 +7696,10 @@
       <c r="Z20" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AA20" s="108" t="s">
+      <c r="AA20" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB20" s="108" t="s">
+      <c r="AB20" s="107" t="s">
         <v>28</v>
       </c>
       <c r="AC20" s="25" t="s">
@@ -7768,7 +7723,7 @@
       <c r="AI20" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ20" s="139" t="s">
+      <c r="AJ20" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK20" s="43" t="s">
@@ -7840,12 +7795,12 @@
         <v>5000</v>
       </c>
       <c r="G21" s="39" t="s">
-        <v>1077</v>
-      </c>
-      <c r="H21" s="133" t="s">
+        <v>1075</v>
+      </c>
+      <c r="H21" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="131" t="s">
+      <c r="I21" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J21" s="43">
@@ -7899,10 +7854,10 @@
       <c r="Z21" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AA21" s="108" t="s">
+      <c r="AA21" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="AB21" s="108" t="s">
+      <c r="AB21" s="107" t="s">
         <v>29</v>
       </c>
       <c r="AC21" s="25" t="s">
@@ -7926,7 +7881,7 @@
       <c r="AI21" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ21" s="139" t="s">
+      <c r="AJ21" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK21" s="43" t="s">
@@ -7983,12 +7938,12 @@
         <v>5000</v>
       </c>
       <c r="G22" s="39" t="s">
-        <v>1079</v>
-      </c>
-      <c r="H22" s="133" t="s">
+        <v>1077</v>
+      </c>
+      <c r="H22" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="I22" s="131" t="s">
+      <c r="I22" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J22" s="43"/>
@@ -8023,7 +7978,7 @@
         <v>28</v>
       </c>
       <c r="AI22" s="25"/>
-      <c r="AJ22" s="139" t="s">
+      <c r="AJ22" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK22" s="43"/>
@@ -8053,7 +8008,7 @@
     <row r="23" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="85" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>1061</v>
@@ -8068,12 +8023,12 @@
         <v>5000</v>
       </c>
       <c r="G23" s="39" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H23" s="133" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H23" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="131" t="s">
+      <c r="I23" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J23" s="43"/>
@@ -8108,7 +8063,7 @@
         <v>28</v>
       </c>
       <c r="AI23" s="25"/>
-      <c r="AJ23" s="139" t="s">
+      <c r="AJ23" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK23" s="43"/>
@@ -8134,7 +8089,7 @@
     <row r="24" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="85" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>1061</v>
@@ -8149,12 +8104,12 @@
         <v>5000</v>
       </c>
       <c r="G24" s="39" t="s">
-        <v>1074</v>
-      </c>
-      <c r="H24" s="133" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H24" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="131" t="s">
+      <c r="I24" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J24" s="43"/>
@@ -8189,7 +8144,7 @@
         <v>28</v>
       </c>
       <c r="AI24" s="25"/>
-      <c r="AJ24" s="139" t="s">
+      <c r="AJ24" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK24" s="43"/>
@@ -8215,7 +8170,7 @@
     <row r="25" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="85" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>1061</v>
@@ -8232,10 +8187,10 @@
       <c r="G25" s="39" t="s">
         <v>1067</v>
       </c>
-      <c r="H25" s="133" t="s">
+      <c r="H25" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="131" t="s">
+      <c r="I25" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J25" s="43"/>
@@ -8270,7 +8225,7 @@
         <v>28</v>
       </c>
       <c r="AI25" s="25"/>
-      <c r="AJ25" s="139" t="s">
+      <c r="AJ25" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK25" s="43"/>
@@ -8300,7 +8255,7 @@
     <row r="26" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="85" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="C26" s="25" t="s">
         <v>1061</v>
@@ -8315,12 +8270,12 @@
         <v>5000</v>
       </c>
       <c r="G26" s="39" t="s">
-        <v>1068</v>
-      </c>
-      <c r="H26" s="133" t="s">
+        <v>1081</v>
+      </c>
+      <c r="H26" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="131" t="s">
+      <c r="I26" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J26" s="43"/>
@@ -8355,7 +8310,7 @@
         <v>28</v>
       </c>
       <c r="AI26" s="25"/>
-      <c r="AJ26" s="139" t="s">
+      <c r="AJ26" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK26" s="43"/>
@@ -8385,7 +8340,7 @@
     <row r="27" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="85" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>1061</v>
@@ -8400,12 +8355,12 @@
         <v>5000</v>
       </c>
       <c r="G27" s="39" t="s">
-        <v>1080</v>
-      </c>
-      <c r="H27" s="133" t="s">
+        <v>1078</v>
+      </c>
+      <c r="H27" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="I27" s="131" t="s">
+      <c r="I27" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J27" s="43"/>
@@ -8440,7 +8395,7 @@
         <v>28</v>
       </c>
       <c r="AI27" s="25"/>
-      <c r="AJ27" s="139" t="s">
+      <c r="AJ27" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK27" s="43"/>
@@ -8470,7 +8425,7 @@
     <row r="28" spans="1:55" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="85" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>1061</v>
@@ -8485,12 +8440,12 @@
         <v>5000</v>
       </c>
       <c r="G28" s="39" t="s">
-        <v>1075</v>
-      </c>
-      <c r="H28" s="133" t="s">
+        <v>1080</v>
+      </c>
+      <c r="H28" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="I28" s="131" t="s">
+      <c r="I28" s="111" t="s">
         <v>22</v>
       </c>
       <c r="J28" s="43"/>
@@ -8525,7 +8480,7 @@
         <v>28</v>
       </c>
       <c r="AI28" s="25"/>
-      <c r="AJ28" s="139" t="s">
+      <c r="AJ28" s="119" t="s">
         <v>29</v>
       </c>
       <c r="AK28" s="43"/>
@@ -8735,14 +8690,14 @@
       <c r="H45" s="11"/>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B46" s="135" t="s">
-        <v>1081</v>
-      </c>
-      <c r="C46" s="134"/>
-      <c r="D46" s="134"/>
-      <c r="E46" s="134"/>
-      <c r="F46" s="134"/>
-      <c r="G46" s="136"/>
+      <c r="B46" s="115" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C46" s="114"/>
+      <c r="D46" s="114"/>
+      <c r="E46" s="114"/>
+      <c r="F46" s="114"/>
+      <c r="G46" s="116"/>
       <c r="H46" s="11"/>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.2">
@@ -8825,42 +8780,42 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A4:BC21 C29:F32 A29:B33 G29:BC31 I33:BC33 I32:K32 M32:BC32 A22:G27 J22:AI27 AK22:BC27">
-    <cfRule type="expression" dxfId="22" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28 J28:AI28 AK28:BC28">
-    <cfRule type="expression" dxfId="20" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="5" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="11" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="19" stopIfTrue="1">
       <formula>$A32="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
       <formula>$A32="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I28">
-    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ22:AJ28">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40306,31 +40261,31 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="C782:C787 C844:C855 C789:C842">
-    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>$A782=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
       <formula>$A782=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B336:C353 B764:C769 B301:C303 B4:C10 B297:C299 B38:C49 B25:C36 B496:C528 B12:C23 B844:B855 B315:C326 B530:C539 B541:C550 B728:C743 B745:C748 B750:C758 B332:C334 B771:C780 B328:C330 B760:C760 B762:C762 B305:C313 B355:C358 B782:B787 B552:C561 B51:C131 B133:C213 B215:C295 B360:C494 B563:C616 B673:C726 B618:C671 B789:B842">
-    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>$A4=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2 D2:Z2">
-    <cfRule type="cellIs" dxfId="14" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A10 A12:A23 A25:A36 A38:A49 A297:A299 A301:A303 A305:A313 A315:A326 A328:A330 A332:A334 A336:A353 A355:A358 A496:A528 A530:A539 A541:A550 A552:A561 A745:A748 A750:A758 A760 A762 A764:A769 A771:A780 A782:A787 A844:A855 A51:A131 A133:A213 A215:A295 A360:A494 A563:A616 A673:A726 A618:A671 A728:A743 A789:A842">
-    <cfRule type="cellIs" dxfId="13" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
+ updated dependencies + created new executables + updated CertTest/TstFiles + added results for test 25
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@751 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -36,7 +36,7 @@
     <definedName name="_Toc46290869" localSheetId="2">Variables!$B$770</definedName>
     <definedName name="_Toc46290870" localSheetId="2">Variables!$B$781</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">TestMatrix!$B$2:$AX$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'TestMatrix (new)'!$B$2:$BH$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'TestMatrix (new)'!$B$2:$BC$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Variables!$B$1:$P$855</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2726" uniqueCount="1111">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3366,10 +3366,22 @@
     <t>Glue-Code Options</t>
   </si>
   <si>
-    <t>Flexible, tip-brake shutdown, steady wind</t>
-  </si>
-  <si>
     <t>NREL 5 MW - OC4-DeepCwind Semi-Submersible</t>
+  </si>
+  <si>
+    <t>Flexible, steady wind</t>
+  </si>
+  <si>
+    <t>Flexible, variable speed control, free yaw, EOG01 event</t>
+  </si>
+  <si>
+    <t>Flexible, variable speed control, free yaw, EDC01 event</t>
+  </si>
+  <si>
+    <t>Flexible, variable speed control, free yaw, turbulence</t>
+  </si>
+  <si>
+    <t>ServoDyn</t>
   </si>
 </sst>
 </file>
@@ -3473,7 +3485,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -4040,12 +4052,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4511,12 +4536,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -4585,118 +4630,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -5208,13 +5141,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BM30"/>
+  <dimension ref="A1:BH61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="AJ4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="BG24" sqref="BG23:BG24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5237,28 +5170,25 @@
     <col min="21" max="22" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="25" width="3.28515625" style="2" customWidth="1"/>
     <col min="26" max="26" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" style="2" customWidth="1"/>
-    <col min="28" max="28" width="4.28515625" style="2" customWidth="1"/>
-    <col min="29" max="29" width="3.28515625" style="2" customWidth="1"/>
-    <col min="30" max="32" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="44" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4.85546875" style="2" customWidth="1"/>
-    <col min="46" max="46" width="3.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4.5703125" style="2" customWidth="1"/>
-    <col min="48" max="57" width="4.85546875" style="2" customWidth="1"/>
-    <col min="58" max="58" width="4.85546875" style="45" customWidth="1"/>
-    <col min="59" max="59" width="4.85546875" style="9" customWidth="1"/>
-    <col min="60" max="61" width="4.85546875" style="2" customWidth="1"/>
-    <col min="62" max="63" width="4.85546875" style="45" customWidth="1"/>
-    <col min="64" max="64" width="6.7109375" style="45" customWidth="1"/>
-    <col min="65" max="65" width="4.85546875" style="2" customWidth="1"/>
-    <col min="66" max="66" width="4.42578125" customWidth="1"/>
-    <col min="67" max="67" width="4.28515625" customWidth="1"/>
+    <col min="27" max="27" width="4.28515625" style="2" customWidth="1"/>
+    <col min="28" max="28" width="3.28515625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="41" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.5703125" style="2" customWidth="1"/>
+    <col min="43" max="52" width="4.85546875" style="2" customWidth="1"/>
+    <col min="53" max="53" width="4.85546875" style="45" customWidth="1"/>
+    <col min="54" max="54" width="4.85546875" style="9" customWidth="1"/>
+    <col min="55" max="56" width="4.85546875" style="2" customWidth="1"/>
+    <col min="57" max="58" width="4.85546875" style="45" customWidth="1"/>
+    <col min="59" max="59" width="6.7109375" style="45" customWidth="1"/>
+    <col min="60" max="60" width="4.85546875" style="2" customWidth="1"/>
+    <col min="61" max="61" width="4.42578125" customWidth="1"/>
+    <col min="62" max="62" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:65" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="120" t="s">
         <v>27</v>
       </c>
@@ -5284,61 +5214,58 @@
       <c r="T2" s="143"/>
       <c r="U2" s="143"/>
       <c r="V2" s="144"/>
-      <c r="W2" s="127"/>
+      <c r="W2" s="127" t="s">
+        <v>1110</v>
+      </c>
       <c r="X2" s="135"/>
       <c r="Y2" s="135"/>
       <c r="Z2" s="135"/>
       <c r="AA2" s="135"/>
       <c r="AB2" s="135"/>
       <c r="AC2" s="135"/>
-      <c r="AD2" s="135"/>
-      <c r="AE2" s="135"/>
-      <c r="AF2" s="135"/>
-      <c r="AG2" s="136"/>
-      <c r="AH2" s="129" t="s">
+      <c r="AD2" s="136"/>
+      <c r="AE2" s="129" t="s">
         <v>4</v>
       </c>
+      <c r="AF2" s="130"/>
+      <c r="AG2" s="130"/>
+      <c r="AH2" s="130"/>
       <c r="AI2" s="130"/>
       <c r="AJ2" s="130"/>
       <c r="AK2" s="130"/>
       <c r="AL2" s="130"/>
       <c r="AM2" s="130"/>
       <c r="AN2" s="130"/>
-      <c r="AO2" s="130"/>
-      <c r="AP2" s="130"/>
-      <c r="AQ2" s="130"/>
-      <c r="AR2" s="130"/>
-      <c r="AS2" s="130"/>
-      <c r="AT2" s="130"/>
-      <c r="AU2" s="123" t="s">
+      <c r="AO2" s="131"/>
+      <c r="AP2" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="AV2" s="137"/>
-      <c r="AW2" s="137"/>
-      <c r="AX2" s="137"/>
-      <c r="AY2" s="137"/>
-      <c r="AZ2" s="138"/>
-      <c r="BA2" s="123" t="s">
+      <c r="AQ2" s="137"/>
+      <c r="AR2" s="137"/>
+      <c r="AS2" s="137"/>
+      <c r="AT2" s="137"/>
+      <c r="AU2" s="138"/>
+      <c r="AV2" s="123" t="s">
         <v>1061</v>
       </c>
-      <c r="BB2" s="124"/>
-      <c r="BC2" s="124"/>
-      <c r="BD2" s="125"/>
-      <c r="BE2" s="132" t="s">
+      <c r="AW2" s="124"/>
+      <c r="AX2" s="124"/>
+      <c r="AY2" s="125"/>
+      <c r="AZ2" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="BF2" s="133"/>
-      <c r="BG2" s="133"/>
-      <c r="BH2" s="134"/>
-      <c r="BI2" s="126" t="s">
+      <c r="BA2" s="133"/>
+      <c r="BB2" s="133"/>
+      <c r="BC2" s="134"/>
+      <c r="BD2" s="126" t="s">
         <v>1047</v>
       </c>
-      <c r="BJ2" s="127"/>
-      <c r="BK2" s="127"/>
-      <c r="BL2" s="127"/>
-      <c r="BM2" s="128"/>
-    </row>
-    <row r="3" spans="1:65" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="BE2" s="127"/>
+      <c r="BF2" s="127"/>
+      <c r="BG2" s="127"/>
+      <c r="BH2" s="128"/>
+    </row>
+    <row r="3" spans="1:60" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
       <c r="B3" s="79" t="s">
         <v>287</v>
@@ -5416,116 +5343,101 @@
         <v>3</v>
       </c>
       <c r="AA3" s="67" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AB3" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC3" s="67" t="s">
         <v>339</v>
       </c>
-      <c r="AD3" s="94" t="s">
-        <v>1058</v>
-      </c>
-      <c r="AE3" s="94" t="s">
-        <v>1057</v>
-      </c>
-      <c r="AF3" s="92" t="s">
+      <c r="AC3" s="92" t="s">
         <v>1055</v>
       </c>
-      <c r="AG3" s="93" t="s">
+      <c r="AD3" s="93" t="s">
         <v>1056</v>
       </c>
-      <c r="AH3" s="82" t="s">
+      <c r="AE3" s="82" t="s">
         <v>5</v>
       </c>
+      <c r="AF3" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG3" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH3" s="83" t="s">
+        <v>8</v>
+      </c>
       <c r="AI3" s="83" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AJ3" s="83" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AK3" s="83" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="AL3" s="83" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AM3" s="83" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AN3" s="83" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO3" s="83" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP3" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="AQ3" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="AR3" s="83" t="s">
+      <c r="AO3" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="AS3" s="101" t="s">
-        <v>1063</v>
-      </c>
-      <c r="AT3" s="84" t="s">
-        <v>16</v>
-      </c>
-      <c r="AU3" s="71" t="s">
+      <c r="AP3" s="169" t="s">
         <v>44</v>
       </c>
-      <c r="AV3" s="72" t="s">
+      <c r="AQ3" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="AW3" s="73" t="s">
+      <c r="AR3" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="AX3" s="73" t="s">
+      <c r="AS3" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="AY3" s="73" t="s">
+      <c r="AT3" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="AZ3" s="74" t="s">
+      <c r="AU3" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="BA3" s="97"/>
-      <c r="BB3" s="73"/>
-      <c r="BC3" s="73"/>
-      <c r="BD3" s="74"/>
-      <c r="BE3" s="75" t="s">
+      <c r="AV3" s="97"/>
+      <c r="AW3" s="73"/>
+      <c r="AX3" s="73"/>
+      <c r="AY3" s="74"/>
+      <c r="AZ3" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="BF3" s="77" t="s">
+      <c r="BA3" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="BG3" s="78" t="s">
+      <c r="BB3" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="BH3" s="76" t="s">
+      <c r="BC3" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="BI3" s="66" t="s">
+      <c r="BD3" s="66" t="s">
         <v>1045</v>
       </c>
-      <c r="BJ3" s="69" t="s">
+      <c r="BE3" s="69" t="s">
         <v>1046</v>
       </c>
-      <c r="BK3" s="70" t="s">
+      <c r="BF3" s="70" t="s">
         <v>1051</v>
       </c>
-      <c r="BL3" s="70" t="s">
+      <c r="BG3" s="70" t="s">
         <v>1054</v>
       </c>
-      <c r="BM3" s="68" t="s">
+      <c r="BH3" s="68" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27"/>
       <c r="B4" s="85" t="s">
         <v>20</v>
@@ -5605,25 +5517,25 @@
       <c r="AA4" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="AB4" s="29" t="s">
+      <c r="AB4" s="29">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="AC4" s="29">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="29" t="s">
+      <c r="AD4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="AE4" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF4" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG4" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH4" s="31" t="s">
+      <c r="AE4" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF4" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG4" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH4" s="32" t="s">
         <v>28</v>
       </c>
       <c r="AI4" s="32" t="s">
@@ -5633,7 +5545,7 @@
         <v>28</v>
       </c>
       <c r="AK4" s="32" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AL4" s="32" t="s">
         <v>28</v>
@@ -5642,78 +5554,63 @@
         <v>28</v>
       </c>
       <c r="AN4" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO4" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="AP4" s="32" t="s">
+      <c r="AO4" s="33" t="s">
         <v>28</v>
       </c>
+      <c r="AP4" s="34" t="s">
+        <v>32</v>
+      </c>
       <c r="AQ4" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR4" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS4" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT4" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU4" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="AV4" s="32" t="s">
+      <c r="AR4" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="AW4" s="35" t="s">
+      <c r="AS4" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT4" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU4" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV4" s="98"/>
+      <c r="AW4" s="35"/>
+      <c r="AX4" s="35"/>
+      <c r="AY4" s="33"/>
+      <c r="AZ4" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="AX4" s="35" t="s">
+      <c r="BA4" s="46">
+        <v>15</v>
+      </c>
+      <c r="BB4" s="37">
+        <v>0.2</v>
+      </c>
+      <c r="BC4" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="AY4" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ4" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA4" s="98"/>
-      <c r="BB4" s="35"/>
-      <c r="BC4" s="35"/>
-      <c r="BD4" s="33"/>
-      <c r="BE4" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="BF4" s="46">
-        <v>15</v>
-      </c>
-      <c r="BG4" s="37">
-        <v>0.2</v>
-      </c>
-      <c r="BH4" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI4" s="59">
-        <v>0</v>
-      </c>
-      <c r="BJ4" s="55">
+      <c r="BD4" s="59">
+        <v>0</v>
+      </c>
+      <c r="BE4" s="55">
         <v>3</v>
       </c>
-      <c r="BK4" s="62">
+      <c r="BF4" s="62">
         <f>Variables!D2</f>
         <v>23</v>
       </c>
-      <c r="BL4" s="62" t="s">
+      <c r="BG4" s="62" t="s">
         <v>1048</v>
       </c>
-      <c r="BM4" s="38" t="s">
+      <c r="BH4" s="38" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
       <c r="B5" s="85" t="s">
         <v>33</v>
@@ -5731,7 +5628,7 @@
         <v>175</v>
       </c>
       <c r="G5" s="166" t="s">
-        <v>498</v>
+        <v>1106</v>
       </c>
       <c r="H5" s="40">
         <v>20</v>
@@ -5790,28 +5687,28 @@
       <c r="Z5" s="25">
         <v>2</v>
       </c>
-      <c r="AA5" s="107" t="s">
+      <c r="AA5" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="AB5" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC5" s="25">
+      <c r="AB5" s="25">
         <v>1</v>
       </c>
-      <c r="AD5" s="107" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE5" s="25" t="s">
+      <c r="AC5" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AF5" s="41" t="s">
+      <c r="AD5" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AG5" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH5" s="40" t="s">
+      <c r="AE5" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF5" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG5" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH5" s="25" t="s">
         <v>28</v>
       </c>
       <c r="AI5" s="25" t="s">
@@ -5821,7 +5718,7 @@
         <v>28</v>
       </c>
       <c r="AK5" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AL5" s="25" t="s">
         <v>28</v>
@@ -5830,78 +5727,63 @@
         <v>28</v>
       </c>
       <c r="AN5" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AP5" s="25" t="s">
+      <c r="AO5" s="42" t="s">
         <v>28</v>
       </c>
+      <c r="AP5" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="AQ5" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR5" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS5" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT5" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU5" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR5" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AV5" s="25" t="s">
+      <c r="AS5" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW5" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="AX5" s="41" t="s">
+      <c r="AT5" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AY5" s="41" t="s">
+      <c r="AU5" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="AZ5" s="42" t="s">
+      <c r="AV5" s="99"/>
+      <c r="AW5" s="41"/>
+      <c r="AX5" s="41"/>
+      <c r="AY5" s="42"/>
+      <c r="AZ5" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BA5" s="99"/>
-      <c r="BB5" s="41"/>
-      <c r="BC5" s="41"/>
-      <c r="BD5" s="42"/>
-      <c r="BE5" s="43" t="s">
+      <c r="BA5" s="47">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="44">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BF5" s="47">
-        <v>0</v>
-      </c>
-      <c r="BG5" s="44">
-        <v>0</v>
-      </c>
-      <c r="BH5" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI5" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ5" s="56">
+      <c r="BD5" s="60">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="56">
         <v>1</v>
       </c>
-      <c r="BK5" s="63">
+      <c r="BF5" s="63">
         <f>Variables!E2</f>
         <v>22</v>
       </c>
-      <c r="BL5" s="63" t="s">
+      <c r="BG5" s="63" t="s">
         <v>1049</v>
       </c>
-      <c r="BM5" s="42" t="s">
+      <c r="BH5" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="85" t="s">
         <v>34</v>
@@ -5981,25 +5863,25 @@
       <c r="AA6" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB6" s="25" t="s">
+      <c r="AB6" s="25">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC6" s="25">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="25" t="s">
+      <c r="AD6" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE6" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF6" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG6" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH6" s="40" t="s">
+      <c r="AE6" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF6" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG6" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH6" s="25" t="s">
         <v>28</v>
       </c>
       <c r="AI6" s="25" t="s">
@@ -6020,76 +5902,61 @@
       <c r="AN6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AO6" s="25" t="s">
+      <c r="AO6" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AP6" s="25" t="s">
-        <v>28</v>
+      <c r="AP6" s="43" t="s">
+        <v>22</v>
       </c>
       <c r="AQ6" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR6" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS6" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT6" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU6" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AV6" s="25" t="s">
+      <c r="AR6" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS6" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW6" s="41" t="s">
+      <c r="AT6" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU6" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV6" s="99"/>
+      <c r="AW6" s="41"/>
+      <c r="AX6" s="41"/>
+      <c r="AY6" s="42"/>
+      <c r="AZ6" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AX6" s="41" t="s">
+      <c r="BA6" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="BB6" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC6" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="AY6" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ6" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA6" s="99"/>
-      <c r="BB6" s="41"/>
-      <c r="BC6" s="41"/>
-      <c r="BD6" s="42"/>
-      <c r="BE6" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="BF6" s="47" t="s">
-        <v>285</v>
-      </c>
-      <c r="BG6" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="BH6" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI6" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ6" s="56">
+      <c r="BD6" s="60">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="56">
         <v>3</v>
       </c>
-      <c r="BK6" s="63">
+      <c r="BF6" s="63">
         <f>Variables!F$2</f>
         <v>23</v>
       </c>
-      <c r="BL6" s="63" t="s">
+      <c r="BG6" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM6" s="42" t="s">
+      <c r="BH6" s="42" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="7" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="85" t="s">
         <v>35</v>
@@ -6169,115 +6036,100 @@
       <c r="AA7" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB7" s="25" t="s">
+      <c r="AB7" s="25">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC7" s="25">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="25" t="s">
+      <c r="AD7" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE7" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF7" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG7" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH7" s="40" t="s">
+      <c r="AE7" s="40" t="s">
         <v>28</v>
       </c>
+      <c r="AF7" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG7" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH7" s="25" t="s">
+        <v>28</v>
+      </c>
       <c r="AI7" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AJ7" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AK7" s="25" t="s">
         <v>28</v>
       </c>
       <c r="AL7" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AM7" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AN7" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AO7" s="25" t="s">
+      <c r="AO7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AP7" s="25" t="s">
-        <v>28</v>
+      <c r="AP7" s="43" t="s">
+        <v>32</v>
       </c>
       <c r="AQ7" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR7" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS7" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT7" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU7" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AV7" s="25" t="s">
+      <c r="AR7" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AW7" s="41" t="s">
+      <c r="AS7" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT7" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU7" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV7" s="99"/>
+      <c r="AW7" s="41"/>
+      <c r="AX7" s="41"/>
+      <c r="AY7" s="42"/>
+      <c r="AZ7" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AX7" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AY7" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ7" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA7" s="99"/>
-      <c r="BB7" s="41"/>
-      <c r="BC7" s="41"/>
-      <c r="BD7" s="42"/>
-      <c r="BE7" s="43" t="s">
+      <c r="BA7" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="BB7" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC7" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BF7" s="47" t="s">
-        <v>285</v>
-      </c>
-      <c r="BG7" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="BH7" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="BI7" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ7" s="56">
+      <c r="BD7" s="60">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="56">
         <v>5</v>
       </c>
-      <c r="BK7" s="63">
+      <c r="BF7" s="63">
         <f>Variables!F$2</f>
         <v>23</v>
       </c>
-      <c r="BL7" s="63" t="s">
+      <c r="BG7" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM7" s="42" t="s">
+      <c r="BH7" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
       <c r="B8" s="85" t="s">
         <v>36</v>
@@ -6295,7 +6147,7 @@
         <v>175</v>
       </c>
       <c r="G8" s="166" t="s">
-        <v>499</v>
+        <v>1106</v>
       </c>
       <c r="H8" s="40">
         <v>30</v>
@@ -6354,28 +6206,28 @@
       <c r="Z8" s="25">
         <v>2</v>
       </c>
-      <c r="AA8" s="107" t="s">
+      <c r="AA8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="AB8" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC8" s="25">
+      <c r="AB8" s="25">
         <v>1</v>
       </c>
-      <c r="AD8" s="25" t="s">
+      <c r="AC8" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE8" s="107" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF8" s="41" t="s">
+      <c r="AD8" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AG8" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH8" s="40" t="s">
+      <c r="AE8" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF8" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG8" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH8" s="25" t="s">
         <v>28</v>
       </c>
       <c r="AI8" s="25" t="s">
@@ -6385,7 +6237,7 @@
         <v>28</v>
       </c>
       <c r="AK8" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AL8" s="25" t="s">
         <v>28</v>
@@ -6394,78 +6246,63 @@
         <v>28</v>
       </c>
       <c r="AN8" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO8" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AP8" s="25" t="s">
+      <c r="AO8" s="42" t="s">
         <v>28</v>
       </c>
+      <c r="AP8" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="AQ8" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR8" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS8" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT8" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU8" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR8" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AV8" s="25" t="s">
+      <c r="AS8" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW8" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="AX8" s="41" t="s">
+      <c r="AT8" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AY8" s="41" t="s">
+      <c r="AU8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="AZ8" s="42" t="s">
+      <c r="AV8" s="99"/>
+      <c r="AW8" s="41"/>
+      <c r="AX8" s="41"/>
+      <c r="AY8" s="42"/>
+      <c r="AZ8" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BA8" s="99"/>
-      <c r="BB8" s="41"/>
-      <c r="BC8" s="41"/>
-      <c r="BD8" s="42"/>
-      <c r="BE8" s="43" t="s">
+      <c r="BA8" s="47">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="44">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BF8" s="47">
-        <v>0</v>
-      </c>
-      <c r="BG8" s="44">
-        <v>0</v>
-      </c>
-      <c r="BH8" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI8" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ8" s="56">
+      <c r="BD8" s="60">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="56">
         <v>3</v>
       </c>
-      <c r="BK8" s="63">
+      <c r="BF8" s="63">
         <f>Variables!G$2</f>
         <v>24</v>
       </c>
-      <c r="BL8" s="63" t="s">
+      <c r="BG8" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM8" s="42" t="s">
+      <c r="BH8" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
       <c r="B9" s="85" t="s">
         <v>37</v>
@@ -6484,7 +6321,7 @@
         <v>50</v>
       </c>
       <c r="G9" s="166" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="H9" s="40">
         <v>35</v>
@@ -6543,29 +6380,29 @@
       <c r="Z9" s="25">
         <v>2</v>
       </c>
-      <c r="AA9" s="107" t="s">
+      <c r="AA9" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="AB9" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC9" s="25">
+      <c r="AB9" s="25">
         <v>1</v>
       </c>
-      <c r="AD9" s="25" t="s">
+      <c r="AC9" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE9" s="107" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF9" s="41" t="s">
+      <c r="AD9" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AG9" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH9" s="40" t="s">
+      <c r="AE9" s="40" t="s">
         <v>28</v>
+      </c>
+      <c r="AF9" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG9" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH9" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="AI9" s="25" t="s">
         <v>28</v>
@@ -6574,87 +6411,72 @@
         <v>28</v>
       </c>
       <c r="AK9" s="25" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="AL9" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AM9" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AN9" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AO9" s="25" t="s">
+      <c r="AO9" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="AP9" s="25" t="s">
-        <v>29</v>
+      <c r="AP9" s="43" t="s">
+        <v>22</v>
       </c>
       <c r="AQ9" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AR9" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AS9" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT9" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU9" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AV9" s="25" t="s">
+      <c r="AR9" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS9" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT9" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW9" s="41" t="s">
+      <c r="AU9" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV9" s="99"/>
+      <c r="AW9" s="41"/>
+      <c r="AX9" s="41"/>
+      <c r="AY9" s="42"/>
+      <c r="AZ9" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AX9" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="AY9" s="41" t="s">
+      <c r="BA9" s="47">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="44">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="AZ9" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA9" s="99"/>
-      <c r="BB9" s="41"/>
-      <c r="BC9" s="41"/>
-      <c r="BD9" s="42"/>
-      <c r="BE9" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="BF9" s="47">
-        <v>0</v>
-      </c>
-      <c r="BG9" s="44">
-        <v>0</v>
-      </c>
-      <c r="BH9" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI9" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ9" s="56">
+      <c r="BD9" s="60">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="56">
         <v>5</v>
       </c>
-      <c r="BK9" s="63">
+      <c r="BF9" s="63">
         <f>Variables!H$2</f>
         <v>22</v>
       </c>
-      <c r="BL9" s="63" t="s">
+      <c r="BG9" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM9" s="42" t="s">
+      <c r="BH9" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
       <c r="B10" s="85" t="s">
         <v>38</v>
@@ -6735,115 +6557,100 @@
       <c r="AA10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB10" s="25" t="s">
+      <c r="AB10" s="25">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC10" s="25">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="25" t="s">
+      <c r="AD10" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE10" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF10" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG10" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH10" s="40" t="s">
+      <c r="AE10" s="40" t="s">
         <v>28</v>
       </c>
+      <c r="AF10" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG10" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH10" s="25" t="s">
+        <v>42</v>
+      </c>
       <c r="AI10" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ10" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK10" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AJ10" s="25" t="s">
+      <c r="AL10" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AK10" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL10" s="25" t="s">
-        <v>29</v>
-      </c>
       <c r="AM10" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AN10" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AO10" s="25" t="s">
+      <c r="AO10" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AP10" s="25" t="s">
-        <v>28</v>
+      <c r="AP10" s="43" t="s">
+        <v>32</v>
       </c>
       <c r="AQ10" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR10" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS10" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT10" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU10" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR10" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AV10" s="25" t="s">
+      <c r="AS10" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT10" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW10" s="41" t="s">
+      <c r="AU10" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV10" s="99"/>
+      <c r="AW10" s="41"/>
+      <c r="AX10" s="41"/>
+      <c r="AY10" s="42"/>
+      <c r="AZ10" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AX10" s="41" t="s">
+      <c r="BA10" s="47">
+        <v>0</v>
+      </c>
+      <c r="BB10" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC10" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="AY10" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ10" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA10" s="99"/>
-      <c r="BB10" s="41"/>
-      <c r="BC10" s="41"/>
-      <c r="BD10" s="42"/>
-      <c r="BE10" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="BF10" s="47">
-        <v>0</v>
-      </c>
-      <c r="BG10" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="BH10" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="BI10" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ10" s="56">
+      <c r="BD10" s="60">
+        <v>0</v>
+      </c>
+      <c r="BE10" s="56">
         <v>3</v>
       </c>
-      <c r="BK10" s="63">
+      <c r="BF10" s="63">
         <f>Variables!I$2</f>
         <v>24</v>
       </c>
-      <c r="BL10" s="63" t="s">
+      <c r="BG10" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM10" s="42" t="s">
+      <c r="BH10" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
       <c r="B11" s="85" t="s">
         <v>39</v>
@@ -6924,115 +6731,100 @@
       <c r="AA11" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB11" s="25" t="s">
+      <c r="AB11" s="25">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC11" s="25">
-        <v>1</v>
-      </c>
-      <c r="AD11" s="25" t="s">
+      <c r="AD11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE11" s="25" t="s">
+      <c r="AE11" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF11" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG11" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH11" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI11" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ11" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK11" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL11" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM11" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN11" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO11" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP11" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ11" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AF11" s="41" t="s">
+      <c r="AR11" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AG11" s="41" t="s">
+      <c r="AT11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AH11" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI11" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ11" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AK11" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL11" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM11" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AN11" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO11" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AP11" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AQ11" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR11" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS11" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT11" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU11" s="43" t="s">
+      <c r="AU11" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV11" s="99"/>
+      <c r="AW11" s="41"/>
+      <c r="AX11" s="41"/>
+      <c r="AY11" s="42"/>
+      <c r="AZ11" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AV11" s="25" t="s">
+      <c r="BA11" s="47">
+        <v>15</v>
+      </c>
+      <c r="BB11" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC11" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="AW11" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="AX11" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AY11" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ11" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA11" s="99"/>
-      <c r="BB11" s="41"/>
-      <c r="BC11" s="41"/>
-      <c r="BD11" s="42"/>
-      <c r="BE11" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="BF11" s="47">
-        <v>15</v>
-      </c>
-      <c r="BG11" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="BH11" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI11" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ11" s="56">
+      <c r="BD11" s="60">
+        <v>0</v>
+      </c>
+      <c r="BE11" s="56">
         <v>2</v>
       </c>
-      <c r="BK11" s="63">
+      <c r="BF11" s="63">
         <f>Variables!J$2</f>
         <v>27</v>
       </c>
-      <c r="BL11" s="63" t="s">
+      <c r="BG11" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM11" s="42" t="s">
+      <c r="BH11" s="42" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="12" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="85" t="s">
         <v>40</v>
@@ -7112,26 +6904,26 @@
       <c r="AA12" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB12" s="25" t="s">
+      <c r="AB12" s="25">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD12" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC12" s="25">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE12" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF12" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG12" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH12" s="40" t="s">
+      <c r="AE12" s="40" t="s">
         <v>28</v>
+      </c>
+      <c r="AF12" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG12" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH12" s="25" t="s">
+        <v>29</v>
       </c>
       <c r="AI12" s="25" t="s">
         <v>28</v>
@@ -7140,7 +6932,7 @@
         <v>28</v>
       </c>
       <c r="AK12" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AL12" s="25" t="s">
         <v>28</v>
@@ -7151,76 +6943,61 @@
       <c r="AN12" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AO12" s="25" t="s">
+      <c r="AO12" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AP12" s="25" t="s">
-        <v>28</v>
+      <c r="AP12" s="43" t="s">
+        <v>22</v>
       </c>
       <c r="AQ12" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR12" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS12" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT12" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU12" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AV12" s="25" t="s">
+      <c r="AR12" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS12" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT12" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU12" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV12" s="99"/>
+      <c r="AW12" s="41"/>
+      <c r="AX12" s="41"/>
+      <c r="AY12" s="42"/>
+      <c r="AZ12" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="BA12" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="BB12" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC12" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="AW12" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="AX12" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="AY12" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="AZ12" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="BA12" s="99"/>
-      <c r="BB12" s="41"/>
-      <c r="BC12" s="41"/>
-      <c r="BD12" s="42"/>
-      <c r="BE12" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="BF12" s="47" t="s">
-        <v>285</v>
-      </c>
-      <c r="BG12" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="BH12" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI12" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ12" s="56">
+      <c r="BD12" s="60">
+        <v>0</v>
+      </c>
+      <c r="BE12" s="56">
         <v>5</v>
       </c>
-      <c r="BK12" s="63">
+      <c r="BF12" s="63">
         <f>Variables!K$2</f>
         <v>26</v>
       </c>
-      <c r="BL12" s="63" t="s">
+      <c r="BG12" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM12" s="42" t="s">
+      <c r="BH12" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="85" t="s">
         <v>41</v>
@@ -7300,25 +7077,25 @@
       <c r="AA13" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB13" s="25" t="s">
+      <c r="AB13" s="25">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC13" s="25">
-        <v>1</v>
-      </c>
-      <c r="AD13" s="25" t="s">
+      <c r="AD13" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE13" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF13" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG13" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH13" s="40" t="s">
+      <c r="AE13" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF13" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG13" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH13" s="25" t="s">
         <v>29</v>
       </c>
       <c r="AI13" s="25" t="s">
@@ -7339,76 +7116,61 @@
       <c r="AN13" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AO13" s="25" t="s">
+      <c r="AO13" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="AP13" s="25" t="s">
-        <v>29</v>
+      <c r="AP13" s="43" t="s">
+        <v>22</v>
       </c>
       <c r="AQ13" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AR13" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AS13" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT13" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU13" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AV13" s="25" t="s">
+      <c r="AR13" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS13" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT13" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW13" s="41" t="s">
+      <c r="AU13" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="AX13" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="AY13" s="41" t="s">
+      <c r="AV13" s="99"/>
+      <c r="AW13" s="41"/>
+      <c r="AX13" s="41"/>
+      <c r="AY13" s="42"/>
+      <c r="AZ13" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="AZ13" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="BA13" s="99"/>
-      <c r="BB13" s="41"/>
-      <c r="BC13" s="41"/>
-      <c r="BD13" s="42"/>
-      <c r="BE13" s="43" t="s">
+      <c r="BA13" s="47">
+        <v>0</v>
+      </c>
+      <c r="BB13" s="44">
+        <v>0</v>
+      </c>
+      <c r="BC13" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BF13" s="47">
-        <v>0</v>
-      </c>
-      <c r="BG13" s="44">
-        <v>0</v>
-      </c>
-      <c r="BH13" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI13" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ13" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK13" s="63">
+      <c r="BD13" s="60">
+        <v>0</v>
+      </c>
+      <c r="BE13" s="56">
+        <v>0</v>
+      </c>
+      <c r="BF13" s="63">
         <f>Variables!L$2</f>
         <v>24</v>
       </c>
-      <c r="BL13" s="63" t="s">
+      <c r="BG13" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM13" s="42" t="s">
+      <c r="BH13" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="85" t="s">
         <v>51</v>
@@ -7488,24 +7250,26 @@
       <c r="AA14" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB14" s="25"/>
-      <c r="AC14" s="25">
+      <c r="AB14" s="25">
         <v>1</v>
       </c>
-      <c r="AD14" s="25" t="s">
+      <c r="AC14" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE14" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF14" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG14" s="41" t="s">
+      <c r="AD14" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AH14" s="40" t="s">
+      <c r="AE14" s="40" t="s">
         <v>28</v>
+      </c>
+      <c r="AF14" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG14" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH14" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="AI14" s="25" t="s">
         <v>28</v>
@@ -7514,7 +7278,7 @@
         <v>28</v>
       </c>
       <c r="AK14" s="25" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="AL14" s="25" t="s">
         <v>28</v>
@@ -7523,78 +7287,63 @@
         <v>28</v>
       </c>
       <c r="AN14" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO14" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AP14" s="25" t="s">
+      <c r="AO14" s="42" t="s">
         <v>28</v>
       </c>
+      <c r="AP14" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="AQ14" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR14" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS14" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT14" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU14" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AV14" s="25" t="s">
+      <c r="AR14" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AW14" s="41" t="s">
+      <c r="AS14" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX14" s="41" t="s">
+      <c r="AT14" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AY14" s="41" t="s">
+      <c r="AU14" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV14" s="99"/>
+      <c r="AW14" s="41"/>
+      <c r="AX14" s="41"/>
+      <c r="AY14" s="42"/>
+      <c r="AZ14" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA14" s="47">
+        <v>0</v>
+      </c>
+      <c r="BB14" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC14" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="AZ14" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA14" s="99"/>
-      <c r="BB14" s="41"/>
-      <c r="BC14" s="41"/>
-      <c r="BD14" s="42"/>
-      <c r="BE14" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="BF14" s="47">
-        <v>0</v>
-      </c>
-      <c r="BG14" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="BH14" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="BI14" s="60">
+      <c r="BD14" s="60">
         <v>2</v>
       </c>
-      <c r="BJ14" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK14" s="63">
+      <c r="BE14" s="56">
+        <v>0</v>
+      </c>
+      <c r="BF14" s="63">
         <f>Variables!M$2</f>
         <v>21</v>
       </c>
-      <c r="BL14" s="63" t="s">
+      <c r="BG14" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM14" s="42" t="s">
+      <c r="BH14" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="85" t="s">
         <v>52</v>
@@ -7674,26 +7423,26 @@
       <c r="AA15" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB15" s="25" t="s">
+      <c r="AB15" s="25">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC15" s="25">
-        <v>1</v>
-      </c>
-      <c r="AD15" s="25" t="s">
+      <c r="AD15" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE15" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF15" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG15" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH15" s="40" t="s">
+      <c r="AE15" s="40" t="s">
         <v>28</v>
+      </c>
+      <c r="AF15" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG15" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH15" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="AI15" s="25" t="s">
         <v>28</v>
@@ -7702,7 +7451,7 @@
         <v>28</v>
       </c>
       <c r="AK15" s="25" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="AL15" s="25" t="s">
         <v>28</v>
@@ -7711,78 +7460,63 @@
         <v>28</v>
       </c>
       <c r="AN15" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO15" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AP15" s="25" t="s">
+      <c r="AO15" s="42" t="s">
         <v>28</v>
       </c>
+      <c r="AP15" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="AQ15" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR15" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS15" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT15" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU15" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AV15" s="25" t="s">
+      <c r="AR15" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AW15" s="41" t="s">
+      <c r="AS15" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX15" s="41" t="s">
+      <c r="AT15" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AY15" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="AZ15" s="42" t="s">
+      <c r="AU15" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BA15" s="99"/>
-      <c r="BB15" s="41"/>
-      <c r="BC15" s="41"/>
-      <c r="BD15" s="42"/>
-      <c r="BE15" s="43" t="s">
+      <c r="AV15" s="99"/>
+      <c r="AW15" s="41"/>
+      <c r="AX15" s="41"/>
+      <c r="AY15" s="42"/>
+      <c r="AZ15" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BF15" s="47" t="s">
+      <c r="BA15" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="BG15" s="44">
+      <c r="BB15" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH15" s="42" t="s">
+      <c r="BC15" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BI15" s="60">
+      <c r="BD15" s="60">
         <v>2</v>
       </c>
-      <c r="BJ15" s="56">
+      <c r="BE15" s="56">
         <v>4</v>
       </c>
-      <c r="BK15" s="63">
+      <c r="BF15" s="63">
         <f>Variables!N$2</f>
         <v>21</v>
       </c>
-      <c r="BL15" s="63" t="s">
+      <c r="BG15" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM15" s="42" t="s">
+      <c r="BH15" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="85" t="s">
         <v>53</v>
@@ -7862,26 +7596,26 @@
       <c r="AA16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB16" s="25" t="s">
+      <c r="AB16" s="25">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC16" s="25">
-        <v>1</v>
-      </c>
-      <c r="AD16" s="25" t="s">
+      <c r="AD16" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE16" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF16" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG16" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH16" s="40" t="s">
+      <c r="AE16" s="40" t="s">
         <v>28</v>
+      </c>
+      <c r="AF16" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG16" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH16" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="AI16" s="25" t="s">
         <v>28</v>
@@ -7890,7 +7624,7 @@
         <v>28</v>
       </c>
       <c r="AK16" s="25" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="AL16" s="25" t="s">
         <v>28</v>
@@ -7899,78 +7633,63 @@
         <v>28</v>
       </c>
       <c r="AN16" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO16" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AP16" s="25" t="s">
+      <c r="AO16" s="42" t="s">
         <v>28</v>
       </c>
+      <c r="AP16" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="AQ16" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR16" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS16" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT16" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU16" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AV16" s="25" t="s">
+      <c r="AR16" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AW16" s="41" t="s">
+      <c r="AS16" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX16" s="41" t="s">
+      <c r="AT16" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AY16" s="41" t="s">
+      <c r="AU16" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV16" s="99"/>
+      <c r="AW16" s="41"/>
+      <c r="AX16" s="41"/>
+      <c r="AY16" s="42"/>
+      <c r="AZ16" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA16" s="47">
+        <v>0</v>
+      </c>
+      <c r="BB16" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC16" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="AZ16" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA16" s="99"/>
-      <c r="BB16" s="41"/>
-      <c r="BC16" s="41"/>
-      <c r="BD16" s="42"/>
-      <c r="BE16" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="BF16" s="47">
-        <v>0</v>
-      </c>
-      <c r="BG16" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="BH16" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="BI16" s="60">
+      <c r="BD16" s="60">
         <v>2</v>
       </c>
-      <c r="BJ16" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK16" s="63">
+      <c r="BE16" s="56">
+        <v>0</v>
+      </c>
+      <c r="BF16" s="63">
         <f>Variables!O$2</f>
         <v>23</v>
       </c>
-      <c r="BL16" s="63" t="s">
+      <c r="BG16" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM16" s="42" t="s">
+      <c r="BH16" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="17" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
       <c r="B17" s="149"/>
       <c r="C17" s="150"/>
@@ -7999,45 +7718,40 @@
       <c r="Z17" s="151"/>
       <c r="AA17" s="151"/>
       <c r="AB17" s="151"/>
-      <c r="AC17" s="151"/>
-      <c r="AD17" s="151"/>
-      <c r="AE17" s="151"/>
-      <c r="AF17" s="153"/>
-      <c r="AG17" s="153"/>
-      <c r="AH17" s="149"/>
+      <c r="AC17" s="153"/>
+      <c r="AD17" s="153"/>
+      <c r="AE17" s="149"/>
+      <c r="AF17" s="151"/>
+      <c r="AG17" s="151"/>
+      <c r="AH17" s="151"/>
       <c r="AI17" s="151"/>
       <c r="AJ17" s="151"/>
       <c r="AK17" s="151"/>
       <c r="AL17" s="151"/>
       <c r="AM17" s="151"/>
       <c r="AN17" s="151"/>
-      <c r="AO17" s="151"/>
-      <c r="AP17" s="151"/>
+      <c r="AO17" s="154"/>
+      <c r="AP17" s="152"/>
       <c r="AQ17" s="151"/>
-      <c r="AR17" s="151"/>
-      <c r="AS17" s="151"/>
-      <c r="AT17" s="151"/>
-      <c r="AU17" s="152"/>
-      <c r="AV17" s="151"/>
+      <c r="AR17" s="153"/>
+      <c r="AS17" s="153"/>
+      <c r="AT17" s="153"/>
+      <c r="AU17" s="154"/>
+      <c r="AV17" s="155"/>
       <c r="AW17" s="153"/>
       <c r="AX17" s="153"/>
-      <c r="AY17" s="153"/>
-      <c r="AZ17" s="154"/>
-      <c r="BA17" s="155"/>
-      <c r="BB17" s="153"/>
-      <c r="BC17" s="153"/>
-      <c r="BD17" s="154"/>
-      <c r="BE17" s="152"/>
-      <c r="BF17" s="156"/>
-      <c r="BG17" s="157"/>
+      <c r="AY17" s="154"/>
+      <c r="AZ17" s="152"/>
+      <c r="BA17" s="156"/>
+      <c r="BB17" s="157"/>
+      <c r="BC17" s="154"/>
+      <c r="BD17" s="158"/>
+      <c r="BE17" s="159"/>
+      <c r="BF17" s="160"/>
+      <c r="BG17" s="160"/>
       <c r="BH17" s="154"/>
-      <c r="BI17" s="158"/>
-      <c r="BJ17" s="159"/>
-      <c r="BK17" s="160"/>
-      <c r="BL17" s="160"/>
-      <c r="BM17" s="154"/>
-    </row>
-    <row r="18" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
       <c r="B18" s="85" t="s">
         <v>289</v>
@@ -8055,7 +7769,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="166" t="s">
-        <v>502</v>
+        <v>1107</v>
       </c>
       <c r="H18" s="40">
         <v>20</v>
@@ -8117,113 +7831,100 @@
       <c r="AA18" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB18" s="25"/>
-      <c r="AC18" s="25">
+      <c r="AB18" s="25">
         <v>1</v>
       </c>
-      <c r="AD18" s="25" t="s">
+      <c r="AC18" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE18" s="25" t="s">
+      <c r="AD18" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AF18" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG18" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH18" s="40" t="s">
+      <c r="AE18" s="40" t="s">
         <v>28</v>
       </c>
+      <c r="AF18" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG18" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH18" s="25" t="s">
+        <v>42</v>
+      </c>
       <c r="AI18" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AJ18" s="25" t="s">
         <v>28</v>
       </c>
       <c r="AK18" s="25" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="AL18" s="25" t="s">
         <v>29</v>
       </c>
       <c r="AM18" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN18" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO18" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP18" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ18" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR18" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS18" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT18" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU18" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV18" s="99"/>
+      <c r="AW18" s="41"/>
+      <c r="AX18" s="41"/>
+      <c r="AY18" s="42"/>
+      <c r="AZ18" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA18" s="53" t="s">
+        <v>285</v>
+      </c>
+      <c r="BB18" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC18" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="BD18" s="60">
+        <v>0</v>
+      </c>
+      <c r="BE18" s="61">
+        <v>0</v>
+      </c>
+      <c r="BF18" s="63">
+        <f>Variables!Q$2</f>
+        <v>0</v>
+      </c>
+      <c r="BG18" s="63" t="s">
+        <v>1048</v>
+      </c>
+      <c r="BH18" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AN18" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AO18" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AP18" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ18" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AR18" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AS18" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT18" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU18" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV18" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="AW18" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="AX18" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AY18" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ18" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA18" s="99"/>
-      <c r="BB18" s="41"/>
-      <c r="BC18" s="41"/>
-      <c r="BD18" s="42"/>
-      <c r="BE18" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="BF18" s="53" t="s">
-        <v>285</v>
-      </c>
-      <c r="BG18" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="BH18" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI18" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ18" s="61">
-        <v>0</v>
-      </c>
-      <c r="BK18" s="63">
-        <f>Variables!Q$2</f>
-        <v>0</v>
-      </c>
-      <c r="BL18" s="63" t="s">
-        <v>1048</v>
-      </c>
-      <c r="BM18" s="42" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
       <c r="B19" s="85" t="s">
         <v>309</v>
@@ -8241,7 +7942,7 @@
         <v>10</v>
       </c>
       <c r="G19" s="166" t="s">
-        <v>503</v>
+        <v>1108</v>
       </c>
       <c r="H19" s="40">
         <v>20</v>
@@ -8303,115 +8004,100 @@
       <c r="AA19" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB19" s="25" t="s">
+      <c r="AB19" s="25">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC19" s="25">
-        <v>1</v>
-      </c>
-      <c r="AD19" s="25" t="s">
+      <c r="AD19" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE19" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF19" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG19" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH19" s="40" t="s">
+      <c r="AE19" s="40" t="s">
         <v>28</v>
       </c>
+      <c r="AF19" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG19" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH19" s="25" t="s">
+        <v>42</v>
+      </c>
       <c r="AI19" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AJ19" s="25" t="s">
         <v>28</v>
       </c>
       <c r="AK19" s="25" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="AL19" s="25" t="s">
         <v>29</v>
       </c>
       <c r="AM19" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AN19" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AO19" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AP19" s="25" t="s">
+      <c r="AO19" s="42" t="s">
         <v>29</v>
       </c>
+      <c r="AP19" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="AQ19" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AR19" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AS19" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT19" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU19" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AV19" s="25" t="s">
+      <c r="AR19" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AW19" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="AX19" s="41" t="s">
+      <c r="AS19" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AY19" s="41" t="s">
+      <c r="AT19" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AZ19" s="42" t="s">
+      <c r="AU19" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BA19" s="99"/>
-      <c r="BB19" s="41"/>
-      <c r="BC19" s="41"/>
-      <c r="BD19" s="42"/>
-      <c r="BE19" s="43" t="s">
+      <c r="AV19" s="99"/>
+      <c r="AW19" s="41"/>
+      <c r="AX19" s="41"/>
+      <c r="AY19" s="42"/>
+      <c r="AZ19" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BF19" s="47" t="s">
+      <c r="BA19" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="BG19" s="44">
+      <c r="BB19" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH19" s="42" t="s">
+      <c r="BC19" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BI19" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ19" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK19" s="63">
+      <c r="BD19" s="60">
+        <v>0</v>
+      </c>
+      <c r="BE19" s="56">
+        <v>0</v>
+      </c>
+      <c r="BF19" s="63">
         <f>Variables!R$2</f>
         <v>25</v>
       </c>
-      <c r="BL19" s="63" t="s">
+      <c r="BG19" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM19" s="42" t="s">
+      <c r="BH19" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="85" t="s">
         <v>336</v>
@@ -8429,7 +8115,7 @@
         <v>10</v>
       </c>
       <c r="G20" s="166" t="s">
-        <v>504</v>
+        <v>1109</v>
       </c>
       <c r="H20" s="40">
         <v>70</v>
@@ -8491,115 +8177,100 @@
       <c r="AA20" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB20" s="25" t="s">
+      <c r="AB20" s="25">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC20" s="25">
-        <v>1</v>
-      </c>
-      <c r="AD20" s="25" t="s">
+      <c r="AD20" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE20" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF20" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG20" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH20" s="40" t="s">
+      <c r="AE20" s="40" t="s">
         <v>28</v>
       </c>
+      <c r="AF20" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG20" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH20" s="25" t="s">
+        <v>42</v>
+      </c>
       <c r="AI20" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AJ20" s="25" t="s">
         <v>28</v>
       </c>
       <c r="AK20" s="25" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="AL20" s="25" t="s">
         <v>29</v>
       </c>
       <c r="AM20" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AN20" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AO20" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="AP20" s="25" t="s">
+      <c r="AO20" s="42" t="s">
         <v>29</v>
       </c>
+      <c r="AP20" s="43" t="s">
+        <v>32</v>
+      </c>
       <c r="AQ20" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AR20" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AS20" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT20" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU20" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AV20" s="25" t="s">
+      <c r="AR20" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AW20" s="41" t="s">
+      <c r="AS20" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT20" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU20" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV20" s="99"/>
+      <c r="AW20" s="41"/>
+      <c r="AX20" s="41"/>
+      <c r="AY20" s="42"/>
+      <c r="AZ20" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA20" s="53" t="s">
+        <v>285</v>
+      </c>
+      <c r="BB20" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC20" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="AX20" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AY20" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ20" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA20" s="99"/>
-      <c r="BB20" s="41"/>
-      <c r="BC20" s="41"/>
-      <c r="BD20" s="42"/>
-      <c r="BE20" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="BF20" s="53" t="s">
-        <v>285</v>
-      </c>
-      <c r="BG20" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="BH20" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="BI20" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ20" s="61">
-        <v>0</v>
-      </c>
-      <c r="BK20" s="63">
+      <c r="BD20" s="60">
+        <v>0</v>
+      </c>
+      <c r="BE20" s="61">
+        <v>0</v>
+      </c>
+      <c r="BF20" s="63">
         <f>Variables!S$2</f>
         <v>25</v>
       </c>
-      <c r="BL20" s="63" t="s">
+      <c r="BG20" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM20" s="42" t="s">
+      <c r="BH20" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="85" t="s">
         <v>1060</v>
@@ -8679,26 +8350,26 @@
       <c r="AA21" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AB21" s="25" t="s">
+      <c r="AB21" s="25">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AC21" s="25">
-        <v>1</v>
-      </c>
-      <c r="AD21" s="25" t="s">
+      <c r="AD21" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AE21" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF21" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG21" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH21" s="40" t="s">
+      <c r="AE21" s="40" t="s">
         <v>28</v>
+      </c>
+      <c r="AF21" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG21" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH21" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="AI21" s="25" t="s">
         <v>28</v>
@@ -8707,7 +8378,7 @@
         <v>28</v>
       </c>
       <c r="AK21" s="25" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="AL21" s="25" t="s">
         <v>28</v>
@@ -8718,61 +8389,46 @@
       <c r="AN21" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AO21" s="25" t="s">
+      <c r="AO21" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AP21" s="25" t="s">
-        <v>28</v>
+      <c r="AP21" s="43" t="s">
+        <v>32</v>
       </c>
       <c r="AQ21" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR21" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS21" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT21" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU21" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="AV21" s="25" t="s">
+      <c r="AR21" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AW21" s="41" t="s">
+      <c r="AS21" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX21" s="41" t="s">
+      <c r="AT21" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AY21" s="41" t="s">
+      <c r="AU21" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="AZ21" s="42" t="s">
+      <c r="AV21" s="99"/>
+      <c r="AW21" s="41"/>
+      <c r="AX21" s="41"/>
+      <c r="AY21" s="42"/>
+      <c r="AZ21" s="43"/>
+      <c r="BA21" s="53"/>
+      <c r="BB21" s="44"/>
+      <c r="BC21" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BA21" s="99"/>
-      <c r="BB21" s="41"/>
-      <c r="BC21" s="41"/>
-      <c r="BD21" s="42"/>
-      <c r="BE21" s="43"/>
-      <c r="BF21" s="53"/>
-      <c r="BG21" s="44"/>
-      <c r="BH21" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="BI21" s="60"/>
-      <c r="BJ21" s="61"/>
-      <c r="BK21" s="63"/>
-      <c r="BL21" s="63" t="s">
+      <c r="BD21" s="60"/>
+      <c r="BE21" s="61"/>
+      <c r="BF21" s="63"/>
+      <c r="BG21" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM21" s="42"/>
-    </row>
-    <row r="22" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BH21" s="42"/>
+    </row>
+    <row r="22" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
       <c r="B22" s="85" t="s">
         <v>1065</v>
@@ -8846,54 +8502,45 @@
       </c>
       <c r="Z22" s="25"/>
       <c r="AA22" s="25"/>
-      <c r="AB22" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC22" s="25"/>
-      <c r="AD22" s="25"/>
-      <c r="AE22" s="25"/>
-      <c r="AF22" s="41"/>
-      <c r="AG22" s="41"/>
-      <c r="AH22" s="40"/>
+      <c r="AB22" s="25"/>
+      <c r="AC22" s="41"/>
+      <c r="AD22" s="41"/>
+      <c r="AE22" s="40"/>
+      <c r="AF22" s="25"/>
+      <c r="AG22" s="25"/>
+      <c r="AH22" s="25"/>
       <c r="AI22" s="25"/>
       <c r="AJ22" s="25"/>
       <c r="AK22" s="25"/>
       <c r="AL22" s="25"/>
       <c r="AM22" s="25"/>
       <c r="AN22" s="25"/>
-      <c r="AO22" s="25"/>
-      <c r="AP22" s="25"/>
+      <c r="AO22" s="42"/>
+      <c r="AP22" s="43"/>
       <c r="AQ22" s="25"/>
-      <c r="AR22" s="25"/>
-      <c r="AS22" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT22" s="25"/>
-      <c r="AU22" s="43"/>
-      <c r="AV22" s="25"/>
+      <c r="AR22" s="41"/>
+      <c r="AS22" s="41"/>
+      <c r="AT22" s="41"/>
+      <c r="AU22" s="42"/>
+      <c r="AV22" s="99"/>
       <c r="AW22" s="41"/>
       <c r="AX22" s="41"/>
-      <c r="AY22" s="41"/>
-      <c r="AZ22" s="42"/>
-      <c r="BA22" s="99"/>
-      <c r="BB22" s="41"/>
-      <c r="BC22" s="41"/>
-      <c r="BD22" s="42"/>
-      <c r="BE22" s="43"/>
-      <c r="BF22" s="53"/>
-      <c r="BG22" s="44"/>
-      <c r="BH22" s="42" t="s">
+      <c r="AY22" s="42"/>
+      <c r="AZ22" s="43"/>
+      <c r="BA22" s="53"/>
+      <c r="BB22" s="44"/>
+      <c r="BC22" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI22" s="60"/>
-      <c r="BJ22" s="61"/>
-      <c r="BK22" s="63"/>
-      <c r="BL22" s="63" t="s">
+      <c r="BD22" s="60"/>
+      <c r="BE22" s="61"/>
+      <c r="BF22" s="63"/>
+      <c r="BG22" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM22" s="42"/>
-    </row>
-    <row r="23" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BH22" s="42"/>
+    </row>
+    <row r="23" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="85" t="s">
         <v>1070</v>
@@ -8968,47 +8615,42 @@
       <c r="Z23" s="25"/>
       <c r="AA23" s="25"/>
       <c r="AB23" s="25"/>
-      <c r="AC23" s="25"/>
-      <c r="AD23" s="25"/>
-      <c r="AE23" s="25"/>
-      <c r="AF23" s="41"/>
-      <c r="AG23" s="41"/>
-      <c r="AH23" s="40"/>
+      <c r="AC23" s="41"/>
+      <c r="AD23" s="41"/>
+      <c r="AE23" s="40"/>
+      <c r="AF23" s="25"/>
+      <c r="AG23" s="25"/>
+      <c r="AH23" s="25"/>
       <c r="AI23" s="25"/>
       <c r="AJ23" s="25"/>
       <c r="AK23" s="25"/>
       <c r="AL23" s="25"/>
       <c r="AM23" s="25"/>
       <c r="AN23" s="25"/>
-      <c r="AO23" s="25"/>
-      <c r="AP23" s="25"/>
+      <c r="AO23" s="42"/>
+      <c r="AP23" s="43"/>
       <c r="AQ23" s="25"/>
-      <c r="AR23" s="25"/>
-      <c r="AS23" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT23" s="25"/>
-      <c r="AU23" s="43"/>
-      <c r="AV23" s="25"/>
+      <c r="AR23" s="41"/>
+      <c r="AS23" s="41"/>
+      <c r="AT23" s="41"/>
+      <c r="AU23" s="42"/>
+      <c r="AV23" s="99"/>
       <c r="AW23" s="41"/>
       <c r="AX23" s="41"/>
-      <c r="AY23" s="41"/>
-      <c r="AZ23" s="42"/>
-      <c r="BA23" s="99"/>
-      <c r="BB23" s="41"/>
-      <c r="BC23" s="41"/>
-      <c r="BD23" s="42"/>
-      <c r="BE23" s="43"/>
-      <c r="BF23" s="53"/>
-      <c r="BG23" s="44"/>
+      <c r="AY23" s="42"/>
+      <c r="AZ23" s="43"/>
+      <c r="BA23" s="53"/>
+      <c r="BB23" s="44"/>
+      <c r="BC23" s="42"/>
+      <c r="BD23" s="60"/>
+      <c r="BE23" s="61"/>
+      <c r="BF23" s="63"/>
+      <c r="BG23" s="63" t="s">
+        <v>1050</v>
+      </c>
       <c r="BH23" s="42"/>
-      <c r="BI23" s="60"/>
-      <c r="BJ23" s="61"/>
-      <c r="BK23" s="63"/>
-      <c r="BL23" s="63"/>
-      <c r="BM23" s="42"/>
-    </row>
-    <row r="24" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="85" t="s">
         <v>1071</v>
@@ -9083,47 +8725,42 @@
       <c r="Z24" s="25"/>
       <c r="AA24" s="25"/>
       <c r="AB24" s="25"/>
-      <c r="AC24" s="25"/>
-      <c r="AD24" s="25"/>
-      <c r="AE24" s="25"/>
-      <c r="AF24" s="41"/>
-      <c r="AG24" s="41"/>
-      <c r="AH24" s="40"/>
+      <c r="AC24" s="41"/>
+      <c r="AD24" s="41"/>
+      <c r="AE24" s="40"/>
+      <c r="AF24" s="25"/>
+      <c r="AG24" s="25"/>
+      <c r="AH24" s="25"/>
       <c r="AI24" s="25"/>
       <c r="AJ24" s="25"/>
       <c r="AK24" s="25"/>
       <c r="AL24" s="25"/>
       <c r="AM24" s="25"/>
       <c r="AN24" s="25"/>
-      <c r="AO24" s="25"/>
-      <c r="AP24" s="25"/>
+      <c r="AO24" s="42"/>
+      <c r="AP24" s="43"/>
       <c r="AQ24" s="25"/>
-      <c r="AR24" s="25"/>
-      <c r="AS24" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT24" s="25"/>
-      <c r="AU24" s="43"/>
-      <c r="AV24" s="25"/>
+      <c r="AR24" s="41"/>
+      <c r="AS24" s="41"/>
+      <c r="AT24" s="41"/>
+      <c r="AU24" s="42"/>
+      <c r="AV24" s="99"/>
       <c r="AW24" s="41"/>
       <c r="AX24" s="41"/>
-      <c r="AY24" s="41"/>
-      <c r="AZ24" s="42"/>
-      <c r="BA24" s="99"/>
-      <c r="BB24" s="41"/>
-      <c r="BC24" s="41"/>
-      <c r="BD24" s="42"/>
-      <c r="BE24" s="43"/>
-      <c r="BF24" s="53"/>
-      <c r="BG24" s="44"/>
+      <c r="AY24" s="42"/>
+      <c r="AZ24" s="43"/>
+      <c r="BA24" s="53"/>
+      <c r="BB24" s="44"/>
+      <c r="BC24" s="42"/>
+      <c r="BD24" s="60"/>
+      <c r="BE24" s="61"/>
+      <c r="BF24" s="63"/>
+      <c r="BG24" s="63" t="s">
+        <v>1050</v>
+      </c>
       <c r="BH24" s="42"/>
-      <c r="BI24" s="60"/>
-      <c r="BJ24" s="61"/>
-      <c r="BK24" s="63"/>
-      <c r="BL24" s="63"/>
-      <c r="BM24" s="42"/>
-    </row>
-    <row r="25" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="85" t="s">
         <v>1069</v>
@@ -9198,51 +8835,44 @@
       <c r="Z25" s="25"/>
       <c r="AA25" s="25"/>
       <c r="AB25" s="25"/>
-      <c r="AC25" s="25"/>
-      <c r="AD25" s="25"/>
-      <c r="AE25" s="25"/>
-      <c r="AF25" s="41"/>
-      <c r="AG25" s="41"/>
-      <c r="AH25" s="40"/>
+      <c r="AC25" s="41"/>
+      <c r="AD25" s="41"/>
+      <c r="AE25" s="40"/>
+      <c r="AF25" s="25"/>
+      <c r="AG25" s="25"/>
+      <c r="AH25" s="25"/>
       <c r="AI25" s="25"/>
       <c r="AJ25" s="25"/>
       <c r="AK25" s="25"/>
       <c r="AL25" s="25"/>
       <c r="AM25" s="25"/>
       <c r="AN25" s="25"/>
-      <c r="AO25" s="25"/>
-      <c r="AP25" s="25"/>
+      <c r="AO25" s="42"/>
+      <c r="AP25" s="43"/>
       <c r="AQ25" s="25"/>
-      <c r="AR25" s="25"/>
-      <c r="AS25" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT25" s="25"/>
-      <c r="AU25" s="43"/>
-      <c r="AV25" s="25"/>
+      <c r="AR25" s="41"/>
+      <c r="AS25" s="41"/>
+      <c r="AT25" s="41"/>
+      <c r="AU25" s="42"/>
+      <c r="AV25" s="99"/>
       <c r="AW25" s="41"/>
       <c r="AX25" s="41"/>
-      <c r="AY25" s="41"/>
-      <c r="AZ25" s="42"/>
-      <c r="BA25" s="99"/>
-      <c r="BB25" s="41"/>
-      <c r="BC25" s="41"/>
-      <c r="BD25" s="42"/>
-      <c r="BE25" s="43"/>
-      <c r="BF25" s="53"/>
-      <c r="BG25" s="44"/>
-      <c r="BH25" s="42" t="s">
+      <c r="AY25" s="42"/>
+      <c r="AZ25" s="43"/>
+      <c r="BA25" s="53"/>
+      <c r="BB25" s="44"/>
+      <c r="BC25" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI25" s="60"/>
-      <c r="BJ25" s="61"/>
-      <c r="BK25" s="63"/>
-      <c r="BL25" s="63" t="s">
+      <c r="BD25" s="60"/>
+      <c r="BE25" s="61"/>
+      <c r="BF25" s="63"/>
+      <c r="BG25" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM25" s="42"/>
-    </row>
-    <row r="26" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BH25" s="42"/>
+    </row>
+    <row r="26" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="85" t="s">
         <v>1068</v>
@@ -9317,51 +8947,44 @@
       <c r="Z26" s="25"/>
       <c r="AA26" s="25"/>
       <c r="AB26" s="25"/>
-      <c r="AC26" s="25"/>
-      <c r="AD26" s="25"/>
-      <c r="AE26" s="25"/>
-      <c r="AF26" s="41"/>
-      <c r="AG26" s="41"/>
-      <c r="AH26" s="40"/>
+      <c r="AC26" s="41"/>
+      <c r="AD26" s="41"/>
+      <c r="AE26" s="40"/>
+      <c r="AF26" s="25"/>
+      <c r="AG26" s="25"/>
+      <c r="AH26" s="25"/>
       <c r="AI26" s="25"/>
       <c r="AJ26" s="25"/>
       <c r="AK26" s="25"/>
       <c r="AL26" s="25"/>
       <c r="AM26" s="25"/>
       <c r="AN26" s="25"/>
-      <c r="AO26" s="25"/>
-      <c r="AP26" s="25"/>
+      <c r="AO26" s="42"/>
+      <c r="AP26" s="43"/>
       <c r="AQ26" s="25"/>
-      <c r="AR26" s="25"/>
-      <c r="AS26" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT26" s="25"/>
-      <c r="AU26" s="43"/>
-      <c r="AV26" s="25"/>
+      <c r="AR26" s="41"/>
+      <c r="AS26" s="41"/>
+      <c r="AT26" s="41"/>
+      <c r="AU26" s="42"/>
+      <c r="AV26" s="99"/>
       <c r="AW26" s="41"/>
       <c r="AX26" s="41"/>
-      <c r="AY26" s="41"/>
-      <c r="AZ26" s="42"/>
-      <c r="BA26" s="99"/>
-      <c r="BB26" s="41"/>
-      <c r="BC26" s="41"/>
-      <c r="BD26" s="42"/>
-      <c r="BE26" s="43"/>
-      <c r="BF26" s="53"/>
-      <c r="BG26" s="44"/>
-      <c r="BH26" s="42" t="s">
+      <c r="AY26" s="42"/>
+      <c r="AZ26" s="43"/>
+      <c r="BA26" s="53"/>
+      <c r="BB26" s="44"/>
+      <c r="BC26" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI26" s="60"/>
-      <c r="BJ26" s="61"/>
-      <c r="BK26" s="63"/>
-      <c r="BL26" s="63" t="s">
+      <c r="BD26" s="60"/>
+      <c r="BE26" s="61"/>
+      <c r="BF26" s="63"/>
+      <c r="BG26" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM26" s="42"/>
-    </row>
-    <row r="27" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BH26" s="42"/>
+    </row>
+    <row r="27" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="85" t="s">
         <v>1067</v>
@@ -9436,57 +9059,50 @@
       <c r="Z27" s="25"/>
       <c r="AA27" s="25"/>
       <c r="AB27" s="25"/>
-      <c r="AC27" s="25"/>
-      <c r="AD27" s="25"/>
-      <c r="AE27" s="25"/>
-      <c r="AF27" s="41"/>
-      <c r="AG27" s="41"/>
-      <c r="AH27" s="40"/>
+      <c r="AC27" s="41"/>
+      <c r="AD27" s="41"/>
+      <c r="AE27" s="40"/>
+      <c r="AF27" s="25"/>
+      <c r="AG27" s="25"/>
+      <c r="AH27" s="25"/>
       <c r="AI27" s="25"/>
       <c r="AJ27" s="25"/>
       <c r="AK27" s="25"/>
       <c r="AL27" s="25"/>
       <c r="AM27" s="25"/>
       <c r="AN27" s="25"/>
-      <c r="AO27" s="25"/>
-      <c r="AP27" s="25"/>
+      <c r="AO27" s="42"/>
+      <c r="AP27" s="43"/>
       <c r="AQ27" s="25"/>
-      <c r="AR27" s="25"/>
-      <c r="AS27" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT27" s="25"/>
-      <c r="AU27" s="43"/>
-      <c r="AV27" s="25"/>
+      <c r="AR27" s="41"/>
+      <c r="AS27" s="41"/>
+      <c r="AT27" s="41"/>
+      <c r="AU27" s="42"/>
+      <c r="AV27" s="99"/>
       <c r="AW27" s="41"/>
       <c r="AX27" s="41"/>
-      <c r="AY27" s="41"/>
-      <c r="AZ27" s="42"/>
-      <c r="BA27" s="99"/>
-      <c r="BB27" s="41"/>
-      <c r="BC27" s="41"/>
-      <c r="BD27" s="42"/>
-      <c r="BE27" s="43"/>
-      <c r="BF27" s="53"/>
-      <c r="BG27" s="44"/>
-      <c r="BH27" s="42" t="s">
+      <c r="AY27" s="42"/>
+      <c r="AZ27" s="43"/>
+      <c r="BA27" s="53"/>
+      <c r="BB27" s="44"/>
+      <c r="BC27" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI27" s="60"/>
-      <c r="BJ27" s="61"/>
-      <c r="BK27" s="63"/>
-      <c r="BL27" s="63" t="s">
+      <c r="BD27" s="60"/>
+      <c r="BE27" s="61"/>
+      <c r="BF27" s="63"/>
+      <c r="BG27" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM27" s="42"/>
-    </row>
-    <row r="28" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BH27" s="42"/>
+    </row>
+    <row r="28" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="85" t="s">
         <v>1073</v>
       </c>
       <c r="C28" s="140" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="D28" s="25">
         <v>3</v>
@@ -9555,51 +9171,44 @@
       <c r="Z28" s="25"/>
       <c r="AA28" s="25"/>
       <c r="AB28" s="25"/>
-      <c r="AC28" s="25"/>
-      <c r="AD28" s="25"/>
-      <c r="AE28" s="25"/>
-      <c r="AF28" s="41"/>
-      <c r="AG28" s="41"/>
-      <c r="AH28" s="40"/>
+      <c r="AC28" s="41"/>
+      <c r="AD28" s="41"/>
+      <c r="AE28" s="40"/>
+      <c r="AF28" s="25"/>
+      <c r="AG28" s="25"/>
+      <c r="AH28" s="25"/>
       <c r="AI28" s="25"/>
       <c r="AJ28" s="25"/>
       <c r="AK28" s="25"/>
       <c r="AL28" s="25"/>
       <c r="AM28" s="25"/>
       <c r="AN28" s="25"/>
-      <c r="AO28" s="25"/>
-      <c r="AP28" s="25"/>
+      <c r="AO28" s="42"/>
+      <c r="AP28" s="43"/>
       <c r="AQ28" s="25"/>
-      <c r="AR28" s="25"/>
-      <c r="AS28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT28" s="25"/>
-      <c r="AU28" s="43"/>
-      <c r="AV28" s="25"/>
+      <c r="AR28" s="41"/>
+      <c r="AS28" s="41"/>
+      <c r="AT28" s="41"/>
+      <c r="AU28" s="42"/>
+      <c r="AV28" s="99"/>
       <c r="AW28" s="41"/>
       <c r="AX28" s="41"/>
-      <c r="AY28" s="41"/>
-      <c r="AZ28" s="42"/>
-      <c r="BA28" s="99"/>
-      <c r="BB28" s="41"/>
-      <c r="BC28" s="41"/>
-      <c r="BD28" s="42"/>
-      <c r="BE28" s="43"/>
-      <c r="BF28" s="53"/>
-      <c r="BG28" s="44"/>
-      <c r="BH28" s="42" t="s">
+      <c r="AY28" s="42"/>
+      <c r="AZ28" s="43"/>
+      <c r="BA28" s="53"/>
+      <c r="BB28" s="44"/>
+      <c r="BC28" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI28" s="60"/>
-      <c r="BJ28" s="61"/>
-      <c r="BK28" s="63"/>
-      <c r="BL28" s="63" t="s">
+      <c r="BD28" s="60"/>
+      <c r="BE28" s="61"/>
+      <c r="BF28" s="63"/>
+      <c r="BG28" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM28" s="42"/>
-    </row>
-    <row r="29" spans="1:65" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="BH28" s="42"/>
+    </row>
+    <row r="29" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="4"/>
       <c r="D29" s="3"/>
@@ -9628,80 +9237,399 @@
       <c r="Y29" s="4"/>
       <c r="Z29" s="4"/>
       <c r="AA29" s="4"/>
-      <c r="AB29" s="25"/>
-      <c r="AC29" s="4"/>
-      <c r="AD29" s="4"/>
-      <c r="AE29" s="4"/>
-      <c r="AF29" s="8"/>
-      <c r="AG29" s="8"/>
-      <c r="AH29" s="5"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="8"/>
+      <c r="AD29" s="8"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="4"/>
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="4"/>
       <c r="AI29" s="4"/>
       <c r="AJ29" s="4"/>
       <c r="AK29" s="4"/>
       <c r="AL29" s="4"/>
       <c r="AM29" s="4"/>
       <c r="AN29" s="4"/>
-      <c r="AO29" s="4"/>
-      <c r="AP29" s="4"/>
+      <c r="AO29" s="6"/>
+      <c r="AP29" s="7"/>
       <c r="AQ29" s="4"/>
-      <c r="AR29" s="4"/>
-      <c r="AS29" s="4"/>
-      <c r="AT29" s="4"/>
-      <c r="AU29" s="7"/>
-      <c r="AV29" s="4"/>
+      <c r="AR29" s="8"/>
+      <c r="AS29" s="8"/>
+      <c r="AT29" s="8"/>
+      <c r="AU29" s="6"/>
+      <c r="AV29" s="100"/>
       <c r="AW29" s="8"/>
       <c r="AX29" s="8"/>
-      <c r="AY29" s="8"/>
-      <c r="AZ29" s="6"/>
-      <c r="BA29" s="100"/>
-      <c r="BB29" s="8"/>
-      <c r="BC29" s="8"/>
-      <c r="BD29" s="6"/>
-      <c r="BE29" s="7"/>
-      <c r="BF29" s="48"/>
-      <c r="BG29" s="10"/>
+      <c r="AY29" s="6"/>
+      <c r="AZ29" s="7"/>
+      <c r="BA29" s="48"/>
+      <c r="BB29" s="10"/>
+      <c r="BC29" s="6"/>
+      <c r="BD29" s="7"/>
+      <c r="BE29" s="48"/>
+      <c r="BF29" s="64"/>
+      <c r="BG29" s="64"/>
       <c r="BH29" s="6"/>
-      <c r="BI29" s="7"/>
-      <c r="BJ29" s="48"/>
-      <c r="BK29" s="64"/>
-      <c r="BL29" s="64"/>
-      <c r="BM29" s="6"/>
-    </row>
-    <row r="30" spans="1:65" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AB30" s="4"/>
+    </row>
+    <row r="33" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY33" s="45"/>
+      <c r="AZ33" s="9"/>
+      <c r="BA33" s="2"/>
+      <c r="BB33" s="2"/>
+      <c r="BC33" s="45"/>
+      <c r="BD33" s="45"/>
+      <c r="BF33" s="2"/>
+      <c r="BG33"/>
+      <c r="BH33"/>
+    </row>
+    <row r="34" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY34" s="45"/>
+      <c r="AZ34" s="9"/>
+      <c r="BA34" s="2"/>
+      <c r="BB34" s="2"/>
+      <c r="BC34" s="45"/>
+      <c r="BD34" s="45"/>
+      <c r="BF34" s="2"/>
+      <c r="BG34"/>
+      <c r="BH34"/>
+    </row>
+    <row r="35" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY35" s="45"/>
+      <c r="AZ35" s="9"/>
+      <c r="BA35" s="2"/>
+      <c r="BB35" s="2"/>
+      <c r="BC35" s="45"/>
+      <c r="BD35" s="45"/>
+      <c r="BF35" s="2"/>
+      <c r="BG35"/>
+      <c r="BH35"/>
+    </row>
+    <row r="36" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY36" s="45"/>
+      <c r="AZ36" s="9"/>
+      <c r="BA36" s="2"/>
+      <c r="BB36" s="2"/>
+      <c r="BC36" s="45"/>
+      <c r="BD36" s="45"/>
+      <c r="BF36" s="2"/>
+      <c r="BG36"/>
+      <c r="BH36"/>
+    </row>
+    <row r="37" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY37" s="45"/>
+      <c r="AZ37" s="9"/>
+      <c r="BA37" s="2"/>
+      <c r="BB37" s="2"/>
+      <c r="BC37" s="45"/>
+      <c r="BD37" s="45"/>
+      <c r="BF37" s="2"/>
+      <c r="BG37"/>
+      <c r="BH37"/>
+    </row>
+    <row r="38" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY38" s="45"/>
+      <c r="AZ38" s="9"/>
+      <c r="BA38" s="2"/>
+      <c r="BB38" s="2"/>
+      <c r="BC38" s="45"/>
+      <c r="BD38" s="45"/>
+      <c r="BF38" s="2"/>
+      <c r="BG38"/>
+      <c r="BH38"/>
+    </row>
+    <row r="39" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY39" s="45"/>
+      <c r="AZ39" s="9"/>
+      <c r="BA39" s="2"/>
+      <c r="BB39" s="2"/>
+      <c r="BC39" s="45"/>
+      <c r="BD39" s="45"/>
+      <c r="BF39" s="2"/>
+      <c r="BG39"/>
+      <c r="BH39"/>
+    </row>
+    <row r="40" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY40" s="45"/>
+      <c r="AZ40" s="9"/>
+      <c r="BA40" s="2"/>
+      <c r="BB40" s="2"/>
+      <c r="BC40" s="45"/>
+      <c r="BD40" s="45"/>
+      <c r="BF40" s="2"/>
+      <c r="BG40"/>
+      <c r="BH40"/>
+    </row>
+    <row r="41" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY41" s="45"/>
+      <c r="AZ41" s="9"/>
+      <c r="BA41" s="2"/>
+      <c r="BB41" s="2"/>
+      <c r="BC41" s="45"/>
+      <c r="BD41" s="45"/>
+      <c r="BF41" s="2"/>
+      <c r="BG41"/>
+      <c r="BH41"/>
+    </row>
+    <row r="42" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY42" s="45"/>
+      <c r="AZ42" s="9"/>
+      <c r="BA42" s="2"/>
+      <c r="BB42" s="2"/>
+      <c r="BC42" s="45"/>
+      <c r="BD42" s="45"/>
+      <c r="BF42" s="2"/>
+      <c r="BG42"/>
+      <c r="BH42"/>
+    </row>
+    <row r="43" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY43" s="45"/>
+      <c r="AZ43" s="9"/>
+      <c r="BA43" s="2"/>
+      <c r="BB43" s="2"/>
+      <c r="BC43" s="45"/>
+      <c r="BD43" s="45"/>
+      <c r="BF43" s="2"/>
+      <c r="BG43"/>
+      <c r="BH43"/>
+    </row>
+    <row r="44" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY44" s="45"/>
+      <c r="AZ44" s="9"/>
+      <c r="BA44" s="2"/>
+      <c r="BB44" s="2"/>
+      <c r="BC44" s="45"/>
+      <c r="BD44" s="45"/>
+      <c r="BF44" s="2"/>
+      <c r="BG44"/>
+      <c r="BH44"/>
+    </row>
+    <row r="45" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY45" s="45"/>
+      <c r="AZ45" s="9"/>
+      <c r="BA45" s="2"/>
+      <c r="BB45" s="2"/>
+      <c r="BC45" s="45"/>
+      <c r="BD45" s="45"/>
+      <c r="BF45" s="2"/>
+      <c r="BG45"/>
+      <c r="BH45"/>
+    </row>
+    <row r="46" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY46" s="45"/>
+      <c r="AZ46" s="9"/>
+      <c r="BA46" s="2"/>
+      <c r="BB46" s="2"/>
+      <c r="BC46" s="45"/>
+      <c r="BD46" s="45"/>
+      <c r="BF46" s="2"/>
+      <c r="BG46"/>
+      <c r="BH46"/>
+    </row>
+    <row r="47" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY47" s="45"/>
+      <c r="AZ47" s="9"/>
+      <c r="BA47" s="2"/>
+      <c r="BB47" s="2"/>
+      <c r="BC47" s="45"/>
+      <c r="BD47" s="45"/>
+      <c r="BF47" s="2"/>
+      <c r="BG47"/>
+      <c r="BH47"/>
+    </row>
+    <row r="48" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY48" s="45"/>
+      <c r="AZ48" s="9"/>
+      <c r="BA48" s="2"/>
+      <c r="BB48" s="2"/>
+      <c r="BC48" s="45"/>
+      <c r="BD48" s="45"/>
+      <c r="BF48" s="2"/>
+      <c r="BG48"/>
+      <c r="BH48"/>
+    </row>
+    <row r="49" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY49" s="45"/>
+      <c r="AZ49" s="9"/>
+      <c r="BA49" s="2"/>
+      <c r="BB49" s="2"/>
+      <c r="BC49" s="45"/>
+      <c r="BD49" s="45"/>
+      <c r="BF49" s="2"/>
+      <c r="BG49"/>
+      <c r="BH49"/>
+    </row>
+    <row r="50" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY50" s="45"/>
+      <c r="AZ50" s="9"/>
+      <c r="BA50" s="2"/>
+      <c r="BB50" s="2"/>
+      <c r="BC50" s="45"/>
+      <c r="BD50" s="45"/>
+      <c r="BF50" s="2"/>
+      <c r="BG50"/>
+      <c r="BH50"/>
+    </row>
+    <row r="51" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY51" s="45"/>
+      <c r="AZ51" s="9"/>
+      <c r="BA51" s="2"/>
+      <c r="BB51" s="2"/>
+      <c r="BC51" s="45"/>
+      <c r="BD51" s="45"/>
+      <c r="BF51" s="2"/>
+      <c r="BG51"/>
+      <c r="BH51"/>
+    </row>
+    <row r="52" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY52" s="45"/>
+      <c r="AZ52" s="9"/>
+      <c r="BA52" s="2"/>
+      <c r="BB52" s="2"/>
+      <c r="BC52" s="45"/>
+      <c r="BD52" s="45"/>
+      <c r="BF52" s="2"/>
+      <c r="BG52"/>
+      <c r="BH52"/>
+    </row>
+    <row r="53" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY53" s="45"/>
+      <c r="AZ53" s="9"/>
+      <c r="BA53" s="2"/>
+      <c r="BB53" s="2"/>
+      <c r="BC53" s="45"/>
+      <c r="BD53" s="45"/>
+      <c r="BF53" s="2"/>
+      <c r="BG53"/>
+      <c r="BH53"/>
+    </row>
+    <row r="54" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY54" s="45"/>
+      <c r="AZ54" s="9"/>
+      <c r="BA54" s="2"/>
+      <c r="BB54" s="2"/>
+      <c r="BC54" s="45"/>
+      <c r="BD54" s="45"/>
+      <c r="BF54" s="2"/>
+      <c r="BG54"/>
+      <c r="BH54"/>
+    </row>
+    <row r="55" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY55" s="45"/>
+      <c r="AZ55" s="9"/>
+      <c r="BA55" s="2"/>
+      <c r="BB55" s="2"/>
+      <c r="BC55" s="45"/>
+      <c r="BD55" s="45"/>
+      <c r="BF55" s="2"/>
+      <c r="BG55"/>
+      <c r="BH55"/>
+    </row>
+    <row r="56" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY56" s="45"/>
+      <c r="AZ56" s="9"/>
+      <c r="BA56" s="2"/>
+      <c r="BB56" s="2"/>
+      <c r="BC56" s="45"/>
+      <c r="BD56" s="45"/>
+      <c r="BF56" s="2"/>
+      <c r="BG56"/>
+      <c r="BH56"/>
+    </row>
+    <row r="57" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY57" s="45"/>
+      <c r="AZ57" s="9"/>
+      <c r="BA57" s="2"/>
+      <c r="BB57" s="2"/>
+      <c r="BC57" s="45"/>
+      <c r="BD57" s="45"/>
+      <c r="BF57" s="2"/>
+      <c r="BG57"/>
+      <c r="BH57"/>
+    </row>
+    <row r="58" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY58" s="45"/>
+      <c r="AZ58" s="9"/>
+      <c r="BA58" s="2"/>
+      <c r="BB58" s="2"/>
+      <c r="BC58" s="45"/>
+      <c r="BD58" s="45"/>
+      <c r="BF58" s="2"/>
+      <c r="BG58"/>
+      <c r="BH58"/>
+    </row>
+    <row r="59" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY59" s="45"/>
+      <c r="AZ59" s="9"/>
+      <c r="BA59" s="2"/>
+      <c r="BB59" s="2"/>
+      <c r="BC59" s="45"/>
+      <c r="BD59" s="45"/>
+      <c r="BF59" s="2"/>
+      <c r="BG59"/>
+      <c r="BH59"/>
+    </row>
+    <row r="60" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY60" s="45"/>
+      <c r="AZ60" s="9"/>
+      <c r="BA60" s="2"/>
+      <c r="BB60" s="2"/>
+      <c r="BC60" s="45"/>
+      <c r="BD60" s="45"/>
+      <c r="BF60" s="2"/>
+      <c r="BG60"/>
+      <c r="BH60"/>
+    </row>
+    <row r="61" spans="51:60" x14ac:dyDescent="0.2">
+      <c r="AY61" s="45"/>
+      <c r="AZ61" s="9"/>
+      <c r="BA61" s="2"/>
+      <c r="BB61" s="2"/>
+      <c r="BC61" s="45"/>
+      <c r="BD61" s="45"/>
+      <c r="BF61" s="2"/>
+      <c r="BG61"/>
+      <c r="BH61"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="BI2:BM2"/>
+    <mergeCell ref="BD2:BH2"/>
     <mergeCell ref="H2:V2"/>
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="W2:AG2"/>
-    <mergeCell ref="AH2:AT2"/>
-    <mergeCell ref="AU2:AZ2"/>
-    <mergeCell ref="BA2:BD2"/>
-    <mergeCell ref="BE2:BH2"/>
+    <mergeCell ref="W2:AD2"/>
+    <mergeCell ref="AE2:AO2"/>
+    <mergeCell ref="AP2:AU2"/>
+    <mergeCell ref="AV2:AY2"/>
+    <mergeCell ref="AZ2:BC2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A29:G30 AB14 W14:AA30 A4:G27 W4:BM13 AC14:BM30 H4:V30">
-    <cfRule type="expression" dxfId="24" priority="11" stopIfTrue="1">
+  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 A4:G27 AA14 AA18:AA29 W4:BH13 AB14:BH30">
+    <cfRule type="expression" dxfId="26" priority="17" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="18" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28">
-    <cfRule type="expression" dxfId="22" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="15" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="16" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB15:AB30">
-    <cfRule type="expression" dxfId="18" priority="23" stopIfTrue="1">
+  <conditionalFormatting sqref="AA16:AA17">
+    <cfRule type="expression" dxfId="22" priority="29" stopIfTrue="1">
+      <formula>$A15="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="30" stopIfTrue="1">
+      <formula>$A15="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA15">
+    <cfRule type="expression" dxfId="20" priority="1" stopIfTrue="1">
       <formula>$A14="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="2" stopIfTrue="1">
       <formula>$A14="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9719,10 +9647,10 @@
   <dimension ref="A1:BC50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="O4" sqref="O4:O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13716,42 +13644,42 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A4:BC21 C29:F32 A29:B33 G29:BC31 I33:BC33 I32:K32 M32:BC32 J22:AI27 AK22:BC27 A22:G27">
-    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="15" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="16" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28 J28:AI28 AK28:BC28">
-    <cfRule type="expression" dxfId="14" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="5" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="6" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="12" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="19" stopIfTrue="1">
       <formula>$A32="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="20" stopIfTrue="1">
       <formula>$A32="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I28">
-    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="3" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ22:AJ28">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="1" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="2" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45197,31 +45125,31 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="C782:C787 C844:C855 C789:C842">
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
       <formula>$A782=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
       <formula>$A782=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B336:C353 B764:C769 B301:C303 B4:C10 B297:C299 B38:C49 B25:C36 B496:C528 B12:C23 B844:B855 B315:C326 B530:C539 B541:C550 B728:C743 B745:C748 B750:C758 B332:C334 B771:C780 B328:C330 B760:C760 B762:C762 B305:C313 B355:C358 B782:B787 B552:C561 B51:C131 B133:C213 B215:C295 B360:C494 B563:C616 B673:C726 B618:C671 B789:B842">
-    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
       <formula>$A4=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2 D2:Z2">
-    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A10 A12:A23 A25:A36 A38:A49 A297:A299 A301:A303 A305:A313 A315:A326 A328:A330 A332:A334 A336:A353 A355:A358 A496:A528 A530:A539 A541:A550 A552:A561 A745:A748 A750:A758 A760 A762 A764:A769 A771:A780 A782:A787 A844:A855 A51:A131 A133:A213 A215:A295 A360:A494 A563:A616 A673:A726 A618:A671 A728:A743 A789:A842">
-    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="7" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
renamed test25 aerodyn input file to have .dat extension instead of .ipt (consistent with other modules/tests)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@753 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="2790" windowWidth="15180" windowHeight="8715" tabRatio="712"/>
+    <workbookView xWindow="5955" yWindow="2850" windowWidth="15180" windowHeight="8655" tabRatio="712"/>
   </bookViews>
   <sheets>
     <sheet name="TestMatrix (new)" sheetId="3" r:id="rId1"/>
@@ -4547,7 +4547,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="35">
     <dxf>
       <font>
         <condense val="0"/>
@@ -4630,34 +4630,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
     </dxf>
     <dxf>
       <font>

</xml_diff>

<commit_message>
+ modified error message so that it's TowerBsHt that must be > 0 on floating systems (not PtfmRefzt). + changed comment on HD input files description of waveMod (updated template file). also fixed the comment line describing the HD input file contents on a couple of models + recompiled, reran certtest, and updated TstFiles/CertTest.out + modified ReadMe based on JMJ comments
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@755 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="2850" windowWidth="15180" windowHeight="8655" tabRatio="712"/>
+    <workbookView xWindow="5955" yWindow="2910" windowWidth="15180" windowHeight="8595" tabRatio="712"/>
   </bookViews>
   <sheets>
     <sheet name="TestMatrix (new)" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2726" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2803" uniqueCount="1122">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3382,6 +3382,39 @@
   </si>
   <si>
     <t>ServoDyn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flexible, DLL control, tower potential flow and drag, turbulence </t>
+  </si>
+  <si>
+    <t>Flexible, DLL control, tower potential flow, turbulence, irregular waves</t>
+  </si>
+  <si>
+    <t>Flexible, DLL control, tower potential flow, turbulence, irregular waves, marine growth</t>
+  </si>
+  <si>
+    <t>Flexible, DLL control, irregular &amp; multidirectional waves, turbulence</t>
+  </si>
+  <si>
+    <t>Flexible, DLL control, turbulence, irregular waves</t>
+  </si>
+  <si>
+    <t>OC4 Load Case (LC) 3.7: steady wind, white noise waves</t>
+  </si>
+  <si>
+    <t>Flexible, DLL control, tower potential flow, steady wind, regular waves with 0 phase</t>
+  </si>
+  <si>
+    <t>Test25</t>
+  </si>
+  <si>
+    <t>Test24</t>
+  </si>
+  <si>
+    <t>Test23</t>
+  </si>
+  <si>
+    <t>Test22</t>
   </si>
 </sst>
 </file>
@@ -4070,7 +4103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4399,63 +4432,6 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4466,12 +4442,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4520,9 +4490,6 @@
     <xf numFmtId="1" fontId="2" fillId="12" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -4532,9 +4499,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
@@ -4542,12 +4506,200 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -4630,62 +4782,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -5116,133 +5212,136 @@
   <dimension ref="A1:BH61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BG24" sqref="BG23:BG24"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8" style="2" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="171" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.28515625" customWidth="1"/>
     <col min="8" max="8" width="3.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="18" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3.28515625" style="2" customWidth="1"/>
     <col min="20" max="20" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="25" width="3.28515625" style="2" customWidth="1"/>
-    <col min="26" max="26" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="4.28515625" style="2" customWidth="1"/>
     <col min="28" max="28" width="3.28515625" style="2" customWidth="1"/>
-    <col min="29" max="29" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="41" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.5703125" style="2" customWidth="1"/>
-    <col min="43" max="52" width="4.85546875" style="2" customWidth="1"/>
-    <col min="53" max="53" width="4.85546875" style="45" customWidth="1"/>
-    <col min="54" max="54" width="4.85546875" style="9" customWidth="1"/>
-    <col min="55" max="56" width="4.85546875" style="2" customWidth="1"/>
-    <col min="57" max="58" width="4.85546875" style="45" customWidth="1"/>
-    <col min="59" max="59" width="6.7109375" style="45" customWidth="1"/>
-    <col min="60" max="60" width="4.85546875" style="2" customWidth="1"/>
+    <col min="29" max="30" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="41" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="47" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="51" width="4.85546875" style="2" customWidth="1"/>
+    <col min="52" max="52" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="4.5703125" style="45" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="3.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="3.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="5.7109375" style="45" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="5" style="2" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="4.42578125" customWidth="1"/>
     <col min="62" max="62" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="161" t="s">
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="149" t="s">
         <v>1104</v>
       </c>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="143"/>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="143"/>
-      <c r="O2" s="143"/>
-      <c r="P2" s="143"/>
-      <c r="Q2" s="143"/>
-      <c r="R2" s="143"/>
-      <c r="S2" s="143"/>
-      <c r="T2" s="143"/>
-      <c r="U2" s="143"/>
-      <c r="V2" s="144"/>
-      <c r="W2" s="127" t="s">
+      <c r="I2" s="150"/>
+      <c r="J2" s="150"/>
+      <c r="K2" s="150"/>
+      <c r="L2" s="150"/>
+      <c r="M2" s="150"/>
+      <c r="N2" s="150"/>
+      <c r="O2" s="150"/>
+      <c r="P2" s="150"/>
+      <c r="Q2" s="150"/>
+      <c r="R2" s="150"/>
+      <c r="S2" s="150"/>
+      <c r="T2" s="150"/>
+      <c r="U2" s="150"/>
+      <c r="V2" s="151"/>
+      <c r="W2" s="147" t="s">
         <v>1110</v>
       </c>
-      <c r="X2" s="135"/>
-      <c r="Y2" s="135"/>
-      <c r="Z2" s="135"/>
-      <c r="AA2" s="135"/>
-      <c r="AB2" s="135"/>
-      <c r="AC2" s="135"/>
-      <c r="AD2" s="136"/>
-      <c r="AE2" s="129" t="s">
+      <c r="X2" s="155"/>
+      <c r="Y2" s="155"/>
+      <c r="Z2" s="155"/>
+      <c r="AA2" s="155"/>
+      <c r="AB2" s="155"/>
+      <c r="AC2" s="155"/>
+      <c r="AD2" s="156"/>
+      <c r="AE2" s="157" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" s="130"/>
-      <c r="AG2" s="130"/>
-      <c r="AH2" s="130"/>
-      <c r="AI2" s="130"/>
-      <c r="AJ2" s="130"/>
-      <c r="AK2" s="130"/>
-      <c r="AL2" s="130"/>
-      <c r="AM2" s="130"/>
-      <c r="AN2" s="130"/>
-      <c r="AO2" s="131"/>
-      <c r="AP2" s="124" t="s">
+      <c r="AF2" s="158"/>
+      <c r="AG2" s="158"/>
+      <c r="AH2" s="158"/>
+      <c r="AI2" s="158"/>
+      <c r="AJ2" s="158"/>
+      <c r="AK2" s="158"/>
+      <c r="AL2" s="158"/>
+      <c r="AM2" s="158"/>
+      <c r="AN2" s="158"/>
+      <c r="AO2" s="159"/>
+      <c r="AP2" s="160" t="s">
         <v>43</v>
       </c>
-      <c r="AQ2" s="137"/>
-      <c r="AR2" s="137"/>
-      <c r="AS2" s="137"/>
-      <c r="AT2" s="137"/>
-      <c r="AU2" s="138"/>
-      <c r="AV2" s="123" t="s">
+      <c r="AQ2" s="161"/>
+      <c r="AR2" s="161"/>
+      <c r="AS2" s="161"/>
+      <c r="AT2" s="161"/>
+      <c r="AU2" s="162"/>
+      <c r="AV2" s="163" t="s">
         <v>1061</v>
       </c>
-      <c r="AW2" s="124"/>
-      <c r="AX2" s="124"/>
-      <c r="AY2" s="125"/>
-      <c r="AZ2" s="132" t="s">
+      <c r="AW2" s="160"/>
+      <c r="AX2" s="160"/>
+      <c r="AY2" s="164"/>
+      <c r="AZ2" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="BA2" s="133"/>
-      <c r="BB2" s="133"/>
-      <c r="BC2" s="134"/>
-      <c r="BD2" s="126" t="s">
+      <c r="BA2" s="166"/>
+      <c r="BB2" s="166"/>
+      <c r="BC2" s="167"/>
+      <c r="BD2" s="146" t="s">
         <v>1047</v>
       </c>
-      <c r="BE2" s="127"/>
-      <c r="BF2" s="127"/>
-      <c r="BG2" s="127"/>
-      <c r="BH2" s="128"/>
-    </row>
-    <row r="3" spans="1:60" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="BE2" s="147"/>
+      <c r="BF2" s="147"/>
+      <c r="BG2" s="147"/>
+      <c r="BH2" s="148"/>
+    </row>
+    <row r="3" spans="1:60" s="1" customFormat="1" ht="85.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
       <c r="B3" s="79" t="s">
         <v>287</v>
       </c>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="122" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="80" t="s">
@@ -5254,52 +5353,52 @@
       <c r="F3" s="80" t="s">
         <v>488</v>
       </c>
-      <c r="G3" s="164" t="s">
+      <c r="G3" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="162" t="s">
+      <c r="H3" s="140" t="s">
         <v>1090</v>
       </c>
-      <c r="I3" s="145" t="s">
+      <c r="I3" s="124" t="s">
         <v>1091</v>
       </c>
-      <c r="J3" s="145" t="s">
+      <c r="J3" s="124" t="s">
         <v>1092</v>
       </c>
-      <c r="K3" s="145" t="s">
+      <c r="K3" s="124" t="s">
         <v>1093</v>
       </c>
-      <c r="L3" s="145" t="s">
+      <c r="L3" s="124" t="s">
         <v>1094</v>
       </c>
-      <c r="M3" s="145" t="s">
+      <c r="M3" s="124" t="s">
         <v>1097</v>
       </c>
-      <c r="N3" s="145" t="s">
+      <c r="N3" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="145" t="s">
+      <c r="O3" s="124" t="s">
         <v>1098</v>
       </c>
-      <c r="P3" s="145" t="s">
+      <c r="P3" s="124" t="s">
         <v>1063</v>
       </c>
-      <c r="Q3" s="145" t="s">
+      <c r="Q3" s="124" t="s">
         <v>1099</v>
       </c>
-      <c r="R3" s="145" t="s">
+      <c r="R3" s="124" t="s">
         <v>1100</v>
       </c>
-      <c r="S3" s="145" t="s">
+      <c r="S3" s="124" t="s">
         <v>1101</v>
       </c>
-      <c r="T3" s="146" t="s">
+      <c r="T3" s="125" t="s">
         <v>1095</v>
       </c>
-      <c r="U3" s="146" t="s">
+      <c r="U3" s="125" t="s">
         <v>1103</v>
       </c>
-      <c r="V3" s="147" t="s">
+      <c r="V3" s="126" t="s">
         <v>1096</v>
       </c>
       <c r="W3" s="66" t="s">
@@ -5356,10 +5455,10 @@
       <c r="AN3" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="AO3" s="170" t="s">
+      <c r="AO3" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="AP3" s="169" t="s">
+      <c r="AP3" s="144" t="s">
         <v>44</v>
       </c>
       <c r="AQ3" s="72" t="s">
@@ -5414,7 +5513,7 @@
       <c r="B4" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="139" t="s">
+      <c r="C4" s="172" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="29">
@@ -5426,13 +5525,13 @@
       <c r="F4" s="55">
         <v>175</v>
       </c>
-      <c r="G4" s="165" t="s">
+      <c r="G4" s="168" t="s">
         <v>497</v>
       </c>
-      <c r="H4" s="163">
+      <c r="H4" s="141">
         <v>20</v>
       </c>
-      <c r="I4" s="139">
+      <c r="I4" s="120">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="J4" s="29">
@@ -5465,7 +5564,7 @@
       <c r="S4" s="25">
         <v>0</v>
       </c>
-      <c r="T4" s="139">
+      <c r="T4" s="120">
         <v>0.02</v>
       </c>
       <c r="U4" s="29">
@@ -5587,7 +5686,7 @@
       <c r="B5" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="139" t="s">
+      <c r="C5" s="172" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="29">
@@ -5599,13 +5698,13 @@
       <c r="F5" s="55">
         <v>175</v>
       </c>
-      <c r="G5" s="166" t="s">
+      <c r="G5" s="169" t="s">
         <v>1106</v>
       </c>
       <c r="H5" s="40">
         <v>20</v>
       </c>
-      <c r="I5" s="140">
+      <c r="I5" s="121">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="J5" s="25">
@@ -5638,10 +5737,10 @@
       <c r="S5" s="25">
         <v>0</v>
       </c>
-      <c r="T5" s="148">
+      <c r="T5" s="127">
         <v>0.04</v>
       </c>
-      <c r="U5" s="142">
+      <c r="U5" s="123">
         <v>5</v>
       </c>
       <c r="V5" s="38">
@@ -5760,7 +5859,7 @@
       <c r="B6" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="139" t="s">
+      <c r="C6" s="172" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="29">
@@ -5772,13 +5871,13 @@
       <c r="F6" s="55">
         <v>175</v>
       </c>
-      <c r="G6" s="166" t="s">
+      <c r="G6" s="169" t="s">
         <v>491</v>
       </c>
       <c r="H6" s="40">
         <v>20</v>
       </c>
-      <c r="I6" s="140">
+      <c r="I6" s="121">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="J6" s="25">
@@ -5811,10 +5910,10 @@
       <c r="S6" s="25">
         <v>0</v>
       </c>
-      <c r="T6" s="148">
+      <c r="T6" s="127">
         <v>0.02</v>
       </c>
-      <c r="U6" s="142">
+      <c r="U6" s="123">
         <v>10</v>
       </c>
       <c r="V6" s="38">
@@ -5933,7 +6032,7 @@
       <c r="B7" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="139" t="s">
+      <c r="C7" s="172" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="29">
@@ -5945,13 +6044,13 @@
       <c r="F7" s="55">
         <v>175</v>
       </c>
-      <c r="G7" s="166" t="s">
+      <c r="G7" s="169" t="s">
         <v>492</v>
       </c>
       <c r="H7" s="40">
         <v>70</v>
       </c>
-      <c r="I7" s="140">
+      <c r="I7" s="121">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="J7" s="25">
@@ -5984,10 +6083,10 @@
       <c r="S7" s="25">
         <v>0</v>
       </c>
-      <c r="T7" s="148">
+      <c r="T7" s="127">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="U7" s="142">
+      <c r="U7" s="123">
         <v>10</v>
       </c>
       <c r="V7" s="38">
@@ -6106,7 +6205,7 @@
       <c r="B8" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="139" t="s">
+      <c r="C8" s="172" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="29">
@@ -6118,13 +6217,13 @@
       <c r="F8" s="55">
         <v>175</v>
       </c>
-      <c r="G8" s="166" t="s">
+      <c r="G8" s="169" t="s">
         <v>1106</v>
       </c>
       <c r="H8" s="40">
         <v>30</v>
       </c>
-      <c r="I8" s="140">
+      <c r="I8" s="121">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="J8" s="25">
@@ -6157,10 +6256,10 @@
       <c r="S8" s="25">
         <v>0</v>
       </c>
-      <c r="T8" s="148">
+      <c r="T8" s="127">
         <v>0.04</v>
       </c>
-      <c r="U8" s="142">
+      <c r="U8" s="123">
         <v>5</v>
       </c>
       <c r="V8" s="38">
@@ -6279,7 +6378,7 @@
       <c r="B9" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="140" t="s">
+      <c r="C9" s="173" t="s">
         <v>279</v>
       </c>
       <c r="D9" s="25">
@@ -6292,13 +6391,13 @@
       <c r="F9" s="25">
         <v>50</v>
       </c>
-      <c r="G9" s="166" t="s">
+      <c r="G9" s="169" t="s">
         <v>1106</v>
       </c>
       <c r="H9" s="40">
         <v>35</v>
       </c>
-      <c r="I9" s="140">
+      <c r="I9" s="121">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J9" s="25">
@@ -6331,10 +6430,10 @@
       <c r="S9" s="25">
         <v>0</v>
       </c>
-      <c r="T9" s="148">
+      <c r="T9" s="127">
         <v>0.05</v>
       </c>
-      <c r="U9" s="142">
+      <c r="U9" s="123">
         <v>5</v>
       </c>
       <c r="V9" s="38">
@@ -6453,7 +6552,7 @@
       <c r="B10" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="140" t="s">
+      <c r="C10" s="173" t="s">
         <v>279</v>
       </c>
       <c r="D10" s="25">
@@ -6466,13 +6565,13 @@
       <c r="F10" s="25">
         <v>50</v>
       </c>
-      <c r="G10" s="166" t="s">
+      <c r="G10" s="169" t="s">
         <v>492</v>
       </c>
       <c r="H10" s="40">
         <v>70</v>
       </c>
-      <c r="I10" s="140">
+      <c r="I10" s="121">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J10" s="25">
@@ -6505,7 +6604,7 @@
       <c r="S10" s="25">
         <v>0</v>
       </c>
-      <c r="T10" s="140">
+      <c r="T10" s="121">
         <v>0.05</v>
       </c>
       <c r="U10" s="25">
@@ -6627,7 +6726,7 @@
       <c r="B11" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="140" t="s">
+      <c r="C11" s="173" t="s">
         <v>279</v>
       </c>
       <c r="D11" s="25">
@@ -6640,13 +6739,13 @@
       <c r="F11" s="25">
         <v>50</v>
       </c>
-      <c r="G11" s="165" t="s">
+      <c r="G11" s="168" t="s">
         <v>497</v>
       </c>
       <c r="H11" s="40">
         <v>20</v>
       </c>
-      <c r="I11" s="140">
+      <c r="I11" s="121">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J11" s="25">
@@ -6679,7 +6778,7 @@
       <c r="S11" s="25">
         <v>0</v>
       </c>
-      <c r="T11" s="140">
+      <c r="T11" s="121">
         <v>0.05</v>
       </c>
       <c r="U11" s="25">
@@ -6801,7 +6900,7 @@
       <c r="B12" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="140" t="s">
+      <c r="C12" s="173" t="s">
         <v>489</v>
       </c>
       <c r="D12" s="25">
@@ -6813,13 +6912,13 @@
       <c r="F12" s="25">
         <v>20</v>
       </c>
-      <c r="G12" s="166" t="s">
+      <c r="G12" s="169" t="s">
         <v>493</v>
       </c>
       <c r="H12" s="40">
         <v>40</v>
       </c>
-      <c r="I12" s="140">
+      <c r="I12" s="121">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="J12" s="25">
@@ -6852,7 +6951,7 @@
       <c r="S12" s="25">
         <v>0</v>
       </c>
-      <c r="T12" s="140">
+      <c r="T12" s="121">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="U12" s="25">
@@ -6974,7 +7073,7 @@
       <c r="B13" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="140" t="s">
+      <c r="C13" s="173" t="s">
         <v>490</v>
       </c>
       <c r="D13" s="25">
@@ -6986,13 +7085,13 @@
       <c r="F13" s="25">
         <v>20</v>
       </c>
-      <c r="G13" s="166" t="s">
+      <c r="G13" s="169" t="s">
         <v>496</v>
       </c>
       <c r="H13" s="40">
         <v>25</v>
       </c>
-      <c r="I13" s="140">
+      <c r="I13" s="121">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="J13" s="25">
@@ -7025,7 +7124,7 @@
       <c r="S13" s="25">
         <v>0</v>
       </c>
-      <c r="T13" s="140">
+      <c r="T13" s="121">
         <v>0.1</v>
       </c>
       <c r="U13" s="25">
@@ -7142,12 +7241,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="140" t="s">
+      <c r="C14" s="173" t="s">
         <v>286</v>
       </c>
       <c r="D14" s="25">
@@ -7159,13 +7258,13 @@
       <c r="F14" s="25">
         <v>1500</v>
       </c>
-      <c r="G14" s="166" t="s">
+      <c r="G14" s="169" t="s">
         <v>500</v>
       </c>
       <c r="H14" s="40">
         <v>20</v>
       </c>
-      <c r="I14" s="140">
+      <c r="I14" s="121">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J14" s="25">
@@ -7198,7 +7297,7 @@
       <c r="S14" s="25">
         <v>0</v>
       </c>
-      <c r="T14" s="140">
+      <c r="T14" s="121">
         <v>0.05</v>
       </c>
       <c r="U14" s="25">
@@ -7315,12 +7414,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="140" t="s">
+      <c r="C15" s="173" t="s">
         <v>286</v>
       </c>
       <c r="D15" s="25">
@@ -7332,13 +7431,13 @@
       <c r="F15" s="25">
         <v>1500</v>
       </c>
-      <c r="G15" s="166" t="s">
+      <c r="G15" s="169" t="s">
         <v>494</v>
       </c>
       <c r="H15" s="40">
         <v>20</v>
       </c>
-      <c r="I15" s="140">
+      <c r="I15" s="121">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J15" s="25">
@@ -7371,7 +7470,7 @@
       <c r="S15" s="25">
         <v>0</v>
       </c>
-      <c r="T15" s="140">
+      <c r="T15" s="121">
         <v>0.05</v>
       </c>
       <c r="U15" s="25">
@@ -7488,12 +7587,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="140" t="s">
+      <c r="C16" s="173" t="s">
         <v>286</v>
       </c>
       <c r="D16" s="25">
@@ -7505,13 +7604,13 @@
       <c r="F16" s="25">
         <v>1500</v>
       </c>
-      <c r="G16" s="166" t="s">
+      <c r="G16" s="169" t="s">
         <v>495</v>
       </c>
       <c r="H16" s="40">
         <v>40</v>
       </c>
-      <c r="I16" s="140">
+      <c r="I16" s="121">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J16" s="25">
@@ -7544,7 +7643,7 @@
       <c r="S16" s="25">
         <v>0</v>
       </c>
-      <c r="T16" s="140">
+      <c r="T16" s="121">
         <v>0.05</v>
       </c>
       <c r="U16" s="25">
@@ -7663,72 +7762,72 @@
     </row>
     <row r="17" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
-      <c r="B17" s="149"/>
-      <c r="C17" s="150"/>
-      <c r="D17" s="151"/>
-      <c r="E17" s="151"/>
-      <c r="F17" s="151"/>
-      <c r="G17" s="167"/>
-      <c r="H17" s="149"/>
-      <c r="I17" s="150"/>
-      <c r="J17" s="151"/>
-      <c r="K17" s="151"/>
-      <c r="L17" s="151"/>
-      <c r="M17" s="151"/>
-      <c r="N17" s="151"/>
-      <c r="O17" s="151"/>
-      <c r="P17" s="151"/>
-      <c r="Q17" s="151"/>
-      <c r="R17" s="151"/>
-      <c r="S17" s="151"/>
-      <c r="T17" s="150"/>
-      <c r="U17" s="151"/>
-      <c r="V17" s="154"/>
-      <c r="W17" s="152"/>
-      <c r="X17" s="151"/>
-      <c r="Y17" s="151"/>
-      <c r="Z17" s="151"/>
-      <c r="AA17" s="151"/>
-      <c r="AB17" s="151"/>
-      <c r="AC17" s="153"/>
-      <c r="AD17" s="153"/>
-      <c r="AE17" s="149"/>
-      <c r="AF17" s="151"/>
-      <c r="AG17" s="151"/>
-      <c r="AH17" s="151"/>
-      <c r="AI17" s="151"/>
-      <c r="AJ17" s="151"/>
-      <c r="AK17" s="151"/>
-      <c r="AL17" s="151"/>
-      <c r="AM17" s="151"/>
-      <c r="AN17" s="151"/>
-      <c r="AO17" s="154"/>
-      <c r="AP17" s="152"/>
-      <c r="AQ17" s="151"/>
-      <c r="AR17" s="153"/>
-      <c r="AS17" s="153"/>
-      <c r="AT17" s="153"/>
-      <c r="AU17" s="154"/>
-      <c r="AV17" s="155"/>
-      <c r="AW17" s="153"/>
-      <c r="AX17" s="153"/>
-      <c r="AY17" s="154"/>
-      <c r="AZ17" s="152"/>
-      <c r="BA17" s="156"/>
-      <c r="BB17" s="157"/>
-      <c r="BC17" s="154"/>
-      <c r="BD17" s="158"/>
-      <c r="BE17" s="159"/>
-      <c r="BF17" s="160"/>
-      <c r="BG17" s="160"/>
-      <c r="BH17" s="154"/>
-    </row>
-    <row r="18" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="128"/>
+      <c r="C17" s="174"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="130"/>
+      <c r="G17" s="170"/>
+      <c r="H17" s="128"/>
+      <c r="I17" s="129"/>
+      <c r="J17" s="130"/>
+      <c r="K17" s="130"/>
+      <c r="L17" s="130"/>
+      <c r="M17" s="130"/>
+      <c r="N17" s="130"/>
+      <c r="O17" s="130"/>
+      <c r="P17" s="130"/>
+      <c r="Q17" s="130"/>
+      <c r="R17" s="130"/>
+      <c r="S17" s="130"/>
+      <c r="T17" s="129"/>
+      <c r="U17" s="130"/>
+      <c r="V17" s="133"/>
+      <c r="W17" s="131"/>
+      <c r="X17" s="130"/>
+      <c r="Y17" s="130"/>
+      <c r="Z17" s="130"/>
+      <c r="AA17" s="130"/>
+      <c r="AB17" s="130"/>
+      <c r="AC17" s="132"/>
+      <c r="AD17" s="132"/>
+      <c r="AE17" s="128"/>
+      <c r="AF17" s="130"/>
+      <c r="AG17" s="130"/>
+      <c r="AH17" s="130"/>
+      <c r="AI17" s="130"/>
+      <c r="AJ17" s="130"/>
+      <c r="AK17" s="130"/>
+      <c r="AL17" s="130"/>
+      <c r="AM17" s="130"/>
+      <c r="AN17" s="130"/>
+      <c r="AO17" s="133"/>
+      <c r="AP17" s="131"/>
+      <c r="AQ17" s="130"/>
+      <c r="AR17" s="132"/>
+      <c r="AS17" s="132"/>
+      <c r="AT17" s="132"/>
+      <c r="AU17" s="133"/>
+      <c r="AV17" s="134"/>
+      <c r="AW17" s="132"/>
+      <c r="AX17" s="132"/>
+      <c r="AY17" s="133"/>
+      <c r="AZ17" s="131"/>
+      <c r="BA17" s="135"/>
+      <c r="BB17" s="136"/>
+      <c r="BC17" s="133"/>
+      <c r="BD17" s="137"/>
+      <c r="BE17" s="138"/>
+      <c r="BF17" s="139"/>
+      <c r="BG17" s="139"/>
+      <c r="BH17" s="133"/>
+    </row>
+    <row r="18" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
       <c r="B18" s="85" t="s">
         <v>289</v>
       </c>
-      <c r="C18" s="140" t="s">
+      <c r="C18" s="173" t="s">
         <v>310</v>
       </c>
       <c r="D18" s="25">
@@ -7740,13 +7839,13 @@
       <c r="F18" s="25">
         <v>10</v>
       </c>
-      <c r="G18" s="166" t="s">
+      <c r="G18" s="169" t="s">
         <v>1107</v>
       </c>
       <c r="H18" s="40">
         <v>20</v>
       </c>
-      <c r="I18" s="140">
+      <c r="I18" s="121">
         <v>1E-3</v>
       </c>
       <c r="J18" s="25">
@@ -7779,7 +7878,7 @@
       <c r="S18" s="25">
         <v>0</v>
       </c>
-      <c r="T18" s="140">
+      <c r="T18" s="121">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="U18" s="25">
@@ -7896,12 +7995,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
       <c r="B19" s="85" t="s">
         <v>309</v>
       </c>
-      <c r="C19" s="140" t="s">
+      <c r="C19" s="173" t="s">
         <v>310</v>
       </c>
       <c r="D19" s="25">
@@ -7913,13 +8012,13 @@
       <c r="F19" s="25">
         <v>10</v>
       </c>
-      <c r="G19" s="166" t="s">
+      <c r="G19" s="169" t="s">
         <v>1108</v>
       </c>
       <c r="H19" s="40">
         <v>20</v>
       </c>
-      <c r="I19" s="140">
+      <c r="I19" s="121">
         <v>1E-3</v>
       </c>
       <c r="J19" s="25">
@@ -7952,7 +8051,7 @@
       <c r="S19" s="25">
         <v>0</v>
       </c>
-      <c r="T19" s="140">
+      <c r="T19" s="121">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="U19" s="25">
@@ -8069,12 +8168,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="85" t="s">
         <v>336</v>
       </c>
-      <c r="C20" s="140" t="s">
+      <c r="C20" s="173" t="s">
         <v>310</v>
       </c>
       <c r="D20" s="25">
@@ -8086,13 +8185,13 @@
       <c r="F20" s="25">
         <v>10</v>
       </c>
-      <c r="G20" s="166" t="s">
+      <c r="G20" s="169" t="s">
         <v>1109</v>
       </c>
       <c r="H20" s="40">
         <v>70</v>
       </c>
-      <c r="I20" s="140">
+      <c r="I20" s="121">
         <v>1E-3</v>
       </c>
       <c r="J20" s="25">
@@ -8125,7 +8224,7 @@
       <c r="S20" s="25">
         <v>0</v>
       </c>
-      <c r="T20" s="140">
+      <c r="T20" s="121">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="U20" s="25">
@@ -8242,12 +8341,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="85" t="s">
         <v>1060</v>
       </c>
-      <c r="C21" s="140" t="s">
+      <c r="C21" s="173" t="s">
         <v>1089</v>
       </c>
       <c r="D21" s="25">
@@ -8259,13 +8358,13 @@
       <c r="F21" s="25">
         <v>5000</v>
       </c>
-      <c r="G21" s="166" t="s">
-        <v>1074</v>
+      <c r="G21" s="169" t="s">
+        <v>1111</v>
       </c>
       <c r="H21" s="40">
         <v>60</v>
       </c>
-      <c r="I21" s="140">
+      <c r="I21" s="121">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="J21" s="25">
@@ -8298,7 +8397,7 @@
       <c r="S21" s="25">
         <v>0</v>
       </c>
-      <c r="T21" s="140">
+      <c r="T21" s="121">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="U21" s="25">
@@ -8400,12 +8499,12 @@
       </c>
       <c r="BH21" s="42"/>
     </row>
-    <row r="22" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
       <c r="B22" s="85" t="s">
         <v>1065</v>
       </c>
-      <c r="C22" s="140" t="s">
+      <c r="C22" s="173" t="s">
         <v>1082</v>
       </c>
       <c r="D22" s="25">
@@ -8417,13 +8516,13 @@
       <c r="F22" s="25">
         <v>5000</v>
       </c>
-      <c r="G22" s="166" t="s">
-        <v>1076</v>
+      <c r="G22" s="169" t="s">
+        <v>1112</v>
       </c>
       <c r="H22" s="40">
         <v>60</v>
       </c>
-      <c r="I22" s="140">
+      <c r="I22" s="121">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J22" s="25">
@@ -8456,7 +8555,7 @@
       <c r="S22" s="25">
         <v>0</v>
       </c>
-      <c r="T22" s="140">
+      <c r="T22" s="121">
         <v>0.05</v>
       </c>
       <c r="U22" s="25">
@@ -8477,17 +8576,39 @@
       <c r="AB22" s="25"/>
       <c r="AC22" s="41"/>
       <c r="AD22" s="41"/>
-      <c r="AE22" s="40"/>
-      <c r="AF22" s="25"/>
-      <c r="AG22" s="25"/>
-      <c r="AH22" s="25"/>
-      <c r="AI22" s="25"/>
-      <c r="AJ22" s="25"/>
-      <c r="AK22" s="25"/>
-      <c r="AL22" s="25"/>
-      <c r="AM22" s="25"/>
-      <c r="AN22" s="25"/>
-      <c r="AO22" s="42"/>
+      <c r="AE22" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF22" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG22" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH22" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI22" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ22" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK22" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL22" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM22" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN22" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO22" s="42" t="s">
+        <v>28</v>
+      </c>
       <c r="AP22" s="43"/>
       <c r="AQ22" s="25"/>
       <c r="AR22" s="41"/>
@@ -8512,12 +8633,12 @@
       </c>
       <c r="BH22" s="42"/>
     </row>
-    <row r="23" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="85" t="s">
         <v>1070</v>
       </c>
-      <c r="C23" s="140" t="s">
+      <c r="C23" s="173" t="s">
         <v>1083</v>
       </c>
       <c r="D23" s="25">
@@ -8529,13 +8650,13 @@
       <c r="F23" s="25">
         <v>5000</v>
       </c>
-      <c r="G23" s="166" t="s">
-        <v>1075</v>
+      <c r="G23" s="169" t="s">
+        <v>1117</v>
       </c>
       <c r="H23" s="40">
         <v>60</v>
       </c>
-      <c r="I23" s="140">
+      <c r="I23" s="121">
         <v>0.01</v>
       </c>
       <c r="J23" s="25">
@@ -8568,7 +8689,7 @@
       <c r="S23" s="25">
         <v>0</v>
       </c>
-      <c r="T23" s="140">
+      <c r="T23" s="121">
         <v>0.05</v>
       </c>
       <c r="U23" s="25">
@@ -8589,17 +8710,39 @@
       <c r="AB23" s="25"/>
       <c r="AC23" s="41"/>
       <c r="AD23" s="41"/>
-      <c r="AE23" s="40"/>
-      <c r="AF23" s="25"/>
-      <c r="AG23" s="25"/>
-      <c r="AH23" s="25"/>
-      <c r="AI23" s="25"/>
-      <c r="AJ23" s="25"/>
-      <c r="AK23" s="25"/>
-      <c r="AL23" s="25"/>
-      <c r="AM23" s="25"/>
-      <c r="AN23" s="25"/>
-      <c r="AO23" s="42"/>
+      <c r="AE23" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF23" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG23" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH23" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI23" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ23" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK23" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL23" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM23" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN23" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO23" s="42" t="s">
+        <v>28</v>
+      </c>
       <c r="AP23" s="43"/>
       <c r="AQ23" s="25"/>
       <c r="AR23" s="41"/>
@@ -8622,12 +8765,12 @@
       </c>
       <c r="BH23" s="42"/>
     </row>
-    <row r="24" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="85" t="s">
         <v>1071</v>
       </c>
-      <c r="C24" s="140" t="s">
+      <c r="C24" s="173" t="s">
         <v>1084</v>
       </c>
       <c r="D24" s="25">
@@ -8639,13 +8782,13 @@
       <c r="F24" s="25">
         <v>5000</v>
       </c>
-      <c r="G24" s="166" t="s">
-        <v>1072</v>
+      <c r="G24" s="169" t="s">
+        <v>1113</v>
       </c>
       <c r="H24" s="40">
         <v>60</v>
       </c>
-      <c r="I24" s="140">
+      <c r="I24" s="121">
         <v>0.01</v>
       </c>
       <c r="J24" s="25">
@@ -8678,7 +8821,7 @@
       <c r="S24" s="25">
         <v>0</v>
       </c>
-      <c r="T24" s="140">
+      <c r="T24" s="121">
         <v>0.05</v>
       </c>
       <c r="U24" s="25">
@@ -8699,17 +8842,39 @@
       <c r="AB24" s="25"/>
       <c r="AC24" s="41"/>
       <c r="AD24" s="41"/>
-      <c r="AE24" s="40"/>
-      <c r="AF24" s="25"/>
-      <c r="AG24" s="25"/>
-      <c r="AH24" s="25"/>
-      <c r="AI24" s="25"/>
-      <c r="AJ24" s="25"/>
-      <c r="AK24" s="25"/>
-      <c r="AL24" s="25"/>
-      <c r="AM24" s="25"/>
-      <c r="AN24" s="25"/>
-      <c r="AO24" s="42"/>
+      <c r="AE24" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF24" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG24" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH24" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI24" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ24" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK24" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL24" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM24" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN24" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO24" s="42" t="s">
+        <v>28</v>
+      </c>
       <c r="AP24" s="43"/>
       <c r="AQ24" s="25"/>
       <c r="AR24" s="41"/>
@@ -8732,12 +8897,12 @@
       </c>
       <c r="BH24" s="42"/>
     </row>
-    <row r="25" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="85" t="s">
-        <v>1069</v>
-      </c>
-      <c r="C25" s="140" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C25" s="173" t="s">
         <v>1085</v>
       </c>
       <c r="D25" s="25">
@@ -8749,13 +8914,13 @@
       <c r="F25" s="25">
         <v>5000</v>
       </c>
-      <c r="G25" s="166" t="s">
-        <v>1066</v>
+      <c r="G25" s="169" t="s">
+        <v>1114</v>
       </c>
       <c r="H25" s="40">
         <v>60</v>
       </c>
-      <c r="I25" s="140">
+      <c r="I25" s="121">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="J25" s="25">
@@ -8788,7 +8953,7 @@
       <c r="S25" s="25">
         <v>0</v>
       </c>
-      <c r="T25" s="140">
+      <c r="T25" s="121">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="U25" s="25">
@@ -8809,17 +8974,39 @@
       <c r="AB25" s="25"/>
       <c r="AC25" s="41"/>
       <c r="AD25" s="41"/>
-      <c r="AE25" s="40"/>
-      <c r="AF25" s="25"/>
-      <c r="AG25" s="25"/>
-      <c r="AH25" s="25"/>
-      <c r="AI25" s="25"/>
-      <c r="AJ25" s="25"/>
-      <c r="AK25" s="25"/>
-      <c r="AL25" s="25"/>
-      <c r="AM25" s="25"/>
-      <c r="AN25" s="25"/>
-      <c r="AO25" s="42"/>
+      <c r="AE25" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF25" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG25" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH25" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI25" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ25" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK25" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL25" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM25" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN25" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO25" s="42" t="s">
+        <v>28</v>
+      </c>
       <c r="AP25" s="43"/>
       <c r="AQ25" s="25"/>
       <c r="AR25" s="41"/>
@@ -8847,9 +9034,9 @@
     <row r="26" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="85" t="s">
-        <v>1068</v>
-      </c>
-      <c r="C26" s="140" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C26" s="173" t="s">
         <v>1086</v>
       </c>
       <c r="D26" s="25">
@@ -8861,13 +9048,13 @@
       <c r="F26" s="25">
         <v>5000</v>
       </c>
-      <c r="G26" s="166" t="s">
-        <v>1080</v>
+      <c r="G26" s="169" t="s">
+        <v>1115</v>
       </c>
       <c r="H26" s="40">
         <v>60</v>
       </c>
-      <c r="I26" s="140">
+      <c r="I26" s="121">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="J26" s="25">
@@ -8900,7 +9087,7 @@
       <c r="S26" s="25">
         <v>0</v>
       </c>
-      <c r="T26" s="140">
+      <c r="T26" s="121">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="U26" s="25">
@@ -8921,17 +9108,39 @@
       <c r="AB26" s="25"/>
       <c r="AC26" s="41"/>
       <c r="AD26" s="41"/>
-      <c r="AE26" s="40"/>
-      <c r="AF26" s="25"/>
-      <c r="AG26" s="25"/>
-      <c r="AH26" s="25"/>
-      <c r="AI26" s="25"/>
-      <c r="AJ26" s="25"/>
-      <c r="AK26" s="25"/>
-      <c r="AL26" s="25"/>
-      <c r="AM26" s="25"/>
-      <c r="AN26" s="25"/>
-      <c r="AO26" s="42"/>
+      <c r="AE26" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF26" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG26" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH26" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI26" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ26" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK26" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL26" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM26" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN26" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO26" s="42" t="s">
+        <v>28</v>
+      </c>
       <c r="AP26" s="43"/>
       <c r="AQ26" s="25"/>
       <c r="AR26" s="41"/>
@@ -8959,9 +9168,9 @@
     <row r="27" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="85" t="s">
-        <v>1067</v>
-      </c>
-      <c r="C27" s="140" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C27" s="173" t="s">
         <v>1087</v>
       </c>
       <c r="D27" s="25">
@@ -8973,13 +9182,13 @@
       <c r="F27" s="25">
         <v>5000</v>
       </c>
-      <c r="G27" s="166" t="s">
-        <v>1077</v>
+      <c r="G27" s="169" t="s">
+        <v>1115</v>
       </c>
       <c r="H27" s="40">
         <v>60</v>
       </c>
-      <c r="I27" s="140">
+      <c r="I27" s="121">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="J27" s="25">
@@ -9012,7 +9221,7 @@
       <c r="S27" s="25">
         <v>0</v>
       </c>
-      <c r="T27" s="140">
+      <c r="T27" s="121">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="U27" s="25">
@@ -9033,17 +9242,39 @@
       <c r="AB27" s="25"/>
       <c r="AC27" s="41"/>
       <c r="AD27" s="41"/>
-      <c r="AE27" s="40"/>
-      <c r="AF27" s="25"/>
-      <c r="AG27" s="25"/>
-      <c r="AH27" s="25"/>
-      <c r="AI27" s="25"/>
-      <c r="AJ27" s="25"/>
-      <c r="AK27" s="25"/>
-      <c r="AL27" s="25"/>
-      <c r="AM27" s="25"/>
-      <c r="AN27" s="25"/>
-      <c r="AO27" s="42"/>
+      <c r="AE27" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH27" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO27" s="42" t="s">
+        <v>28</v>
+      </c>
       <c r="AP27" s="43"/>
       <c r="AQ27" s="25"/>
       <c r="AR27" s="41"/>
@@ -9068,12 +9299,12 @@
       </c>
       <c r="BH27" s="42"/>
     </row>
-    <row r="28" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="85" t="s">
-        <v>1073</v>
-      </c>
-      <c r="C28" s="140" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C28" s="173" t="s">
         <v>1105</v>
       </c>
       <c r="D28" s="25">
@@ -9085,13 +9316,13 @@
       <c r="F28" s="25">
         <v>5000</v>
       </c>
-      <c r="G28" s="166" t="s">
-        <v>1079</v>
+      <c r="G28" s="169" t="s">
+        <v>1116</v>
       </c>
       <c r="H28" s="40">
         <v>60</v>
       </c>
-      <c r="I28" s="140">
+      <c r="I28" s="121">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="J28" s="25">
@@ -9124,7 +9355,7 @@
       <c r="S28" s="25">
         <v>0</v>
       </c>
-      <c r="T28" s="140">
+      <c r="T28" s="121">
         <v>0.05</v>
       </c>
       <c r="U28" s="25">
@@ -9145,17 +9376,39 @@
       <c r="AB28" s="25"/>
       <c r="AC28" s="41"/>
       <c r="AD28" s="41"/>
-      <c r="AE28" s="40"/>
-      <c r="AF28" s="25"/>
-      <c r="AG28" s="25"/>
-      <c r="AH28" s="25"/>
-      <c r="AI28" s="25"/>
-      <c r="AJ28" s="25"/>
-      <c r="AK28" s="25"/>
-      <c r="AL28" s="25"/>
-      <c r="AM28" s="25"/>
-      <c r="AN28" s="25"/>
-      <c r="AO28" s="42"/>
+      <c r="AE28" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH28" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO28" s="42" t="s">
+        <v>28</v>
+      </c>
       <c r="AP28" s="43"/>
       <c r="AQ28" s="25"/>
       <c r="AR28" s="41"/>
@@ -9182,11 +9435,11 @@
     </row>
     <row r="29" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="4"/>
+      <c r="C29" s="175"/>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="168"/>
+      <c r="G29" s="143"/>
       <c r="H29" s="5"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -9573,35 +9826,35 @@
     <mergeCell ref="AV2:AY2"/>
     <mergeCell ref="AZ2:BC2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 A4:G27 AA14 AA18:AA29 W4:BH13 AB14:BH30">
-    <cfRule type="expression" dxfId="26" priority="17" stopIfTrue="1">
+  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 AA18:AA29 W4:BH13 A4:G27 AB14:BH30">
+    <cfRule type="expression" dxfId="40" priority="17" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="18" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28">
-    <cfRule type="expression" dxfId="24" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="15" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="16" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA16:AA17">
-    <cfRule type="expression" dxfId="22" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="29" stopIfTrue="1">
       <formula>$A15="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="30" stopIfTrue="1">
       <formula>$A15="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA15">
-    <cfRule type="expression" dxfId="20" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="1" stopIfTrue="1">
       <formula>$A14="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="2" stopIfTrue="1">
       <formula>$A14="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9662,74 +9915,74 @@
   <sheetData>
     <row r="1" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="126" t="s">
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="146" t="s">
         <v>1062</v>
       </c>
-      <c r="J2" s="127"/>
-      <c r="K2" s="135"/>
-      <c r="L2" s="135"/>
-      <c r="M2" s="135"/>
-      <c r="N2" s="135"/>
-      <c r="O2" s="135"/>
-      <c r="P2" s="135"/>
-      <c r="Q2" s="135"/>
-      <c r="R2" s="135"/>
-      <c r="S2" s="135"/>
-      <c r="T2" s="136"/>
-      <c r="U2" s="129" t="s">
+      <c r="J2" s="147"/>
+      <c r="K2" s="155"/>
+      <c r="L2" s="155"/>
+      <c r="M2" s="155"/>
+      <c r="N2" s="155"/>
+      <c r="O2" s="155"/>
+      <c r="P2" s="155"/>
+      <c r="Q2" s="155"/>
+      <c r="R2" s="155"/>
+      <c r="S2" s="155"/>
+      <c r="T2" s="156"/>
+      <c r="U2" s="157" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="130"/>
-      <c r="W2" s="130"/>
-      <c r="X2" s="130"/>
-      <c r="Y2" s="130"/>
-      <c r="Z2" s="130"/>
-      <c r="AA2" s="130"/>
-      <c r="AB2" s="130"/>
-      <c r="AC2" s="130"/>
-      <c r="AD2" s="130"/>
-      <c r="AE2" s="130"/>
-      <c r="AF2" s="130"/>
-      <c r="AG2" s="130"/>
-      <c r="AH2" s="130"/>
-      <c r="AI2" s="130"/>
-      <c r="AJ2" s="131"/>
-      <c r="AK2" s="123" t="s">
+      <c r="V2" s="158"/>
+      <c r="W2" s="158"/>
+      <c r="X2" s="158"/>
+      <c r="Y2" s="158"/>
+      <c r="Z2" s="158"/>
+      <c r="AA2" s="158"/>
+      <c r="AB2" s="158"/>
+      <c r="AC2" s="158"/>
+      <c r="AD2" s="158"/>
+      <c r="AE2" s="158"/>
+      <c r="AF2" s="158"/>
+      <c r="AG2" s="158"/>
+      <c r="AH2" s="158"/>
+      <c r="AI2" s="158"/>
+      <c r="AJ2" s="159"/>
+      <c r="AK2" s="163" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="137"/>
-      <c r="AM2" s="137"/>
-      <c r="AN2" s="137"/>
-      <c r="AO2" s="137"/>
-      <c r="AP2" s="138"/>
-      <c r="AQ2" s="123" t="s">
+      <c r="AL2" s="161"/>
+      <c r="AM2" s="161"/>
+      <c r="AN2" s="161"/>
+      <c r="AO2" s="161"/>
+      <c r="AP2" s="162"/>
+      <c r="AQ2" s="163" t="s">
         <v>1061</v>
       </c>
-      <c r="AR2" s="124"/>
-      <c r="AS2" s="124"/>
-      <c r="AT2" s="125"/>
-      <c r="AU2" s="132" t="s">
+      <c r="AR2" s="160"/>
+      <c r="AS2" s="160"/>
+      <c r="AT2" s="164"/>
+      <c r="AU2" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="AV2" s="133"/>
-      <c r="AW2" s="133"/>
-      <c r="AX2" s="134"/>
-      <c r="AY2" s="126" t="s">
+      <c r="AV2" s="166"/>
+      <c r="AW2" s="166"/>
+      <c r="AX2" s="167"/>
+      <c r="AY2" s="146" t="s">
         <v>1047</v>
       </c>
-      <c r="AZ2" s="127"/>
-      <c r="BA2" s="127"/>
-      <c r="BB2" s="127"/>
-      <c r="BC2" s="128"/>
+      <c r="AZ2" s="147"/>
+      <c r="BA2" s="147"/>
+      <c r="BB2" s="147"/>
+      <c r="BC2" s="148"/>
     </row>
     <row r="3" spans="1:55" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -9897,7 +10150,7 @@
       <c r="B4" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="139" t="s">
+      <c r="C4" s="120" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="29">
@@ -10057,7 +10310,7 @@
       <c r="B5" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="139" t="s">
+      <c r="C5" s="120" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="29">
@@ -10217,7 +10470,7 @@
       <c r="B6" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="139" t="s">
+      <c r="C6" s="120" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="29">
@@ -10377,7 +10630,7 @@
       <c r="B7" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="139" t="s">
+      <c r="C7" s="120" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="29">
@@ -10537,7 +10790,7 @@
       <c r="B8" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="139" t="s">
+      <c r="C8" s="120" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="29">
@@ -10697,7 +10950,7 @@
       <c r="B9" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="140" t="s">
+      <c r="C9" s="121" t="s">
         <v>279</v>
       </c>
       <c r="D9" s="25">
@@ -10858,7 +11111,7 @@
       <c r="B10" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="140" t="s">
+      <c r="C10" s="121" t="s">
         <v>279</v>
       </c>
       <c r="D10" s="25">
@@ -11019,7 +11272,7 @@
       <c r="B11" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="140" t="s">
+      <c r="C11" s="121" t="s">
         <v>279</v>
       </c>
       <c r="D11" s="25">
@@ -11180,7 +11433,7 @@
       <c r="B12" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="140" t="s">
+      <c r="C12" s="121" t="s">
         <v>489</v>
       </c>
       <c r="D12" s="25">
@@ -11340,7 +11593,7 @@
       <c r="B13" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="140" t="s">
+      <c r="C13" s="121" t="s">
         <v>490</v>
       </c>
       <c r="D13" s="25">
@@ -11500,7 +11753,7 @@
       <c r="B14" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="140" t="s">
+      <c r="C14" s="121" t="s">
         <v>286</v>
       </c>
       <c r="D14" s="25">
@@ -11660,7 +11913,7 @@
       <c r="B15" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="140" t="s">
+      <c r="C15" s="121" t="s">
         <v>286</v>
       </c>
       <c r="D15" s="25">
@@ -11820,7 +12073,7 @@
       <c r="B16" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="140" t="s">
+      <c r="C16" s="121" t="s">
         <v>286</v>
       </c>
       <c r="D16" s="25">
@@ -11980,7 +12233,7 @@
       <c r="B17" s="85" t="s">
         <v>288</v>
       </c>
-      <c r="C17" s="140" t="s">
+      <c r="C17" s="121" t="s">
         <v>286</v>
       </c>
       <c r="D17" s="25">
@@ -12140,7 +12393,7 @@
       <c r="B18" s="85" t="s">
         <v>289</v>
       </c>
-      <c r="C18" s="140" t="s">
+      <c r="C18" s="121" t="s">
         <v>310</v>
       </c>
       <c r="D18" s="25">
@@ -12300,7 +12553,7 @@
       <c r="B19" s="85" t="s">
         <v>309</v>
       </c>
-      <c r="C19" s="140" t="s">
+      <c r="C19" s="121" t="s">
         <v>310</v>
       </c>
       <c r="D19" s="25">
@@ -12460,7 +12713,7 @@
       <c r="B20" s="85" t="s">
         <v>336</v>
       </c>
-      <c r="C20" s="140" t="s">
+      <c r="C20" s="121" t="s">
         <v>310</v>
       </c>
       <c r="D20" s="25">
@@ -12618,7 +12871,7 @@
       <c r="B21" s="85" t="s">
         <v>1060</v>
       </c>
-      <c r="C21" s="140" t="s">
+      <c r="C21" s="121" t="s">
         <v>1081</v>
       </c>
       <c r="D21" s="25">
@@ -12761,7 +13014,7 @@
       <c r="B22" s="85" t="s">
         <v>1065</v>
       </c>
-      <c r="C22" s="140" t="s">
+      <c r="C22" s="121" t="s">
         <v>1082</v>
       </c>
       <c r="D22" s="25">
@@ -12846,7 +13099,7 @@
       <c r="B23" s="85" t="s">
         <v>1070</v>
       </c>
-      <c r="C23" s="140" t="s">
+      <c r="C23" s="121" t="s">
         <v>1083</v>
       </c>
       <c r="D23" s="25">
@@ -12927,7 +13180,7 @@
       <c r="B24" s="85" t="s">
         <v>1071</v>
       </c>
-      <c r="C24" s="140" t="s">
+      <c r="C24" s="121" t="s">
         <v>1084</v>
       </c>
       <c r="D24" s="25">
@@ -13008,7 +13261,7 @@
       <c r="B25" s="85" t="s">
         <v>1069</v>
       </c>
-      <c r="C25" s="140" t="s">
+      <c r="C25" s="121" t="s">
         <v>1085</v>
       </c>
       <c r="D25" s="25">
@@ -13093,7 +13346,7 @@
       <c r="B26" s="85" t="s">
         <v>1068</v>
       </c>
-      <c r="C26" s="140" t="s">
+      <c r="C26" s="121" t="s">
         <v>1086</v>
       </c>
       <c r="D26" s="25">
@@ -13178,7 +13431,7 @@
       <c r="B27" s="85" t="s">
         <v>1067</v>
       </c>
-      <c r="C27" s="140" t="s">
+      <c r="C27" s="121" t="s">
         <v>1087</v>
       </c>
       <c r="D27" s="25">
@@ -13263,7 +13516,7 @@
       <c r="B28" s="85" t="s">
         <v>1073</v>
       </c>
-      <c r="C28" s="140" t="s">
+      <c r="C28" s="121" t="s">
         <v>1088</v>
       </c>
       <c r="D28" s="25">
@@ -13616,42 +13869,42 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A4:BC21 C29:F32 A29:B33 G29:BC31 I33:BC33 I32:K32 M32:BC32 J22:AI27 AK22:BC27 A22:G27">
-    <cfRule type="expression" dxfId="18" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="15" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="16" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28 J28:AI28 AK28:BC28">
-    <cfRule type="expression" dxfId="16" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="5" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="6" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="14" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="19" stopIfTrue="1">
       <formula>$A32="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="20" stopIfTrue="1">
       <formula>$A32="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I28">
-    <cfRule type="expression" dxfId="12" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="3" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="4" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ22:AJ28">
-    <cfRule type="expression" dxfId="10" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="1" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="2" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45097,31 +45350,31 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="C782:C787 C844:C855 C789:C842">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="1" stopIfTrue="1">
       <formula>$A782=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="2" stopIfTrue="1">
       <formula>$A782=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B336:C353 B764:C769 B301:C303 B4:C10 B297:C299 B38:C49 B25:C36 B496:C528 B12:C23 B844:B855 B315:C326 B530:C539 B541:C550 B728:C743 B745:C748 B750:C758 B332:C334 B771:C780 B328:C330 B760:C760 B762:C762 B305:C313 B355:C358 B782:B787 B552:C561 B51:C131 B133:C213 B215:C295 B360:C494 B563:C616 B673:C726 B618:C671 B789:B842">
-    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
       <formula>$A4=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="4" stopIfTrue="1">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2 D2:Z2">
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A10 A12:A23 A25:A36 A38:A49 A297:A299 A301:A303 A305:A313 A315:A326 A328:A330 A332:A334 A336:A353 A355:A358 A496:A528 A530:A539 A541:A550 A552:A561 A745:A748 A750:A758 A760 A762 A764:A769 A771:A780 A782:A787 A844:A855 A51:A131 A133:A213 A215:A295 A360:A494 A563:A616 A673:A726 A618:A671 A728:A743 A789:A842">
-    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
+ updated tripod, Test20, with files from Jason J and Rick D, fixing the tower.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@788 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -4506,6 +4506,30 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4572,148 +4596,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="41">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <font>
         <condense val="0"/>
@@ -5215,14 +5103,14 @@
       <pane xSplit="7" ySplit="3" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" style="171" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="149" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.140625" style="2" bestFit="1" customWidth="1"/>
@@ -5260,81 +5148,81 @@
   <sheetData>
     <row r="1" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="149" t="s">
+      <c r="C2" s="161"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="161"/>
+      <c r="F2" s="161"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="157" t="s">
         <v>1104</v>
       </c>
-      <c r="I2" s="150"/>
-      <c r="J2" s="150"/>
-      <c r="K2" s="150"/>
-      <c r="L2" s="150"/>
-      <c r="M2" s="150"/>
-      <c r="N2" s="150"/>
-      <c r="O2" s="150"/>
-      <c r="P2" s="150"/>
-      <c r="Q2" s="150"/>
-      <c r="R2" s="150"/>
-      <c r="S2" s="150"/>
-      <c r="T2" s="150"/>
-      <c r="U2" s="150"/>
-      <c r="V2" s="151"/>
-      <c r="W2" s="147" t="s">
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="158"/>
+      <c r="L2" s="158"/>
+      <c r="M2" s="158"/>
+      <c r="N2" s="158"/>
+      <c r="O2" s="158"/>
+      <c r="P2" s="158"/>
+      <c r="Q2" s="158"/>
+      <c r="R2" s="158"/>
+      <c r="S2" s="158"/>
+      <c r="T2" s="158"/>
+      <c r="U2" s="158"/>
+      <c r="V2" s="159"/>
+      <c r="W2" s="155" t="s">
         <v>1110</v>
       </c>
-      <c r="X2" s="155"/>
-      <c r="Y2" s="155"/>
-      <c r="Z2" s="155"/>
-      <c r="AA2" s="155"/>
-      <c r="AB2" s="155"/>
-      <c r="AC2" s="155"/>
-      <c r="AD2" s="156"/>
-      <c r="AE2" s="157" t="s">
+      <c r="X2" s="163"/>
+      <c r="Y2" s="163"/>
+      <c r="Z2" s="163"/>
+      <c r="AA2" s="163"/>
+      <c r="AB2" s="163"/>
+      <c r="AC2" s="163"/>
+      <c r="AD2" s="164"/>
+      <c r="AE2" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" s="158"/>
-      <c r="AG2" s="158"/>
-      <c r="AH2" s="158"/>
-      <c r="AI2" s="158"/>
-      <c r="AJ2" s="158"/>
-      <c r="AK2" s="158"/>
-      <c r="AL2" s="158"/>
-      <c r="AM2" s="158"/>
-      <c r="AN2" s="158"/>
-      <c r="AO2" s="159"/>
-      <c r="AP2" s="160" t="s">
+      <c r="AF2" s="166"/>
+      <c r="AG2" s="166"/>
+      <c r="AH2" s="166"/>
+      <c r="AI2" s="166"/>
+      <c r="AJ2" s="166"/>
+      <c r="AK2" s="166"/>
+      <c r="AL2" s="166"/>
+      <c r="AM2" s="166"/>
+      <c r="AN2" s="166"/>
+      <c r="AO2" s="167"/>
+      <c r="AP2" s="168" t="s">
         <v>43</v>
       </c>
-      <c r="AQ2" s="161"/>
-      <c r="AR2" s="161"/>
-      <c r="AS2" s="161"/>
-      <c r="AT2" s="161"/>
-      <c r="AU2" s="162"/>
-      <c r="AV2" s="163" t="s">
+      <c r="AQ2" s="169"/>
+      <c r="AR2" s="169"/>
+      <c r="AS2" s="169"/>
+      <c r="AT2" s="169"/>
+      <c r="AU2" s="170"/>
+      <c r="AV2" s="171" t="s">
         <v>1061</v>
       </c>
-      <c r="AW2" s="160"/>
-      <c r="AX2" s="160"/>
-      <c r="AY2" s="164"/>
-      <c r="AZ2" s="165" t="s">
+      <c r="AW2" s="168"/>
+      <c r="AX2" s="168"/>
+      <c r="AY2" s="172"/>
+      <c r="AZ2" s="173" t="s">
         <v>18</v>
       </c>
-      <c r="BA2" s="166"/>
-      <c r="BB2" s="166"/>
-      <c r="BC2" s="167"/>
-      <c r="BD2" s="146" t="s">
+      <c r="BA2" s="174"/>
+      <c r="BB2" s="174"/>
+      <c r="BC2" s="175"/>
+      <c r="BD2" s="154" t="s">
         <v>1047</v>
       </c>
-      <c r="BE2" s="147"/>
-      <c r="BF2" s="147"/>
-      <c r="BG2" s="147"/>
-      <c r="BH2" s="148"/>
+      <c r="BE2" s="155"/>
+      <c r="BF2" s="155"/>
+      <c r="BG2" s="155"/>
+      <c r="BH2" s="156"/>
     </row>
     <row r="3" spans="1:60" s="1" customFormat="1" ht="85.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
@@ -5513,7 +5401,7 @@
       <c r="B4" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="172" t="s">
+      <c r="C4" s="150" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="29">
@@ -5525,7 +5413,7 @@
       <c r="F4" s="55">
         <v>175</v>
       </c>
-      <c r="G4" s="168" t="s">
+      <c r="G4" s="146" t="s">
         <v>497</v>
       </c>
       <c r="H4" s="141">
@@ -5686,7 +5574,7 @@
       <c r="B5" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="172" t="s">
+      <c r="C5" s="150" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="29">
@@ -5698,7 +5586,7 @@
       <c r="F5" s="55">
         <v>175</v>
       </c>
-      <c r="G5" s="169" t="s">
+      <c r="G5" s="147" t="s">
         <v>1106</v>
       </c>
       <c r="H5" s="40">
@@ -5859,7 +5747,7 @@
       <c r="B6" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="172" t="s">
+      <c r="C6" s="150" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="29">
@@ -5871,7 +5759,7 @@
       <c r="F6" s="55">
         <v>175</v>
       </c>
-      <c r="G6" s="169" t="s">
+      <c r="G6" s="147" t="s">
         <v>491</v>
       </c>
       <c r="H6" s="40">
@@ -6032,7 +5920,7 @@
       <c r="B7" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="172" t="s">
+      <c r="C7" s="150" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="29">
@@ -6044,7 +5932,7 @@
       <c r="F7" s="55">
         <v>175</v>
       </c>
-      <c r="G7" s="169" t="s">
+      <c r="G7" s="147" t="s">
         <v>492</v>
       </c>
       <c r="H7" s="40">
@@ -6205,7 +6093,7 @@
       <c r="B8" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="172" t="s">
+      <c r="C8" s="150" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="29">
@@ -6217,7 +6105,7 @@
       <c r="F8" s="55">
         <v>175</v>
       </c>
-      <c r="G8" s="169" t="s">
+      <c r="G8" s="147" t="s">
         <v>1106</v>
       </c>
       <c r="H8" s="40">
@@ -6378,7 +6266,7 @@
       <c r="B9" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="173" t="s">
+      <c r="C9" s="151" t="s">
         <v>279</v>
       </c>
       <c r="D9" s="25">
@@ -6391,7 +6279,7 @@
       <c r="F9" s="25">
         <v>50</v>
       </c>
-      <c r="G9" s="169" t="s">
+      <c r="G9" s="147" t="s">
         <v>1106</v>
       </c>
       <c r="H9" s="40">
@@ -6552,7 +6440,7 @@
       <c r="B10" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="173" t="s">
+      <c r="C10" s="151" t="s">
         <v>279</v>
       </c>
       <c r="D10" s="25">
@@ -6565,7 +6453,7 @@
       <c r="F10" s="25">
         <v>50</v>
       </c>
-      <c r="G10" s="169" t="s">
+      <c r="G10" s="147" t="s">
         <v>492</v>
       </c>
       <c r="H10" s="40">
@@ -6726,7 +6614,7 @@
       <c r="B11" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="173" t="s">
+      <c r="C11" s="151" t="s">
         <v>279</v>
       </c>
       <c r="D11" s="25">
@@ -6739,7 +6627,7 @@
       <c r="F11" s="25">
         <v>50</v>
       </c>
-      <c r="G11" s="168" t="s">
+      <c r="G11" s="146" t="s">
         <v>497</v>
       </c>
       <c r="H11" s="40">
@@ -6900,7 +6788,7 @@
       <c r="B12" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="173" t="s">
+      <c r="C12" s="151" t="s">
         <v>489</v>
       </c>
       <c r="D12" s="25">
@@ -6912,7 +6800,7 @@
       <c r="F12" s="25">
         <v>20</v>
       </c>
-      <c r="G12" s="169" t="s">
+      <c r="G12" s="147" t="s">
         <v>493</v>
       </c>
       <c r="H12" s="40">
@@ -7073,7 +6961,7 @@
       <c r="B13" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="173" t="s">
+      <c r="C13" s="151" t="s">
         <v>490</v>
       </c>
       <c r="D13" s="25">
@@ -7085,7 +6973,7 @@
       <c r="F13" s="25">
         <v>20</v>
       </c>
-      <c r="G13" s="169" t="s">
+      <c r="G13" s="147" t="s">
         <v>496</v>
       </c>
       <c r="H13" s="40">
@@ -7246,7 +7134,7 @@
       <c r="B14" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="173" t="s">
+      <c r="C14" s="151" t="s">
         <v>286</v>
       </c>
       <c r="D14" s="25">
@@ -7258,7 +7146,7 @@
       <c r="F14" s="25">
         <v>1500</v>
       </c>
-      <c r="G14" s="169" t="s">
+      <c r="G14" s="147" t="s">
         <v>500</v>
       </c>
       <c r="H14" s="40">
@@ -7419,7 +7307,7 @@
       <c r="B15" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="173" t="s">
+      <c r="C15" s="151" t="s">
         <v>286</v>
       </c>
       <c r="D15" s="25">
@@ -7431,7 +7319,7 @@
       <c r="F15" s="25">
         <v>1500</v>
       </c>
-      <c r="G15" s="169" t="s">
+      <c r="G15" s="147" t="s">
         <v>494</v>
       </c>
       <c r="H15" s="40">
@@ -7592,7 +7480,7 @@
       <c r="B16" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="173" t="s">
+      <c r="C16" s="151" t="s">
         <v>286</v>
       </c>
       <c r="D16" s="25">
@@ -7604,7 +7492,7 @@
       <c r="F16" s="25">
         <v>1500</v>
       </c>
-      <c r="G16" s="169" t="s">
+      <c r="G16" s="147" t="s">
         <v>495</v>
       </c>
       <c r="H16" s="40">
@@ -7763,11 +7651,11 @@
     <row r="17" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
       <c r="B17" s="128"/>
-      <c r="C17" s="174"/>
+      <c r="C17" s="152"/>
       <c r="D17" s="130"/>
       <c r="E17" s="130"/>
       <c r="F17" s="130"/>
-      <c r="G17" s="170"/>
+      <c r="G17" s="148"/>
       <c r="H17" s="128"/>
       <c r="I17" s="129"/>
       <c r="J17" s="130"/>
@@ -7827,7 +7715,7 @@
       <c r="B18" s="85" t="s">
         <v>289</v>
       </c>
-      <c r="C18" s="173" t="s">
+      <c r="C18" s="151" t="s">
         <v>310</v>
       </c>
       <c r="D18" s="25">
@@ -7839,7 +7727,7 @@
       <c r="F18" s="25">
         <v>10</v>
       </c>
-      <c r="G18" s="169" t="s">
+      <c r="G18" s="147" t="s">
         <v>1107</v>
       </c>
       <c r="H18" s="40">
@@ -8000,7 +7888,7 @@
       <c r="B19" s="85" t="s">
         <v>309</v>
       </c>
-      <c r="C19" s="173" t="s">
+      <c r="C19" s="151" t="s">
         <v>310</v>
       </c>
       <c r="D19" s="25">
@@ -8012,7 +7900,7 @@
       <c r="F19" s="25">
         <v>10</v>
       </c>
-      <c r="G19" s="169" t="s">
+      <c r="G19" s="147" t="s">
         <v>1108</v>
       </c>
       <c r="H19" s="40">
@@ -8173,7 +8061,7 @@
       <c r="B20" s="85" t="s">
         <v>336</v>
       </c>
-      <c r="C20" s="173" t="s">
+      <c r="C20" s="151" t="s">
         <v>310</v>
       </c>
       <c r="D20" s="25">
@@ -8185,7 +8073,7 @@
       <c r="F20" s="25">
         <v>10</v>
       </c>
-      <c r="G20" s="169" t="s">
+      <c r="G20" s="147" t="s">
         <v>1109</v>
       </c>
       <c r="H20" s="40">
@@ -8346,7 +8234,7 @@
       <c r="B21" s="85" t="s">
         <v>1060</v>
       </c>
-      <c r="C21" s="173" t="s">
+      <c r="C21" s="151" t="s">
         <v>1089</v>
       </c>
       <c r="D21" s="25">
@@ -8358,7 +8246,7 @@
       <c r="F21" s="25">
         <v>5000</v>
       </c>
-      <c r="G21" s="169" t="s">
+      <c r="G21" s="147" t="s">
         <v>1111</v>
       </c>
       <c r="H21" s="40">
@@ -8504,7 +8392,7 @@
       <c r="B22" s="85" t="s">
         <v>1065</v>
       </c>
-      <c r="C22" s="173" t="s">
+      <c r="C22" s="151" t="s">
         <v>1082</v>
       </c>
       <c r="D22" s="25">
@@ -8516,7 +8404,7 @@
       <c r="F22" s="25">
         <v>5000</v>
       </c>
-      <c r="G22" s="169" t="s">
+      <c r="G22" s="147" t="s">
         <v>1112</v>
       </c>
       <c r="H22" s="40">
@@ -8638,7 +8526,7 @@
       <c r="B23" s="85" t="s">
         <v>1070</v>
       </c>
-      <c r="C23" s="173" t="s">
+      <c r="C23" s="151" t="s">
         <v>1083</v>
       </c>
       <c r="D23" s="25">
@@ -8650,14 +8538,14 @@
       <c r="F23" s="25">
         <v>5000</v>
       </c>
-      <c r="G23" s="169" t="s">
+      <c r="G23" s="147" t="s">
         <v>1117</v>
       </c>
       <c r="H23" s="40">
         <v>60</v>
       </c>
       <c r="I23" s="121">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="J23" s="25">
         <v>2</v>
@@ -8690,7 +8578,7 @@
         <v>0</v>
       </c>
       <c r="T23" s="121">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="U23" s="25">
         <v>0</v>
@@ -8770,7 +8658,7 @@
       <c r="B24" s="85" t="s">
         <v>1071</v>
       </c>
-      <c r="C24" s="173" t="s">
+      <c r="C24" s="151" t="s">
         <v>1084</v>
       </c>
       <c r="D24" s="25">
@@ -8782,7 +8670,7 @@
       <c r="F24" s="25">
         <v>5000</v>
       </c>
-      <c r="G24" s="169" t="s">
+      <c r="G24" s="147" t="s">
         <v>1113</v>
       </c>
       <c r="H24" s="40">
@@ -8902,7 +8790,7 @@
       <c r="B25" s="85" t="s">
         <v>1121</v>
       </c>
-      <c r="C25" s="173" t="s">
+      <c r="C25" s="151" t="s">
         <v>1085</v>
       </c>
       <c r="D25" s="25">
@@ -8914,7 +8802,7 @@
       <c r="F25" s="25">
         <v>5000</v>
       </c>
-      <c r="G25" s="169" t="s">
+      <c r="G25" s="147" t="s">
         <v>1114</v>
       </c>
       <c r="H25" s="40">
@@ -9036,7 +8924,7 @@
       <c r="B26" s="85" t="s">
         <v>1120</v>
       </c>
-      <c r="C26" s="173" t="s">
+      <c r="C26" s="151" t="s">
         <v>1086</v>
       </c>
       <c r="D26" s="25">
@@ -9048,7 +8936,7 @@
       <c r="F26" s="25">
         <v>5000</v>
       </c>
-      <c r="G26" s="169" t="s">
+      <c r="G26" s="147" t="s">
         <v>1115</v>
       </c>
       <c r="H26" s="40">
@@ -9170,7 +9058,7 @@
       <c r="B27" s="85" t="s">
         <v>1119</v>
       </c>
-      <c r="C27" s="173" t="s">
+      <c r="C27" s="151" t="s">
         <v>1087</v>
       </c>
       <c r="D27" s="25">
@@ -9182,7 +9070,7 @@
       <c r="F27" s="25">
         <v>5000</v>
       </c>
-      <c r="G27" s="169" t="s">
+      <c r="G27" s="147" t="s">
         <v>1115</v>
       </c>
       <c r="H27" s="40">
@@ -9304,7 +9192,7 @@
       <c r="B28" s="85" t="s">
         <v>1118</v>
       </c>
-      <c r="C28" s="173" t="s">
+      <c r="C28" s="151" t="s">
         <v>1105</v>
       </c>
       <c r="D28" s="25">
@@ -9316,7 +9204,7 @@
       <c r="F28" s="25">
         <v>5000</v>
       </c>
-      <c r="G28" s="169" t="s">
+      <c r="G28" s="147" t="s">
         <v>1116</v>
       </c>
       <c r="H28" s="40">
@@ -9435,7 +9323,7 @@
     </row>
     <row r="29" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="175"/>
+      <c r="C29" s="153"/>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -9827,34 +9715,34 @@
     <mergeCell ref="AZ2:BC2"/>
   </mergeCells>
   <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 AA18:AA29 W4:BH13 A4:G27 AB14:BH30">
-    <cfRule type="expression" dxfId="40" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="17" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="18" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28">
-    <cfRule type="expression" dxfId="38" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="15" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="16" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA16:AA17">
-    <cfRule type="expression" dxfId="36" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="29" stopIfTrue="1">
       <formula>$A15="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="30" stopIfTrue="1">
       <formula>$A15="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA15">
-    <cfRule type="expression" dxfId="34" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
       <formula>$A14="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
       <formula>$A14="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9915,74 +9803,74 @@
   <sheetData>
     <row r="1" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="146" t="s">
+      <c r="C2" s="161"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="161"/>
+      <c r="F2" s="161"/>
+      <c r="G2" s="161"/>
+      <c r="H2" s="162"/>
+      <c r="I2" s="154" t="s">
         <v>1062</v>
       </c>
-      <c r="J2" s="147"/>
-      <c r="K2" s="155"/>
-      <c r="L2" s="155"/>
-      <c r="M2" s="155"/>
-      <c r="N2" s="155"/>
-      <c r="O2" s="155"/>
-      <c r="P2" s="155"/>
-      <c r="Q2" s="155"/>
-      <c r="R2" s="155"/>
-      <c r="S2" s="155"/>
-      <c r="T2" s="156"/>
-      <c r="U2" s="157" t="s">
+      <c r="J2" s="155"/>
+      <c r="K2" s="163"/>
+      <c r="L2" s="163"/>
+      <c r="M2" s="163"/>
+      <c r="N2" s="163"/>
+      <c r="O2" s="163"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="164"/>
+      <c r="U2" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="158"/>
-      <c r="W2" s="158"/>
-      <c r="X2" s="158"/>
-      <c r="Y2" s="158"/>
-      <c r="Z2" s="158"/>
-      <c r="AA2" s="158"/>
-      <c r="AB2" s="158"/>
-      <c r="AC2" s="158"/>
-      <c r="AD2" s="158"/>
-      <c r="AE2" s="158"/>
-      <c r="AF2" s="158"/>
-      <c r="AG2" s="158"/>
-      <c r="AH2" s="158"/>
-      <c r="AI2" s="158"/>
-      <c r="AJ2" s="159"/>
-      <c r="AK2" s="163" t="s">
+      <c r="V2" s="166"/>
+      <c r="W2" s="166"/>
+      <c r="X2" s="166"/>
+      <c r="Y2" s="166"/>
+      <c r="Z2" s="166"/>
+      <c r="AA2" s="166"/>
+      <c r="AB2" s="166"/>
+      <c r="AC2" s="166"/>
+      <c r="AD2" s="166"/>
+      <c r="AE2" s="166"/>
+      <c r="AF2" s="166"/>
+      <c r="AG2" s="166"/>
+      <c r="AH2" s="166"/>
+      <c r="AI2" s="166"/>
+      <c r="AJ2" s="167"/>
+      <c r="AK2" s="171" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="161"/>
-      <c r="AM2" s="161"/>
-      <c r="AN2" s="161"/>
-      <c r="AO2" s="161"/>
-      <c r="AP2" s="162"/>
-      <c r="AQ2" s="163" t="s">
+      <c r="AL2" s="169"/>
+      <c r="AM2" s="169"/>
+      <c r="AN2" s="169"/>
+      <c r="AO2" s="169"/>
+      <c r="AP2" s="170"/>
+      <c r="AQ2" s="171" t="s">
         <v>1061</v>
       </c>
-      <c r="AR2" s="160"/>
-      <c r="AS2" s="160"/>
-      <c r="AT2" s="164"/>
-      <c r="AU2" s="165" t="s">
+      <c r="AR2" s="168"/>
+      <c r="AS2" s="168"/>
+      <c r="AT2" s="172"/>
+      <c r="AU2" s="173" t="s">
         <v>18</v>
       </c>
-      <c r="AV2" s="166"/>
-      <c r="AW2" s="166"/>
-      <c r="AX2" s="167"/>
-      <c r="AY2" s="146" t="s">
+      <c r="AV2" s="174"/>
+      <c r="AW2" s="174"/>
+      <c r="AX2" s="175"/>
+      <c r="AY2" s="154" t="s">
         <v>1047</v>
       </c>
-      <c r="AZ2" s="147"/>
-      <c r="BA2" s="147"/>
-      <c r="BB2" s="147"/>
-      <c r="BC2" s="148"/>
+      <c r="AZ2" s="155"/>
+      <c r="BA2" s="155"/>
+      <c r="BB2" s="155"/>
+      <c r="BC2" s="156"/>
     </row>
     <row r="3" spans="1:55" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -13869,42 +13757,42 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A4:BC21 C29:F32 A29:B33 G29:BC31 I33:BC33 I32:K32 M32:BC32 J22:AI27 AK22:BC27 A22:G27">
-    <cfRule type="expression" dxfId="32" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28 J28:AI28 AK28:BC28">
-    <cfRule type="expression" dxfId="30" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="5" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="28" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="19" stopIfTrue="1">
       <formula>$A32="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
       <formula>$A32="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I28">
-    <cfRule type="expression" dxfId="26" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ22:AJ28">
-    <cfRule type="expression" dxfId="24" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45350,31 +45238,31 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="C782:C787 C844:C855 C789:C842">
-    <cfRule type="expression" dxfId="22" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>$A782=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
       <formula>$A782=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B336:C353 B764:C769 B301:C303 B4:C10 B297:C299 B38:C49 B25:C36 B496:C528 B12:C23 B844:B855 B315:C326 B530:C539 B541:C550 B728:C743 B745:C748 B750:C758 B332:C334 B771:C780 B328:C330 B760:C760 B762:C762 B305:C313 B355:C358 B782:B787 B552:C561 B51:C131 B133:C213 B215:C295 B360:C494 B563:C616 B673:C726 B618:C671 B789:B842">
-    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>$A4=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2 D2:Z2">
-    <cfRule type="cellIs" dxfId="18" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A10 A12:A23 A25:A36 A38:A49 A297:A299 A301:A303 A305:A313 A315:A326 A328:A330 A332:A334 A336:A353 A355:A358 A496:A528 A530:A539 A541:A550 A552:A561 A745:A748 A750:A758 A760 A762 A764:A769 A771:A780 A782:A787 A844:A855 A51:A131 A133:A213 A215:A295 A360:A494 A563:A616 A673:A726 A618:A671 A728:A743 A789:A842">
-    <cfRule type="cellIs" dxfId="17" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fixed missing files in Archive. removed mbuhl paths from batch files. replaced MAP with MAP++ files (source files & input files); haven't updated x64 version, yet added some HD inputs to CertTest case list (FASTCertTestCases.xlsx) removed Source/dependencies/Blank_MAP_DLL
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@845 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="2910" windowWidth="15180" windowHeight="8595" tabRatio="712"/>
+    <workbookView xWindow="5955" yWindow="2970" windowWidth="15180" windowHeight="8535" tabRatio="712"/>
   </bookViews>
   <sheets>
     <sheet name="TestMatrix (new)" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="_Toc46290869" localSheetId="2">Variables!$B$770</definedName>
     <definedName name="_Toc46290870" localSheetId="2">Variables!$B$781</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">TestMatrix!$B$2:$AX$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'TestMatrix (new)'!$B$2:$BC$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'TestMatrix (new)'!$B$2:$BH$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Variables!$B$1:$P$855</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2803" uniqueCount="1122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2808" uniqueCount="1127">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3415,6 +3415,21 @@
   </si>
   <si>
     <t>Test22</t>
+  </si>
+  <si>
+    <t>Water Depth (m)</t>
+  </si>
+  <si>
+    <t>WaveMod</t>
+  </si>
+  <si>
+    <t>WaveHS</t>
+  </si>
+  <si>
+    <t>WaveTp</t>
+  </si>
+  <si>
+    <t>1P0.0</t>
   </si>
 </sst>
 </file>
@@ -3443,6 +3458,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -4103,7 +4119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4595,6 +4611,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5097,13 +5119,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BH61"/>
+  <dimension ref="A1:BM61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="U4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="AQ34" sqref="AQ34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5133,21 +5155,23 @@
     <col min="34" max="34" width="4.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="35" max="41" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="42" max="47" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="51" width="4.85546875" style="2" customWidth="1"/>
-    <col min="52" max="52" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="4.5703125" style="45" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="3.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="57" max="58" width="3.28515625" style="45" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="5.7109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="4.42578125" customWidth="1"/>
-    <col min="62" max="62" width="4.28515625" customWidth="1"/>
+    <col min="48" max="48" width="4.85546875" style="2" customWidth="1"/>
+    <col min="49" max="49" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="56" width="4.85546875" style="2" customWidth="1"/>
+    <col min="57" max="57" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="4.5703125" style="45" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="3.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="62" max="63" width="3.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.7109375" style="45" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="4.42578125" customWidth="1"/>
+    <col min="67" max="67" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:65" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="160" t="s">
         <v>27</v>
       </c>
@@ -5209,22 +5233,27 @@
       </c>
       <c r="AW2" s="168"/>
       <c r="AX2" s="168"/>
-      <c r="AY2" s="172"/>
-      <c r="AZ2" s="173" t="s">
+      <c r="AY2" s="168"/>
+      <c r="AZ2" s="168"/>
+      <c r="BA2" s="168"/>
+      <c r="BB2" s="168"/>
+      <c r="BC2" s="168"/>
+      <c r="BD2" s="172"/>
+      <c r="BE2" s="173" t="s">
         <v>18</v>
       </c>
-      <c r="BA2" s="174"/>
-      <c r="BB2" s="174"/>
-      <c r="BC2" s="175"/>
-      <c r="BD2" s="154" t="s">
+      <c r="BF2" s="174"/>
+      <c r="BG2" s="174"/>
+      <c r="BH2" s="175"/>
+      <c r="BI2" s="154" t="s">
         <v>1047</v>
       </c>
-      <c r="BE2" s="155"/>
-      <c r="BF2" s="155"/>
-      <c r="BG2" s="155"/>
-      <c r="BH2" s="156"/>
-    </row>
-    <row r="3" spans="1:60" s="1" customFormat="1" ht="85.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="BJ2" s="155"/>
+      <c r="BK2" s="155"/>
+      <c r="BL2" s="155"/>
+      <c r="BM2" s="156"/>
+    </row>
+    <row r="3" spans="1:65" s="1" customFormat="1" ht="85.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
       <c r="B3" s="79" t="s">
         <v>287</v>
@@ -5364,39 +5393,52 @@
       <c r="AU3" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="AV3" s="97"/>
-      <c r="AW3" s="73"/>
-      <c r="AX3" s="73"/>
-      <c r="AY3" s="74"/>
-      <c r="AZ3" s="75" t="s">
+      <c r="AV3" s="176" t="s">
+        <v>1122</v>
+      </c>
+      <c r="AW3" s="177" t="s">
+        <v>1123</v>
+      </c>
+      <c r="AX3" s="177" t="s">
+        <v>1124</v>
+      </c>
+      <c r="AY3" s="177" t="s">
+        <v>1125</v>
+      </c>
+      <c r="AZ3" s="177"/>
+      <c r="BA3" s="177"/>
+      <c r="BB3" s="177"/>
+      <c r="BC3" s="73"/>
+      <c r="BD3" s="74"/>
+      <c r="BE3" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="BA3" s="77" t="s">
+      <c r="BF3" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="BB3" s="78" t="s">
+      <c r="BG3" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="BC3" s="76" t="s">
+      <c r="BH3" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="BD3" s="66" t="s">
+      <c r="BI3" s="66" t="s">
         <v>1045</v>
       </c>
-      <c r="BE3" s="69" t="s">
+      <c r="BJ3" s="69" t="s">
         <v>1046</v>
       </c>
-      <c r="BF3" s="70" t="s">
+      <c r="BK3" s="70" t="s">
         <v>1051</v>
       </c>
-      <c r="BG3" s="70" t="s">
+      <c r="BL3" s="70" t="s">
         <v>1054</v>
       </c>
-      <c r="BH3" s="68" t="s">
+      <c r="BM3" s="68" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27"/>
       <c r="B4" s="85" t="s">
         <v>20</v>
@@ -5539,37 +5581,42 @@
       <c r="AV4" s="98"/>
       <c r="AW4" s="35"/>
       <c r="AX4" s="35"/>
-      <c r="AY4" s="33"/>
-      <c r="AZ4" s="36" t="s">
+      <c r="AY4" s="35"/>
+      <c r="AZ4" s="35"/>
+      <c r="BA4" s="35"/>
+      <c r="BB4" s="35"/>
+      <c r="BC4" s="35"/>
+      <c r="BD4" s="33"/>
+      <c r="BE4" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="BA4" s="46">
+      <c r="BF4" s="46">
         <v>15</v>
       </c>
-      <c r="BB4" s="37">
+      <c r="BG4" s="37">
         <v>0.2</v>
       </c>
-      <c r="BC4" s="38" t="s">
+      <c r="BH4" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="BD4" s="59">
-        <v>0</v>
-      </c>
-      <c r="BE4" s="55">
+      <c r="BI4" s="59">
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="55">
         <v>3</v>
       </c>
-      <c r="BF4" s="62">
+      <c r="BK4" s="62">
         <f>Variables!D2</f>
         <v>23</v>
       </c>
-      <c r="BG4" s="62" t="s">
+      <c r="BL4" s="62" t="s">
         <v>1048</v>
       </c>
-      <c r="BH4" s="38" t="s">
+      <c r="BM4" s="38" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
       <c r="B5" s="85" t="s">
         <v>33</v>
@@ -5712,37 +5759,42 @@
       <c r="AV5" s="99"/>
       <c r="AW5" s="41"/>
       <c r="AX5" s="41"/>
-      <c r="AY5" s="42"/>
-      <c r="AZ5" s="43" t="s">
+      <c r="AY5" s="41"/>
+      <c r="AZ5" s="41"/>
+      <c r="BA5" s="41"/>
+      <c r="BB5" s="41"/>
+      <c r="BC5" s="41"/>
+      <c r="BD5" s="42"/>
+      <c r="BE5" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BA5" s="47">
-        <v>0</v>
-      </c>
-      <c r="BB5" s="44">
-        <v>0</v>
-      </c>
-      <c r="BC5" s="42" t="s">
+      <c r="BF5" s="47">
+        <v>0</v>
+      </c>
+      <c r="BG5" s="44">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD5" s="60">
-        <v>0</v>
-      </c>
-      <c r="BE5" s="56">
+      <c r="BI5" s="60">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="56">
         <v>1</v>
       </c>
-      <c r="BF5" s="63">
+      <c r="BK5" s="63">
         <f>Variables!E2</f>
         <v>22</v>
       </c>
-      <c r="BG5" s="63" t="s">
+      <c r="BL5" s="63" t="s">
         <v>1049</v>
       </c>
-      <c r="BH5" s="42" t="s">
+      <c r="BM5" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="85" t="s">
         <v>34</v>
@@ -5885,37 +5937,42 @@
       <c r="AV6" s="99"/>
       <c r="AW6" s="41"/>
       <c r="AX6" s="41"/>
-      <c r="AY6" s="42"/>
-      <c r="AZ6" s="43" t="s">
+      <c r="AY6" s="41"/>
+      <c r="AZ6" s="41"/>
+      <c r="BA6" s="41"/>
+      <c r="BB6" s="41"/>
+      <c r="BC6" s="41"/>
+      <c r="BD6" s="42"/>
+      <c r="BE6" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="BA6" s="47" t="s">
+      <c r="BF6" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="BB6" s="44">
+      <c r="BG6" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC6" s="42" t="s">
+      <c r="BH6" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD6" s="60">
-        <v>0</v>
-      </c>
-      <c r="BE6" s="56">
+      <c r="BI6" s="60">
+        <v>0</v>
+      </c>
+      <c r="BJ6" s="56">
         <v>3</v>
       </c>
-      <c r="BF6" s="63">
+      <c r="BK6" s="63">
         <f>Variables!F$2</f>
         <v>23</v>
       </c>
-      <c r="BG6" s="63" t="s">
+      <c r="BL6" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH6" s="42" t="s">
+      <c r="BM6" s="42" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="7" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="85" t="s">
         <v>35</v>
@@ -6058,37 +6115,42 @@
       <c r="AV7" s="99"/>
       <c r="AW7" s="41"/>
       <c r="AX7" s="41"/>
-      <c r="AY7" s="42"/>
-      <c r="AZ7" s="43" t="s">
+      <c r="AY7" s="41"/>
+      <c r="AZ7" s="41"/>
+      <c r="BA7" s="41"/>
+      <c r="BB7" s="41"/>
+      <c r="BC7" s="41"/>
+      <c r="BD7" s="42"/>
+      <c r="BE7" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="BA7" s="47" t="s">
+      <c r="BF7" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="BB7" s="44">
+      <c r="BG7" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC7" s="42" t="s">
+      <c r="BH7" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD7" s="60">
-        <v>0</v>
-      </c>
-      <c r="BE7" s="56">
+      <c r="BI7" s="60">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="56">
         <v>5</v>
       </c>
-      <c r="BF7" s="63">
+      <c r="BK7" s="63">
         <f>Variables!F$2</f>
         <v>23</v>
       </c>
-      <c r="BG7" s="63" t="s">
+      <c r="BL7" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BH7" s="42" t="s">
+      <c r="BM7" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
       <c r="B8" s="85" t="s">
         <v>36</v>
@@ -6231,37 +6293,42 @@
       <c r="AV8" s="99"/>
       <c r="AW8" s="41"/>
       <c r="AX8" s="41"/>
-      <c r="AY8" s="42"/>
-      <c r="AZ8" s="43" t="s">
+      <c r="AY8" s="41"/>
+      <c r="AZ8" s="41"/>
+      <c r="BA8" s="41"/>
+      <c r="BB8" s="41"/>
+      <c r="BC8" s="41"/>
+      <c r="BD8" s="42"/>
+      <c r="BE8" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BA8" s="47">
-        <v>0</v>
-      </c>
-      <c r="BB8" s="44">
-        <v>0</v>
-      </c>
-      <c r="BC8" s="42" t="s">
+      <c r="BF8" s="47">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="44">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD8" s="60">
-        <v>0</v>
-      </c>
-      <c r="BE8" s="56">
+      <c r="BI8" s="60">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="56">
         <v>3</v>
       </c>
-      <c r="BF8" s="63">
+      <c r="BK8" s="63">
         <f>Variables!G$2</f>
         <v>24</v>
       </c>
-      <c r="BG8" s="63" t="s">
+      <c r="BL8" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH8" s="42" t="s">
+      <c r="BM8" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
       <c r="B9" s="85" t="s">
         <v>37</v>
@@ -6405,37 +6472,42 @@
       <c r="AV9" s="99"/>
       <c r="AW9" s="41"/>
       <c r="AX9" s="41"/>
-      <c r="AY9" s="42"/>
-      <c r="AZ9" s="43" t="s">
+      <c r="AY9" s="41"/>
+      <c r="AZ9" s="41"/>
+      <c r="BA9" s="41"/>
+      <c r="BB9" s="41"/>
+      <c r="BC9" s="41"/>
+      <c r="BD9" s="42"/>
+      <c r="BE9" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="BA9" s="47">
-        <v>0</v>
-      </c>
-      <c r="BB9" s="44">
-        <v>0</v>
-      </c>
-      <c r="BC9" s="42" t="s">
+      <c r="BF9" s="47">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="44">
+        <v>0</v>
+      </c>
+      <c r="BH9" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD9" s="60">
-        <v>0</v>
-      </c>
-      <c r="BE9" s="56">
+      <c r="BI9" s="60">
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="56">
         <v>5</v>
       </c>
-      <c r="BF9" s="63">
+      <c r="BK9" s="63">
         <f>Variables!H$2</f>
         <v>22</v>
       </c>
-      <c r="BG9" s="63" t="s">
+      <c r="BL9" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH9" s="42" t="s">
+      <c r="BM9" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
       <c r="B10" s="85" t="s">
         <v>38</v>
@@ -6579,37 +6651,42 @@
       <c r="AV10" s="99"/>
       <c r="AW10" s="41"/>
       <c r="AX10" s="41"/>
-      <c r="AY10" s="42"/>
-      <c r="AZ10" s="43" t="s">
+      <c r="AY10" s="41"/>
+      <c r="AZ10" s="41"/>
+      <c r="BA10" s="41"/>
+      <c r="BB10" s="41"/>
+      <c r="BC10" s="41"/>
+      <c r="BD10" s="42"/>
+      <c r="BE10" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="BA10" s="47">
-        <v>0</v>
-      </c>
-      <c r="BB10" s="44">
+      <c r="BF10" s="47">
+        <v>0</v>
+      </c>
+      <c r="BG10" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC10" s="42" t="s">
+      <c r="BH10" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD10" s="60">
-        <v>0</v>
-      </c>
-      <c r="BE10" s="56">
+      <c r="BI10" s="60">
+        <v>0</v>
+      </c>
+      <c r="BJ10" s="56">
         <v>3</v>
       </c>
-      <c r="BF10" s="63">
+      <c r="BK10" s="63">
         <f>Variables!I$2</f>
         <v>24</v>
       </c>
-      <c r="BG10" s="63" t="s">
+      <c r="BL10" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH10" s="42" t="s">
+      <c r="BM10" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
       <c r="B11" s="85" t="s">
         <v>39</v>
@@ -6753,37 +6830,42 @@
       <c r="AV11" s="99"/>
       <c r="AW11" s="41"/>
       <c r="AX11" s="41"/>
-      <c r="AY11" s="42"/>
-      <c r="AZ11" s="43" t="s">
+      <c r="AY11" s="41"/>
+      <c r="AZ11" s="41"/>
+      <c r="BA11" s="41"/>
+      <c r="BB11" s="41"/>
+      <c r="BC11" s="41"/>
+      <c r="BD11" s="42"/>
+      <c r="BE11" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="BA11" s="47">
+      <c r="BF11" s="47">
         <v>15</v>
       </c>
-      <c r="BB11" s="44">
+      <c r="BG11" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC11" s="42" t="s">
+      <c r="BH11" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD11" s="60">
-        <v>0</v>
-      </c>
-      <c r="BE11" s="56">
+      <c r="BI11" s="60">
+        <v>0</v>
+      </c>
+      <c r="BJ11" s="56">
         <v>2</v>
       </c>
-      <c r="BF11" s="63">
+      <c r="BK11" s="63">
         <f>Variables!J$2</f>
         <v>27</v>
       </c>
-      <c r="BG11" s="63" t="s">
+      <c r="BL11" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH11" s="42" t="s">
+      <c r="BM11" s="42" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="12" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="85" t="s">
         <v>40</v>
@@ -6926,37 +7008,42 @@
       <c r="AV12" s="99"/>
       <c r="AW12" s="41"/>
       <c r="AX12" s="41"/>
-      <c r="AY12" s="42"/>
-      <c r="AZ12" s="43" t="s">
+      <c r="AY12" s="41"/>
+      <c r="AZ12" s="41"/>
+      <c r="BA12" s="41"/>
+      <c r="BB12" s="41"/>
+      <c r="BC12" s="41"/>
+      <c r="BD12" s="42"/>
+      <c r="BE12" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="BA12" s="47" t="s">
+      <c r="BF12" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="BB12" s="44">
+      <c r="BG12" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC12" s="42" t="s">
+      <c r="BH12" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD12" s="60">
-        <v>0</v>
-      </c>
-      <c r="BE12" s="56">
+      <c r="BI12" s="60">
+        <v>0</v>
+      </c>
+      <c r="BJ12" s="56">
         <v>5</v>
       </c>
-      <c r="BF12" s="63">
+      <c r="BK12" s="63">
         <f>Variables!K$2</f>
         <v>26</v>
       </c>
-      <c r="BG12" s="63" t="s">
+      <c r="BL12" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH12" s="42" t="s">
+      <c r="BM12" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="85" t="s">
         <v>41</v>
@@ -7099,37 +7186,42 @@
       <c r="AV13" s="99"/>
       <c r="AW13" s="41"/>
       <c r="AX13" s="41"/>
-      <c r="AY13" s="42"/>
-      <c r="AZ13" s="43" t="s">
+      <c r="AY13" s="41"/>
+      <c r="AZ13" s="41"/>
+      <c r="BA13" s="41"/>
+      <c r="BB13" s="41"/>
+      <c r="BC13" s="41"/>
+      <c r="BD13" s="42"/>
+      <c r="BE13" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BA13" s="47">
-        <v>0</v>
-      </c>
-      <c r="BB13" s="44">
-        <v>0</v>
-      </c>
-      <c r="BC13" s="42" t="s">
+      <c r="BF13" s="47">
+        <v>0</v>
+      </c>
+      <c r="BG13" s="44">
+        <v>0</v>
+      </c>
+      <c r="BH13" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD13" s="60">
-        <v>0</v>
-      </c>
-      <c r="BE13" s="56">
-        <v>0</v>
-      </c>
-      <c r="BF13" s="63">
+      <c r="BI13" s="60">
+        <v>0</v>
+      </c>
+      <c r="BJ13" s="56">
+        <v>0</v>
+      </c>
+      <c r="BK13" s="63">
         <f>Variables!L$2</f>
         <v>24</v>
       </c>
-      <c r="BG13" s="63" t="s">
+      <c r="BL13" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH13" s="42" t="s">
+      <c r="BM13" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="85" t="s">
         <v>51</v>
@@ -7272,37 +7364,42 @@
       <c r="AV14" s="99"/>
       <c r="AW14" s="41"/>
       <c r="AX14" s="41"/>
-      <c r="AY14" s="42"/>
-      <c r="AZ14" s="43" t="s">
+      <c r="AY14" s="41"/>
+      <c r="AZ14" s="41"/>
+      <c r="BA14" s="41"/>
+      <c r="BB14" s="41"/>
+      <c r="BC14" s="41"/>
+      <c r="BD14" s="42"/>
+      <c r="BE14" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BA14" s="47">
-        <v>0</v>
-      </c>
-      <c r="BB14" s="44">
+      <c r="BF14" s="47">
+        <v>0</v>
+      </c>
+      <c r="BG14" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC14" s="42" t="s">
+      <c r="BH14" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD14" s="60">
+      <c r="BI14" s="60">
         <v>2</v>
       </c>
-      <c r="BE14" s="56">
-        <v>0</v>
-      </c>
-      <c r="BF14" s="63">
+      <c r="BJ14" s="56">
+        <v>0</v>
+      </c>
+      <c r="BK14" s="63">
         <f>Variables!M$2</f>
         <v>21</v>
       </c>
-      <c r="BG14" s="63" t="s">
+      <c r="BL14" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH14" s="42" t="s">
+      <c r="BM14" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="85" t="s">
         <v>52</v>
@@ -7445,37 +7542,42 @@
       <c r="AV15" s="99"/>
       <c r="AW15" s="41"/>
       <c r="AX15" s="41"/>
-      <c r="AY15" s="42"/>
-      <c r="AZ15" s="43" t="s">
+      <c r="AY15" s="41"/>
+      <c r="AZ15" s="41"/>
+      <c r="BA15" s="41"/>
+      <c r="BB15" s="41"/>
+      <c r="BC15" s="41"/>
+      <c r="BD15" s="42"/>
+      <c r="BE15" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BA15" s="47" t="s">
+      <c r="BF15" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="BB15" s="44">
+      <c r="BG15" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC15" s="42" t="s">
+      <c r="BH15" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD15" s="60">
+      <c r="BI15" s="60">
         <v>2</v>
       </c>
-      <c r="BE15" s="56">
+      <c r="BJ15" s="56">
         <v>4</v>
       </c>
-      <c r="BF15" s="63">
+      <c r="BK15" s="63">
         <f>Variables!N$2</f>
         <v>21</v>
       </c>
-      <c r="BG15" s="63" t="s">
+      <c r="BL15" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH15" s="42" t="s">
+      <c r="BM15" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="85" t="s">
         <v>53</v>
@@ -7618,37 +7720,42 @@
       <c r="AV16" s="99"/>
       <c r="AW16" s="41"/>
       <c r="AX16" s="41"/>
-      <c r="AY16" s="42"/>
-      <c r="AZ16" s="43" t="s">
+      <c r="AY16" s="41"/>
+      <c r="AZ16" s="41"/>
+      <c r="BA16" s="41"/>
+      <c r="BB16" s="41"/>
+      <c r="BC16" s="41"/>
+      <c r="BD16" s="42"/>
+      <c r="BE16" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BA16" s="47">
-        <v>0</v>
-      </c>
-      <c r="BB16" s="44">
+      <c r="BF16" s="47">
+        <v>0</v>
+      </c>
+      <c r="BG16" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC16" s="42" t="s">
+      <c r="BH16" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD16" s="60">
+      <c r="BI16" s="60">
         <v>2</v>
       </c>
-      <c r="BE16" s="56">
-        <v>0</v>
-      </c>
-      <c r="BF16" s="63">
+      <c r="BJ16" s="56">
+        <v>0</v>
+      </c>
+      <c r="BK16" s="63">
         <f>Variables!O$2</f>
         <v>23</v>
       </c>
-      <c r="BG16" s="63" t="s">
+      <c r="BL16" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH16" s="42" t="s">
+      <c r="BM16" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="17" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
       <c r="B17" s="128"/>
       <c r="C17" s="152"/>
@@ -7699,18 +7806,23 @@
       <c r="AV17" s="134"/>
       <c r="AW17" s="132"/>
       <c r="AX17" s="132"/>
-      <c r="AY17" s="133"/>
-      <c r="AZ17" s="131"/>
-      <c r="BA17" s="135"/>
-      <c r="BB17" s="136"/>
-      <c r="BC17" s="133"/>
-      <c r="BD17" s="137"/>
-      <c r="BE17" s="138"/>
-      <c r="BF17" s="139"/>
-      <c r="BG17" s="139"/>
+      <c r="AY17" s="132"/>
+      <c r="AZ17" s="132"/>
+      <c r="BA17" s="132"/>
+      <c r="BB17" s="132"/>
+      <c r="BC17" s="132"/>
+      <c r="BD17" s="133"/>
+      <c r="BE17" s="131"/>
+      <c r="BF17" s="135"/>
+      <c r="BG17" s="136"/>
       <c r="BH17" s="133"/>
-    </row>
-    <row r="18" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="BI17" s="137"/>
+      <c r="BJ17" s="138"/>
+      <c r="BK17" s="139"/>
+      <c r="BL17" s="139"/>
+      <c r="BM17" s="133"/>
+    </row>
+    <row r="18" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
       <c r="B18" s="85" t="s">
         <v>289</v>
@@ -7853,37 +7965,42 @@
       <c r="AV18" s="99"/>
       <c r="AW18" s="41"/>
       <c r="AX18" s="41"/>
-      <c r="AY18" s="42"/>
-      <c r="AZ18" s="43" t="s">
+      <c r="AY18" s="41"/>
+      <c r="AZ18" s="41"/>
+      <c r="BA18" s="41"/>
+      <c r="BB18" s="41"/>
+      <c r="BC18" s="41"/>
+      <c r="BD18" s="42"/>
+      <c r="BE18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BA18" s="53" t="s">
+      <c r="BF18" s="53" t="s">
         <v>285</v>
       </c>
-      <c r="BB18" s="44">
+      <c r="BG18" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC18" s="42" t="s">
+      <c r="BH18" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD18" s="60">
-        <v>0</v>
-      </c>
-      <c r="BE18" s="61">
-        <v>0</v>
-      </c>
-      <c r="BF18" s="63">
+      <c r="BI18" s="60">
+        <v>0</v>
+      </c>
+      <c r="BJ18" s="61">
+        <v>0</v>
+      </c>
+      <c r="BK18" s="63">
         <f>Variables!Q$2</f>
         <v>0</v>
       </c>
-      <c r="BG18" s="63" t="s">
+      <c r="BL18" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH18" s="42" t="s">
+      <c r="BM18" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
       <c r="B19" s="85" t="s">
         <v>309</v>
@@ -8026,37 +8143,42 @@
       <c r="AV19" s="99"/>
       <c r="AW19" s="41"/>
       <c r="AX19" s="41"/>
-      <c r="AY19" s="42"/>
-      <c r="AZ19" s="43" t="s">
+      <c r="AY19" s="41"/>
+      <c r="AZ19" s="41"/>
+      <c r="BA19" s="41"/>
+      <c r="BB19" s="41"/>
+      <c r="BC19" s="41"/>
+      <c r="BD19" s="42"/>
+      <c r="BE19" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BA19" s="47" t="s">
+      <c r="BF19" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="BB19" s="44">
+      <c r="BG19" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC19" s="42" t="s">
+      <c r="BH19" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD19" s="60">
-        <v>0</v>
-      </c>
-      <c r="BE19" s="56">
-        <v>0</v>
-      </c>
-      <c r="BF19" s="63">
+      <c r="BI19" s="60">
+        <v>0</v>
+      </c>
+      <c r="BJ19" s="56">
+        <v>0</v>
+      </c>
+      <c r="BK19" s="63">
         <f>Variables!R$2</f>
         <v>25</v>
       </c>
-      <c r="BG19" s="63" t="s">
+      <c r="BL19" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH19" s="42" t="s">
+      <c r="BM19" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="85" t="s">
         <v>336</v>
@@ -8199,37 +8321,42 @@
       <c r="AV20" s="99"/>
       <c r="AW20" s="41"/>
       <c r="AX20" s="41"/>
-      <c r="AY20" s="42"/>
-      <c r="AZ20" s="43" t="s">
+      <c r="AY20" s="41"/>
+      <c r="AZ20" s="41"/>
+      <c r="BA20" s="41"/>
+      <c r="BB20" s="41"/>
+      <c r="BC20" s="41"/>
+      <c r="BD20" s="42"/>
+      <c r="BE20" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="BA20" s="53" t="s">
+      <c r="BF20" s="53" t="s">
         <v>285</v>
       </c>
-      <c r="BB20" s="44">
+      <c r="BG20" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC20" s="42" t="s">
+      <c r="BH20" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD20" s="60">
-        <v>0</v>
-      </c>
-      <c r="BE20" s="61">
-        <v>0</v>
-      </c>
-      <c r="BF20" s="63">
+      <c r="BI20" s="60">
+        <v>0</v>
+      </c>
+      <c r="BJ20" s="61">
+        <v>0</v>
+      </c>
+      <c r="BK20" s="63">
         <f>Variables!S$2</f>
         <v>25</v>
       </c>
-      <c r="BG20" s="63" t="s">
+      <c r="BL20" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BH20" s="42" t="s">
+      <c r="BM20" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="85" t="s">
         <v>1060</v>
@@ -8372,22 +8499,27 @@
       <c r="AV21" s="99"/>
       <c r="AW21" s="41"/>
       <c r="AX21" s="41"/>
-      <c r="AY21" s="42"/>
-      <c r="AZ21" s="43"/>
-      <c r="BA21" s="53"/>
-      <c r="BB21" s="44"/>
-      <c r="BC21" s="42" t="s">
+      <c r="AY21" s="41"/>
+      <c r="AZ21" s="41"/>
+      <c r="BA21" s="41"/>
+      <c r="BB21" s="41"/>
+      <c r="BC21" s="41"/>
+      <c r="BD21" s="42"/>
+      <c r="BE21" s="43"/>
+      <c r="BF21" s="53"/>
+      <c r="BG21" s="44"/>
+      <c r="BH21" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD21" s="60"/>
-      <c r="BE21" s="61"/>
-      <c r="BF21" s="63"/>
-      <c r="BG21" s="63" t="s">
+      <c r="BI21" s="60"/>
+      <c r="BJ21" s="61"/>
+      <c r="BK21" s="63"/>
+      <c r="BL21" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BH21" s="42"/>
-    </row>
-    <row r="22" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="BM21" s="42"/>
+    </row>
+    <row r="22" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
       <c r="B22" s="85" t="s">
         <v>1065</v>
@@ -8503,25 +8635,38 @@
       <c r="AS22" s="41"/>
       <c r="AT22" s="41"/>
       <c r="AU22" s="42"/>
-      <c r="AV22" s="99"/>
-      <c r="AW22" s="41"/>
-      <c r="AX22" s="41"/>
-      <c r="AY22" s="42"/>
-      <c r="AZ22" s="43"/>
-      <c r="BA22" s="53"/>
-      <c r="BB22" s="44"/>
-      <c r="BC22" s="42" t="s">
+      <c r="AV22" s="99">
+        <v>20</v>
+      </c>
+      <c r="AW22" s="41">
+        <v>2</v>
+      </c>
+      <c r="AX22" s="41">
+        <v>6</v>
+      </c>
+      <c r="AY22" s="41">
+        <v>10</v>
+      </c>
+      <c r="AZ22" s="41"/>
+      <c r="BA22" s="41"/>
+      <c r="BB22" s="41"/>
+      <c r="BC22" s="41"/>
+      <c r="BD22" s="42"/>
+      <c r="BE22" s="43"/>
+      <c r="BF22" s="53"/>
+      <c r="BG22" s="44"/>
+      <c r="BH22" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD22" s="60"/>
-      <c r="BE22" s="61"/>
-      <c r="BF22" s="63"/>
-      <c r="BG22" s="63" t="s">
+      <c r="BI22" s="60"/>
+      <c r="BJ22" s="61"/>
+      <c r="BK22" s="63"/>
+      <c r="BL22" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BH22" s="42"/>
-    </row>
-    <row r="23" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="BM22" s="42"/>
+    </row>
+    <row r="23" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="85" t="s">
         <v>1070</v>
@@ -8637,23 +8782,32 @@
       <c r="AS23" s="41"/>
       <c r="AT23" s="41"/>
       <c r="AU23" s="42"/>
-      <c r="AV23" s="99"/>
-      <c r="AW23" s="41"/>
+      <c r="AV23" s="99">
+        <v>45</v>
+      </c>
+      <c r="AW23" s="41" t="s">
+        <v>1126</v>
+      </c>
       <c r="AX23" s="41"/>
-      <c r="AY23" s="42"/>
-      <c r="AZ23" s="43"/>
-      <c r="BA23" s="53"/>
-      <c r="BB23" s="44"/>
-      <c r="BC23" s="42"/>
-      <c r="BD23" s="60"/>
-      <c r="BE23" s="61"/>
-      <c r="BF23" s="63"/>
-      <c r="BG23" s="63" t="s">
+      <c r="AY23" s="41"/>
+      <c r="AZ23" s="41"/>
+      <c r="BA23" s="41"/>
+      <c r="BB23" s="41"/>
+      <c r="BC23" s="41"/>
+      <c r="BD23" s="42"/>
+      <c r="BE23" s="43"/>
+      <c r="BF23" s="53"/>
+      <c r="BG23" s="44"/>
+      <c r="BH23" s="42"/>
+      <c r="BI23" s="60"/>
+      <c r="BJ23" s="61"/>
+      <c r="BK23" s="63"/>
+      <c r="BL23" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BH23" s="42"/>
-    </row>
-    <row r="24" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="BM23" s="42"/>
+    </row>
+    <row r="24" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="85" t="s">
         <v>1071</v>
@@ -8769,23 +8923,36 @@
       <c r="AS24" s="41"/>
       <c r="AT24" s="41"/>
       <c r="AU24" s="42"/>
-      <c r="AV24" s="99"/>
-      <c r="AW24" s="41"/>
-      <c r="AX24" s="41"/>
-      <c r="AY24" s="42"/>
-      <c r="AZ24" s="43"/>
-      <c r="BA24" s="53"/>
-      <c r="BB24" s="44"/>
-      <c r="BC24" s="42"/>
-      <c r="BD24" s="60"/>
-      <c r="BE24" s="61"/>
-      <c r="BF24" s="63"/>
-      <c r="BG24" s="63" t="s">
+      <c r="AV24" s="99">
+        <v>50</v>
+      </c>
+      <c r="AW24" s="41">
+        <v>2</v>
+      </c>
+      <c r="AX24" s="41">
+        <v>8</v>
+      </c>
+      <c r="AY24" s="41">
+        <v>10</v>
+      </c>
+      <c r="AZ24" s="41"/>
+      <c r="BA24" s="41"/>
+      <c r="BB24" s="41"/>
+      <c r="BC24" s="41"/>
+      <c r="BD24" s="42"/>
+      <c r="BE24" s="43"/>
+      <c r="BF24" s="53"/>
+      <c r="BG24" s="44"/>
+      <c r="BH24" s="42"/>
+      <c r="BI24" s="60"/>
+      <c r="BJ24" s="61"/>
+      <c r="BK24" s="63"/>
+      <c r="BL24" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BH24" s="42"/>
-    </row>
-    <row r="25" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="BM24" s="42"/>
+    </row>
+    <row r="25" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="85" t="s">
         <v>1121</v>
@@ -8904,22 +9071,27 @@
       <c r="AV25" s="99"/>
       <c r="AW25" s="41"/>
       <c r="AX25" s="41"/>
-      <c r="AY25" s="42"/>
-      <c r="AZ25" s="43"/>
-      <c r="BA25" s="53"/>
-      <c r="BB25" s="44"/>
-      <c r="BC25" s="42" t="s">
+      <c r="AY25" s="41"/>
+      <c r="AZ25" s="41"/>
+      <c r="BA25" s="41"/>
+      <c r="BB25" s="41"/>
+      <c r="BC25" s="41"/>
+      <c r="BD25" s="42"/>
+      <c r="BE25" s="43"/>
+      <c r="BF25" s="53"/>
+      <c r="BG25" s="44"/>
+      <c r="BH25" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD25" s="60"/>
-      <c r="BE25" s="61"/>
-      <c r="BF25" s="63"/>
-      <c r="BG25" s="63" t="s">
+      <c r="BI25" s="60"/>
+      <c r="BJ25" s="61"/>
+      <c r="BK25" s="63"/>
+      <c r="BL25" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BH25" s="42"/>
-    </row>
-    <row r="26" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BM25" s="42"/>
+    </row>
+    <row r="26" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="85" t="s">
         <v>1120</v>
@@ -9038,22 +9210,27 @@
       <c r="AV26" s="99"/>
       <c r="AW26" s="41"/>
       <c r="AX26" s="41"/>
-      <c r="AY26" s="42"/>
-      <c r="AZ26" s="43"/>
-      <c r="BA26" s="53"/>
-      <c r="BB26" s="44"/>
-      <c r="BC26" s="42" t="s">
+      <c r="AY26" s="41"/>
+      <c r="AZ26" s="41"/>
+      <c r="BA26" s="41"/>
+      <c r="BB26" s="41"/>
+      <c r="BC26" s="41"/>
+      <c r="BD26" s="42"/>
+      <c r="BE26" s="43"/>
+      <c r="BF26" s="53"/>
+      <c r="BG26" s="44"/>
+      <c r="BH26" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD26" s="60"/>
-      <c r="BE26" s="61"/>
-      <c r="BF26" s="63"/>
-      <c r="BG26" s="63" t="s">
+      <c r="BI26" s="60"/>
+      <c r="BJ26" s="61"/>
+      <c r="BK26" s="63"/>
+      <c r="BL26" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BH26" s="42"/>
-    </row>
-    <row r="27" spans="1:60" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BM26" s="42"/>
+    </row>
+    <row r="27" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="85" t="s">
         <v>1119</v>
@@ -9172,22 +9349,27 @@
       <c r="AV27" s="99"/>
       <c r="AW27" s="41"/>
       <c r="AX27" s="41"/>
-      <c r="AY27" s="42"/>
-      <c r="AZ27" s="43"/>
-      <c r="BA27" s="53"/>
-      <c r="BB27" s="44"/>
-      <c r="BC27" s="42" t="s">
+      <c r="AY27" s="41"/>
+      <c r="AZ27" s="41"/>
+      <c r="BA27" s="41"/>
+      <c r="BB27" s="41"/>
+      <c r="BC27" s="41"/>
+      <c r="BD27" s="42"/>
+      <c r="BE27" s="43"/>
+      <c r="BF27" s="53"/>
+      <c r="BG27" s="44"/>
+      <c r="BH27" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD27" s="60"/>
-      <c r="BE27" s="61"/>
-      <c r="BF27" s="63"/>
-      <c r="BG27" s="63" t="s">
+      <c r="BI27" s="60"/>
+      <c r="BJ27" s="61"/>
+      <c r="BK27" s="63"/>
+      <c r="BL27" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BH27" s="42"/>
-    </row>
-    <row r="28" spans="1:60" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="BM27" s="42"/>
+    </row>
+    <row r="28" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="85" t="s">
         <v>1118</v>
@@ -9306,22 +9488,27 @@
       <c r="AV28" s="99"/>
       <c r="AW28" s="41"/>
       <c r="AX28" s="41"/>
-      <c r="AY28" s="42"/>
-      <c r="AZ28" s="43"/>
-      <c r="BA28" s="53"/>
-      <c r="BB28" s="44"/>
-      <c r="BC28" s="42" t="s">
+      <c r="AY28" s="41"/>
+      <c r="AZ28" s="41"/>
+      <c r="BA28" s="41"/>
+      <c r="BB28" s="41"/>
+      <c r="BC28" s="41"/>
+      <c r="BD28" s="42"/>
+      <c r="BE28" s="43"/>
+      <c r="BF28" s="53"/>
+      <c r="BG28" s="44"/>
+      <c r="BH28" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD28" s="60"/>
-      <c r="BE28" s="61"/>
-      <c r="BF28" s="63"/>
-      <c r="BG28" s="63" t="s">
+      <c r="BI28" s="60"/>
+      <c r="BJ28" s="61"/>
+      <c r="BK28" s="63"/>
+      <c r="BL28" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BH28" s="42"/>
-    </row>
-    <row r="29" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="BM28" s="42"/>
+    </row>
+    <row r="29" spans="1:65" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="153"/>
       <c r="D29" s="3"/>
@@ -9373,348 +9560,353 @@
       <c r="AV29" s="100"/>
       <c r="AW29" s="8"/>
       <c r="AX29" s="8"/>
-      <c r="AY29" s="6"/>
-      <c r="AZ29" s="7"/>
-      <c r="BA29" s="48"/>
-      <c r="BB29" s="10"/>
-      <c r="BC29" s="6"/>
-      <c r="BD29" s="7"/>
-      <c r="BE29" s="48"/>
-      <c r="BF29" s="64"/>
-      <c r="BG29" s="64"/>
+      <c r="AY29" s="8"/>
+      <c r="AZ29" s="8"/>
+      <c r="BA29" s="8"/>
+      <c r="BB29" s="8"/>
+      <c r="BC29" s="8"/>
+      <c r="BD29" s="6"/>
+      <c r="BE29" s="7"/>
+      <c r="BF29" s="48"/>
+      <c r="BG29" s="10"/>
       <c r="BH29" s="6"/>
-    </row>
-    <row r="33" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY33" s="45"/>
-      <c r="AZ33" s="9"/>
-      <c r="BA33" s="2"/>
-      <c r="BB33" s="2"/>
-      <c r="BC33" s="45"/>
+      <c r="BI29" s="7"/>
+      <c r="BJ29" s="48"/>
+      <c r="BK29" s="64"/>
+      <c r="BL29" s="64"/>
+      <c r="BM29" s="6"/>
+    </row>
+    <row r="33" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD33" s="45"/>
+      <c r="BE33" s="9"/>
       <c r="BF33" s="2"/>
-      <c r="BG33"/>
-      <c r="BH33"/>
-    </row>
-    <row r="34" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY34" s="45"/>
-      <c r="AZ34" s="9"/>
-      <c r="BA34" s="2"/>
-      <c r="BB34" s="2"/>
-      <c r="BC34" s="45"/>
+      <c r="BG33" s="2"/>
+      <c r="BH33" s="45"/>
+      <c r="BI33" s="45"/>
+      <c r="BK33" s="2"/>
+      <c r="BL33"/>
+      <c r="BM33"/>
+    </row>
+    <row r="34" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD34" s="45"/>
+      <c r="BE34" s="9"/>
       <c r="BF34" s="2"/>
-      <c r="BG34"/>
-      <c r="BH34"/>
-    </row>
-    <row r="35" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY35" s="45"/>
-      <c r="AZ35" s="9"/>
-      <c r="BA35" s="2"/>
-      <c r="BB35" s="2"/>
-      <c r="BC35" s="45"/>
+      <c r="BG34" s="2"/>
+      <c r="BH34" s="45"/>
+      <c r="BI34" s="45"/>
+      <c r="BK34" s="2"/>
+      <c r="BL34"/>
+      <c r="BM34"/>
+    </row>
+    <row r="35" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD35" s="45"/>
+      <c r="BE35" s="9"/>
       <c r="BF35" s="2"/>
-      <c r="BG35"/>
-      <c r="BH35"/>
-    </row>
-    <row r="36" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY36" s="45"/>
-      <c r="AZ36" s="9"/>
-      <c r="BA36" s="2"/>
-      <c r="BB36" s="2"/>
-      <c r="BC36" s="45"/>
+      <c r="BG35" s="2"/>
+      <c r="BH35" s="45"/>
+      <c r="BI35" s="45"/>
+      <c r="BK35" s="2"/>
+      <c r="BL35"/>
+      <c r="BM35"/>
+    </row>
+    <row r="36" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD36" s="45"/>
+      <c r="BE36" s="9"/>
       <c r="BF36" s="2"/>
-      <c r="BG36"/>
-      <c r="BH36"/>
-    </row>
-    <row r="37" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY37" s="45"/>
-      <c r="AZ37" s="9"/>
-      <c r="BA37" s="2"/>
-      <c r="BB37" s="2"/>
-      <c r="BC37" s="45"/>
+      <c r="BG36" s="2"/>
+      <c r="BH36" s="45"/>
+      <c r="BI36" s="45"/>
+      <c r="BK36" s="2"/>
+      <c r="BL36"/>
+      <c r="BM36"/>
+    </row>
+    <row r="37" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD37" s="45"/>
+      <c r="BE37" s="9"/>
       <c r="BF37" s="2"/>
-      <c r="BG37"/>
-      <c r="BH37"/>
-    </row>
-    <row r="38" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY38" s="45"/>
-      <c r="AZ38" s="9"/>
-      <c r="BA38" s="2"/>
-      <c r="BB38" s="2"/>
-      <c r="BC38" s="45"/>
+      <c r="BG37" s="2"/>
+      <c r="BH37" s="45"/>
+      <c r="BI37" s="45"/>
+      <c r="BK37" s="2"/>
+      <c r="BL37"/>
+      <c r="BM37"/>
+    </row>
+    <row r="38" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD38" s="45"/>
+      <c r="BE38" s="9"/>
       <c r="BF38" s="2"/>
-      <c r="BG38"/>
-      <c r="BH38"/>
-    </row>
-    <row r="39" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY39" s="45"/>
-      <c r="AZ39" s="9"/>
-      <c r="BA39" s="2"/>
-      <c r="BB39" s="2"/>
-      <c r="BC39" s="45"/>
+      <c r="BG38" s="2"/>
+      <c r="BH38" s="45"/>
+      <c r="BI38" s="45"/>
+      <c r="BK38" s="2"/>
+      <c r="BL38"/>
+      <c r="BM38"/>
+    </row>
+    <row r="39" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD39" s="45"/>
+      <c r="BE39" s="9"/>
       <c r="BF39" s="2"/>
-      <c r="BG39"/>
-      <c r="BH39"/>
-    </row>
-    <row r="40" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY40" s="45"/>
-      <c r="AZ40" s="9"/>
-      <c r="BA40" s="2"/>
-      <c r="BB40" s="2"/>
-      <c r="BC40" s="45"/>
+      <c r="BG39" s="2"/>
+      <c r="BH39" s="45"/>
+      <c r="BI39" s="45"/>
+      <c r="BK39" s="2"/>
+      <c r="BL39"/>
+      <c r="BM39"/>
+    </row>
+    <row r="40" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD40" s="45"/>
+      <c r="BE40" s="9"/>
       <c r="BF40" s="2"/>
-      <c r="BG40"/>
-      <c r="BH40"/>
-    </row>
-    <row r="41" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY41" s="45"/>
-      <c r="AZ41" s="9"/>
-      <c r="BA41" s="2"/>
-      <c r="BB41" s="2"/>
-      <c r="BC41" s="45"/>
+      <c r="BG40" s="2"/>
+      <c r="BH40" s="45"/>
+      <c r="BI40" s="45"/>
+      <c r="BK40" s="2"/>
+      <c r="BL40"/>
+      <c r="BM40"/>
+    </row>
+    <row r="41" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD41" s="45"/>
+      <c r="BE41" s="9"/>
       <c r="BF41" s="2"/>
-      <c r="BG41"/>
-      <c r="BH41"/>
-    </row>
-    <row r="42" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY42" s="45"/>
-      <c r="AZ42" s="9"/>
-      <c r="BA42" s="2"/>
-      <c r="BB42" s="2"/>
-      <c r="BC42" s="45"/>
+      <c r="BG41" s="2"/>
+      <c r="BH41" s="45"/>
+      <c r="BI41" s="45"/>
+      <c r="BK41" s="2"/>
+      <c r="BL41"/>
+      <c r="BM41"/>
+    </row>
+    <row r="42" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD42" s="45"/>
+      <c r="BE42" s="9"/>
       <c r="BF42" s="2"/>
-      <c r="BG42"/>
-      <c r="BH42"/>
-    </row>
-    <row r="43" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY43" s="45"/>
-      <c r="AZ43" s="9"/>
-      <c r="BA43" s="2"/>
-      <c r="BB43" s="2"/>
-      <c r="BC43" s="45"/>
+      <c r="BG42" s="2"/>
+      <c r="BH42" s="45"/>
+      <c r="BI42" s="45"/>
+      <c r="BK42" s="2"/>
+      <c r="BL42"/>
+      <c r="BM42"/>
+    </row>
+    <row r="43" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD43" s="45"/>
+      <c r="BE43" s="9"/>
       <c r="BF43" s="2"/>
-      <c r="BG43"/>
-      <c r="BH43"/>
-    </row>
-    <row r="44" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY44" s="45"/>
-      <c r="AZ44" s="9"/>
-      <c r="BA44" s="2"/>
-      <c r="BB44" s="2"/>
-      <c r="BC44" s="45"/>
+      <c r="BG43" s="2"/>
+      <c r="BH43" s="45"/>
+      <c r="BI43" s="45"/>
+      <c r="BK43" s="2"/>
+      <c r="BL43"/>
+      <c r="BM43"/>
+    </row>
+    <row r="44" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD44" s="45"/>
+      <c r="BE44" s="9"/>
       <c r="BF44" s="2"/>
-      <c r="BG44"/>
-      <c r="BH44"/>
-    </row>
-    <row r="45" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY45" s="45"/>
-      <c r="AZ45" s="9"/>
-      <c r="BA45" s="2"/>
-      <c r="BB45" s="2"/>
-      <c r="BC45" s="45"/>
+      <c r="BG44" s="2"/>
+      <c r="BH44" s="45"/>
+      <c r="BI44" s="45"/>
+      <c r="BK44" s="2"/>
+      <c r="BL44"/>
+      <c r="BM44"/>
+    </row>
+    <row r="45" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD45" s="45"/>
+      <c r="BE45" s="9"/>
       <c r="BF45" s="2"/>
-      <c r="BG45"/>
-      <c r="BH45"/>
-    </row>
-    <row r="46" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY46" s="45"/>
-      <c r="AZ46" s="9"/>
-      <c r="BA46" s="2"/>
-      <c r="BB46" s="2"/>
-      <c r="BC46" s="45"/>
+      <c r="BG45" s="2"/>
+      <c r="BH45" s="45"/>
+      <c r="BI45" s="45"/>
+      <c r="BK45" s="2"/>
+      <c r="BL45"/>
+      <c r="BM45"/>
+    </row>
+    <row r="46" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD46" s="45"/>
+      <c r="BE46" s="9"/>
       <c r="BF46" s="2"/>
-      <c r="BG46"/>
-      <c r="BH46"/>
-    </row>
-    <row r="47" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY47" s="45"/>
-      <c r="AZ47" s="9"/>
-      <c r="BA47" s="2"/>
-      <c r="BB47" s="2"/>
-      <c r="BC47" s="45"/>
+      <c r="BG46" s="2"/>
+      <c r="BH46" s="45"/>
+      <c r="BI46" s="45"/>
+      <c r="BK46" s="2"/>
+      <c r="BL46"/>
+      <c r="BM46"/>
+    </row>
+    <row r="47" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD47" s="45"/>
+      <c r="BE47" s="9"/>
       <c r="BF47" s="2"/>
-      <c r="BG47"/>
-      <c r="BH47"/>
-    </row>
-    <row r="48" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY48" s="45"/>
-      <c r="AZ48" s="9"/>
-      <c r="BA48" s="2"/>
-      <c r="BB48" s="2"/>
-      <c r="BC48" s="45"/>
+      <c r="BG47" s="2"/>
+      <c r="BH47" s="45"/>
+      <c r="BI47" s="45"/>
+      <c r="BK47" s="2"/>
+      <c r="BL47"/>
+      <c r="BM47"/>
+    </row>
+    <row r="48" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD48" s="45"/>
+      <c r="BE48" s="9"/>
       <c r="BF48" s="2"/>
-      <c r="BG48"/>
-      <c r="BH48"/>
-    </row>
-    <row r="49" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY49" s="45"/>
-      <c r="AZ49" s="9"/>
-      <c r="BA49" s="2"/>
-      <c r="BB49" s="2"/>
-      <c r="BC49" s="45"/>
+      <c r="BG48" s="2"/>
+      <c r="BH48" s="45"/>
+      <c r="BI48" s="45"/>
+      <c r="BK48" s="2"/>
+      <c r="BL48"/>
+      <c r="BM48"/>
+    </row>
+    <row r="49" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD49" s="45"/>
+      <c r="BE49" s="9"/>
       <c r="BF49" s="2"/>
-      <c r="BG49"/>
-      <c r="BH49"/>
-    </row>
-    <row r="50" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY50" s="45"/>
-      <c r="AZ50" s="9"/>
-      <c r="BA50" s="2"/>
-      <c r="BB50" s="2"/>
-      <c r="BC50" s="45"/>
+      <c r="BG49" s="2"/>
+      <c r="BH49" s="45"/>
+      <c r="BI49" s="45"/>
+      <c r="BK49" s="2"/>
+      <c r="BL49"/>
+      <c r="BM49"/>
+    </row>
+    <row r="50" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD50" s="45"/>
+      <c r="BE50" s="9"/>
       <c r="BF50" s="2"/>
-      <c r="BG50"/>
-      <c r="BH50"/>
-    </row>
-    <row r="51" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY51" s="45"/>
-      <c r="AZ51" s="9"/>
-      <c r="BA51" s="2"/>
-      <c r="BB51" s="2"/>
-      <c r="BC51" s="45"/>
+      <c r="BG50" s="2"/>
+      <c r="BH50" s="45"/>
+      <c r="BI50" s="45"/>
+      <c r="BK50" s="2"/>
+      <c r="BL50"/>
+      <c r="BM50"/>
+    </row>
+    <row r="51" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD51" s="45"/>
+      <c r="BE51" s="9"/>
       <c r="BF51" s="2"/>
-      <c r="BG51"/>
-      <c r="BH51"/>
-    </row>
-    <row r="52" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY52" s="45"/>
-      <c r="AZ52" s="9"/>
-      <c r="BA52" s="2"/>
-      <c r="BB52" s="2"/>
-      <c r="BC52" s="45"/>
+      <c r="BG51" s="2"/>
+      <c r="BH51" s="45"/>
+      <c r="BI51" s="45"/>
+      <c r="BK51" s="2"/>
+      <c r="BL51"/>
+      <c r="BM51"/>
+    </row>
+    <row r="52" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD52" s="45"/>
+      <c r="BE52" s="9"/>
       <c r="BF52" s="2"/>
-      <c r="BG52"/>
-      <c r="BH52"/>
-    </row>
-    <row r="53" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY53" s="45"/>
-      <c r="AZ53" s="9"/>
-      <c r="BA53" s="2"/>
-      <c r="BB53" s="2"/>
-      <c r="BC53" s="45"/>
+      <c r="BG52" s="2"/>
+      <c r="BH52" s="45"/>
+      <c r="BI52" s="45"/>
+      <c r="BK52" s="2"/>
+      <c r="BL52"/>
+      <c r="BM52"/>
+    </row>
+    <row r="53" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD53" s="45"/>
+      <c r="BE53" s="9"/>
       <c r="BF53" s="2"/>
-      <c r="BG53"/>
-      <c r="BH53"/>
-    </row>
-    <row r="54" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY54" s="45"/>
-      <c r="AZ54" s="9"/>
-      <c r="BA54" s="2"/>
-      <c r="BB54" s="2"/>
-      <c r="BC54" s="45"/>
+      <c r="BG53" s="2"/>
+      <c r="BH53" s="45"/>
+      <c r="BI53" s="45"/>
+      <c r="BK53" s="2"/>
+      <c r="BL53"/>
+      <c r="BM53"/>
+    </row>
+    <row r="54" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD54" s="45"/>
+      <c r="BE54" s="9"/>
       <c r="BF54" s="2"/>
-      <c r="BG54"/>
-      <c r="BH54"/>
-    </row>
-    <row r="55" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY55" s="45"/>
-      <c r="AZ55" s="9"/>
-      <c r="BA55" s="2"/>
-      <c r="BB55" s="2"/>
-      <c r="BC55" s="45"/>
+      <c r="BG54" s="2"/>
+      <c r="BH54" s="45"/>
+      <c r="BI54" s="45"/>
+      <c r="BK54" s="2"/>
+      <c r="BL54"/>
+      <c r="BM54"/>
+    </row>
+    <row r="55" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD55" s="45"/>
+      <c r="BE55" s="9"/>
       <c r="BF55" s="2"/>
-      <c r="BG55"/>
-      <c r="BH55"/>
-    </row>
-    <row r="56" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY56" s="45"/>
-      <c r="AZ56" s="9"/>
-      <c r="BA56" s="2"/>
-      <c r="BB56" s="2"/>
-      <c r="BC56" s="45"/>
+      <c r="BG55" s="2"/>
+      <c r="BH55" s="45"/>
+      <c r="BI55" s="45"/>
+      <c r="BK55" s="2"/>
+      <c r="BL55"/>
+      <c r="BM55"/>
+    </row>
+    <row r="56" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD56" s="45"/>
+      <c r="BE56" s="9"/>
       <c r="BF56" s="2"/>
-      <c r="BG56"/>
-      <c r="BH56"/>
-    </row>
-    <row r="57" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY57" s="45"/>
-      <c r="AZ57" s="9"/>
-      <c r="BA57" s="2"/>
-      <c r="BB57" s="2"/>
-      <c r="BC57" s="45"/>
+      <c r="BG56" s="2"/>
+      <c r="BH56" s="45"/>
+      <c r="BI56" s="45"/>
+      <c r="BK56" s="2"/>
+      <c r="BL56"/>
+      <c r="BM56"/>
+    </row>
+    <row r="57" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD57" s="45"/>
+      <c r="BE57" s="9"/>
       <c r="BF57" s="2"/>
-      <c r="BG57"/>
-      <c r="BH57"/>
-    </row>
-    <row r="58" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY58" s="45"/>
-      <c r="AZ58" s="9"/>
-      <c r="BA58" s="2"/>
-      <c r="BB58" s="2"/>
-      <c r="BC58" s="45"/>
+      <c r="BG57" s="2"/>
+      <c r="BH57" s="45"/>
+      <c r="BI57" s="45"/>
+      <c r="BK57" s="2"/>
+      <c r="BL57"/>
+      <c r="BM57"/>
+    </row>
+    <row r="58" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD58" s="45"/>
+      <c r="BE58" s="9"/>
       <c r="BF58" s="2"/>
-      <c r="BG58"/>
-      <c r="BH58"/>
-    </row>
-    <row r="59" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY59" s="45"/>
-      <c r="AZ59" s="9"/>
-      <c r="BA59" s="2"/>
-      <c r="BB59" s="2"/>
-      <c r="BC59" s="45"/>
+      <c r="BG58" s="2"/>
+      <c r="BH58" s="45"/>
+      <c r="BI58" s="45"/>
+      <c r="BK58" s="2"/>
+      <c r="BL58"/>
+      <c r="BM58"/>
+    </row>
+    <row r="59" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD59" s="45"/>
+      <c r="BE59" s="9"/>
       <c r="BF59" s="2"/>
-      <c r="BG59"/>
-      <c r="BH59"/>
-    </row>
-    <row r="60" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY60" s="45"/>
-      <c r="AZ60" s="9"/>
-      <c r="BA60" s="2"/>
-      <c r="BB60" s="2"/>
-      <c r="BC60" s="45"/>
+      <c r="BG59" s="2"/>
+      <c r="BH59" s="45"/>
+      <c r="BI59" s="45"/>
+      <c r="BK59" s="2"/>
+      <c r="BL59"/>
+      <c r="BM59"/>
+    </row>
+    <row r="60" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD60" s="45"/>
+      <c r="BE60" s="9"/>
       <c r="BF60" s="2"/>
-      <c r="BG60"/>
-      <c r="BH60"/>
-    </row>
-    <row r="61" spans="51:60" x14ac:dyDescent="0.2">
-      <c r="AY61" s="45"/>
-      <c r="AZ61" s="9"/>
-      <c r="BA61" s="2"/>
-      <c r="BB61" s="2"/>
-      <c r="BC61" s="45"/>
+      <c r="BG60" s="2"/>
+      <c r="BH60" s="45"/>
+      <c r="BI60" s="45"/>
+      <c r="BK60" s="2"/>
+      <c r="BL60"/>
+      <c r="BM60"/>
+    </row>
+    <row r="61" spans="56:65" x14ac:dyDescent="0.2">
       <c r="BD61" s="45"/>
+      <c r="BE61" s="9"/>
       <c r="BF61" s="2"/>
-      <c r="BG61"/>
-      <c r="BH61"/>
+      <c r="BG61" s="2"/>
+      <c r="BH61" s="45"/>
+      <c r="BI61" s="45"/>
+      <c r="BK61" s="2"/>
+      <c r="BL61"/>
+      <c r="BM61"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="BD2:BH2"/>
+    <mergeCell ref="BI2:BM2"/>
     <mergeCell ref="H2:V2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="W2:AD2"/>
     <mergeCell ref="AE2:AO2"/>
     <mergeCell ref="AP2:AU2"/>
-    <mergeCell ref="AV2:AY2"/>
-    <mergeCell ref="AZ2:BC2"/>
+    <mergeCell ref="AV2:BD2"/>
+    <mergeCell ref="BE2:BH2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 AA18:AA29 W4:BH13 A4:G27 AB14:BH30">
+  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 AA18:AA29 W4:BM13 A4:G27 AB14:BM30">
     <cfRule type="expression" dxfId="24" priority="17" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>

</xml_diff>

<commit_message>
+ updated switches in ServoDyn (user routines from subroutines are option 3 for ALL control types) + added two lines in ServoDyn input file for future use with TMD model + added scripts to convert input files, and ran them to update CertTest files + added Lidar files to FAST_Gateway.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@902 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -40,6 +40,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">Variables!$B$1:$P$855</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -4546,6 +4547,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4611,12 +4618,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5125,7 +5126,7 @@
       <pane xSplit="7" ySplit="3" topLeftCell="U4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AQ34" sqref="AQ34"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5172,86 +5173,86 @@
   <sheetData>
     <row r="1" spans="1:65" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:65" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="162" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="161"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="157" t="s">
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="159" t="s">
         <v>1104</v>
       </c>
-      <c r="I2" s="158"/>
-      <c r="J2" s="158"/>
-      <c r="K2" s="158"/>
-      <c r="L2" s="158"/>
-      <c r="M2" s="158"/>
-      <c r="N2" s="158"/>
-      <c r="O2" s="158"/>
-      <c r="P2" s="158"/>
-      <c r="Q2" s="158"/>
-      <c r="R2" s="158"/>
-      <c r="S2" s="158"/>
-      <c r="T2" s="158"/>
-      <c r="U2" s="158"/>
-      <c r="V2" s="159"/>
-      <c r="W2" s="155" t="s">
+      <c r="I2" s="160"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="160"/>
+      <c r="L2" s="160"/>
+      <c r="M2" s="160"/>
+      <c r="N2" s="160"/>
+      <c r="O2" s="160"/>
+      <c r="P2" s="160"/>
+      <c r="Q2" s="160"/>
+      <c r="R2" s="160"/>
+      <c r="S2" s="160"/>
+      <c r="T2" s="160"/>
+      <c r="U2" s="160"/>
+      <c r="V2" s="161"/>
+      <c r="W2" s="157" t="s">
         <v>1110</v>
       </c>
-      <c r="X2" s="163"/>
-      <c r="Y2" s="163"/>
-      <c r="Z2" s="163"/>
-      <c r="AA2" s="163"/>
-      <c r="AB2" s="163"/>
-      <c r="AC2" s="163"/>
-      <c r="AD2" s="164"/>
-      <c r="AE2" s="165" t="s">
+      <c r="X2" s="165"/>
+      <c r="Y2" s="165"/>
+      <c r="Z2" s="165"/>
+      <c r="AA2" s="165"/>
+      <c r="AB2" s="165"/>
+      <c r="AC2" s="165"/>
+      <c r="AD2" s="166"/>
+      <c r="AE2" s="167" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" s="166"/>
-      <c r="AG2" s="166"/>
-      <c r="AH2" s="166"/>
-      <c r="AI2" s="166"/>
-      <c r="AJ2" s="166"/>
-      <c r="AK2" s="166"/>
-      <c r="AL2" s="166"/>
-      <c r="AM2" s="166"/>
-      <c r="AN2" s="166"/>
-      <c r="AO2" s="167"/>
-      <c r="AP2" s="168" t="s">
+      <c r="AF2" s="168"/>
+      <c r="AG2" s="168"/>
+      <c r="AH2" s="168"/>
+      <c r="AI2" s="168"/>
+      <c r="AJ2" s="168"/>
+      <c r="AK2" s="168"/>
+      <c r="AL2" s="168"/>
+      <c r="AM2" s="168"/>
+      <c r="AN2" s="168"/>
+      <c r="AO2" s="169"/>
+      <c r="AP2" s="170" t="s">
         <v>43</v>
       </c>
-      <c r="AQ2" s="169"/>
-      <c r="AR2" s="169"/>
-      <c r="AS2" s="169"/>
-      <c r="AT2" s="169"/>
-      <c r="AU2" s="170"/>
-      <c r="AV2" s="171" t="s">
+      <c r="AQ2" s="171"/>
+      <c r="AR2" s="171"/>
+      <c r="AS2" s="171"/>
+      <c r="AT2" s="171"/>
+      <c r="AU2" s="172"/>
+      <c r="AV2" s="173" t="s">
         <v>1061</v>
       </c>
-      <c r="AW2" s="168"/>
-      <c r="AX2" s="168"/>
-      <c r="AY2" s="168"/>
-      <c r="AZ2" s="168"/>
-      <c r="BA2" s="168"/>
-      <c r="BB2" s="168"/>
-      <c r="BC2" s="168"/>
-      <c r="BD2" s="172"/>
-      <c r="BE2" s="173" t="s">
+      <c r="AW2" s="170"/>
+      <c r="AX2" s="170"/>
+      <c r="AY2" s="170"/>
+      <c r="AZ2" s="170"/>
+      <c r="BA2" s="170"/>
+      <c r="BB2" s="170"/>
+      <c r="BC2" s="170"/>
+      <c r="BD2" s="174"/>
+      <c r="BE2" s="175" t="s">
         <v>18</v>
       </c>
-      <c r="BF2" s="174"/>
-      <c r="BG2" s="174"/>
-      <c r="BH2" s="175"/>
-      <c r="BI2" s="154" t="s">
+      <c r="BF2" s="176"/>
+      <c r="BG2" s="176"/>
+      <c r="BH2" s="177"/>
+      <c r="BI2" s="156" t="s">
         <v>1047</v>
       </c>
-      <c r="BJ2" s="155"/>
-      <c r="BK2" s="155"/>
-      <c r="BL2" s="155"/>
-      <c r="BM2" s="156"/>
+      <c r="BJ2" s="157"/>
+      <c r="BK2" s="157"/>
+      <c r="BL2" s="157"/>
+      <c r="BM2" s="158"/>
     </row>
     <row r="3" spans="1:65" s="1" customFormat="1" ht="85.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
@@ -5393,21 +5394,21 @@
       <c r="AU3" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="AV3" s="176" t="s">
+      <c r="AV3" s="154" t="s">
         <v>1122</v>
       </c>
-      <c r="AW3" s="177" t="s">
+      <c r="AW3" s="155" t="s">
         <v>1123</v>
       </c>
-      <c r="AX3" s="177" t="s">
+      <c r="AX3" s="155" t="s">
         <v>1124</v>
       </c>
-      <c r="AY3" s="177" t="s">
+      <c r="AY3" s="155" t="s">
         <v>1125</v>
       </c>
-      <c r="AZ3" s="177"/>
-      <c r="BA3" s="177"/>
-      <c r="BB3" s="177"/>
+      <c r="AZ3" s="155"/>
+      <c r="BA3" s="155"/>
+      <c r="BB3" s="155"/>
       <c r="BC3" s="73"/>
       <c r="BD3" s="74"/>
       <c r="BE3" s="75" t="s">
@@ -9995,74 +9996,74 @@
   <sheetData>
     <row r="1" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="162" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="161"/>
-      <c r="G2" s="161"/>
-      <c r="H2" s="162"/>
-      <c r="I2" s="154" t="s">
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="156" t="s">
         <v>1062</v>
       </c>
-      <c r="J2" s="155"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="164"/>
-      <c r="U2" s="165" t="s">
+      <c r="J2" s="157"/>
+      <c r="K2" s="165"/>
+      <c r="L2" s="165"/>
+      <c r="M2" s="165"/>
+      <c r="N2" s="165"/>
+      <c r="O2" s="165"/>
+      <c r="P2" s="165"/>
+      <c r="Q2" s="165"/>
+      <c r="R2" s="165"/>
+      <c r="S2" s="165"/>
+      <c r="T2" s="166"/>
+      <c r="U2" s="167" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="166"/>
-      <c r="W2" s="166"/>
-      <c r="X2" s="166"/>
-      <c r="Y2" s="166"/>
-      <c r="Z2" s="166"/>
-      <c r="AA2" s="166"/>
-      <c r="AB2" s="166"/>
-      <c r="AC2" s="166"/>
-      <c r="AD2" s="166"/>
-      <c r="AE2" s="166"/>
-      <c r="AF2" s="166"/>
-      <c r="AG2" s="166"/>
-      <c r="AH2" s="166"/>
-      <c r="AI2" s="166"/>
-      <c r="AJ2" s="167"/>
-      <c r="AK2" s="171" t="s">
+      <c r="V2" s="168"/>
+      <c r="W2" s="168"/>
+      <c r="X2" s="168"/>
+      <c r="Y2" s="168"/>
+      <c r="Z2" s="168"/>
+      <c r="AA2" s="168"/>
+      <c r="AB2" s="168"/>
+      <c r="AC2" s="168"/>
+      <c r="AD2" s="168"/>
+      <c r="AE2" s="168"/>
+      <c r="AF2" s="168"/>
+      <c r="AG2" s="168"/>
+      <c r="AH2" s="168"/>
+      <c r="AI2" s="168"/>
+      <c r="AJ2" s="169"/>
+      <c r="AK2" s="173" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="169"/>
-      <c r="AM2" s="169"/>
-      <c r="AN2" s="169"/>
-      <c r="AO2" s="169"/>
-      <c r="AP2" s="170"/>
-      <c r="AQ2" s="171" t="s">
+      <c r="AL2" s="171"/>
+      <c r="AM2" s="171"/>
+      <c r="AN2" s="171"/>
+      <c r="AO2" s="171"/>
+      <c r="AP2" s="172"/>
+      <c r="AQ2" s="173" t="s">
         <v>1061</v>
       </c>
-      <c r="AR2" s="168"/>
-      <c r="AS2" s="168"/>
-      <c r="AT2" s="172"/>
-      <c r="AU2" s="173" t="s">
+      <c r="AR2" s="170"/>
+      <c r="AS2" s="170"/>
+      <c r="AT2" s="174"/>
+      <c r="AU2" s="175" t="s">
         <v>18</v>
       </c>
-      <c r="AV2" s="174"/>
-      <c r="AW2" s="174"/>
-      <c r="AX2" s="175"/>
-      <c r="AY2" s="154" t="s">
+      <c r="AV2" s="176"/>
+      <c r="AW2" s="176"/>
+      <c r="AX2" s="177"/>
+      <c r="AY2" s="156" t="s">
         <v>1047</v>
       </c>
-      <c r="AZ2" s="155"/>
-      <c r="BA2" s="155"/>
-      <c r="BB2" s="155"/>
-      <c r="BC2" s="156"/>
+      <c r="AZ2" s="157"/>
+      <c r="BA2" s="157"/>
+      <c r="BB2" s="157"/>
+      <c r="BC2" s="158"/>
     </row>
     <row r="3" spans="1:55" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">

</xml_diff>

<commit_message>
added mws to FASTCertTestCases.xlsx; fixed typo in NRELOffshrBsline5MW_Onshore_ElastoDyn.dat; updated dependencies
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@927 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -36,16 +36,15 @@
     <definedName name="_Toc46290869" localSheetId="2">Variables!$B$770</definedName>
     <definedName name="_Toc46290870" localSheetId="2">Variables!$B$781</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">TestMatrix!$B$2:$AX$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'TestMatrix (new)'!$B$2:$BH$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'TestMatrix (new)'!$B$2:$BI$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Variables!$B$1:$P$855</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2808" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2811" uniqueCount="1128">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3431,6 +3430,9 @@
   </si>
   <si>
     <t>1P0.0</t>
+  </si>
+  <si>
+    <t>Mean Wind Speed</t>
   </si>
 </sst>
 </file>
@@ -4120,7 +4122,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4619,6 +4621,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="12" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5120,13 +5131,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BM61"/>
+  <dimension ref="A1:BN61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="U4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A27" sqref="A27:XFD27"/>
+      <selection pane="bottomRight" activeCell="BM26" sqref="BM26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5162,17 +5173,18 @@
     <col min="57" max="57" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="4.5703125" style="45" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="3.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="62" max="63" width="3.28515625" style="45" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="5.7109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="4.42578125" customWidth="1"/>
-    <col min="67" max="67" width="4.28515625" customWidth="1"/>
+    <col min="60" max="60" width="4.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="3.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="5.7109375" style="45" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="4.42578125" customWidth="1"/>
+    <col min="68" max="68" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:65" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:66" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="162" t="s">
         <v>27</v>
       </c>
@@ -5245,16 +5257,17 @@
       </c>
       <c r="BF2" s="176"/>
       <c r="BG2" s="176"/>
-      <c r="BH2" s="177"/>
-      <c r="BI2" s="156" t="s">
+      <c r="BH2" s="176"/>
+      <c r="BI2" s="177"/>
+      <c r="BJ2" s="156" t="s">
         <v>1047</v>
       </c>
-      <c r="BJ2" s="157"/>
       <c r="BK2" s="157"/>
       <c r="BL2" s="157"/>
-      <c r="BM2" s="158"/>
-    </row>
-    <row r="3" spans="1:65" s="1" customFormat="1" ht="85.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="BM2" s="157"/>
+      <c r="BN2" s="158"/>
+    </row>
+    <row r="3" spans="1:66" s="1" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
       <c r="B3" s="79" t="s">
         <v>287</v>
@@ -5420,26 +5433,29 @@
       <c r="BG3" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="BH3" s="76" t="s">
+      <c r="BH3" s="178" t="s">
+        <v>1127</v>
+      </c>
+      <c r="BI3" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="BI3" s="66" t="s">
+      <c r="BJ3" s="66" t="s">
         <v>1045</v>
       </c>
-      <c r="BJ3" s="69" t="s">
+      <c r="BK3" s="69" t="s">
         <v>1046</v>
       </c>
-      <c r="BK3" s="70" t="s">
+      <c r="BL3" s="70" t="s">
         <v>1051</v>
       </c>
-      <c r="BL3" s="70" t="s">
+      <c r="BM3" s="70" t="s">
         <v>1054</v>
       </c>
-      <c r="BM3" s="68" t="s">
+      <c r="BN3" s="68" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27"/>
       <c r="B4" s="85" t="s">
         <v>20</v>
@@ -5597,27 +5613,28 @@
       <c r="BG4" s="37">
         <v>0.2</v>
       </c>
-      <c r="BH4" s="38" t="s">
+      <c r="BH4" s="179"/>
+      <c r="BI4" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="BI4" s="59">
-        <v>0</v>
-      </c>
-      <c r="BJ4" s="55">
+      <c r="BJ4" s="59">
+        <v>0</v>
+      </c>
+      <c r="BK4" s="55">
         <v>3</v>
       </c>
-      <c r="BK4" s="62">
+      <c r="BL4" s="62">
         <f>Variables!D2</f>
         <v>23</v>
       </c>
-      <c r="BL4" s="62" t="s">
+      <c r="BM4" s="62" t="s">
         <v>1048</v>
       </c>
-      <c r="BM4" s="38" t="s">
+      <c r="BN4" s="38" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
       <c r="B5" s="85" t="s">
         <v>33</v>
@@ -5775,27 +5792,28 @@
       <c r="BG5" s="44">
         <v>0</v>
       </c>
-      <c r="BH5" s="42" t="s">
+      <c r="BH5" s="180"/>
+      <c r="BI5" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BI5" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ5" s="56">
+      <c r="BJ5" s="60">
+        <v>0</v>
+      </c>
+      <c r="BK5" s="56">
         <v>1</v>
       </c>
-      <c r="BK5" s="63">
+      <c r="BL5" s="63">
         <f>Variables!E2</f>
         <v>22</v>
       </c>
-      <c r="BL5" s="63" t="s">
+      <c r="BM5" s="63" t="s">
         <v>1049</v>
       </c>
-      <c r="BM5" s="42" t="s">
+      <c r="BN5" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="85" t="s">
         <v>34</v>
@@ -5953,27 +5971,28 @@
       <c r="BG6" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH6" s="42" t="s">
+      <c r="BH6" s="180"/>
+      <c r="BI6" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BI6" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ6" s="56">
+      <c r="BJ6" s="60">
+        <v>0</v>
+      </c>
+      <c r="BK6" s="56">
         <v>3</v>
       </c>
-      <c r="BK6" s="63">
+      <c r="BL6" s="63">
         <f>Variables!F$2</f>
         <v>23</v>
       </c>
-      <c r="BL6" s="63" t="s">
+      <c r="BM6" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM6" s="42" t="s">
+      <c r="BN6" s="42" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="7" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="85" t="s">
         <v>35</v>
@@ -6131,27 +6150,28 @@
       <c r="BG7" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH7" s="42" t="s">
+      <c r="BH7" s="180"/>
+      <c r="BI7" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI7" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ7" s="56">
+      <c r="BJ7" s="60">
+        <v>0</v>
+      </c>
+      <c r="BK7" s="56">
         <v>5</v>
       </c>
-      <c r="BK7" s="63">
+      <c r="BL7" s="63">
         <f>Variables!F$2</f>
         <v>23</v>
       </c>
-      <c r="BL7" s="63" t="s">
+      <c r="BM7" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM7" s="42" t="s">
+      <c r="BN7" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
       <c r="B8" s="85" t="s">
         <v>36</v>
@@ -6309,27 +6329,28 @@
       <c r="BG8" s="44">
         <v>0</v>
       </c>
-      <c r="BH8" s="42" t="s">
+      <c r="BH8" s="180"/>
+      <c r="BI8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BI8" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ8" s="56">
+      <c r="BJ8" s="60">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="56">
         <v>3</v>
       </c>
-      <c r="BK8" s="63">
+      <c r="BL8" s="63">
         <f>Variables!G$2</f>
         <v>24</v>
       </c>
-      <c r="BL8" s="63" t="s">
+      <c r="BM8" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM8" s="42" t="s">
+      <c r="BN8" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
       <c r="B9" s="85" t="s">
         <v>37</v>
@@ -6488,27 +6509,28 @@
       <c r="BG9" s="44">
         <v>0</v>
       </c>
-      <c r="BH9" s="42" t="s">
+      <c r="BH9" s="180"/>
+      <c r="BI9" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BI9" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ9" s="56">
+      <c r="BJ9" s="60">
+        <v>0</v>
+      </c>
+      <c r="BK9" s="56">
         <v>5</v>
       </c>
-      <c r="BK9" s="63">
+      <c r="BL9" s="63">
         <f>Variables!H$2</f>
         <v>22</v>
       </c>
-      <c r="BL9" s="63" t="s">
+      <c r="BM9" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM9" s="42" t="s">
+      <c r="BN9" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
       <c r="B10" s="85" t="s">
         <v>38</v>
@@ -6667,27 +6689,28 @@
       <c r="BG10" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH10" s="42" t="s">
+      <c r="BH10" s="180"/>
+      <c r="BI10" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI10" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ10" s="56">
+      <c r="BJ10" s="60">
+        <v>0</v>
+      </c>
+      <c r="BK10" s="56">
         <v>3</v>
       </c>
-      <c r="BK10" s="63">
+      <c r="BL10" s="63">
         <f>Variables!I$2</f>
         <v>24</v>
       </c>
-      <c r="BL10" s="63" t="s">
+      <c r="BM10" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM10" s="42" t="s">
+      <c r="BN10" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
       <c r="B11" s="85" t="s">
         <v>39</v>
@@ -6846,27 +6869,28 @@
       <c r="BG11" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH11" s="42" t="s">
+      <c r="BH11" s="180"/>
+      <c r="BI11" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BI11" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ11" s="56">
+      <c r="BJ11" s="60">
+        <v>0</v>
+      </c>
+      <c r="BK11" s="56">
         <v>2</v>
       </c>
-      <c r="BK11" s="63">
+      <c r="BL11" s="63">
         <f>Variables!J$2</f>
         <v>27</v>
       </c>
-      <c r="BL11" s="63" t="s">
+      <c r="BM11" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM11" s="42" t="s">
+      <c r="BN11" s="42" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="12" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="85" t="s">
         <v>40</v>
@@ -7024,27 +7048,28 @@
       <c r="BG12" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH12" s="42" t="s">
+      <c r="BH12" s="180"/>
+      <c r="BI12" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BI12" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ12" s="56">
+      <c r="BJ12" s="60">
+        <v>0</v>
+      </c>
+      <c r="BK12" s="56">
         <v>5</v>
       </c>
-      <c r="BK12" s="63">
+      <c r="BL12" s="63">
         <f>Variables!K$2</f>
         <v>26</v>
       </c>
-      <c r="BL12" s="63" t="s">
+      <c r="BM12" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM12" s="42" t="s">
+      <c r="BN12" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="85" t="s">
         <v>41</v>
@@ -7202,27 +7227,28 @@
       <c r="BG13" s="44">
         <v>0</v>
       </c>
-      <c r="BH13" s="42" t="s">
+      <c r="BH13" s="180"/>
+      <c r="BI13" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BI13" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ13" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK13" s="63">
+      <c r="BJ13" s="60">
+        <v>0</v>
+      </c>
+      <c r="BK13" s="56">
+        <v>0</v>
+      </c>
+      <c r="BL13" s="63">
         <f>Variables!L$2</f>
         <v>24</v>
       </c>
-      <c r="BL13" s="63" t="s">
+      <c r="BM13" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM13" s="42" t="s">
+      <c r="BN13" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:66" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="85" t="s">
         <v>51</v>
@@ -7380,27 +7406,28 @@
       <c r="BG14" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH14" s="42" t="s">
+      <c r="BH14" s="180"/>
+      <c r="BI14" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI14" s="60">
+      <c r="BJ14" s="60">
         <v>2</v>
       </c>
-      <c r="BJ14" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK14" s="63">
+      <c r="BK14" s="56">
+        <v>0</v>
+      </c>
+      <c r="BL14" s="63">
         <f>Variables!M$2</f>
         <v>21</v>
       </c>
-      <c r="BL14" s="63" t="s">
+      <c r="BM14" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM14" s="42" t="s">
+      <c r="BN14" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:66" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="85" t="s">
         <v>52</v>
@@ -7558,27 +7585,28 @@
       <c r="BG15" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH15" s="42" t="s">
+      <c r="BH15" s="180"/>
+      <c r="BI15" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BI15" s="60">
+      <c r="BJ15" s="60">
         <v>2</v>
       </c>
-      <c r="BJ15" s="56">
+      <c r="BK15" s="56">
         <v>4</v>
       </c>
-      <c r="BK15" s="63">
+      <c r="BL15" s="63">
         <f>Variables!N$2</f>
         <v>21</v>
       </c>
-      <c r="BL15" s="63" t="s">
+      <c r="BM15" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM15" s="42" t="s">
+      <c r="BN15" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:66" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="85" t="s">
         <v>53</v>
@@ -7736,27 +7764,28 @@
       <c r="BG16" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH16" s="42" t="s">
+      <c r="BH16" s="180"/>
+      <c r="BI16" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI16" s="60">
+      <c r="BJ16" s="60">
         <v>2</v>
       </c>
-      <c r="BJ16" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK16" s="63">
+      <c r="BK16" s="56">
+        <v>0</v>
+      </c>
+      <c r="BL16" s="63">
         <f>Variables!O$2</f>
         <v>23</v>
       </c>
-      <c r="BL16" s="63" t="s">
+      <c r="BM16" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM16" s="42" t="s">
+      <c r="BN16" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="17" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
       <c r="B17" s="128"/>
       <c r="C17" s="152"/>
@@ -7816,14 +7845,15 @@
       <c r="BE17" s="131"/>
       <c r="BF17" s="135"/>
       <c r="BG17" s="136"/>
-      <c r="BH17" s="133"/>
-      <c r="BI17" s="137"/>
-      <c r="BJ17" s="138"/>
-      <c r="BK17" s="139"/>
+      <c r="BH17" s="181"/>
+      <c r="BI17" s="133"/>
+      <c r="BJ17" s="137"/>
+      <c r="BK17" s="138"/>
       <c r="BL17" s="139"/>
-      <c r="BM17" s="133"/>
-    </row>
-    <row r="18" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="BM17" s="139"/>
+      <c r="BN17" s="133"/>
+    </row>
+    <row r="18" spans="1:66" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
       <c r="B18" s="85" t="s">
         <v>289</v>
@@ -7981,27 +8011,28 @@
       <c r="BG18" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH18" s="42" t="s">
+      <c r="BH18" s="180"/>
+      <c r="BI18" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BI18" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ18" s="61">
-        <v>0</v>
-      </c>
-      <c r="BK18" s="63">
+      <c r="BJ18" s="60">
+        <v>0</v>
+      </c>
+      <c r="BK18" s="61">
+        <v>0</v>
+      </c>
+      <c r="BL18" s="63">
         <f>Variables!Q$2</f>
         <v>0</v>
       </c>
-      <c r="BL18" s="63" t="s">
+      <c r="BM18" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM18" s="42" t="s">
+      <c r="BN18" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:66" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
       <c r="B19" s="85" t="s">
         <v>309</v>
@@ -8159,27 +8190,28 @@
       <c r="BG19" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH19" s="42" t="s">
+      <c r="BH19" s="180"/>
+      <c r="BI19" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BI19" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ19" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK19" s="63">
+      <c r="BJ19" s="60">
+        <v>0</v>
+      </c>
+      <c r="BK19" s="56">
+        <v>0</v>
+      </c>
+      <c r="BL19" s="63">
         <f>Variables!R$2</f>
         <v>25</v>
       </c>
-      <c r="BL19" s="63" t="s">
+      <c r="BM19" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM19" s="42" t="s">
+      <c r="BN19" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:66" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="85" t="s">
         <v>336</v>
@@ -8337,27 +8369,28 @@
       <c r="BG20" s="44">
         <v>0.2</v>
       </c>
-      <c r="BH20" s="42" t="s">
+      <c r="BH20" s="180"/>
+      <c r="BI20" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI20" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ20" s="61">
-        <v>0</v>
-      </c>
-      <c r="BK20" s="63">
+      <c r="BJ20" s="60">
+        <v>0</v>
+      </c>
+      <c r="BK20" s="61">
+        <v>0</v>
+      </c>
+      <c r="BL20" s="63">
         <f>Variables!S$2</f>
         <v>25</v>
       </c>
-      <c r="BL20" s="63" t="s">
+      <c r="BM20" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM20" s="42" t="s">
+      <c r="BN20" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:66" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="85" t="s">
         <v>1060</v>
@@ -8509,18 +8542,21 @@
       <c r="BE21" s="43"/>
       <c r="BF21" s="53"/>
       <c r="BG21" s="44"/>
-      <c r="BH21" s="42" t="s">
+      <c r="BH21" s="180">
+        <v>12</v>
+      </c>
+      <c r="BI21" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI21" s="60"/>
-      <c r="BJ21" s="61"/>
-      <c r="BK21" s="63"/>
-      <c r="BL21" s="63" t="s">
+      <c r="BJ21" s="60"/>
+      <c r="BK21" s="61"/>
+      <c r="BL21" s="63"/>
+      <c r="BM21" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM21" s="42"/>
-    </row>
-    <row r="22" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="BN21" s="42"/>
+    </row>
+    <row r="22" spans="1:66" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
       <c r="B22" s="85" t="s">
         <v>1065</v>
@@ -8656,18 +8692,21 @@
       <c r="BE22" s="43"/>
       <c r="BF22" s="53"/>
       <c r="BG22" s="44"/>
-      <c r="BH22" s="42" t="s">
+      <c r="BH22" s="180">
+        <v>12</v>
+      </c>
+      <c r="BI22" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI22" s="60"/>
-      <c r="BJ22" s="61"/>
-      <c r="BK22" s="63"/>
-      <c r="BL22" s="63" t="s">
+      <c r="BJ22" s="60"/>
+      <c r="BK22" s="61"/>
+      <c r="BL22" s="63"/>
+      <c r="BM22" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM22" s="42"/>
-    </row>
-    <row r="23" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="BN22" s="42"/>
+    </row>
+    <row r="23" spans="1:66" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="85" t="s">
         <v>1070</v>
@@ -8799,16 +8838,21 @@
       <c r="BE23" s="43"/>
       <c r="BF23" s="53"/>
       <c r="BG23" s="44"/>
-      <c r="BH23" s="42"/>
-      <c r="BI23" s="60"/>
-      <c r="BJ23" s="61"/>
-      <c r="BK23" s="63"/>
-      <c r="BL23" s="63" t="s">
+      <c r="BH23" s="180">
+        <v>8</v>
+      </c>
+      <c r="BI23" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="BJ23" s="60"/>
+      <c r="BK23" s="61"/>
+      <c r="BL23" s="63"/>
+      <c r="BM23" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM23" s="42"/>
-    </row>
-    <row r="24" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="BN23" s="42"/>
+    </row>
+    <row r="24" spans="1:66" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="85" t="s">
         <v>1071</v>
@@ -8944,16 +8988,21 @@
       <c r="BE24" s="43"/>
       <c r="BF24" s="53"/>
       <c r="BG24" s="44"/>
-      <c r="BH24" s="42"/>
-      <c r="BI24" s="60"/>
-      <c r="BJ24" s="61"/>
-      <c r="BK24" s="63"/>
-      <c r="BL24" s="63" t="s">
+      <c r="BH24" s="180">
+        <v>12</v>
+      </c>
+      <c r="BI24" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="BJ24" s="60"/>
+      <c r="BK24" s="61"/>
+      <c r="BL24" s="63"/>
+      <c r="BM24" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM24" s="42"/>
-    </row>
-    <row r="25" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="BN24" s="42"/>
+    </row>
+    <row r="25" spans="1:66" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="85" t="s">
         <v>1121</v>
@@ -9081,18 +9130,21 @@
       <c r="BE25" s="43"/>
       <c r="BF25" s="53"/>
       <c r="BG25" s="44"/>
-      <c r="BH25" s="42" t="s">
+      <c r="BH25" s="180">
+        <v>12</v>
+      </c>
+      <c r="BI25" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI25" s="60"/>
-      <c r="BJ25" s="61"/>
-      <c r="BK25" s="63"/>
-      <c r="BL25" s="63" t="s">
+      <c r="BJ25" s="60"/>
+      <c r="BK25" s="61"/>
+      <c r="BL25" s="63"/>
+      <c r="BM25" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM25" s="42"/>
-    </row>
-    <row r="26" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BN25" s="42"/>
+    </row>
+    <row r="26" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="85" t="s">
         <v>1120</v>
@@ -9220,18 +9272,21 @@
       <c r="BE26" s="43"/>
       <c r="BF26" s="53"/>
       <c r="BG26" s="44"/>
-      <c r="BH26" s="42" t="s">
+      <c r="BH26" s="180">
+        <v>12</v>
+      </c>
+      <c r="BI26" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI26" s="60"/>
-      <c r="BJ26" s="61"/>
-      <c r="BK26" s="63"/>
-      <c r="BL26" s="63" t="s">
+      <c r="BJ26" s="60"/>
+      <c r="BK26" s="61"/>
+      <c r="BL26" s="63"/>
+      <c r="BM26" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM26" s="42"/>
-    </row>
-    <row r="27" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BN26" s="42"/>
+    </row>
+    <row r="27" spans="1:66" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="85" t="s">
         <v>1119</v>
@@ -9359,18 +9414,21 @@
       <c r="BE27" s="43"/>
       <c r="BF27" s="53"/>
       <c r="BG27" s="44"/>
-      <c r="BH27" s="42" t="s">
+      <c r="BH27" s="180">
+        <v>12</v>
+      </c>
+      <c r="BI27" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BI27" s="60"/>
-      <c r="BJ27" s="61"/>
-      <c r="BK27" s="63"/>
-      <c r="BL27" s="63" t="s">
+      <c r="BJ27" s="60"/>
+      <c r="BK27" s="61"/>
+      <c r="BL27" s="63"/>
+      <c r="BM27" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM27" s="42"/>
-    </row>
-    <row r="28" spans="1:65" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="BN27" s="42"/>
+    </row>
+    <row r="28" spans="1:66" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="85" t="s">
         <v>1118</v>
@@ -9498,18 +9556,21 @@
       <c r="BE28" s="43"/>
       <c r="BF28" s="53"/>
       <c r="BG28" s="44"/>
-      <c r="BH28" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="BI28" s="60"/>
-      <c r="BJ28" s="61"/>
-      <c r="BK28" s="63"/>
-      <c r="BL28" s="63" t="s">
+      <c r="BH28" s="180">
+        <v>8</v>
+      </c>
+      <c r="BI28" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="BJ28" s="60"/>
+      <c r="BK28" s="61"/>
+      <c r="BL28" s="63"/>
+      <c r="BM28" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM28" s="42"/>
-    </row>
-    <row r="29" spans="1:65" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="BN28" s="42"/>
+    </row>
+    <row r="29" spans="1:66" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="153"/>
       <c r="D29" s="3"/>
@@ -9570,344 +9631,374 @@
       <c r="BE29" s="7"/>
       <c r="BF29" s="48"/>
       <c r="BG29" s="10"/>
-      <c r="BH29" s="6"/>
-      <c r="BI29" s="7"/>
-      <c r="BJ29" s="48"/>
-      <c r="BK29" s="64"/>
+      <c r="BH29" s="182"/>
+      <c r="BI29" s="6"/>
+      <c r="BJ29" s="7"/>
+      <c r="BK29" s="48"/>
       <c r="BL29" s="64"/>
-      <c r="BM29" s="6"/>
-    </row>
-    <row r="33" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BM29" s="64"/>
+      <c r="BN29" s="6"/>
+    </row>
+    <row r="33" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD33" s="45"/>
       <c r="BE33" s="9"/>
       <c r="BF33" s="2"/>
       <c r="BG33" s="2"/>
-      <c r="BH33" s="45"/>
+      <c r="BH33" s="2"/>
       <c r="BI33" s="45"/>
-      <c r="BK33" s="2"/>
-      <c r="BL33"/>
+      <c r="BJ33" s="45"/>
+      <c r="BL33" s="2"/>
       <c r="BM33"/>
-    </row>
-    <row r="34" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN33"/>
+    </row>
+    <row r="34" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD34" s="45"/>
       <c r="BE34" s="9"/>
       <c r="BF34" s="2"/>
       <c r="BG34" s="2"/>
-      <c r="BH34" s="45"/>
+      <c r="BH34" s="2"/>
       <c r="BI34" s="45"/>
-      <c r="BK34" s="2"/>
-      <c r="BL34"/>
+      <c r="BJ34" s="45"/>
+      <c r="BL34" s="2"/>
       <c r="BM34"/>
-    </row>
-    <row r="35" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN34"/>
+    </row>
+    <row r="35" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD35" s="45"/>
       <c r="BE35" s="9"/>
       <c r="BF35" s="2"/>
       <c r="BG35" s="2"/>
-      <c r="BH35" s="45"/>
+      <c r="BH35" s="2"/>
       <c r="BI35" s="45"/>
-      <c r="BK35" s="2"/>
-      <c r="BL35"/>
+      <c r="BJ35" s="45"/>
+      <c r="BL35" s="2"/>
       <c r="BM35"/>
-    </row>
-    <row r="36" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN35"/>
+    </row>
+    <row r="36" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD36" s="45"/>
       <c r="BE36" s="9"/>
       <c r="BF36" s="2"/>
       <c r="BG36" s="2"/>
-      <c r="BH36" s="45"/>
+      <c r="BH36" s="2"/>
       <c r="BI36" s="45"/>
-      <c r="BK36" s="2"/>
-      <c r="BL36"/>
+      <c r="BJ36" s="45"/>
+      <c r="BL36" s="2"/>
       <c r="BM36"/>
-    </row>
-    <row r="37" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN36"/>
+    </row>
+    <row r="37" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD37" s="45"/>
       <c r="BE37" s="9"/>
       <c r="BF37" s="2"/>
       <c r="BG37" s="2"/>
-      <c r="BH37" s="45"/>
+      <c r="BH37" s="2"/>
       <c r="BI37" s="45"/>
-      <c r="BK37" s="2"/>
-      <c r="BL37"/>
+      <c r="BJ37" s="45"/>
+      <c r="BL37" s="2"/>
       <c r="BM37"/>
-    </row>
-    <row r="38" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN37"/>
+    </row>
+    <row r="38" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD38" s="45"/>
       <c r="BE38" s="9"/>
       <c r="BF38" s="2"/>
       <c r="BG38" s="2"/>
-      <c r="BH38" s="45"/>
+      <c r="BH38" s="2"/>
       <c r="BI38" s="45"/>
-      <c r="BK38" s="2"/>
-      <c r="BL38"/>
+      <c r="BJ38" s="45"/>
+      <c r="BL38" s="2"/>
       <c r="BM38"/>
-    </row>
-    <row r="39" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN38"/>
+    </row>
+    <row r="39" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD39" s="45"/>
       <c r="BE39" s="9"/>
       <c r="BF39" s="2"/>
       <c r="BG39" s="2"/>
-      <c r="BH39" s="45"/>
+      <c r="BH39" s="2"/>
       <c r="BI39" s="45"/>
-      <c r="BK39" s="2"/>
-      <c r="BL39"/>
+      <c r="BJ39" s="45"/>
+      <c r="BL39" s="2"/>
       <c r="BM39"/>
-    </row>
-    <row r="40" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN39"/>
+    </row>
+    <row r="40" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD40" s="45"/>
       <c r="BE40" s="9"/>
       <c r="BF40" s="2"/>
       <c r="BG40" s="2"/>
-      <c r="BH40" s="45"/>
+      <c r="BH40" s="2"/>
       <c r="BI40" s="45"/>
-      <c r="BK40" s="2"/>
-      <c r="BL40"/>
+      <c r="BJ40" s="45"/>
+      <c r="BL40" s="2"/>
       <c r="BM40"/>
-    </row>
-    <row r="41" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN40"/>
+    </row>
+    <row r="41" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD41" s="45"/>
       <c r="BE41" s="9"/>
       <c r="BF41" s="2"/>
       <c r="BG41" s="2"/>
-      <c r="BH41" s="45"/>
+      <c r="BH41" s="2"/>
       <c r="BI41" s="45"/>
-      <c r="BK41" s="2"/>
-      <c r="BL41"/>
+      <c r="BJ41" s="45"/>
+      <c r="BL41" s="2"/>
       <c r="BM41"/>
-    </row>
-    <row r="42" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN41"/>
+    </row>
+    <row r="42" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD42" s="45"/>
       <c r="BE42" s="9"/>
       <c r="BF42" s="2"/>
       <c r="BG42" s="2"/>
-      <c r="BH42" s="45"/>
+      <c r="BH42" s="2"/>
       <c r="BI42" s="45"/>
-      <c r="BK42" s="2"/>
-      <c r="BL42"/>
+      <c r="BJ42" s="45"/>
+      <c r="BL42" s="2"/>
       <c r="BM42"/>
-    </row>
-    <row r="43" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN42"/>
+    </row>
+    <row r="43" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD43" s="45"/>
       <c r="BE43" s="9"/>
       <c r="BF43" s="2"/>
       <c r="BG43" s="2"/>
-      <c r="BH43" s="45"/>
+      <c r="BH43" s="2"/>
       <c r="BI43" s="45"/>
-      <c r="BK43" s="2"/>
-      <c r="BL43"/>
+      <c r="BJ43" s="45"/>
+      <c r="BL43" s="2"/>
       <c r="BM43"/>
-    </row>
-    <row r="44" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN43"/>
+    </row>
+    <row r="44" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD44" s="45"/>
       <c r="BE44" s="9"/>
       <c r="BF44" s="2"/>
       <c r="BG44" s="2"/>
-      <c r="BH44" s="45"/>
+      <c r="BH44" s="2"/>
       <c r="BI44" s="45"/>
-      <c r="BK44" s="2"/>
-      <c r="BL44"/>
+      <c r="BJ44" s="45"/>
+      <c r="BL44" s="2"/>
       <c r="BM44"/>
-    </row>
-    <row r="45" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN44"/>
+    </row>
+    <row r="45" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD45" s="45"/>
       <c r="BE45" s="9"/>
       <c r="BF45" s="2"/>
       <c r="BG45" s="2"/>
-      <c r="BH45" s="45"/>
+      <c r="BH45" s="2"/>
       <c r="BI45" s="45"/>
-      <c r="BK45" s="2"/>
-      <c r="BL45"/>
+      <c r="BJ45" s="45"/>
+      <c r="BL45" s="2"/>
       <c r="BM45"/>
-    </row>
-    <row r="46" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN45"/>
+    </row>
+    <row r="46" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD46" s="45"/>
       <c r="BE46" s="9"/>
       <c r="BF46" s="2"/>
       <c r="BG46" s="2"/>
-      <c r="BH46" s="45"/>
+      <c r="BH46" s="2"/>
       <c r="BI46" s="45"/>
-      <c r="BK46" s="2"/>
-      <c r="BL46"/>
+      <c r="BJ46" s="45"/>
+      <c r="BL46" s="2"/>
       <c r="BM46"/>
-    </row>
-    <row r="47" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN46"/>
+    </row>
+    <row r="47" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD47" s="45"/>
       <c r="BE47" s="9"/>
       <c r="BF47" s="2"/>
       <c r="BG47" s="2"/>
-      <c r="BH47" s="45"/>
+      <c r="BH47" s="2"/>
       <c r="BI47" s="45"/>
-      <c r="BK47" s="2"/>
-      <c r="BL47"/>
+      <c r="BJ47" s="45"/>
+      <c r="BL47" s="2"/>
       <c r="BM47"/>
-    </row>
-    <row r="48" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN47"/>
+    </row>
+    <row r="48" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD48" s="45"/>
       <c r="BE48" s="9"/>
       <c r="BF48" s="2"/>
       <c r="BG48" s="2"/>
-      <c r="BH48" s="45"/>
+      <c r="BH48" s="2"/>
       <c r="BI48" s="45"/>
-      <c r="BK48" s="2"/>
-      <c r="BL48"/>
+      <c r="BJ48" s="45"/>
+      <c r="BL48" s="2"/>
       <c r="BM48"/>
-    </row>
-    <row r="49" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN48"/>
+    </row>
+    <row r="49" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD49" s="45"/>
       <c r="BE49" s="9"/>
       <c r="BF49" s="2"/>
       <c r="BG49" s="2"/>
-      <c r="BH49" s="45"/>
+      <c r="BH49" s="2"/>
       <c r="BI49" s="45"/>
-      <c r="BK49" s="2"/>
-      <c r="BL49"/>
+      <c r="BJ49" s="45"/>
+      <c r="BL49" s="2"/>
       <c r="BM49"/>
-    </row>
-    <row r="50" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN49"/>
+    </row>
+    <row r="50" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD50" s="45"/>
       <c r="BE50" s="9"/>
       <c r="BF50" s="2"/>
       <c r="BG50" s="2"/>
-      <c r="BH50" s="45"/>
+      <c r="BH50" s="2"/>
       <c r="BI50" s="45"/>
-      <c r="BK50" s="2"/>
-      <c r="BL50"/>
+      <c r="BJ50" s="45"/>
+      <c r="BL50" s="2"/>
       <c r="BM50"/>
-    </row>
-    <row r="51" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN50"/>
+    </row>
+    <row r="51" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD51" s="45"/>
       <c r="BE51" s="9"/>
       <c r="BF51" s="2"/>
       <c r="BG51" s="2"/>
-      <c r="BH51" s="45"/>
+      <c r="BH51" s="2"/>
       <c r="BI51" s="45"/>
-      <c r="BK51" s="2"/>
-      <c r="BL51"/>
+      <c r="BJ51" s="45"/>
+      <c r="BL51" s="2"/>
       <c r="BM51"/>
-    </row>
-    <row r="52" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN51"/>
+    </row>
+    <row r="52" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD52" s="45"/>
       <c r="BE52" s="9"/>
       <c r="BF52" s="2"/>
       <c r="BG52" s="2"/>
-      <c r="BH52" s="45"/>
+      <c r="BH52" s="2"/>
       <c r="BI52" s="45"/>
-      <c r="BK52" s="2"/>
-      <c r="BL52"/>
+      <c r="BJ52" s="45"/>
+      <c r="BL52" s="2"/>
       <c r="BM52"/>
-    </row>
-    <row r="53" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN52"/>
+    </row>
+    <row r="53" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD53" s="45"/>
       <c r="BE53" s="9"/>
       <c r="BF53" s="2"/>
       <c r="BG53" s="2"/>
-      <c r="BH53" s="45"/>
+      <c r="BH53" s="2"/>
       <c r="BI53" s="45"/>
-      <c r="BK53" s="2"/>
-      <c r="BL53"/>
+      <c r="BJ53" s="45"/>
+      <c r="BL53" s="2"/>
       <c r="BM53"/>
-    </row>
-    <row r="54" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN53"/>
+    </row>
+    <row r="54" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD54" s="45"/>
       <c r="BE54" s="9"/>
       <c r="BF54" s="2"/>
       <c r="BG54" s="2"/>
-      <c r="BH54" s="45"/>
+      <c r="BH54" s="2"/>
       <c r="BI54" s="45"/>
-      <c r="BK54" s="2"/>
-      <c r="BL54"/>
+      <c r="BJ54" s="45"/>
+      <c r="BL54" s="2"/>
       <c r="BM54"/>
-    </row>
-    <row r="55" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN54"/>
+    </row>
+    <row r="55" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD55" s="45"/>
       <c r="BE55" s="9"/>
       <c r="BF55" s="2"/>
       <c r="BG55" s="2"/>
-      <c r="BH55" s="45"/>
+      <c r="BH55" s="2"/>
       <c r="BI55" s="45"/>
-      <c r="BK55" s="2"/>
-      <c r="BL55"/>
+      <c r="BJ55" s="45"/>
+      <c r="BL55" s="2"/>
       <c r="BM55"/>
-    </row>
-    <row r="56" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN55"/>
+    </row>
+    <row r="56" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD56" s="45"/>
       <c r="BE56" s="9"/>
       <c r="BF56" s="2"/>
       <c r="BG56" s="2"/>
-      <c r="BH56" s="45"/>
+      <c r="BH56" s="2"/>
       <c r="BI56" s="45"/>
-      <c r="BK56" s="2"/>
-      <c r="BL56"/>
+      <c r="BJ56" s="45"/>
+      <c r="BL56" s="2"/>
       <c r="BM56"/>
-    </row>
-    <row r="57" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN56"/>
+    </row>
+    <row r="57" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD57" s="45"/>
       <c r="BE57" s="9"/>
       <c r="BF57" s="2"/>
       <c r="BG57" s="2"/>
-      <c r="BH57" s="45"/>
+      <c r="BH57" s="2"/>
       <c r="BI57" s="45"/>
-      <c r="BK57" s="2"/>
-      <c r="BL57"/>
+      <c r="BJ57" s="45"/>
+      <c r="BL57" s="2"/>
       <c r="BM57"/>
-    </row>
-    <row r="58" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN57"/>
+    </row>
+    <row r="58" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD58" s="45"/>
       <c r="BE58" s="9"/>
       <c r="BF58" s="2"/>
       <c r="BG58" s="2"/>
-      <c r="BH58" s="45"/>
+      <c r="BH58" s="2"/>
       <c r="BI58" s="45"/>
-      <c r="BK58" s="2"/>
-      <c r="BL58"/>
+      <c r="BJ58" s="45"/>
+      <c r="BL58" s="2"/>
       <c r="BM58"/>
-    </row>
-    <row r="59" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN58"/>
+    </row>
+    <row r="59" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD59" s="45"/>
       <c r="BE59" s="9"/>
       <c r="BF59" s="2"/>
       <c r="BG59" s="2"/>
-      <c r="BH59" s="45"/>
+      <c r="BH59" s="2"/>
       <c r="BI59" s="45"/>
-      <c r="BK59" s="2"/>
-      <c r="BL59"/>
+      <c r="BJ59" s="45"/>
+      <c r="BL59" s="2"/>
       <c r="BM59"/>
-    </row>
-    <row r="60" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN59"/>
+    </row>
+    <row r="60" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD60" s="45"/>
       <c r="BE60" s="9"/>
       <c r="BF60" s="2"/>
       <c r="BG60" s="2"/>
-      <c r="BH60" s="45"/>
+      <c r="BH60" s="2"/>
       <c r="BI60" s="45"/>
-      <c r="BK60" s="2"/>
-      <c r="BL60"/>
+      <c r="BJ60" s="45"/>
+      <c r="BL60" s="2"/>
       <c r="BM60"/>
-    </row>
-    <row r="61" spans="56:65" x14ac:dyDescent="0.2">
+      <c r="BN60"/>
+    </row>
+    <row r="61" spans="56:66" x14ac:dyDescent="0.2">
       <c r="BD61" s="45"/>
       <c r="BE61" s="9"/>
       <c r="BF61" s="2"/>
       <c r="BG61" s="2"/>
-      <c r="BH61" s="45"/>
+      <c r="BH61" s="2"/>
       <c r="BI61" s="45"/>
-      <c r="BK61" s="2"/>
-      <c r="BL61"/>
+      <c r="BJ61" s="45"/>
+      <c r="BL61" s="2"/>
       <c r="BM61"/>
+      <c r="BN61"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="BI2:BM2"/>
+    <mergeCell ref="BJ2:BN2"/>
     <mergeCell ref="H2:V2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="W2:AD2"/>
     <mergeCell ref="AE2:AO2"/>
     <mergeCell ref="AP2:AU2"/>
     <mergeCell ref="AV2:BD2"/>
-    <mergeCell ref="BE2:BH2"/>
+    <mergeCell ref="BE2:BI2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 AA18:AA29 W4:BM13 A4:G27 AB14:BM30">
+  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 AA18:AA29 W4:BN13 A4:G27 AB14:BN30">
     <cfRule type="expression" dxfId="24" priority="17" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>

</xml_diff>

<commit_message>
+ removed unused (and now invalid) ServoDyn HSSBrTq outputs from some of the 5MW models + added anchor-tension outputs to MoorDyn input files + use matt_current branch of MoorDyn + modified scripts to put executables in the \bin directory + updated documentation + modified PlotFASToutput.m so it doesn't crash if you give it a non-existent channel name to plot.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@952 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2812" uniqueCount="1130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2812" uniqueCount="1131">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3439,6 +3439,9 @@
   </si>
   <si>
     <t>Integrator</t>
+  </si>
+  <si>
+    <t>Flexible, steady wind, high-speed shaft brake shutdown</t>
   </si>
 </sst>
 </file>
@@ -5154,10 +5157,10 @@
   <dimension ref="A1:BO61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="V15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AB30" sqref="AB30"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5661,7 +5664,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="27"/>
       <c r="B5" s="85" t="s">
         <v>33</v>
@@ -5679,7 +5682,7 @@
         <v>175</v>
       </c>
       <c r="G5" s="147" t="s">
-        <v>1106</v>
+        <v>1130</v>
       </c>
       <c r="H5" s="40">
         <v>20</v>

</xml_diff>

<commit_message>
replaced InflowWind v2.0 with InflowWind v3.0; it has an input file listed in the primary FAST file. (didn't update makefile or VS project, yet)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@987 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -36,7 +36,7 @@
     <definedName name="_Toc46290869" localSheetId="2">Variables!$B$770</definedName>
     <definedName name="_Toc46290870" localSheetId="2">Variables!$B$781</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">TestMatrix!$B$2:$AX$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'TestMatrix (new)'!$B$2:$BA$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'TestMatrix (new)'!$B$2:$BC$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Variables!$B$1:$P$855</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2904" uniqueCount="1133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2911" uniqueCount="1141">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3429,9 +3429,6 @@
     <t>1P0.0</t>
   </si>
   <si>
-    <t>Mean Wind Speed</t>
-  </si>
-  <si>
     <t>ElastoDyn</t>
   </si>
   <si>
@@ -3448,6 +3445,33 @@
   </si>
   <si>
     <t>OC4 Load Case (LC) 3.7: steady wind, white noise second-order waves</t>
+  </si>
+  <si>
+    <t>Direction (deg)</t>
+  </si>
+  <si>
+    <t>5-25</t>
+  </si>
+  <si>
+    <t>0-61</t>
+  </si>
+  <si>
+    <t>11-27</t>
+  </si>
+  <si>
+    <t>11-20</t>
+  </si>
+  <si>
+    <t>-50-0</t>
+  </si>
+  <si>
+    <t>InflowWind</t>
+  </si>
+  <si>
+    <t>Wind Type</t>
+  </si>
+  <si>
+    <t>Mean Wind Speed (m/s)</t>
   </si>
 </sst>
 </file>
@@ -4154,7 +4178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4519,9 +4543,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="12" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4572,9 +4593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -4582,6 +4600,21 @@
     <xf numFmtId="164" fontId="2" fillId="12" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4635,10 +4668,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4650,28 +4686,22 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4679,7 +4709,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="37">
     <dxf>
       <font>
         <condense val="0"/>
@@ -4748,216 +4778,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -5469,20 +5289,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BM61"/>
+  <dimension ref="A1:BO61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="O10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="AP4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomRight" activeCell="BA4" sqref="BA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" style="146" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" style="145" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.109375" style="2" bestFit="1" customWidth="1"/>
@@ -5506,107 +5326,111 @@
     <col min="33" max="34" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="4.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="36" max="42" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="43" max="49" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="4.5546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="3.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="4.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="4.88671875" style="2" customWidth="1"/>
-    <col min="55" max="55" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="57" width="4.88671875" style="2" customWidth="1"/>
-    <col min="58" max="60" width="1.88671875" style="2" customWidth="1"/>
-    <col min="61" max="61" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="62" max="63" width="3.33203125" style="45" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="5.6640625" style="45" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="4.44140625" customWidth="1"/>
-    <col min="67" max="67" width="4.33203125" customWidth="1"/>
+    <col min="43" max="47" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="4.33203125" style="2" customWidth="1"/>
+    <col min="50" max="51" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="5.33203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="5.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="3.33203125" style="185" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="4.88671875" style="2" customWidth="1"/>
+    <col min="57" max="57" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="4.88671875" style="2" customWidth="1"/>
+    <col min="60" max="62" width="1.88671875" style="2" customWidth="1"/>
+    <col min="63" max="63" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="64" max="65" width="3.33203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="5.6640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="4.44140625" customWidth="1"/>
+    <col min="69" max="69" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:65" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="163" t="s">
+    <row r="1" spans="1:67" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:67" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="166" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="160" t="s">
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="168"/>
+      <c r="H2" s="163" t="s">
         <v>1104</v>
       </c>
-      <c r="I2" s="161"/>
-      <c r="J2" s="161"/>
-      <c r="K2" s="161"/>
-      <c r="L2" s="161"/>
-      <c r="M2" s="161"/>
-      <c r="N2" s="161"/>
-      <c r="O2" s="161"/>
-      <c r="P2" s="161"/>
-      <c r="Q2" s="161"/>
-      <c r="R2" s="161"/>
-      <c r="S2" s="161"/>
-      <c r="T2" s="161"/>
-      <c r="U2" s="161"/>
-      <c r="V2" s="162"/>
-      <c r="W2" s="158" t="s">
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
+      <c r="K2" s="164"/>
+      <c r="L2" s="164"/>
+      <c r="M2" s="164"/>
+      <c r="N2" s="164"/>
+      <c r="O2" s="164"/>
+      <c r="P2" s="164"/>
+      <c r="Q2" s="164"/>
+      <c r="R2" s="164"/>
+      <c r="S2" s="164"/>
+      <c r="T2" s="164"/>
+      <c r="U2" s="164"/>
+      <c r="V2" s="165"/>
+      <c r="W2" s="161" t="s">
         <v>1110</v>
       </c>
-      <c r="X2" s="166"/>
-      <c r="Y2" s="166"/>
-      <c r="Z2" s="166"/>
-      <c r="AA2" s="166"/>
-      <c r="AB2" s="166"/>
-      <c r="AC2" s="166"/>
-      <c r="AD2" s="167"/>
-      <c r="AE2" s="168" t="s">
-        <v>1127</v>
-      </c>
-      <c r="AF2" s="169"/>
-      <c r="AG2" s="169"/>
-      <c r="AH2" s="169"/>
-      <c r="AI2" s="169"/>
-      <c r="AJ2" s="169"/>
-      <c r="AK2" s="169"/>
-      <c r="AL2" s="169"/>
-      <c r="AM2" s="169"/>
-      <c r="AN2" s="169"/>
-      <c r="AO2" s="169"/>
-      <c r="AP2" s="170"/>
-      <c r="AQ2" s="171" t="s">
-        <v>1131</v>
-      </c>
-      <c r="AR2" s="172"/>
-      <c r="AS2" s="172"/>
-      <c r="AT2" s="172"/>
-      <c r="AU2" s="172"/>
-      <c r="AV2" s="173"/>
-      <c r="AW2" s="176" t="s">
-        <v>18</v>
-      </c>
-      <c r="AX2" s="177"/>
-      <c r="AY2" s="177"/>
-      <c r="AZ2" s="177"/>
-      <c r="BA2" s="178"/>
-      <c r="BB2" s="181" t="s">
+      <c r="X2" s="169"/>
+      <c r="Y2" s="169"/>
+      <c r="Z2" s="169"/>
+      <c r="AA2" s="169"/>
+      <c r="AB2" s="169"/>
+      <c r="AC2" s="169"/>
+      <c r="AD2" s="170"/>
+      <c r="AE2" s="171" t="s">
+        <v>1126</v>
+      </c>
+      <c r="AF2" s="172"/>
+      <c r="AG2" s="172"/>
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="172"/>
+      <c r="AK2" s="172"/>
+      <c r="AL2" s="172"/>
+      <c r="AM2" s="172"/>
+      <c r="AN2" s="172"/>
+      <c r="AO2" s="172"/>
+      <c r="AP2" s="173"/>
+      <c r="AQ2" s="174" t="s">
         <v>1130</v>
       </c>
+      <c r="AR2" s="175"/>
+      <c r="AS2" s="175"/>
+      <c r="AT2" s="175"/>
+      <c r="AU2" s="175"/>
+      <c r="AV2" s="175"/>
+      <c r="AW2" s="175"/>
+      <c r="AX2" s="176"/>
+      <c r="AY2" s="180" t="s">
+        <v>1138</v>
+      </c>
+      <c r="AZ2" s="181"/>
+      <c r="BA2" s="181"/>
+      <c r="BB2" s="181"/>
       <c r="BC2" s="182"/>
-      <c r="BD2" s="182"/>
-      <c r="BE2" s="182"/>
-      <c r="BF2" s="182"/>
-      <c r="BG2" s="182"/>
-      <c r="BH2" s="183"/>
-      <c r="BI2" s="157" t="s">
+      <c r="BD2" s="177" t="s">
+        <v>1129</v>
+      </c>
+      <c r="BE2" s="178"/>
+      <c r="BF2" s="178"/>
+      <c r="BG2" s="178"/>
+      <c r="BH2" s="178"/>
+      <c r="BI2" s="178"/>
+      <c r="BJ2" s="179"/>
+      <c r="BK2" s="160" t="s">
         <v>1047</v>
       </c>
-      <c r="BJ2" s="158"/>
-      <c r="BK2" s="158"/>
-      <c r="BL2" s="158"/>
-      <c r="BM2" s="159"/>
-    </row>
-    <row r="3" spans="1:65" s="1" customFormat="1" ht="88.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL2" s="161"/>
+      <c r="BM2" s="161"/>
+      <c r="BN2" s="161"/>
+      <c r="BO2" s="162"/>
+    </row>
+    <row r="3" spans="1:67" s="1" customFormat="1" ht="88.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
       <c r="B3" s="79" t="s">
         <v>287</v>
@@ -5623,10 +5447,10 @@
       <c r="F3" s="80" t="s">
         <v>488</v>
       </c>
-      <c r="G3" s="139" t="s">
+      <c r="G3" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="137" t="s">
+      <c r="H3" s="136" t="s">
         <v>1090</v>
       </c>
       <c r="I3" s="121" t="s">
@@ -5696,9 +5520,9 @@
         <v>1056</v>
       </c>
       <c r="AE3" s="82" t="s">
-        <v>1128</v>
-      </c>
-      <c r="AF3" s="156" t="s">
+        <v>1127</v>
+      </c>
+      <c r="AF3" s="154" t="s">
         <v>5</v>
       </c>
       <c r="AG3" s="83" t="s">
@@ -5728,10 +5552,10 @@
       <c r="AO3" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="AP3" s="142" t="s">
+      <c r="AP3" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="AQ3" s="141" t="s">
+      <c r="AQ3" s="140" t="s">
         <v>44</v>
       </c>
       <c r="AR3" s="72" t="s">
@@ -5746,61 +5570,67 @@
       <c r="AU3" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="AV3" s="74" t="s">
+      <c r="AV3" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="AW3" s="75" t="s">
+      <c r="AW3" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="AX3" s="77" t="s">
+      <c r="AX3" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="AY3" s="78" t="s">
+      <c r="AY3" s="75" t="s">
+        <v>1139</v>
+      </c>
+      <c r="AZ3" s="189" t="s">
+        <v>1132</v>
+      </c>
+      <c r="BA3" s="190" t="s">
+        <v>1140</v>
+      </c>
+      <c r="BB3" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="AZ3" s="151" t="s">
-        <v>1126</v>
-      </c>
-      <c r="BA3" s="76" t="s">
+      <c r="BC3" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="BB3" s="184" t="s">
+      <c r="BD3" s="157" t="s">
         <v>1121</v>
       </c>
-      <c r="BC3" s="185" t="s">
+      <c r="BE3" s="158" t="s">
         <v>1122</v>
       </c>
-      <c r="BD3" s="185" t="s">
+      <c r="BF3" s="158" t="s">
         <v>1123</v>
       </c>
-      <c r="BE3" s="185" t="s">
+      <c r="BG3" s="158" t="s">
         <v>1124</v>
       </c>
-      <c r="BF3" s="185"/>
-      <c r="BG3" s="185"/>
-      <c r="BH3" s="186"/>
-      <c r="BI3" s="66" t="s">
+      <c r="BH3" s="158"/>
+      <c r="BI3" s="158"/>
+      <c r="BJ3" s="159"/>
+      <c r="BK3" s="66" t="s">
         <v>1045</v>
       </c>
-      <c r="BJ3" s="69" t="s">
+      <c r="BL3" s="69" t="s">
         <v>1046</v>
       </c>
-      <c r="BK3" s="70" t="s">
+      <c r="BM3" s="70" t="s">
         <v>1051</v>
       </c>
-      <c r="BL3" s="70" t="s">
+      <c r="BN3" s="70" t="s">
         <v>1054</v>
       </c>
-      <c r="BM3" s="68" t="s">
+      <c r="BO3" s="68" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="147" t="s">
+      <c r="C4" s="146" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="29">
@@ -5812,10 +5642,10 @@
       <c r="F4" s="55">
         <v>175</v>
       </c>
-      <c r="G4" s="143" t="s">
+      <c r="G4" s="142" t="s">
         <v>497</v>
       </c>
-      <c r="H4" s="138">
+      <c r="H4" s="137">
         <v>20</v>
       </c>
       <c r="I4" s="117">
@@ -5933,60 +5763,68 @@
       <c r="AU4" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="AV4" s="33" t="s">
+      <c r="AV4" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="AW4" s="36" t="s">
+      <c r="AW4" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="AX4" s="46">
+      <c r="AX4" s="33">
         <v>15</v>
       </c>
-      <c r="AY4" s="37">
+      <c r="AY4" s="36">
+        <v>2</v>
+      </c>
+      <c r="AZ4" s="150">
+        <v>30</v>
+      </c>
+      <c r="BA4" s="150">
+        <v>12</v>
+      </c>
+      <c r="BB4" s="37">
         <v>0.2</v>
       </c>
-      <c r="AZ4" s="152"/>
-      <c r="BA4" s="38" t="s">
+      <c r="BC4" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="BB4" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC4" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD4" s="41" t="s">
+      <c r="BD4" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE4" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF4" s="35"/>
-      <c r="BG4" s="35"/>
-      <c r="BH4" s="33"/>
-      <c r="BI4" s="59">
-        <v>0</v>
-      </c>
-      <c r="BJ4" s="55">
+      <c r="BF4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH4" s="35"/>
+      <c r="BI4" s="35"/>
+      <c r="BJ4" s="33"/>
+      <c r="BK4" s="59">
+        <v>0</v>
+      </c>
+      <c r="BL4" s="55">
         <v>3</v>
       </c>
-      <c r="BK4" s="62">
+      <c r="BM4" s="62">
         <f>Variables!D2</f>
         <v>23</v>
       </c>
-      <c r="BL4" s="62" t="s">
+      <c r="BN4" s="62" t="s">
         <v>1048</v>
       </c>
-      <c r="BM4" s="38" t="s">
+      <c r="BO4" s="38" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:65" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="27"/>
       <c r="B5" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="147" t="s">
+      <c r="C5" s="146" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="29">
@@ -5998,8 +5836,8 @@
       <c r="F5" s="55">
         <v>175</v>
       </c>
-      <c r="G5" s="144" t="s">
-        <v>1129</v>
+      <c r="G5" s="143" t="s">
+        <v>1128</v>
       </c>
       <c r="H5" s="40">
         <v>20</v>
@@ -6119,60 +5957,68 @@
       <c r="AU5" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AV5" s="42" t="s">
+      <c r="AV5" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW5" s="43" t="s">
+      <c r="AW5" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX5" s="47">
-        <v>0</v>
-      </c>
-      <c r="AY5" s="44">
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="153"/>
-      <c r="BA5" s="42" t="s">
+      <c r="AX5" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="43">
+        <v>1</v>
+      </c>
+      <c r="AZ5" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="151">
+        <v>12</v>
+      </c>
+      <c r="BB5" s="44">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BB5" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC5" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD5" s="41" t="s">
+      <c r="BD5" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE5" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF5" s="41"/>
-      <c r="BG5" s="41"/>
-      <c r="BH5" s="42"/>
-      <c r="BI5" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ5" s="56">
+      <c r="BF5" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG5" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH5" s="41"/>
+      <c r="BI5" s="41"/>
+      <c r="BJ5" s="42"/>
+      <c r="BK5" s="60">
+        <v>0</v>
+      </c>
+      <c r="BL5" s="56">
         <v>1</v>
       </c>
-      <c r="BK5" s="63">
+      <c r="BM5" s="63">
         <f>Variables!E2</f>
         <v>22</v>
       </c>
-      <c r="BL5" s="63" t="s">
+      <c r="BN5" s="63" t="s">
         <v>1049</v>
       </c>
-      <c r="BM5" s="42" t="s">
+      <c r="BO5" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
       <c r="B6" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="147" t="s">
+      <c r="C6" s="146" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="29">
@@ -6184,7 +6030,7 @@
       <c r="F6" s="55">
         <v>175</v>
       </c>
-      <c r="G6" s="144" t="s">
+      <c r="G6" s="143" t="s">
         <v>491</v>
       </c>
       <c r="H6" s="40">
@@ -6305,60 +6151,68 @@
       <c r="AU6" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AV6" s="42" t="s">
+      <c r="AV6" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW6" s="43" t="s">
+      <c r="AW6" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX6" s="47" t="s">
+      <c r="AX6" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY6" s="44">
+      <c r="AY6" s="43">
+        <v>2</v>
+      </c>
+      <c r="AZ6" s="151">
+        <v>30</v>
+      </c>
+      <c r="BA6" s="151">
+        <v>12</v>
+      </c>
+      <c r="BB6" s="44">
         <v>0.2</v>
       </c>
-      <c r="AZ6" s="153"/>
-      <c r="BA6" s="42" t="s">
+      <c r="BC6" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BB6" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC6" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD6" s="41" t="s">
+      <c r="BD6" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE6" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF6" s="41"/>
-      <c r="BG6" s="41"/>
-      <c r="BH6" s="42"/>
-      <c r="BI6" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ6" s="56">
+      <c r="BF6" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG6" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH6" s="41"/>
+      <c r="BI6" s="41"/>
+      <c r="BJ6" s="42"/>
+      <c r="BK6" s="60">
+        <v>0</v>
+      </c>
+      <c r="BL6" s="56">
         <v>3</v>
       </c>
-      <c r="BK6" s="63">
+      <c r="BM6" s="63">
         <f>Variables!F$2</f>
         <v>23</v>
       </c>
-      <c r="BL6" s="63" t="s">
+      <c r="BN6" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM6" s="42" t="s">
+      <c r="BO6" s="42" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="7" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
       <c r="B7" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="147" t="s">
+      <c r="C7" s="146" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="29">
@@ -6370,7 +6224,7 @@
       <c r="F7" s="55">
         <v>175</v>
       </c>
-      <c r="G7" s="144" t="s">
+      <c r="G7" s="143" t="s">
         <v>492</v>
       </c>
       <c r="H7" s="40">
@@ -6491,60 +6345,68 @@
       <c r="AU7" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AV7" s="42" t="s">
+      <c r="AV7" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW7" s="43" t="s">
+      <c r="AW7" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX7" s="47" t="s">
+      <c r="AX7" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY7" s="44">
+      <c r="AY7" s="43">
+        <v>4</v>
+      </c>
+      <c r="AZ7" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="151">
+        <v>12</v>
+      </c>
+      <c r="BB7" s="44">
         <v>0.2</v>
       </c>
-      <c r="AZ7" s="153"/>
-      <c r="BA7" s="42" t="s">
+      <c r="BC7" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BB7" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC7" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD7" s="41" t="s">
+      <c r="BD7" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE7" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF7" s="41"/>
-      <c r="BG7" s="41"/>
-      <c r="BH7" s="42"/>
-      <c r="BI7" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ7" s="56">
+      <c r="BF7" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG7" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH7" s="41"/>
+      <c r="BI7" s="41"/>
+      <c r="BJ7" s="42"/>
+      <c r="BK7" s="60">
+        <v>0</v>
+      </c>
+      <c r="BL7" s="56">
         <v>5</v>
       </c>
-      <c r="BK7" s="63">
+      <c r="BM7" s="63">
         <f>Variables!F$2</f>
         <v>23</v>
       </c>
-      <c r="BL7" s="63" t="s">
+      <c r="BN7" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM7" s="42" t="s">
+      <c r="BO7" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="147" t="s">
+      <c r="C8" s="146" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="29">
@@ -6556,7 +6418,7 @@
       <c r="F8" s="55">
         <v>175</v>
       </c>
-      <c r="G8" s="144" t="s">
+      <c r="G8" s="143" t="s">
         <v>1106</v>
       </c>
       <c r="H8" s="40">
@@ -6677,60 +6539,68 @@
       <c r="AU8" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AV8" s="42" t="s">
+      <c r="AV8" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW8" s="43" t="s">
+      <c r="AW8" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX8" s="47">
-        <v>0</v>
-      </c>
-      <c r="AY8" s="44">
-        <v>0</v>
-      </c>
-      <c r="AZ8" s="153"/>
-      <c r="BA8" s="42" t="s">
+      <c r="AX8" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="43">
+        <v>2</v>
+      </c>
+      <c r="AZ8" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="151">
+        <v>12</v>
+      </c>
+      <c r="BB8" s="44">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BB8" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC8" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD8" s="41" t="s">
+      <c r="BD8" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE8" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF8" s="41"/>
-      <c r="BG8" s="41"/>
-      <c r="BH8" s="42"/>
-      <c r="BI8" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ8" s="56">
+      <c r="BF8" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG8" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH8" s="41"/>
+      <c r="BI8" s="41"/>
+      <c r="BJ8" s="42"/>
+      <c r="BK8" s="60">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="56">
         <v>3</v>
       </c>
-      <c r="BK8" s="63">
+      <c r="BM8" s="63">
         <f>Variables!G$2</f>
         <v>24</v>
       </c>
-      <c r="BL8" s="63" t="s">
+      <c r="BN8" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM8" s="42" t="s">
+      <c r="BO8" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="148" t="s">
+      <c r="C9" s="147" t="s">
         <v>279</v>
       </c>
       <c r="D9" s="25">
@@ -6743,7 +6613,7 @@
       <c r="F9" s="25">
         <v>50</v>
       </c>
-      <c r="G9" s="144" t="s">
+      <c r="G9" s="143" t="s">
         <v>1106</v>
       </c>
       <c r="H9" s="40">
@@ -6864,60 +6734,68 @@
       <c r="AU9" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AV9" s="42" t="s">
+      <c r="AV9" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW9" s="43" t="s">
+      <c r="AW9" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX9" s="47">
-        <v>0</v>
-      </c>
-      <c r="AY9" s="44">
-        <v>0</v>
-      </c>
-      <c r="AZ9" s="153"/>
-      <c r="BA9" s="42" t="s">
+      <c r="AX9" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="43">
+        <v>2</v>
+      </c>
+      <c r="AZ9" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="151">
+        <v>12</v>
+      </c>
+      <c r="BB9" s="44">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BB9" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC9" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD9" s="41" t="s">
+      <c r="BD9" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE9" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF9" s="41"/>
-      <c r="BG9" s="41"/>
-      <c r="BH9" s="42"/>
-      <c r="BI9" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ9" s="56">
+      <c r="BF9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH9" s="41"/>
+      <c r="BI9" s="41"/>
+      <c r="BJ9" s="42"/>
+      <c r="BK9" s="60">
+        <v>0</v>
+      </c>
+      <c r="BL9" s="56">
         <v>5</v>
       </c>
-      <c r="BK9" s="63">
+      <c r="BM9" s="63">
         <f>Variables!H$2</f>
         <v>22</v>
       </c>
-      <c r="BL9" s="63" t="s">
+      <c r="BN9" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM9" s="42" t="s">
+      <c r="BO9" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="148" t="s">
+      <c r="C10" s="147" t="s">
         <v>279</v>
       </c>
       <c r="D10" s="25">
@@ -6930,7 +6808,7 @@
       <c r="F10" s="25">
         <v>50</v>
       </c>
-      <c r="G10" s="144" t="s">
+      <c r="G10" s="143" t="s">
         <v>492</v>
       </c>
       <c r="H10" s="40">
@@ -7051,60 +6929,68 @@
       <c r="AU10" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AV10" s="42" t="s">
+      <c r="AV10" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW10" s="43" t="s">
+      <c r="AW10" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX10" s="47">
-        <v>0</v>
-      </c>
-      <c r="AY10" s="44">
+      <c r="AX10" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="43">
+        <v>4</v>
+      </c>
+      <c r="AZ10" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="151">
+        <v>12</v>
+      </c>
+      <c r="BB10" s="44">
         <v>0.2</v>
       </c>
-      <c r="AZ10" s="153"/>
-      <c r="BA10" s="42" t="s">
+      <c r="BC10" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BB10" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC10" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD10" s="41" t="s">
+      <c r="BD10" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE10" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF10" s="41"/>
-      <c r="BG10" s="41"/>
-      <c r="BH10" s="42"/>
-      <c r="BI10" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ10" s="56">
+      <c r="BF10" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG10" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH10" s="41"/>
+      <c r="BI10" s="41"/>
+      <c r="BJ10" s="42"/>
+      <c r="BK10" s="60">
+        <v>0</v>
+      </c>
+      <c r="BL10" s="56">
         <v>3</v>
       </c>
-      <c r="BK10" s="63">
+      <c r="BM10" s="63">
         <f>Variables!I$2</f>
         <v>24</v>
       </c>
-      <c r="BL10" s="63" t="s">
+      <c r="BN10" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM10" s="42" t="s">
+      <c r="BO10" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
       <c r="B11" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="148" t="s">
+      <c r="C11" s="147" t="s">
         <v>279</v>
       </c>
       <c r="D11" s="25">
@@ -7117,7 +7003,7 @@
       <c r="F11" s="25">
         <v>50</v>
       </c>
-      <c r="G11" s="143" t="s">
+      <c r="G11" s="142" t="s">
         <v>497</v>
       </c>
       <c r="H11" s="40">
@@ -7238,60 +7124,68 @@
       <c r="AU11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AV11" s="42" t="s">
+      <c r="AV11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW11" s="43" t="s">
+      <c r="AW11" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX11" s="47">
+      <c r="AX11" s="42">
         <v>15</v>
       </c>
-      <c r="AY11" s="44">
+      <c r="AY11" s="43">
+        <v>1</v>
+      </c>
+      <c r="AZ11" s="151">
+        <v>30</v>
+      </c>
+      <c r="BA11" s="151">
+        <v>11</v>
+      </c>
+      <c r="BB11" s="44">
         <v>0.2</v>
       </c>
-      <c r="AZ11" s="153"/>
-      <c r="BA11" s="42" t="s">
+      <c r="BC11" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BB11" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC11" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD11" s="41" t="s">
+      <c r="BD11" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE11" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF11" s="41"/>
-      <c r="BG11" s="41"/>
-      <c r="BH11" s="42"/>
-      <c r="BI11" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ11" s="56">
+      <c r="BF11" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG11" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH11" s="41"/>
+      <c r="BI11" s="41"/>
+      <c r="BJ11" s="42"/>
+      <c r="BK11" s="60">
+        <v>0</v>
+      </c>
+      <c r="BL11" s="56">
         <v>2</v>
       </c>
-      <c r="BK11" s="63">
+      <c r="BM11" s="63">
         <f>Variables!J$2</f>
         <v>27</v>
       </c>
-      <c r="BL11" s="63" t="s">
+      <c r="BN11" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM11" s="42" t="s">
+      <c r="BO11" s="42" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="12" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
       <c r="B12" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="148" t="s">
+      <c r="C12" s="147" t="s">
         <v>489</v>
       </c>
       <c r="D12" s="25">
@@ -7303,7 +7197,7 @@
       <c r="F12" s="25">
         <v>20</v>
       </c>
-      <c r="G12" s="144" t="s">
+      <c r="G12" s="143" t="s">
         <v>493</v>
       </c>
       <c r="H12" s="40">
@@ -7424,60 +7318,68 @@
       <c r="AU12" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AV12" s="42" t="s">
+      <c r="AV12" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AW12" s="43" t="s">
+      <c r="AW12" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX12" s="47" t="s">
+      <c r="AX12" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY12" s="44">
+      <c r="AY12" s="43">
+        <v>2</v>
+      </c>
+      <c r="AZ12" s="151">
+        <v>30</v>
+      </c>
+      <c r="BA12" s="151">
+        <v>11</v>
+      </c>
+      <c r="BB12" s="44">
         <v>0.2</v>
       </c>
-      <c r="AZ12" s="153"/>
-      <c r="BA12" s="42" t="s">
+      <c r="BC12" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BB12" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC12" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD12" s="41" t="s">
+      <c r="BD12" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE12" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF12" s="41"/>
-      <c r="BG12" s="41"/>
-      <c r="BH12" s="42"/>
-      <c r="BI12" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ12" s="56">
+      <c r="BF12" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG12" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH12" s="41"/>
+      <c r="BI12" s="41"/>
+      <c r="BJ12" s="42"/>
+      <c r="BK12" s="60">
+        <v>0</v>
+      </c>
+      <c r="BL12" s="56">
         <v>5</v>
       </c>
-      <c r="BK12" s="63">
+      <c r="BM12" s="63">
         <f>Variables!K$2</f>
         <v>26</v>
       </c>
-      <c r="BL12" s="63" t="s">
+      <c r="BN12" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM12" s="42" t="s">
+      <c r="BO12" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27"/>
       <c r="B13" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="148" t="s">
+      <c r="C13" s="147" t="s">
         <v>490</v>
       </c>
       <c r="D13" s="25">
@@ -7489,7 +7391,7 @@
       <c r="F13" s="25">
         <v>20</v>
       </c>
-      <c r="G13" s="144" t="s">
+      <c r="G13" s="143" t="s">
         <v>496</v>
       </c>
       <c r="H13" s="40">
@@ -7610,60 +7512,68 @@
       <c r="AU13" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AV13" s="42" t="s">
+      <c r="AV13" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AW13" s="43" t="s">
+      <c r="AW13" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX13" s="47">
-        <v>0</v>
-      </c>
-      <c r="AY13" s="44">
-        <v>0</v>
-      </c>
-      <c r="AZ13" s="153"/>
-      <c r="BA13" s="42" t="s">
+      <c r="AX13" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY13" s="43">
+        <v>2</v>
+      </c>
+      <c r="AZ13" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA13" s="188" t="s">
+        <v>1133</v>
+      </c>
+      <c r="BB13" s="44">
+        <v>0</v>
+      </c>
+      <c r="BC13" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BB13" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC13" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD13" s="41" t="s">
+      <c r="BD13" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE13" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF13" s="41"/>
-      <c r="BG13" s="41"/>
-      <c r="BH13" s="42"/>
-      <c r="BI13" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ13" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK13" s="63">
+      <c r="BF13" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG13" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH13" s="41"/>
+      <c r="BI13" s="41"/>
+      <c r="BJ13" s="42"/>
+      <c r="BK13" s="60">
+        <v>0</v>
+      </c>
+      <c r="BL13" s="56">
+        <v>0</v>
+      </c>
+      <c r="BM13" s="63">
         <f>Variables!L$2</f>
         <v>24</v>
       </c>
-      <c r="BL13" s="63" t="s">
+      <c r="BN13" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM13" s="42" t="s">
+      <c r="BO13" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:65" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="148" t="s">
+      <c r="C14" s="147" t="s">
         <v>286</v>
       </c>
       <c r="D14" s="25">
@@ -7675,7 +7585,7 @@
       <c r="F14" s="25">
         <v>1500</v>
       </c>
-      <c r="G14" s="144" t="s">
+      <c r="G14" s="143" t="s">
         <v>500</v>
       </c>
       <c r="H14" s="40">
@@ -7796,60 +7706,68 @@
       <c r="AU14" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AV14" s="42" t="s">
+      <c r="AV14" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW14" s="43" t="s">
+      <c r="AW14" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX14" s="47">
-        <v>0</v>
-      </c>
-      <c r="AY14" s="44">
+      <c r="AX14" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY14" s="43">
+        <v>4</v>
+      </c>
+      <c r="AZ14" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA14" s="151">
+        <v>12</v>
+      </c>
+      <c r="BB14" s="44">
         <v>0.2</v>
       </c>
-      <c r="AZ14" s="153"/>
-      <c r="BA14" s="42" t="s">
+      <c r="BC14" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BB14" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC14" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD14" s="41" t="s">
+      <c r="BD14" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE14" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF14" s="41"/>
-      <c r="BG14" s="41"/>
-      <c r="BH14" s="42"/>
-      <c r="BI14" s="60">
+      <c r="BF14" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG14" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH14" s="41"/>
+      <c r="BI14" s="41"/>
+      <c r="BJ14" s="42"/>
+      <c r="BK14" s="60">
         <v>2</v>
       </c>
-      <c r="BJ14" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK14" s="63">
+      <c r="BL14" s="56">
+        <v>0</v>
+      </c>
+      <c r="BM14" s="63">
         <f>Variables!M$2</f>
         <v>21</v>
       </c>
-      <c r="BL14" s="63" t="s">
+      <c r="BN14" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM14" s="42" t="s">
+      <c r="BO14" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27"/>
       <c r="B15" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="148" t="s">
+      <c r="C15" s="147" t="s">
         <v>286</v>
       </c>
       <c r="D15" s="25">
@@ -7861,7 +7779,7 @@
       <c r="F15" s="25">
         <v>1500</v>
       </c>
-      <c r="G15" s="144" t="s">
+      <c r="G15" s="143" t="s">
         <v>494</v>
       </c>
       <c r="H15" s="40">
@@ -7982,60 +7900,68 @@
       <c r="AU15" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AV15" s="42" t="s">
+      <c r="AV15" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW15" s="43" t="s">
+      <c r="AW15" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX15" s="47" t="s">
+      <c r="AX15" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY15" s="44">
+      <c r="AY15" s="43">
+        <v>2</v>
+      </c>
+      <c r="AZ15" s="188" t="s">
+        <v>1134</v>
+      </c>
+      <c r="BA15" s="188" t="s">
+        <v>1135</v>
+      </c>
+      <c r="BB15" s="44">
         <v>0.2</v>
       </c>
-      <c r="AZ15" s="153"/>
-      <c r="BA15" s="42" t="s">
+      <c r="BC15" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BB15" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC15" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD15" s="41" t="s">
+      <c r="BD15" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE15" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF15" s="41"/>
-      <c r="BG15" s="41"/>
-      <c r="BH15" s="42"/>
-      <c r="BI15" s="60">
+      <c r="BF15" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG15" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH15" s="41"/>
+      <c r="BI15" s="41"/>
+      <c r="BJ15" s="42"/>
+      <c r="BK15" s="60">
         <v>2</v>
       </c>
-      <c r="BJ15" s="56">
+      <c r="BL15" s="56">
         <v>4</v>
       </c>
-      <c r="BK15" s="63">
+      <c r="BM15" s="63">
         <f>Variables!N$2</f>
         <v>21</v>
       </c>
-      <c r="BL15" s="63" t="s">
+      <c r="BN15" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM15" s="42" t="s">
+      <c r="BO15" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27"/>
       <c r="B16" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="148" t="s">
+      <c r="C16" s="147" t="s">
         <v>286</v>
       </c>
       <c r="D16" s="25">
@@ -8047,7 +7973,7 @@
       <c r="F16" s="25">
         <v>1500</v>
       </c>
-      <c r="G16" s="144" t="s">
+      <c r="G16" s="143" t="s">
         <v>495</v>
       </c>
       <c r="H16" s="40">
@@ -8168,62 +8094,70 @@
       <c r="AU16" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AV16" s="42" t="s">
+      <c r="AV16" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW16" s="43" t="s">
+      <c r="AW16" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX16" s="47">
-        <v>0</v>
-      </c>
-      <c r="AY16" s="44">
+      <c r="AX16" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY16" s="43">
+        <v>4</v>
+      </c>
+      <c r="AZ16" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA16" s="151">
+        <v>12</v>
+      </c>
+      <c r="BB16" s="44">
         <v>0.2</v>
       </c>
-      <c r="AZ16" s="153"/>
-      <c r="BA16" s="42" t="s">
+      <c r="BC16" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BB16" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC16" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD16" s="41" t="s">
+      <c r="BD16" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE16" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF16" s="41"/>
-      <c r="BG16" s="41"/>
-      <c r="BH16" s="42"/>
-      <c r="BI16" s="60">
+      <c r="BF16" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG16" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH16" s="41"/>
+      <c r="BI16" s="41"/>
+      <c r="BJ16" s="42"/>
+      <c r="BK16" s="60">
         <v>2</v>
       </c>
-      <c r="BJ16" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK16" s="63">
+      <c r="BL16" s="56">
+        <v>0</v>
+      </c>
+      <c r="BM16" s="63">
         <f>Variables!O$2</f>
         <v>23</v>
       </c>
-      <c r="BL16" s="63" t="s">
+      <c r="BN16" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM16" s="42" t="s">
+      <c r="BO16" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="17" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="125"/>
-      <c r="C17" s="149"/>
+      <c r="C17" s="148"/>
       <c r="D17" s="127"/>
       <c r="E17" s="127"/>
       <c r="F17" s="127"/>
-      <c r="G17" s="145"/>
+      <c r="G17" s="144"/>
       <c r="H17" s="125"/>
       <c r="I17" s="126"/>
       <c r="J17" s="127"/>
@@ -8264,31 +8198,33 @@
       <c r="AS17" s="129"/>
       <c r="AT17" s="129"/>
       <c r="AU17" s="129"/>
-      <c r="AV17" s="130"/>
-      <c r="AW17" s="128"/>
-      <c r="AX17" s="132"/>
-      <c r="AY17" s="133"/>
-      <c r="AZ17" s="154"/>
-      <c r="BA17" s="130"/>
-      <c r="BB17" s="131"/>
-      <c r="BC17" s="129"/>
-      <c r="BD17" s="129"/>
+      <c r="AV17" s="129"/>
+      <c r="AW17" s="129"/>
+      <c r="AX17" s="130"/>
+      <c r="AY17" s="128"/>
+      <c r="AZ17" s="152"/>
+      <c r="BA17" s="152"/>
+      <c r="BB17" s="132"/>
+      <c r="BC17" s="130"/>
+      <c r="BD17" s="131"/>
       <c r="BE17" s="129"/>
       <c r="BF17" s="129"/>
       <c r="BG17" s="129"/>
-      <c r="BH17" s="130"/>
-      <c r="BI17" s="134"/>
-      <c r="BJ17" s="135"/>
-      <c r="BK17" s="136"/>
-      <c r="BL17" s="136"/>
-      <c r="BM17" s="130"/>
-    </row>
-    <row r="18" spans="1:65" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="BH17" s="129"/>
+      <c r="BI17" s="129"/>
+      <c r="BJ17" s="130"/>
+      <c r="BK17" s="133"/>
+      <c r="BL17" s="134"/>
+      <c r="BM17" s="135"/>
+      <c r="BN17" s="135"/>
+      <c r="BO17" s="130"/>
+    </row>
+    <row r="18" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="27"/>
       <c r="B18" s="85" t="s">
         <v>289</v>
       </c>
-      <c r="C18" s="148" t="s">
+      <c r="C18" s="147" t="s">
         <v>310</v>
       </c>
       <c r="D18" s="25">
@@ -8300,7 +8236,7 @@
       <c r="F18" s="25">
         <v>10</v>
       </c>
-      <c r="G18" s="144" t="s">
+      <c r="G18" s="143" t="s">
         <v>1107</v>
       </c>
       <c r="H18" s="40">
@@ -8421,60 +8357,68 @@
       <c r="AU18" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AV18" s="42" t="s">
+      <c r="AV18" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW18" s="43" t="s">
+      <c r="AW18" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX18" s="53" t="s">
+      <c r="AX18" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY18" s="44">
+      <c r="AY18" s="43">
+        <v>2</v>
+      </c>
+      <c r="AZ18" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA18" s="188" t="s">
+        <v>1136</v>
+      </c>
+      <c r="BB18" s="44">
         <v>0.2</v>
       </c>
-      <c r="AZ18" s="153"/>
-      <c r="BA18" s="42" t="s">
+      <c r="BC18" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BB18" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC18" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD18" s="41" t="s">
+      <c r="BD18" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE18" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF18" s="41"/>
-      <c r="BG18" s="41"/>
-      <c r="BH18" s="42"/>
-      <c r="BI18" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ18" s="61">
-        <v>0</v>
-      </c>
-      <c r="BK18" s="63">
+      <c r="BF18" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG18" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH18" s="41"/>
+      <c r="BI18" s="41"/>
+      <c r="BJ18" s="42"/>
+      <c r="BK18" s="60">
+        <v>0</v>
+      </c>
+      <c r="BL18" s="61">
+        <v>0</v>
+      </c>
+      <c r="BM18" s="63">
         <f>Variables!Q$2</f>
         <v>0</v>
       </c>
-      <c r="BL18" s="63" t="s">
+      <c r="BN18" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM18" s="42" t="s">
+      <c r="BO18" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:65" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="27"/>
       <c r="B19" s="85" t="s">
         <v>309</v>
       </c>
-      <c r="C19" s="148" t="s">
+      <c r="C19" s="147" t="s">
         <v>310</v>
       </c>
       <c r="D19" s="25">
@@ -8486,7 +8430,7 @@
       <c r="F19" s="25">
         <v>10</v>
       </c>
-      <c r="G19" s="144" t="s">
+      <c r="G19" s="143" t="s">
         <v>1108</v>
       </c>
       <c r="H19" s="40">
@@ -8607,60 +8551,68 @@
       <c r="AU19" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AV19" s="42" t="s">
+      <c r="AV19" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW19" s="43" t="s">
+      <c r="AW19" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX19" s="47" t="s">
+      <c r="AX19" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY19" s="44">
+      <c r="AY19" s="43">
+        <v>2</v>
+      </c>
+      <c r="AZ19" s="188" t="s">
+        <v>1137</v>
+      </c>
+      <c r="BA19" s="151">
+        <v>11.9</v>
+      </c>
+      <c r="BB19" s="44">
         <v>0.2</v>
       </c>
-      <c r="AZ19" s="153"/>
-      <c r="BA19" s="42" t="s">
+      <c r="BC19" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BB19" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC19" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD19" s="41" t="s">
+      <c r="BD19" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE19" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF19" s="41"/>
-      <c r="BG19" s="41"/>
-      <c r="BH19" s="42"/>
-      <c r="BI19" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ19" s="56">
-        <v>0</v>
-      </c>
-      <c r="BK19" s="63">
+      <c r="BF19" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG19" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH19" s="41"/>
+      <c r="BI19" s="41"/>
+      <c r="BJ19" s="42"/>
+      <c r="BK19" s="60">
+        <v>0</v>
+      </c>
+      <c r="BL19" s="56">
+        <v>0</v>
+      </c>
+      <c r="BM19" s="63">
         <f>Variables!R$2</f>
         <v>25</v>
       </c>
-      <c r="BL19" s="63" t="s">
+      <c r="BN19" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM19" s="42" t="s">
+      <c r="BO19" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:65" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="27"/>
       <c r="B20" s="85" t="s">
         <v>336</v>
       </c>
-      <c r="C20" s="148" t="s">
+      <c r="C20" s="147" t="s">
         <v>310</v>
       </c>
       <c r="D20" s="25">
@@ -8672,7 +8624,7 @@
       <c r="F20" s="25">
         <v>10</v>
       </c>
-      <c r="G20" s="144" t="s">
+      <c r="G20" s="143" t="s">
         <v>1109</v>
       </c>
       <c r="H20" s="40">
@@ -8793,60 +8745,68 @@
       <c r="AU20" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AV20" s="42" t="s">
+      <c r="AV20" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AW20" s="43" t="s">
+      <c r="AW20" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX20" s="53" t="s">
+      <c r="AX20" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY20" s="44">
+      <c r="AY20" s="43">
+        <v>4</v>
+      </c>
+      <c r="AZ20" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA20" s="151">
+        <v>16</v>
+      </c>
+      <c r="BB20" s="44">
         <v>0.2</v>
       </c>
-      <c r="AZ20" s="153"/>
-      <c r="BA20" s="42" t="s">
+      <c r="BC20" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BB20" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC20" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD20" s="41" t="s">
+      <c r="BD20" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE20" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF20" s="41"/>
-      <c r="BG20" s="41"/>
-      <c r="BH20" s="42"/>
-      <c r="BI20" s="60">
-        <v>0</v>
-      </c>
-      <c r="BJ20" s="61">
-        <v>0</v>
-      </c>
-      <c r="BK20" s="63">
+      <c r="BF20" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG20" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH20" s="41"/>
+      <c r="BI20" s="41"/>
+      <c r="BJ20" s="42"/>
+      <c r="BK20" s="60">
+        <v>0</v>
+      </c>
+      <c r="BL20" s="61">
+        <v>0</v>
+      </c>
+      <c r="BM20" s="63">
         <f>Variables!S$2</f>
         <v>25</v>
       </c>
-      <c r="BL20" s="63" t="s">
+      <c r="BN20" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BM20" s="42" t="s">
+      <c r="BO20" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:65" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="85" t="s">
         <v>1060</v>
       </c>
-      <c r="C21" s="148" t="s">
+      <c r="C21" s="147" t="s">
         <v>1089</v>
       </c>
       <c r="D21" s="25">
@@ -8858,7 +8818,7 @@
       <c r="F21" s="25">
         <v>5000</v>
       </c>
-      <c r="G21" s="144" t="s">
+      <c r="G21" s="143" t="s">
         <v>1111</v>
       </c>
       <c r="H21" s="40">
@@ -8979,47 +8939,55 @@
       <c r="AU21" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AV21" s="42" t="s">
+      <c r="AV21" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AW21" s="43"/>
-      <c r="AX21" s="53"/>
-      <c r="AY21" s="44"/>
-      <c r="AZ21" s="153">
+      <c r="AW21" s="41"/>
+      <c r="AX21" s="42"/>
+      <c r="AY21" s="43">
+        <v>3</v>
+      </c>
+      <c r="AZ21" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA21" s="151">
         <v>12</v>
       </c>
-      <c r="BA21" s="42" t="s">
+      <c r="BB21" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC21" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BB21" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC21" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD21" s="41" t="s">
+      <c r="BD21" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BE21" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF21" s="41"/>
-      <c r="BG21" s="41"/>
-      <c r="BH21" s="42"/>
-      <c r="BI21" s="60"/>
-      <c r="BJ21" s="61"/>
-      <c r="BK21" s="63"/>
-      <c r="BL21" s="63" t="s">
+      <c r="BF21" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG21" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH21" s="41"/>
+      <c r="BI21" s="41"/>
+      <c r="BJ21" s="42"/>
+      <c r="BK21" s="60"/>
+      <c r="BL21" s="61"/>
+      <c r="BM21" s="63"/>
+      <c r="BN21" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM21" s="42"/>
-    </row>
-    <row r="22" spans="1:65" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="BO21" s="42"/>
+    </row>
+    <row r="22" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
       <c r="B22" s="85" t="s">
         <v>1065</v>
       </c>
-      <c r="C22" s="148" t="s">
+      <c r="C22" s="147" t="s">
         <v>1082</v>
       </c>
       <c r="D22" s="25">
@@ -9031,7 +8999,7 @@
       <c r="F22" s="25">
         <v>5000</v>
       </c>
-      <c r="G22" s="144" t="s">
+      <c r="G22" s="143" t="s">
         <v>1112</v>
       </c>
       <c r="H22" s="40">
@@ -9138,45 +9106,53 @@
       <c r="AS22" s="41"/>
       <c r="AT22" s="41"/>
       <c r="AU22" s="41"/>
-      <c r="AV22" s="42"/>
-      <c r="AW22" s="43"/>
-      <c r="AX22" s="53"/>
-      <c r="AY22" s="44"/>
-      <c r="AZ22" s="153">
+      <c r="AV22" s="41"/>
+      <c r="AW22" s="41"/>
+      <c r="AX22" s="42"/>
+      <c r="AY22" s="43">
+        <v>3</v>
+      </c>
+      <c r="AZ22" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA22" s="151">
         <v>12</v>
       </c>
-      <c r="BA22" s="42" t="s">
+      <c r="BB22" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC22" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BB22" s="99">
+      <c r="BD22" s="99">
         <v>20</v>
       </c>
-      <c r="BC22" s="41">
+      <c r="BE22" s="41">
         <v>2</v>
       </c>
-      <c r="BD22" s="41">
+      <c r="BF22" s="41">
         <v>6</v>
       </c>
-      <c r="BE22" s="41">
+      <c r="BG22" s="41">
         <v>10</v>
       </c>
-      <c r="BF22" s="41"/>
-      <c r="BG22" s="41"/>
-      <c r="BH22" s="42"/>
-      <c r="BI22" s="60"/>
-      <c r="BJ22" s="61"/>
-      <c r="BK22" s="63"/>
-      <c r="BL22" s="63" t="s">
+      <c r="BH22" s="41"/>
+      <c r="BI22" s="41"/>
+      <c r="BJ22" s="42"/>
+      <c r="BK22" s="60"/>
+      <c r="BL22" s="61"/>
+      <c r="BM22" s="63"/>
+      <c r="BN22" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM22" s="42"/>
-    </row>
-    <row r="23" spans="1:65" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="BO22" s="42"/>
+    </row>
+    <row r="23" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="85" t="s">
         <v>1070</v>
       </c>
-      <c r="C23" s="148" t="s">
+      <c r="C23" s="147" t="s">
         <v>1083</v>
       </c>
       <c r="D23" s="25">
@@ -9188,7 +9164,7 @@
       <c r="F23" s="25">
         <v>5000</v>
       </c>
-      <c r="G23" s="144" t="s">
+      <c r="G23" s="143" t="s">
         <v>1116</v>
       </c>
       <c r="H23" s="40">
@@ -9295,45 +9271,53 @@
       <c r="AS23" s="41"/>
       <c r="AT23" s="41"/>
       <c r="AU23" s="41"/>
-      <c r="AV23" s="42"/>
-      <c r="AW23" s="43"/>
-      <c r="AX23" s="53"/>
-      <c r="AY23" s="44"/>
-      <c r="AZ23" s="153">
+      <c r="AV23" s="41"/>
+      <c r="AW23" s="41"/>
+      <c r="AX23" s="42"/>
+      <c r="AY23" s="43">
+        <v>1</v>
+      </c>
+      <c r="AZ23" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA23" s="151">
         <v>8</v>
       </c>
-      <c r="BA23" s="42" t="s">
+      <c r="BB23" s="44">
+        <v>0</v>
+      </c>
+      <c r="BC23" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BB23" s="99">
+      <c r="BD23" s="99">
         <v>45</v>
       </c>
-      <c r="BC23" s="41" t="s">
+      <c r="BE23" s="41" t="s">
         <v>1125</v>
       </c>
-      <c r="BD23" s="41" t="s">
+      <c r="BF23" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BE23" s="41" t="s">
+      <c r="BG23" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF23" s="41"/>
-      <c r="BG23" s="41"/>
-      <c r="BH23" s="42"/>
-      <c r="BI23" s="60"/>
-      <c r="BJ23" s="61"/>
-      <c r="BK23" s="63"/>
-      <c r="BL23" s="63" t="s">
+      <c r="BH23" s="41"/>
+      <c r="BI23" s="41"/>
+      <c r="BJ23" s="42"/>
+      <c r="BK23" s="60"/>
+      <c r="BL23" s="61"/>
+      <c r="BM23" s="63"/>
+      <c r="BN23" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM23" s="42"/>
-    </row>
-    <row r="24" spans="1:65" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="BO23" s="42"/>
+    </row>
+    <row r="24" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="27"/>
       <c r="B24" s="85" t="s">
         <v>1071</v>
       </c>
-      <c r="C24" s="148" t="s">
+      <c r="C24" s="147" t="s">
         <v>1084</v>
       </c>
       <c r="D24" s="25">
@@ -9345,7 +9329,7 @@
       <c r="F24" s="25">
         <v>5000</v>
       </c>
-      <c r="G24" s="144" t="s">
+      <c r="G24" s="143" t="s">
         <v>1113</v>
       </c>
       <c r="H24" s="40">
@@ -9452,45 +9436,53 @@
       <c r="AS24" s="41"/>
       <c r="AT24" s="41"/>
       <c r="AU24" s="41"/>
-      <c r="AV24" s="42"/>
-      <c r="AW24" s="43"/>
-      <c r="AX24" s="53"/>
-      <c r="AY24" s="44"/>
-      <c r="AZ24" s="153">
+      <c r="AV24" s="41"/>
+      <c r="AW24" s="41"/>
+      <c r="AX24" s="42"/>
+      <c r="AY24" s="43">
+        <v>3</v>
+      </c>
+      <c r="AZ24" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA24" s="151">
         <v>12</v>
       </c>
-      <c r="BA24" s="42" t="s">
+      <c r="BB24" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC24" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BB24" s="99">
+      <c r="BD24" s="99">
         <v>50</v>
       </c>
-      <c r="BC24" s="41">
+      <c r="BE24" s="41">
         <v>2</v>
       </c>
-      <c r="BD24" s="41">
+      <c r="BF24" s="41">
         <v>8</v>
       </c>
-      <c r="BE24" s="41">
+      <c r="BG24" s="41">
         <v>10</v>
       </c>
-      <c r="BF24" s="41"/>
-      <c r="BG24" s="41"/>
-      <c r="BH24" s="42"/>
-      <c r="BI24" s="60"/>
-      <c r="BJ24" s="61"/>
-      <c r="BK24" s="63"/>
-      <c r="BL24" s="63" t="s">
+      <c r="BH24" s="41"/>
+      <c r="BI24" s="41"/>
+      <c r="BJ24" s="42"/>
+      <c r="BK24" s="60"/>
+      <c r="BL24" s="61"/>
+      <c r="BM24" s="63"/>
+      <c r="BN24" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM24" s="42"/>
-    </row>
-    <row r="25" spans="1:65" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="BO24" s="42"/>
+    </row>
+    <row r="25" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
       <c r="B25" s="85" t="s">
         <v>1120</v>
       </c>
-      <c r="C25" s="148" t="s">
+      <c r="C25" s="147" t="s">
         <v>1085</v>
       </c>
       <c r="D25" s="25">
@@ -9502,7 +9494,7 @@
       <c r="F25" s="25">
         <v>5000</v>
       </c>
-      <c r="G25" s="144" t="s">
+      <c r="G25" s="143" t="s">
         <v>1114</v>
       </c>
       <c r="H25" s="40">
@@ -9609,45 +9601,53 @@
       <c r="AS25" s="41"/>
       <c r="AT25" s="41"/>
       <c r="AU25" s="41"/>
-      <c r="AV25" s="42"/>
-      <c r="AW25" s="43"/>
-      <c r="AX25" s="53"/>
-      <c r="AY25" s="44"/>
-      <c r="AZ25" s="153">
+      <c r="AV25" s="41"/>
+      <c r="AW25" s="41"/>
+      <c r="AX25" s="42"/>
+      <c r="AY25" s="43">
+        <v>3</v>
+      </c>
+      <c r="AZ25" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA25" s="151">
         <v>12</v>
       </c>
-      <c r="BA25" s="42" t="s">
+      <c r="BB25" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC25" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BB25" s="99">
+      <c r="BD25" s="99">
         <v>150</v>
       </c>
-      <c r="BC25" s="41">
+      <c r="BE25" s="41">
         <v>2</v>
       </c>
-      <c r="BD25" s="41">
+      <c r="BF25" s="41">
         <v>5</v>
       </c>
-      <c r="BE25" s="41">
+      <c r="BG25" s="41">
         <v>12.4</v>
       </c>
-      <c r="BF25" s="41"/>
-      <c r="BG25" s="41"/>
-      <c r="BH25" s="42"/>
-      <c r="BI25" s="60"/>
-      <c r="BJ25" s="61"/>
-      <c r="BK25" s="63"/>
-      <c r="BL25" s="63" t="s">
+      <c r="BH25" s="41"/>
+      <c r="BI25" s="41"/>
+      <c r="BJ25" s="42"/>
+      <c r="BK25" s="60"/>
+      <c r="BL25" s="61"/>
+      <c r="BM25" s="63"/>
+      <c r="BN25" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM25" s="42"/>
-    </row>
-    <row r="26" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BO25" s="42"/>
+    </row>
+    <row r="26" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="85" t="s">
         <v>1119</v>
       </c>
-      <c r="C26" s="148" t="s">
+      <c r="C26" s="147" t="s">
         <v>1086</v>
       </c>
       <c r="D26" s="25">
@@ -9659,7 +9659,7 @@
       <c r="F26" s="25">
         <v>5000</v>
       </c>
-      <c r="G26" s="144" t="s">
+      <c r="G26" s="143" t="s">
         <v>1115</v>
       </c>
       <c r="H26" s="40">
@@ -9766,45 +9766,53 @@
       <c r="AS26" s="41"/>
       <c r="AT26" s="41"/>
       <c r="AU26" s="41"/>
-      <c r="AV26" s="42"/>
-      <c r="AW26" s="43"/>
-      <c r="AX26" s="53"/>
-      <c r="AY26" s="44"/>
-      <c r="AZ26" s="153">
+      <c r="AV26" s="41"/>
+      <c r="AW26" s="41"/>
+      <c r="AX26" s="42"/>
+      <c r="AY26" s="43">
+        <v>3</v>
+      </c>
+      <c r="AZ26" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA26" s="151">
         <v>12</v>
       </c>
-      <c r="BA26" s="42" t="s">
+      <c r="BB26" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC26" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BB26" s="99">
+      <c r="BD26" s="99">
         <v>200</v>
       </c>
-      <c r="BC26" s="41">
+      <c r="BE26" s="41">
         <v>2</v>
       </c>
-      <c r="BD26" s="41">
+      <c r="BF26" s="41">
         <v>6</v>
       </c>
-      <c r="BE26" s="41">
+      <c r="BG26" s="41">
         <v>10</v>
       </c>
-      <c r="BF26" s="41"/>
-      <c r="BG26" s="41"/>
-      <c r="BH26" s="42"/>
-      <c r="BI26" s="60"/>
-      <c r="BJ26" s="61"/>
-      <c r="BK26" s="63"/>
-      <c r="BL26" s="63" t="s">
+      <c r="BH26" s="41"/>
+      <c r="BI26" s="41"/>
+      <c r="BJ26" s="42"/>
+      <c r="BK26" s="60"/>
+      <c r="BL26" s="61"/>
+      <c r="BM26" s="63"/>
+      <c r="BN26" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM26" s="42"/>
-    </row>
-    <row r="27" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BO26" s="42"/>
+    </row>
+    <row r="27" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
       <c r="B27" s="85" t="s">
         <v>1118</v>
       </c>
-      <c r="C27" s="148" t="s">
+      <c r="C27" s="147" t="s">
         <v>1087</v>
       </c>
       <c r="D27" s="25">
@@ -9816,7 +9824,7 @@
       <c r="F27" s="25">
         <v>5000</v>
       </c>
-      <c r="G27" s="144" t="s">
+      <c r="G27" s="143" t="s">
         <v>1115</v>
       </c>
       <c r="H27" s="40">
@@ -9923,45 +9931,53 @@
       <c r="AS27" s="41"/>
       <c r="AT27" s="41"/>
       <c r="AU27" s="41"/>
-      <c r="AV27" s="42"/>
-      <c r="AW27" s="43"/>
-      <c r="AX27" s="53"/>
-      <c r="AY27" s="44"/>
-      <c r="AZ27" s="153">
+      <c r="AV27" s="41"/>
+      <c r="AW27" s="41"/>
+      <c r="AX27" s="42"/>
+      <c r="AY27" s="43">
+        <v>3</v>
+      </c>
+      <c r="AZ27" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA27" s="151">
         <v>12</v>
       </c>
-      <c r="BA27" s="42" t="s">
+      <c r="BB27" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BC27" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BB27" s="99">
+      <c r="BD27" s="99">
         <v>320</v>
       </c>
-      <c r="BC27" s="41">
+      <c r="BE27" s="41">
         <v>2</v>
       </c>
-      <c r="BD27" s="41">
+      <c r="BF27" s="41">
         <v>6</v>
       </c>
-      <c r="BE27" s="41">
+      <c r="BG27" s="41">
         <v>10</v>
       </c>
-      <c r="BF27" s="41"/>
-      <c r="BG27" s="41"/>
-      <c r="BH27" s="42"/>
-      <c r="BI27" s="60"/>
-      <c r="BJ27" s="61"/>
-      <c r="BK27" s="63"/>
-      <c r="BL27" s="63" t="s">
+      <c r="BH27" s="41"/>
+      <c r="BI27" s="41"/>
+      <c r="BJ27" s="42"/>
+      <c r="BK27" s="60"/>
+      <c r="BL27" s="61"/>
+      <c r="BM27" s="63"/>
+      <c r="BN27" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM27" s="42"/>
-    </row>
-    <row r="28" spans="1:65" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="BO27" s="42"/>
+    </row>
+    <row r="28" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="27"/>
       <c r="B28" s="85" t="s">
         <v>1117</v>
       </c>
-      <c r="C28" s="148" t="s">
+      <c r="C28" s="147" t="s">
         <v>1105</v>
       </c>
       <c r="D28" s="25">
@@ -9973,8 +9989,8 @@
       <c r="F28" s="25">
         <v>5000</v>
       </c>
-      <c r="G28" s="144" t="s">
-        <v>1132</v>
+      <c r="G28" s="143" t="s">
+        <v>1131</v>
       </c>
       <c r="H28" s="40">
         <v>60</v>
@@ -10080,46 +10096,54 @@
       <c r="AS28" s="41"/>
       <c r="AT28" s="41"/>
       <c r="AU28" s="41"/>
-      <c r="AV28" s="42"/>
-      <c r="AW28" s="43"/>
-      <c r="AX28" s="53"/>
-      <c r="AY28" s="44"/>
-      <c r="AZ28" s="153">
+      <c r="AV28" s="41"/>
+      <c r="AW28" s="41"/>
+      <c r="AX28" s="42"/>
+      <c r="AY28" s="43">
+        <v>1</v>
+      </c>
+      <c r="AZ28" s="151">
+        <v>0</v>
+      </c>
+      <c r="BA28" s="151">
         <v>8</v>
       </c>
-      <c r="BA28" s="42" t="s">
+      <c r="BB28" s="44">
+        <v>0</v>
+      </c>
+      <c r="BC28" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BB28" s="99">
+      <c r="BD28" s="99">
         <v>200</v>
       </c>
-      <c r="BC28" s="41">
+      <c r="BE28" s="41">
         <v>3</v>
       </c>
-      <c r="BD28" s="41">
+      <c r="BF28" s="41">
         <v>1.2645999999999999</v>
       </c>
-      <c r="BE28" s="41" t="s">
+      <c r="BG28" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BF28" s="41"/>
-      <c r="BG28" s="41"/>
-      <c r="BH28" s="42"/>
-      <c r="BI28" s="60"/>
-      <c r="BJ28" s="61"/>
-      <c r="BK28" s="63"/>
-      <c r="BL28" s="63" t="s">
+      <c r="BH28" s="41"/>
+      <c r="BI28" s="41"/>
+      <c r="BJ28" s="42"/>
+      <c r="BK28" s="60"/>
+      <c r="BL28" s="61"/>
+      <c r="BM28" s="63"/>
+      <c r="BN28" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BM28" s="42"/>
-    </row>
-    <row r="29" spans="1:65" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BO28" s="42"/>
+    </row>
+    <row r="29" spans="1:67" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
-      <c r="C29" s="150"/>
+      <c r="C29" s="149"/>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="140"/>
+      <c r="G29" s="139"/>
       <c r="H29" s="5"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -10162,429 +10186,447 @@
       <c r="AS29" s="8"/>
       <c r="AT29" s="8"/>
       <c r="AU29" s="8"/>
-      <c r="AV29" s="6"/>
-      <c r="AW29" s="7"/>
-      <c r="AX29" s="48"/>
-      <c r="AY29" s="10"/>
-      <c r="AZ29" s="155"/>
-      <c r="BA29" s="6"/>
-      <c r="BB29" s="100"/>
-      <c r="BC29" s="8"/>
-      <c r="BD29" s="8"/>
+      <c r="AV29" s="8"/>
+      <c r="AW29" s="8"/>
+      <c r="AX29" s="6"/>
+      <c r="AY29" s="7"/>
+      <c r="AZ29" s="153"/>
+      <c r="BA29" s="153"/>
+      <c r="BB29" s="186"/>
+      <c r="BC29" s="6"/>
+      <c r="BD29" s="100"/>
       <c r="BE29" s="8"/>
       <c r="BF29" s="8"/>
       <c r="BG29" s="8"/>
-      <c r="BH29" s="6"/>
-      <c r="BI29" s="7"/>
-      <c r="BJ29" s="48"/>
-      <c r="BK29" s="64"/>
-      <c r="BL29" s="64"/>
-      <c r="BM29" s="6"/>
-    </row>
-    <row r="33" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW33" s="9"/>
-      <c r="AX33" s="2"/>
-      <c r="AY33" s="2"/>
+      <c r="BH29" s="8"/>
+      <c r="BI29" s="8"/>
+      <c r="BJ29" s="6"/>
+      <c r="BK29" s="7"/>
+      <c r="BL29" s="48"/>
+      <c r="BM29" s="64"/>
+      <c r="BN29" s="64"/>
+      <c r="BO29" s="6"/>
+    </row>
+    <row r="33" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY33" s="9"/>
       <c r="AZ33" s="2"/>
-      <c r="BA33" s="45"/>
-      <c r="BH33" s="45"/>
-      <c r="BI33" s="45"/>
-      <c r="BK33" s="2"/>
-      <c r="BL33"/>
-      <c r="BM33"/>
-    </row>
-    <row r="34" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW34" s="9"/>
-      <c r="AX34" s="2"/>
-      <c r="AY34" s="2"/>
+      <c r="BA33" s="2"/>
+      <c r="BB33" s="187"/>
+      <c r="BC33" s="45"/>
+      <c r="BJ33" s="45"/>
+      <c r="BK33" s="45"/>
+      <c r="BM33" s="2"/>
+      <c r="BN33"/>
+      <c r="BO33"/>
+    </row>
+    <row r="34" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY34" s="9"/>
       <c r="AZ34" s="2"/>
-      <c r="BA34" s="45"/>
-      <c r="BH34" s="45"/>
-      <c r="BI34" s="45"/>
-      <c r="BK34" s="2"/>
-      <c r="BL34"/>
-      <c r="BM34"/>
-    </row>
-    <row r="35" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW35" s="9"/>
-      <c r="AX35" s="2"/>
-      <c r="AY35" s="2"/>
+      <c r="BA34" s="2"/>
+      <c r="BB34" s="187"/>
+      <c r="BC34" s="45"/>
+      <c r="BJ34" s="45"/>
+      <c r="BK34" s="45"/>
+      <c r="BM34" s="2"/>
+      <c r="BN34"/>
+      <c r="BO34"/>
+    </row>
+    <row r="35" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY35" s="9"/>
       <c r="AZ35" s="2"/>
-      <c r="BA35" s="45"/>
-      <c r="BH35" s="45"/>
-      <c r="BI35" s="45"/>
-      <c r="BK35" s="2"/>
-      <c r="BL35"/>
-      <c r="BM35"/>
-    </row>
-    <row r="36" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW36" s="9"/>
-      <c r="AX36" s="2"/>
-      <c r="AY36" s="2"/>
+      <c r="BA35" s="2"/>
+      <c r="BB35" s="187"/>
+      <c r="BC35" s="45"/>
+      <c r="BJ35" s="45"/>
+      <c r="BK35" s="45"/>
+      <c r="BM35" s="2"/>
+      <c r="BN35"/>
+      <c r="BO35"/>
+    </row>
+    <row r="36" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY36" s="9"/>
       <c r="AZ36" s="2"/>
-      <c r="BA36" s="45"/>
-      <c r="BH36" s="45"/>
-      <c r="BI36" s="45"/>
-      <c r="BK36" s="2"/>
-      <c r="BL36"/>
-      <c r="BM36"/>
-    </row>
-    <row r="37" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW37" s="9"/>
-      <c r="AX37" s="2"/>
-      <c r="AY37" s="2"/>
+      <c r="BA36" s="2"/>
+      <c r="BB36" s="187"/>
+      <c r="BC36" s="45"/>
+      <c r="BJ36" s="45"/>
+      <c r="BK36" s="45"/>
+      <c r="BM36" s="2"/>
+      <c r="BN36"/>
+      <c r="BO36"/>
+    </row>
+    <row r="37" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY37" s="9"/>
       <c r="AZ37" s="2"/>
-      <c r="BA37" s="45"/>
-      <c r="BH37" s="45"/>
-      <c r="BI37" s="45"/>
-      <c r="BK37" s="2"/>
-      <c r="BL37"/>
-      <c r="BM37"/>
-    </row>
-    <row r="38" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW38" s="9"/>
-      <c r="AX38" s="2"/>
-      <c r="AY38" s="2"/>
+      <c r="BA37" s="2"/>
+      <c r="BB37" s="187"/>
+      <c r="BC37" s="45"/>
+      <c r="BJ37" s="45"/>
+      <c r="BK37" s="45"/>
+      <c r="BM37" s="2"/>
+      <c r="BN37"/>
+      <c r="BO37"/>
+    </row>
+    <row r="38" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY38" s="9"/>
       <c r="AZ38" s="2"/>
-      <c r="BA38" s="45"/>
-      <c r="BH38" s="45"/>
-      <c r="BI38" s="45"/>
-      <c r="BK38" s="2"/>
-      <c r="BL38"/>
-      <c r="BM38"/>
-    </row>
-    <row r="39" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW39" s="9"/>
-      <c r="AX39" s="2"/>
-      <c r="AY39" s="2"/>
+      <c r="BA38" s="2"/>
+      <c r="BB38" s="187"/>
+      <c r="BC38" s="45"/>
+      <c r="BJ38" s="45"/>
+      <c r="BK38" s="45"/>
+      <c r="BM38" s="2"/>
+      <c r="BN38"/>
+      <c r="BO38"/>
+    </row>
+    <row r="39" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY39" s="9"/>
       <c r="AZ39" s="2"/>
-      <c r="BA39" s="45"/>
-      <c r="BH39" s="45"/>
-      <c r="BI39" s="45"/>
-      <c r="BK39" s="2"/>
-      <c r="BL39"/>
-      <c r="BM39"/>
-    </row>
-    <row r="40" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW40" s="9"/>
-      <c r="AX40" s="2"/>
-      <c r="AY40" s="2"/>
+      <c r="BA39" s="2"/>
+      <c r="BB39" s="187"/>
+      <c r="BC39" s="45"/>
+      <c r="BJ39" s="45"/>
+      <c r="BK39" s="45"/>
+      <c r="BM39" s="2"/>
+      <c r="BN39"/>
+      <c r="BO39"/>
+    </row>
+    <row r="40" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY40" s="9"/>
       <c r="AZ40" s="2"/>
-      <c r="BA40" s="45"/>
-      <c r="BH40" s="45"/>
-      <c r="BI40" s="45"/>
-      <c r="BK40" s="2"/>
-      <c r="BL40"/>
-      <c r="BM40"/>
-    </row>
-    <row r="41" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW41" s="9"/>
-      <c r="AX41" s="2"/>
-      <c r="AY41" s="2"/>
+      <c r="BA40" s="2"/>
+      <c r="BB40" s="187"/>
+      <c r="BC40" s="45"/>
+      <c r="BJ40" s="45"/>
+      <c r="BK40" s="45"/>
+      <c r="BM40" s="2"/>
+      <c r="BN40"/>
+      <c r="BO40"/>
+    </row>
+    <row r="41" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY41" s="9"/>
       <c r="AZ41" s="2"/>
-      <c r="BA41" s="45"/>
-      <c r="BH41" s="45"/>
-      <c r="BI41" s="45"/>
-      <c r="BK41" s="2"/>
-      <c r="BL41"/>
-      <c r="BM41"/>
-    </row>
-    <row r="42" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW42" s="9"/>
-      <c r="AX42" s="2"/>
-      <c r="AY42" s="2"/>
+      <c r="BA41" s="2"/>
+      <c r="BB41" s="187"/>
+      <c r="BC41" s="45"/>
+      <c r="BJ41" s="45"/>
+      <c r="BK41" s="45"/>
+      <c r="BM41" s="2"/>
+      <c r="BN41"/>
+      <c r="BO41"/>
+    </row>
+    <row r="42" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY42" s="9"/>
       <c r="AZ42" s="2"/>
-      <c r="BA42" s="45"/>
-      <c r="BH42" s="45"/>
-      <c r="BI42" s="45"/>
-      <c r="BK42" s="2"/>
-      <c r="BL42"/>
-      <c r="BM42"/>
-    </row>
-    <row r="43" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW43" s="9"/>
-      <c r="AX43" s="2"/>
-      <c r="AY43" s="2"/>
+      <c r="BA42" s="2"/>
+      <c r="BB42" s="187"/>
+      <c r="BC42" s="45"/>
+      <c r="BJ42" s="45"/>
+      <c r="BK42" s="45"/>
+      <c r="BM42" s="2"/>
+      <c r="BN42"/>
+      <c r="BO42"/>
+    </row>
+    <row r="43" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY43" s="9"/>
       <c r="AZ43" s="2"/>
-      <c r="BA43" s="45"/>
-      <c r="BH43" s="45"/>
-      <c r="BI43" s="45"/>
-      <c r="BK43" s="2"/>
-      <c r="BL43"/>
-      <c r="BM43"/>
-    </row>
-    <row r="44" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW44" s="9"/>
-      <c r="AX44" s="2"/>
-      <c r="AY44" s="2"/>
+      <c r="BA43" s="2"/>
+      <c r="BB43" s="187"/>
+      <c r="BC43" s="45"/>
+      <c r="BJ43" s="45"/>
+      <c r="BK43" s="45"/>
+      <c r="BM43" s="2"/>
+      <c r="BN43"/>
+      <c r="BO43"/>
+    </row>
+    <row r="44" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY44" s="9"/>
       <c r="AZ44" s="2"/>
-      <c r="BA44" s="45"/>
-      <c r="BH44" s="45"/>
-      <c r="BI44" s="45"/>
-      <c r="BK44" s="2"/>
-      <c r="BL44"/>
-      <c r="BM44"/>
-    </row>
-    <row r="45" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW45" s="9"/>
-      <c r="AX45" s="2"/>
-      <c r="AY45" s="2"/>
+      <c r="BA44" s="2"/>
+      <c r="BB44" s="187"/>
+      <c r="BC44" s="45"/>
+      <c r="BJ44" s="45"/>
+      <c r="BK44" s="45"/>
+      <c r="BM44" s="2"/>
+      <c r="BN44"/>
+      <c r="BO44"/>
+    </row>
+    <row r="45" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY45" s="9"/>
       <c r="AZ45" s="2"/>
-      <c r="BA45" s="45"/>
-      <c r="BH45" s="45"/>
-      <c r="BI45" s="45"/>
-      <c r="BK45" s="2"/>
-      <c r="BL45"/>
-      <c r="BM45"/>
-    </row>
-    <row r="46" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW46" s="9"/>
-      <c r="AX46" s="2"/>
-      <c r="AY46" s="2"/>
+      <c r="BA45" s="2"/>
+      <c r="BB45" s="187"/>
+      <c r="BC45" s="45"/>
+      <c r="BJ45" s="45"/>
+      <c r="BK45" s="45"/>
+      <c r="BM45" s="2"/>
+      <c r="BN45"/>
+      <c r="BO45"/>
+    </row>
+    <row r="46" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY46" s="9"/>
       <c r="AZ46" s="2"/>
-      <c r="BA46" s="45"/>
-      <c r="BH46" s="45"/>
-      <c r="BI46" s="45"/>
-      <c r="BK46" s="2"/>
-      <c r="BL46"/>
-      <c r="BM46"/>
-    </row>
-    <row r="47" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW47" s="9"/>
-      <c r="AX47" s="2"/>
-      <c r="AY47" s="2"/>
+      <c r="BA46" s="2"/>
+      <c r="BB46" s="187"/>
+      <c r="BC46" s="45"/>
+      <c r="BJ46" s="45"/>
+      <c r="BK46" s="45"/>
+      <c r="BM46" s="2"/>
+      <c r="BN46"/>
+      <c r="BO46"/>
+    </row>
+    <row r="47" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY47" s="9"/>
       <c r="AZ47" s="2"/>
-      <c r="BA47" s="45"/>
-      <c r="BH47" s="45"/>
-      <c r="BI47" s="45"/>
-      <c r="BK47" s="2"/>
-      <c r="BL47"/>
-      <c r="BM47"/>
-    </row>
-    <row r="48" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW48" s="9"/>
-      <c r="AX48" s="2"/>
-      <c r="AY48" s="2"/>
+      <c r="BA47" s="2"/>
+      <c r="BB47" s="187"/>
+      <c r="BC47" s="45"/>
+      <c r="BJ47" s="45"/>
+      <c r="BK47" s="45"/>
+      <c r="BM47" s="2"/>
+      <c r="BN47"/>
+      <c r="BO47"/>
+    </row>
+    <row r="48" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY48" s="9"/>
       <c r="AZ48" s="2"/>
-      <c r="BA48" s="45"/>
-      <c r="BH48" s="45"/>
-      <c r="BI48" s="45"/>
-      <c r="BK48" s="2"/>
-      <c r="BL48"/>
-      <c r="BM48"/>
-    </row>
-    <row r="49" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW49" s="9"/>
-      <c r="AX49" s="2"/>
-      <c r="AY49" s="2"/>
+      <c r="BA48" s="2"/>
+      <c r="BB48" s="187"/>
+      <c r="BC48" s="45"/>
+      <c r="BJ48" s="45"/>
+      <c r="BK48" s="45"/>
+      <c r="BM48" s="2"/>
+      <c r="BN48"/>
+      <c r="BO48"/>
+    </row>
+    <row r="49" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY49" s="9"/>
       <c r="AZ49" s="2"/>
-      <c r="BA49" s="45"/>
-      <c r="BH49" s="45"/>
-      <c r="BI49" s="45"/>
-      <c r="BK49" s="2"/>
-      <c r="BL49"/>
-      <c r="BM49"/>
-    </row>
-    <row r="50" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW50" s="9"/>
-      <c r="AX50" s="2"/>
-      <c r="AY50" s="2"/>
+      <c r="BA49" s="2"/>
+      <c r="BB49" s="187"/>
+      <c r="BC49" s="45"/>
+      <c r="BJ49" s="45"/>
+      <c r="BK49" s="45"/>
+      <c r="BM49" s="2"/>
+      <c r="BN49"/>
+      <c r="BO49"/>
+    </row>
+    <row r="50" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY50" s="9"/>
       <c r="AZ50" s="2"/>
-      <c r="BA50" s="45"/>
-      <c r="BH50" s="45"/>
-      <c r="BI50" s="45"/>
-      <c r="BK50" s="2"/>
-      <c r="BL50"/>
-      <c r="BM50"/>
-    </row>
-    <row r="51" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW51" s="9"/>
-      <c r="AX51" s="2"/>
-      <c r="AY51" s="2"/>
+      <c r="BA50" s="2"/>
+      <c r="BB50" s="187"/>
+      <c r="BC50" s="45"/>
+      <c r="BJ50" s="45"/>
+      <c r="BK50" s="45"/>
+      <c r="BM50" s="2"/>
+      <c r="BN50"/>
+      <c r="BO50"/>
+    </row>
+    <row r="51" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY51" s="9"/>
       <c r="AZ51" s="2"/>
-      <c r="BA51" s="45"/>
-      <c r="BH51" s="45"/>
-      <c r="BI51" s="45"/>
-      <c r="BK51" s="2"/>
-      <c r="BL51"/>
-      <c r="BM51"/>
-    </row>
-    <row r="52" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW52" s="9"/>
-      <c r="AX52" s="2"/>
-      <c r="AY52" s="2"/>
+      <c r="BA51" s="2"/>
+      <c r="BB51" s="187"/>
+      <c r="BC51" s="45"/>
+      <c r="BJ51" s="45"/>
+      <c r="BK51" s="45"/>
+      <c r="BM51" s="2"/>
+      <c r="BN51"/>
+      <c r="BO51"/>
+    </row>
+    <row r="52" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY52" s="9"/>
       <c r="AZ52" s="2"/>
-      <c r="BA52" s="45"/>
-      <c r="BH52" s="45"/>
-      <c r="BI52" s="45"/>
-      <c r="BK52" s="2"/>
-      <c r="BL52"/>
-      <c r="BM52"/>
-    </row>
-    <row r="53" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW53" s="9"/>
-      <c r="AX53" s="2"/>
-      <c r="AY53" s="2"/>
+      <c r="BA52" s="2"/>
+      <c r="BB52" s="187"/>
+      <c r="BC52" s="45"/>
+      <c r="BJ52" s="45"/>
+      <c r="BK52" s="45"/>
+      <c r="BM52" s="2"/>
+      <c r="BN52"/>
+      <c r="BO52"/>
+    </row>
+    <row r="53" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY53" s="9"/>
       <c r="AZ53" s="2"/>
-      <c r="BA53" s="45"/>
-      <c r="BH53" s="45"/>
-      <c r="BI53" s="45"/>
-      <c r="BK53" s="2"/>
-      <c r="BL53"/>
-      <c r="BM53"/>
-    </row>
-    <row r="54" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW54" s="9"/>
-      <c r="AX54" s="2"/>
-      <c r="AY54" s="2"/>
+      <c r="BA53" s="2"/>
+      <c r="BB53" s="187"/>
+      <c r="BC53" s="45"/>
+      <c r="BJ53" s="45"/>
+      <c r="BK53" s="45"/>
+      <c r="BM53" s="2"/>
+      <c r="BN53"/>
+      <c r="BO53"/>
+    </row>
+    <row r="54" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY54" s="9"/>
       <c r="AZ54" s="2"/>
-      <c r="BA54" s="45"/>
-      <c r="BH54" s="45"/>
-      <c r="BI54" s="45"/>
-      <c r="BK54" s="2"/>
-      <c r="BL54"/>
-      <c r="BM54"/>
-    </row>
-    <row r="55" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW55" s="9"/>
-      <c r="AX55" s="2"/>
-      <c r="AY55" s="2"/>
+      <c r="BA54" s="2"/>
+      <c r="BB54" s="187"/>
+      <c r="BC54" s="45"/>
+      <c r="BJ54" s="45"/>
+      <c r="BK54" s="45"/>
+      <c r="BM54" s="2"/>
+      <c r="BN54"/>
+      <c r="BO54"/>
+    </row>
+    <row r="55" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY55" s="9"/>
       <c r="AZ55" s="2"/>
-      <c r="BA55" s="45"/>
-      <c r="BH55" s="45"/>
-      <c r="BI55" s="45"/>
-      <c r="BK55" s="2"/>
-      <c r="BL55"/>
-      <c r="BM55"/>
-    </row>
-    <row r="56" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW56" s="9"/>
-      <c r="AX56" s="2"/>
-      <c r="AY56" s="2"/>
+      <c r="BA55" s="2"/>
+      <c r="BB55" s="187"/>
+      <c r="BC55" s="45"/>
+      <c r="BJ55" s="45"/>
+      <c r="BK55" s="45"/>
+      <c r="BM55" s="2"/>
+      <c r="BN55"/>
+      <c r="BO55"/>
+    </row>
+    <row r="56" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY56" s="9"/>
       <c r="AZ56" s="2"/>
-      <c r="BA56" s="45"/>
-      <c r="BH56" s="45"/>
-      <c r="BI56" s="45"/>
-      <c r="BK56" s="2"/>
-      <c r="BL56"/>
-      <c r="BM56"/>
-    </row>
-    <row r="57" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW57" s="9"/>
-      <c r="AX57" s="2"/>
-      <c r="AY57" s="2"/>
+      <c r="BA56" s="2"/>
+      <c r="BB56" s="187"/>
+      <c r="BC56" s="45"/>
+      <c r="BJ56" s="45"/>
+      <c r="BK56" s="45"/>
+      <c r="BM56" s="2"/>
+      <c r="BN56"/>
+      <c r="BO56"/>
+    </row>
+    <row r="57" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY57" s="9"/>
       <c r="AZ57" s="2"/>
-      <c r="BA57" s="45"/>
-      <c r="BH57" s="45"/>
-      <c r="BI57" s="45"/>
-      <c r="BK57" s="2"/>
-      <c r="BL57"/>
-      <c r="BM57"/>
-    </row>
-    <row r="58" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW58" s="9"/>
-      <c r="AX58" s="2"/>
-      <c r="AY58" s="2"/>
+      <c r="BA57" s="2"/>
+      <c r="BB57" s="187"/>
+      <c r="BC57" s="45"/>
+      <c r="BJ57" s="45"/>
+      <c r="BK57" s="45"/>
+      <c r="BM57" s="2"/>
+      <c r="BN57"/>
+      <c r="BO57"/>
+    </row>
+    <row r="58" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY58" s="9"/>
       <c r="AZ58" s="2"/>
-      <c r="BA58" s="45"/>
-      <c r="BH58" s="45"/>
-      <c r="BI58" s="45"/>
-      <c r="BK58" s="2"/>
-      <c r="BL58"/>
-      <c r="BM58"/>
-    </row>
-    <row r="59" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW59" s="9"/>
-      <c r="AX59" s="2"/>
-      <c r="AY59" s="2"/>
+      <c r="BA58" s="2"/>
+      <c r="BB58" s="187"/>
+      <c r="BC58" s="45"/>
+      <c r="BJ58" s="45"/>
+      <c r="BK58" s="45"/>
+      <c r="BM58" s="2"/>
+      <c r="BN58"/>
+      <c r="BO58"/>
+    </row>
+    <row r="59" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY59" s="9"/>
       <c r="AZ59" s="2"/>
-      <c r="BA59" s="45"/>
-      <c r="BH59" s="45"/>
-      <c r="BI59" s="45"/>
-      <c r="BK59" s="2"/>
-      <c r="BL59"/>
-      <c r="BM59"/>
-    </row>
-    <row r="60" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW60" s="9"/>
-      <c r="AX60" s="2"/>
-      <c r="AY60" s="2"/>
+      <c r="BA59" s="2"/>
+      <c r="BB59" s="187"/>
+      <c r="BC59" s="45"/>
+      <c r="BJ59" s="45"/>
+      <c r="BK59" s="45"/>
+      <c r="BM59" s="2"/>
+      <c r="BN59"/>
+      <c r="BO59"/>
+    </row>
+    <row r="60" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY60" s="9"/>
       <c r="AZ60" s="2"/>
-      <c r="BA60" s="45"/>
-      <c r="BH60" s="45"/>
-      <c r="BI60" s="45"/>
-      <c r="BK60" s="2"/>
-      <c r="BL60"/>
-      <c r="BM60"/>
-    </row>
-    <row r="61" spans="49:65" x14ac:dyDescent="0.25">
-      <c r="AW61" s="9"/>
-      <c r="AX61" s="2"/>
-      <c r="AY61" s="2"/>
+      <c r="BA60" s="2"/>
+      <c r="BB60" s="187"/>
+      <c r="BC60" s="45"/>
+      <c r="BJ60" s="45"/>
+      <c r="BK60" s="45"/>
+      <c r="BM60" s="2"/>
+      <c r="BN60"/>
+      <c r="BO60"/>
+    </row>
+    <row r="61" spans="51:67" x14ac:dyDescent="0.25">
+      <c r="AY61" s="9"/>
       <c r="AZ61" s="2"/>
-      <c r="BA61" s="45"/>
-      <c r="BH61" s="45"/>
-      <c r="BI61" s="45"/>
-      <c r="BK61" s="2"/>
-      <c r="BL61"/>
-      <c r="BM61"/>
+      <c r="BA61" s="2"/>
+      <c r="BB61" s="187"/>
+      <c r="BC61" s="45"/>
+      <c r="BJ61" s="45"/>
+      <c r="BK61" s="45"/>
+      <c r="BM61" s="2"/>
+      <c r="BN61"/>
+      <c r="BO61"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="BI2:BM2"/>
+    <mergeCell ref="BK2:BO2"/>
     <mergeCell ref="H2:V2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="W2:AD2"/>
     <mergeCell ref="AE2:AP2"/>
-    <mergeCell ref="AQ2:AV2"/>
-    <mergeCell ref="BB2:BH2"/>
-    <mergeCell ref="AW2:BA2"/>
+    <mergeCell ref="AQ2:AX2"/>
+    <mergeCell ref="BD2:BJ2"/>
+    <mergeCell ref="AY2:BC2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 A4:G27 AA18:AA29 W4:AB13 AB14:AB30 BI4:BM30 AW4:BA16 BD4:BH16 AC4:AV30 BB4 AW17:BH30">
-    <cfRule type="expression" dxfId="34" priority="31" stopIfTrue="1">
+  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 A4:G27 AA18:AA29 W4:AB13 AB14:AB30 BK4:BO30 BF4:BJ16 AC4:AX30 BD4 AY4:AY29 BC4:BC16 BC17:BJ28 AY30:AZ30 BA29:BJ30 BA4:BA28">
+    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="36" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28">
-    <cfRule type="expression" dxfId="32" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="33" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="34" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA16:AA17">
-    <cfRule type="expression" dxfId="30" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="47" stopIfTrue="1">
       <formula>$A15="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="48" stopIfTrue="1">
       <formula>$A15="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA15">
-    <cfRule type="expression" dxfId="28" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="19" stopIfTrue="1">
       <formula>$A14="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="20" stopIfTrue="1">
       <formula>$A14="p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BB5:BB16">
-    <cfRule type="expression" dxfId="26" priority="13" stopIfTrue="1">
+  <conditionalFormatting sqref="BD5:BD16">
+    <cfRule type="expression" dxfId="24" priority="17" stopIfTrue="1">
       <formula>$A5="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="18" stopIfTrue="1">
       <formula>$A5="p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BC4:BC16">
-    <cfRule type="expression" dxfId="24" priority="11" stopIfTrue="1">
+  <conditionalFormatting sqref="BE4:BE16">
+    <cfRule type="expression" dxfId="22" priority="15" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="16" stopIfTrue="1">
+      <formula>$A4="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AZ4:AZ29">
+    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
+      <formula>$A4="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="4" stopIfTrue="1">
+      <formula>$A4="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB4:BB28">
+    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
+      <formula>$A4="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10645,74 +10687,74 @@
   <sheetData>
     <row r="1" spans="1:55" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:55" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="163" t="s">
+      <c r="B2" s="166" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="157" t="s">
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="168"/>
+      <c r="I2" s="160" t="s">
         <v>1062</v>
       </c>
-      <c r="J2" s="158"/>
-      <c r="K2" s="166"/>
-      <c r="L2" s="166"/>
-      <c r="M2" s="166"/>
-      <c r="N2" s="166"/>
-      <c r="O2" s="166"/>
-      <c r="P2" s="166"/>
-      <c r="Q2" s="166"/>
-      <c r="R2" s="166"/>
-      <c r="S2" s="166"/>
-      <c r="T2" s="167"/>
-      <c r="U2" s="168" t="s">
+      <c r="J2" s="161"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="169"/>
+      <c r="R2" s="169"/>
+      <c r="S2" s="169"/>
+      <c r="T2" s="170"/>
+      <c r="U2" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="169"/>
-      <c r="W2" s="169"/>
-      <c r="X2" s="169"/>
-      <c r="Y2" s="169"/>
-      <c r="Z2" s="169"/>
-      <c r="AA2" s="169"/>
-      <c r="AB2" s="169"/>
-      <c r="AC2" s="169"/>
-      <c r="AD2" s="169"/>
-      <c r="AE2" s="169"/>
-      <c r="AF2" s="169"/>
-      <c r="AG2" s="169"/>
-      <c r="AH2" s="169"/>
-      <c r="AI2" s="169"/>
-      <c r="AJ2" s="170"/>
-      <c r="AK2" s="174" t="s">
+      <c r="V2" s="172"/>
+      <c r="W2" s="172"/>
+      <c r="X2" s="172"/>
+      <c r="Y2" s="172"/>
+      <c r="Z2" s="172"/>
+      <c r="AA2" s="172"/>
+      <c r="AB2" s="172"/>
+      <c r="AC2" s="172"/>
+      <c r="AD2" s="172"/>
+      <c r="AE2" s="172"/>
+      <c r="AF2" s="172"/>
+      <c r="AG2" s="172"/>
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="173"/>
+      <c r="AK2" s="183" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="172"/>
-      <c r="AM2" s="172"/>
-      <c r="AN2" s="172"/>
-      <c r="AO2" s="172"/>
-      <c r="AP2" s="173"/>
-      <c r="AQ2" s="174" t="s">
+      <c r="AL2" s="175"/>
+      <c r="AM2" s="175"/>
+      <c r="AN2" s="175"/>
+      <c r="AO2" s="175"/>
+      <c r="AP2" s="176"/>
+      <c r="AQ2" s="183" t="s">
         <v>1061</v>
       </c>
-      <c r="AR2" s="171"/>
-      <c r="AS2" s="171"/>
-      <c r="AT2" s="175"/>
-      <c r="AU2" s="176" t="s">
+      <c r="AR2" s="174"/>
+      <c r="AS2" s="174"/>
+      <c r="AT2" s="184"/>
+      <c r="AU2" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="AV2" s="177"/>
-      <c r="AW2" s="177"/>
-      <c r="AX2" s="178"/>
-      <c r="AY2" s="157" t="s">
+      <c r="AV2" s="181"/>
+      <c r="AW2" s="181"/>
+      <c r="AX2" s="182"/>
+      <c r="AY2" s="160" t="s">
         <v>1047</v>
       </c>
-      <c r="AZ2" s="158"/>
-      <c r="BA2" s="158"/>
-      <c r="BB2" s="158"/>
-      <c r="BC2" s="159"/>
+      <c r="AZ2" s="161"/>
+      <c r="BA2" s="161"/>
+      <c r="BB2" s="161"/>
+      <c r="BC2" s="162"/>
     </row>
     <row r="3" spans="1:55" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -10895,7 +10937,7 @@
       <c r="G4" s="28" t="s">
         <v>497</v>
       </c>
-      <c r="H4" s="179" t="s">
+      <c r="H4" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I4" s="109" t="s">
@@ -11055,7 +11097,7 @@
       <c r="G5" s="39" t="s">
         <v>498</v>
       </c>
-      <c r="H5" s="180" t="s">
+      <c r="H5" s="156" t="s">
         <v>32</v>
       </c>
       <c r="I5" s="110" t="s">
@@ -11215,7 +11257,7 @@
       <c r="G6" s="39" t="s">
         <v>491</v>
       </c>
-      <c r="H6" s="179" t="s">
+      <c r="H6" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I6" s="110" t="s">
@@ -11375,7 +11417,7 @@
       <c r="G7" s="39" t="s">
         <v>492</v>
       </c>
-      <c r="H7" s="179" t="s">
+      <c r="H7" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I7" s="110" t="s">
@@ -11535,7 +11577,7 @@
       <c r="G8" s="39" t="s">
         <v>499</v>
       </c>
-      <c r="H8" s="179" t="s">
+      <c r="H8" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I8" s="110" t="s">
@@ -11696,7 +11738,7 @@
       <c r="G9" s="39" t="s">
         <v>499</v>
       </c>
-      <c r="H9" s="179" t="s">
+      <c r="H9" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I9" s="110" t="s">
@@ -11857,7 +11899,7 @@
       <c r="G10" s="39" t="s">
         <v>492</v>
       </c>
-      <c r="H10" s="179" t="s">
+      <c r="H10" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I10" s="110" t="s">
@@ -12018,7 +12060,7 @@
       <c r="G11" s="28" t="s">
         <v>497</v>
       </c>
-      <c r="H11" s="179" t="s">
+      <c r="H11" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I11" s="110" t="s">
@@ -12178,7 +12220,7 @@
       <c r="G12" s="39" t="s">
         <v>493</v>
       </c>
-      <c r="H12" s="179" t="s">
+      <c r="H12" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I12" s="110" t="s">
@@ -12338,7 +12380,7 @@
       <c r="G13" s="39" t="s">
         <v>496</v>
       </c>
-      <c r="H13" s="179" t="s">
+      <c r="H13" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I13" s="110" t="s">
@@ -12498,7 +12540,7 @@
       <c r="G14" s="39" t="s">
         <v>500</v>
       </c>
-      <c r="H14" s="179" t="s">
+      <c r="H14" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I14" s="110" t="s">
@@ -12658,7 +12700,7 @@
       <c r="G15" s="39" t="s">
         <v>494</v>
       </c>
-      <c r="H15" s="179" t="s">
+      <c r="H15" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I15" s="110" t="s">
@@ -12818,7 +12860,7 @@
       <c r="G16" s="39" t="s">
         <v>495</v>
       </c>
-      <c r="H16" s="179" t="s">
+      <c r="H16" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I16" s="110" t="s">
@@ -12978,7 +13020,7 @@
       <c r="G17" s="108" t="s">
         <v>501</v>
       </c>
-      <c r="H17" s="180" t="s">
+      <c r="H17" s="156" t="s">
         <v>22</v>
       </c>
       <c r="I17" s="110" t="s">
@@ -13138,7 +13180,7 @@
       <c r="G18" s="39" t="s">
         <v>502</v>
       </c>
-      <c r="H18" s="179" t="s">
+      <c r="H18" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I18" s="110" t="s">
@@ -13298,7 +13340,7 @@
       <c r="G19" s="39" t="s">
         <v>503</v>
       </c>
-      <c r="H19" s="179" t="s">
+      <c r="H19" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I19" s="110" t="s">
@@ -13458,7 +13500,7 @@
       <c r="G20" s="39" t="s">
         <v>504</v>
       </c>
-      <c r="H20" s="179" t="s">
+      <c r="H20" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I20" s="110" t="s">
@@ -13616,7 +13658,7 @@
       <c r="G21" s="39" t="s">
         <v>1074</v>
       </c>
-      <c r="H21" s="179" t="s">
+      <c r="H21" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I21" s="110" t="s">
@@ -13759,7 +13801,7 @@
       <c r="G22" s="39" t="s">
         <v>1076</v>
       </c>
-      <c r="H22" s="179" t="s">
+      <c r="H22" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I22" s="110" t="s">
@@ -13844,7 +13886,7 @@
       <c r="G23" s="39" t="s">
         <v>1075</v>
       </c>
-      <c r="H23" s="179" t="s">
+      <c r="H23" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I23" s="110" t="s">
@@ -13925,7 +13967,7 @@
       <c r="G24" s="39" t="s">
         <v>1072</v>
       </c>
-      <c r="H24" s="179" t="s">
+      <c r="H24" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I24" s="110" t="s">
@@ -14006,7 +14048,7 @@
       <c r="G25" s="39" t="s">
         <v>1066</v>
       </c>
-      <c r="H25" s="179" t="s">
+      <c r="H25" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I25" s="110" t="s">
@@ -14091,7 +14133,7 @@
       <c r="G26" s="39" t="s">
         <v>1080</v>
       </c>
-      <c r="H26" s="179" t="s">
+      <c r="H26" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I26" s="110" t="s">
@@ -14176,7 +14218,7 @@
       <c r="G27" s="39" t="s">
         <v>1077</v>
       </c>
-      <c r="H27" s="179" t="s">
+      <c r="H27" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I27" s="110" t="s">
@@ -14261,7 +14303,7 @@
       <c r="G28" s="39" t="s">
         <v>1079</v>
       </c>
-      <c r="H28" s="179" t="s">
+      <c r="H28" s="155" t="s">
         <v>32</v>
       </c>
       <c r="I28" s="110" t="s">

</xml_diff>

<commit_message>
added UA coefficients for 5MW airfoils; did not use rrd's latest (with some different comments) added AD15 test cases (i.e., cert test run with AD15 instead of AD14): needs some work as I currently get lots of brent warnings and the SWRT multiple table option is not yet supported in AFI. commented out the additional tables in the SWRT airfoil files modified tests 3,6,9,10, and 15 with correct value for AFAeroMod modified location of last blade element in AD15 for UAE and WP_Baseline (both were just a teeny bit longer than the ED blade and were causing mesh mapping errors because the last node didn't project onto an element on the other mesh)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1046 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2911" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2954" uniqueCount="1141">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -4617,6 +4617,18 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4692,24 +4704,96 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -4778,34 +4862,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -5292,10 +5348,10 @@
   <dimension ref="A1:BO61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="AP4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="AM16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BA4" sqref="BA4"/>
+      <selection pane="bottomRight" activeCell="AS22" sqref="AS22:AT28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5331,7 +5387,7 @@
     <col min="50" max="51" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="5.33203125" style="45" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="5.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="3.33203125" style="185" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="3.33203125" style="160" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="4.88671875" style="2" customWidth="1"/>
     <col min="57" max="57" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
@@ -5347,88 +5403,88 @@
   <sheetData>
     <row r="1" spans="1:67" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:67" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="166" t="s">
+      <c r="B2" s="172" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="168"/>
-      <c r="H2" s="163" t="s">
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="173"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="169" t="s">
         <v>1104</v>
       </c>
-      <c r="I2" s="164"/>
-      <c r="J2" s="164"/>
-      <c r="K2" s="164"/>
-      <c r="L2" s="164"/>
-      <c r="M2" s="164"/>
-      <c r="N2" s="164"/>
-      <c r="O2" s="164"/>
-      <c r="P2" s="164"/>
-      <c r="Q2" s="164"/>
-      <c r="R2" s="164"/>
-      <c r="S2" s="164"/>
-      <c r="T2" s="164"/>
-      <c r="U2" s="164"/>
-      <c r="V2" s="165"/>
-      <c r="W2" s="161" t="s">
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
+      <c r="K2" s="170"/>
+      <c r="L2" s="170"/>
+      <c r="M2" s="170"/>
+      <c r="N2" s="170"/>
+      <c r="O2" s="170"/>
+      <c r="P2" s="170"/>
+      <c r="Q2" s="170"/>
+      <c r="R2" s="170"/>
+      <c r="S2" s="170"/>
+      <c r="T2" s="170"/>
+      <c r="U2" s="170"/>
+      <c r="V2" s="171"/>
+      <c r="W2" s="167" t="s">
         <v>1110</v>
       </c>
-      <c r="X2" s="169"/>
-      <c r="Y2" s="169"/>
-      <c r="Z2" s="169"/>
-      <c r="AA2" s="169"/>
-      <c r="AB2" s="169"/>
-      <c r="AC2" s="169"/>
-      <c r="AD2" s="170"/>
-      <c r="AE2" s="171" t="s">
+      <c r="X2" s="175"/>
+      <c r="Y2" s="175"/>
+      <c r="Z2" s="175"/>
+      <c r="AA2" s="175"/>
+      <c r="AB2" s="175"/>
+      <c r="AC2" s="175"/>
+      <c r="AD2" s="176"/>
+      <c r="AE2" s="177" t="s">
         <v>1126</v>
       </c>
-      <c r="AF2" s="172"/>
-      <c r="AG2" s="172"/>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="172"/>
-      <c r="AK2" s="172"/>
-      <c r="AL2" s="172"/>
-      <c r="AM2" s="172"/>
-      <c r="AN2" s="172"/>
-      <c r="AO2" s="172"/>
-      <c r="AP2" s="173"/>
-      <c r="AQ2" s="174" t="s">
+      <c r="AF2" s="178"/>
+      <c r="AG2" s="178"/>
+      <c r="AH2" s="178"/>
+      <c r="AI2" s="178"/>
+      <c r="AJ2" s="178"/>
+      <c r="AK2" s="178"/>
+      <c r="AL2" s="178"/>
+      <c r="AM2" s="178"/>
+      <c r="AN2" s="178"/>
+      <c r="AO2" s="178"/>
+      <c r="AP2" s="179"/>
+      <c r="AQ2" s="180" t="s">
         <v>1130</v>
       </c>
-      <c r="AR2" s="175"/>
-      <c r="AS2" s="175"/>
-      <c r="AT2" s="175"/>
-      <c r="AU2" s="175"/>
-      <c r="AV2" s="175"/>
-      <c r="AW2" s="175"/>
-      <c r="AX2" s="176"/>
-      <c r="AY2" s="180" t="s">
+      <c r="AR2" s="181"/>
+      <c r="AS2" s="181"/>
+      <c r="AT2" s="181"/>
+      <c r="AU2" s="181"/>
+      <c r="AV2" s="181"/>
+      <c r="AW2" s="181"/>
+      <c r="AX2" s="182"/>
+      <c r="AY2" s="186" t="s">
         <v>1138</v>
       </c>
-      <c r="AZ2" s="181"/>
-      <c r="BA2" s="181"/>
-      <c r="BB2" s="181"/>
-      <c r="BC2" s="182"/>
-      <c r="BD2" s="177" t="s">
+      <c r="AZ2" s="187"/>
+      <c r="BA2" s="187"/>
+      <c r="BB2" s="187"/>
+      <c r="BC2" s="188"/>
+      <c r="BD2" s="183" t="s">
         <v>1129</v>
       </c>
-      <c r="BE2" s="178"/>
-      <c r="BF2" s="178"/>
-      <c r="BG2" s="178"/>
-      <c r="BH2" s="178"/>
-      <c r="BI2" s="178"/>
-      <c r="BJ2" s="179"/>
-      <c r="BK2" s="160" t="s">
+      <c r="BE2" s="184"/>
+      <c r="BF2" s="184"/>
+      <c r="BG2" s="184"/>
+      <c r="BH2" s="184"/>
+      <c r="BI2" s="184"/>
+      <c r="BJ2" s="185"/>
+      <c r="BK2" s="166" t="s">
         <v>1047</v>
       </c>
-      <c r="BL2" s="161"/>
-      <c r="BM2" s="161"/>
-      <c r="BN2" s="161"/>
-      <c r="BO2" s="162"/>
+      <c r="BL2" s="167"/>
+      <c r="BM2" s="167"/>
+      <c r="BN2" s="167"/>
+      <c r="BO2" s="168"/>
     </row>
     <row r="3" spans="1:67" s="1" customFormat="1" ht="88.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
@@ -5582,10 +5638,10 @@
       <c r="AY3" s="75" t="s">
         <v>1139</v>
       </c>
-      <c r="AZ3" s="189" t="s">
+      <c r="AZ3" s="164" t="s">
         <v>1132</v>
       </c>
-      <c r="BA3" s="190" t="s">
+      <c r="BA3" s="165" t="s">
         <v>1140</v>
       </c>
       <c r="BB3" s="77" t="s">
@@ -7527,7 +7583,7 @@
       <c r="AZ13" s="151">
         <v>0</v>
       </c>
-      <c r="BA13" s="188" t="s">
+      <c r="BA13" s="163" t="s">
         <v>1133</v>
       </c>
       <c r="BB13" s="44">
@@ -7912,10 +7968,10 @@
       <c r="AY15" s="43">
         <v>2</v>
       </c>
-      <c r="AZ15" s="188" t="s">
+      <c r="AZ15" s="163" t="s">
         <v>1134</v>
       </c>
-      <c r="BA15" s="188" t="s">
+      <c r="BA15" s="163" t="s">
         <v>1135</v>
       </c>
       <c r="BB15" s="44">
@@ -8372,7 +8428,7 @@
       <c r="AZ18" s="151">
         <v>0</v>
       </c>
-      <c r="BA18" s="188" t="s">
+      <c r="BA18" s="163" t="s">
         <v>1136</v>
       </c>
       <c r="BB18" s="44">
@@ -8563,7 +8619,7 @@
       <c r="AY19" s="43">
         <v>2</v>
       </c>
-      <c r="AZ19" s="188" t="s">
+      <c r="AZ19" s="163" t="s">
         <v>1137</v>
       </c>
       <c r="BA19" s="151">
@@ -8942,7 +8998,9 @@
       <c r="AV21" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AW21" s="41"/>
+      <c r="AW21" s="41" t="s">
+        <v>22</v>
+      </c>
       <c r="AX21" s="42"/>
       <c r="AY21" s="43">
         <v>3</v>
@@ -9101,13 +9159,25 @@
       <c r="AP22" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AQ22" s="43"/>
-      <c r="AR22" s="25"/>
-      <c r="AS22" s="41"/>
-      <c r="AT22" s="41"/>
-      <c r="AU22" s="41"/>
+      <c r="AQ22" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR22" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS22" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT22" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU22" s="41" t="s">
+        <v>32</v>
+      </c>
       <c r="AV22" s="41"/>
-      <c r="AW22" s="41"/>
+      <c r="AW22" s="41" t="s">
+        <v>22</v>
+      </c>
       <c r="AX22" s="42"/>
       <c r="AY22" s="43">
         <v>3</v>
@@ -9266,13 +9336,25 @@
       <c r="AP23" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AQ23" s="43"/>
-      <c r="AR23" s="25"/>
-      <c r="AS23" s="41"/>
-      <c r="AT23" s="41"/>
-      <c r="AU23" s="41"/>
+      <c r="AQ23" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR23" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS23" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT23" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU23" s="41" t="s">
+        <v>32</v>
+      </c>
       <c r="AV23" s="41"/>
-      <c r="AW23" s="41"/>
+      <c r="AW23" s="41" t="s">
+        <v>22</v>
+      </c>
       <c r="AX23" s="42"/>
       <c r="AY23" s="43">
         <v>1</v>
@@ -9431,13 +9513,25 @@
       <c r="AP24" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AQ24" s="43"/>
-      <c r="AR24" s="25"/>
-      <c r="AS24" s="41"/>
-      <c r="AT24" s="41"/>
-      <c r="AU24" s="41"/>
+      <c r="AQ24" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR24" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS24" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT24" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU24" s="41" t="s">
+        <v>32</v>
+      </c>
       <c r="AV24" s="41"/>
-      <c r="AW24" s="41"/>
+      <c r="AW24" s="41" t="s">
+        <v>22</v>
+      </c>
       <c r="AX24" s="42"/>
       <c r="AY24" s="43">
         <v>3</v>
@@ -9596,13 +9690,25 @@
       <c r="AP25" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AQ25" s="43"/>
-      <c r="AR25" s="25"/>
-      <c r="AS25" s="41"/>
-      <c r="AT25" s="41"/>
-      <c r="AU25" s="41"/>
+      <c r="AQ25" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR25" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS25" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT25" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU25" s="41" t="s">
+        <v>32</v>
+      </c>
       <c r="AV25" s="41"/>
-      <c r="AW25" s="41"/>
+      <c r="AW25" s="41" t="s">
+        <v>22</v>
+      </c>
       <c r="AX25" s="42"/>
       <c r="AY25" s="43">
         <v>3</v>
@@ -9761,13 +9867,25 @@
       <c r="AP26" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AQ26" s="43"/>
-      <c r="AR26" s="25"/>
-      <c r="AS26" s="41"/>
-      <c r="AT26" s="41"/>
-      <c r="AU26" s="41"/>
+      <c r="AQ26" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR26" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS26" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT26" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU26" s="41" t="s">
+        <v>32</v>
+      </c>
       <c r="AV26" s="41"/>
-      <c r="AW26" s="41"/>
+      <c r="AW26" s="41" t="s">
+        <v>22</v>
+      </c>
       <c r="AX26" s="42"/>
       <c r="AY26" s="43">
         <v>3</v>
@@ -9926,13 +10044,25 @@
       <c r="AP27" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AQ27" s="43"/>
-      <c r="AR27" s="25"/>
-      <c r="AS27" s="41"/>
-      <c r="AT27" s="41"/>
-      <c r="AU27" s="41"/>
+      <c r="AQ27" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR27" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS27" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT27" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU27" s="41" t="s">
+        <v>32</v>
+      </c>
       <c r="AV27" s="41"/>
-      <c r="AW27" s="41"/>
+      <c r="AW27" s="41" t="s">
+        <v>22</v>
+      </c>
       <c r="AX27" s="42"/>
       <c r="AY27" s="43">
         <v>3</v>
@@ -10091,13 +10221,25 @@
       <c r="AP28" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="AQ28" s="43"/>
-      <c r="AR28" s="25"/>
-      <c r="AS28" s="41"/>
-      <c r="AT28" s="41"/>
-      <c r="AU28" s="41"/>
+      <c r="AQ28" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR28" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS28" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT28" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU28" s="41" t="s">
+        <v>32</v>
+      </c>
       <c r="AV28" s="41"/>
-      <c r="AW28" s="41"/>
+      <c r="AW28" s="41" t="s">
+        <v>22</v>
+      </c>
       <c r="AX28" s="42"/>
       <c r="AY28" s="43">
         <v>1</v>
@@ -10192,7 +10334,7 @@
       <c r="AY29" s="7"/>
       <c r="AZ29" s="153"/>
       <c r="BA29" s="153"/>
-      <c r="BB29" s="186"/>
+      <c r="BB29" s="161"/>
       <c r="BC29" s="6"/>
       <c r="BD29" s="100"/>
       <c r="BE29" s="8"/>
@@ -10211,7 +10353,7 @@
       <c r="AY33" s="9"/>
       <c r="AZ33" s="2"/>
       <c r="BA33" s="2"/>
-      <c r="BB33" s="187"/>
+      <c r="BB33" s="162"/>
       <c r="BC33" s="45"/>
       <c r="BJ33" s="45"/>
       <c r="BK33" s="45"/>
@@ -10223,7 +10365,7 @@
       <c r="AY34" s="9"/>
       <c r="AZ34" s="2"/>
       <c r="BA34" s="2"/>
-      <c r="BB34" s="187"/>
+      <c r="BB34" s="162"/>
       <c r="BC34" s="45"/>
       <c r="BJ34" s="45"/>
       <c r="BK34" s="45"/>
@@ -10235,7 +10377,7 @@
       <c r="AY35" s="9"/>
       <c r="AZ35" s="2"/>
       <c r="BA35" s="2"/>
-      <c r="BB35" s="187"/>
+      <c r="BB35" s="162"/>
       <c r="BC35" s="45"/>
       <c r="BJ35" s="45"/>
       <c r="BK35" s="45"/>
@@ -10247,7 +10389,7 @@
       <c r="AY36" s="9"/>
       <c r="AZ36" s="2"/>
       <c r="BA36" s="2"/>
-      <c r="BB36" s="187"/>
+      <c r="BB36" s="162"/>
       <c r="BC36" s="45"/>
       <c r="BJ36" s="45"/>
       <c r="BK36" s="45"/>
@@ -10259,7 +10401,7 @@
       <c r="AY37" s="9"/>
       <c r="AZ37" s="2"/>
       <c r="BA37" s="2"/>
-      <c r="BB37" s="187"/>
+      <c r="BB37" s="162"/>
       <c r="BC37" s="45"/>
       <c r="BJ37" s="45"/>
       <c r="BK37" s="45"/>
@@ -10271,7 +10413,7 @@
       <c r="AY38" s="9"/>
       <c r="AZ38" s="2"/>
       <c r="BA38" s="2"/>
-      <c r="BB38" s="187"/>
+      <c r="BB38" s="162"/>
       <c r="BC38" s="45"/>
       <c r="BJ38" s="45"/>
       <c r="BK38" s="45"/>
@@ -10283,7 +10425,7 @@
       <c r="AY39" s="9"/>
       <c r="AZ39" s="2"/>
       <c r="BA39" s="2"/>
-      <c r="BB39" s="187"/>
+      <c r="BB39" s="162"/>
       <c r="BC39" s="45"/>
       <c r="BJ39" s="45"/>
       <c r="BK39" s="45"/>
@@ -10295,7 +10437,7 @@
       <c r="AY40" s="9"/>
       <c r="AZ40" s="2"/>
       <c r="BA40" s="2"/>
-      <c r="BB40" s="187"/>
+      <c r="BB40" s="162"/>
       <c r="BC40" s="45"/>
       <c r="BJ40" s="45"/>
       <c r="BK40" s="45"/>
@@ -10307,7 +10449,7 @@
       <c r="AY41" s="9"/>
       <c r="AZ41" s="2"/>
       <c r="BA41" s="2"/>
-      <c r="BB41" s="187"/>
+      <c r="BB41" s="162"/>
       <c r="BC41" s="45"/>
       <c r="BJ41" s="45"/>
       <c r="BK41" s="45"/>
@@ -10319,7 +10461,7 @@
       <c r="AY42" s="9"/>
       <c r="AZ42" s="2"/>
       <c r="BA42" s="2"/>
-      <c r="BB42" s="187"/>
+      <c r="BB42" s="162"/>
       <c r="BC42" s="45"/>
       <c r="BJ42" s="45"/>
       <c r="BK42" s="45"/>
@@ -10331,7 +10473,7 @@
       <c r="AY43" s="9"/>
       <c r="AZ43" s="2"/>
       <c r="BA43" s="2"/>
-      <c r="BB43" s="187"/>
+      <c r="BB43" s="162"/>
       <c r="BC43" s="45"/>
       <c r="BJ43" s="45"/>
       <c r="BK43" s="45"/>
@@ -10343,7 +10485,7 @@
       <c r="AY44" s="9"/>
       <c r="AZ44" s="2"/>
       <c r="BA44" s="2"/>
-      <c r="BB44" s="187"/>
+      <c r="BB44" s="162"/>
       <c r="BC44" s="45"/>
       <c r="BJ44" s="45"/>
       <c r="BK44" s="45"/>
@@ -10355,7 +10497,7 @@
       <c r="AY45" s="9"/>
       <c r="AZ45" s="2"/>
       <c r="BA45" s="2"/>
-      <c r="BB45" s="187"/>
+      <c r="BB45" s="162"/>
       <c r="BC45" s="45"/>
       <c r="BJ45" s="45"/>
       <c r="BK45" s="45"/>
@@ -10367,7 +10509,7 @@
       <c r="AY46" s="9"/>
       <c r="AZ46" s="2"/>
       <c r="BA46" s="2"/>
-      <c r="BB46" s="187"/>
+      <c r="BB46" s="162"/>
       <c r="BC46" s="45"/>
       <c r="BJ46" s="45"/>
       <c r="BK46" s="45"/>
@@ -10379,7 +10521,7 @@
       <c r="AY47" s="9"/>
       <c r="AZ47" s="2"/>
       <c r="BA47" s="2"/>
-      <c r="BB47" s="187"/>
+      <c r="BB47" s="162"/>
       <c r="BC47" s="45"/>
       <c r="BJ47" s="45"/>
       <c r="BK47" s="45"/>
@@ -10391,7 +10533,7 @@
       <c r="AY48" s="9"/>
       <c r="AZ48" s="2"/>
       <c r="BA48" s="2"/>
-      <c r="BB48" s="187"/>
+      <c r="BB48" s="162"/>
       <c r="BC48" s="45"/>
       <c r="BJ48" s="45"/>
       <c r="BK48" s="45"/>
@@ -10403,7 +10545,7 @@
       <c r="AY49" s="9"/>
       <c r="AZ49" s="2"/>
       <c r="BA49" s="2"/>
-      <c r="BB49" s="187"/>
+      <c r="BB49" s="162"/>
       <c r="BC49" s="45"/>
       <c r="BJ49" s="45"/>
       <c r="BK49" s="45"/>
@@ -10415,7 +10557,7 @@
       <c r="AY50" s="9"/>
       <c r="AZ50" s="2"/>
       <c r="BA50" s="2"/>
-      <c r="BB50" s="187"/>
+      <c r="BB50" s="162"/>
       <c r="BC50" s="45"/>
       <c r="BJ50" s="45"/>
       <c r="BK50" s="45"/>
@@ -10427,7 +10569,7 @@
       <c r="AY51" s="9"/>
       <c r="AZ51" s="2"/>
       <c r="BA51" s="2"/>
-      <c r="BB51" s="187"/>
+      <c r="BB51" s="162"/>
       <c r="BC51" s="45"/>
       <c r="BJ51" s="45"/>
       <c r="BK51" s="45"/>
@@ -10439,7 +10581,7 @@
       <c r="AY52" s="9"/>
       <c r="AZ52" s="2"/>
       <c r="BA52" s="2"/>
-      <c r="BB52" s="187"/>
+      <c r="BB52" s="162"/>
       <c r="BC52" s="45"/>
       <c r="BJ52" s="45"/>
       <c r="BK52" s="45"/>
@@ -10451,7 +10593,7 @@
       <c r="AY53" s="9"/>
       <c r="AZ53" s="2"/>
       <c r="BA53" s="2"/>
-      <c r="BB53" s="187"/>
+      <c r="BB53" s="162"/>
       <c r="BC53" s="45"/>
       <c r="BJ53" s="45"/>
       <c r="BK53" s="45"/>
@@ -10463,7 +10605,7 @@
       <c r="AY54" s="9"/>
       <c r="AZ54" s="2"/>
       <c r="BA54" s="2"/>
-      <c r="BB54" s="187"/>
+      <c r="BB54" s="162"/>
       <c r="BC54" s="45"/>
       <c r="BJ54" s="45"/>
       <c r="BK54" s="45"/>
@@ -10475,7 +10617,7 @@
       <c r="AY55" s="9"/>
       <c r="AZ55" s="2"/>
       <c r="BA55" s="2"/>
-      <c r="BB55" s="187"/>
+      <c r="BB55" s="162"/>
       <c r="BC55" s="45"/>
       <c r="BJ55" s="45"/>
       <c r="BK55" s="45"/>
@@ -10487,7 +10629,7 @@
       <c r="AY56" s="9"/>
       <c r="AZ56" s="2"/>
       <c r="BA56" s="2"/>
-      <c r="BB56" s="187"/>
+      <c r="BB56" s="162"/>
       <c r="BC56" s="45"/>
       <c r="BJ56" s="45"/>
       <c r="BK56" s="45"/>
@@ -10499,7 +10641,7 @@
       <c r="AY57" s="9"/>
       <c r="AZ57" s="2"/>
       <c r="BA57" s="2"/>
-      <c r="BB57" s="187"/>
+      <c r="BB57" s="162"/>
       <c r="BC57" s="45"/>
       <c r="BJ57" s="45"/>
       <c r="BK57" s="45"/>
@@ -10511,7 +10653,7 @@
       <c r="AY58" s="9"/>
       <c r="AZ58" s="2"/>
       <c r="BA58" s="2"/>
-      <c r="BB58" s="187"/>
+      <c r="BB58" s="162"/>
       <c r="BC58" s="45"/>
       <c r="BJ58" s="45"/>
       <c r="BK58" s="45"/>
@@ -10523,7 +10665,7 @@
       <c r="AY59" s="9"/>
       <c r="AZ59" s="2"/>
       <c r="BA59" s="2"/>
-      <c r="BB59" s="187"/>
+      <c r="BB59" s="162"/>
       <c r="BC59" s="45"/>
       <c r="BJ59" s="45"/>
       <c r="BK59" s="45"/>
@@ -10535,7 +10677,7 @@
       <c r="AY60" s="9"/>
       <c r="AZ60" s="2"/>
       <c r="BA60" s="2"/>
-      <c r="BB60" s="187"/>
+      <c r="BB60" s="162"/>
       <c r="BC60" s="45"/>
       <c r="BJ60" s="45"/>
       <c r="BK60" s="45"/>
@@ -10547,7 +10689,7 @@
       <c r="AY61" s="9"/>
       <c r="AZ61" s="2"/>
       <c r="BA61" s="2"/>
-      <c r="BB61" s="187"/>
+      <c r="BB61" s="162"/>
       <c r="BC61" s="45"/>
       <c r="BJ61" s="45"/>
       <c r="BK61" s="45"/>
@@ -10566,67 +10708,67 @@
     <mergeCell ref="BD2:BJ2"/>
     <mergeCell ref="AY2:BC2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 A4:G27 AA18:AA29 W4:AB13 AB14:AB30 BK4:BO30 BF4:BJ16 AC4:AX30 BD4 AY4:AY29 BC4:BC16 BC17:BJ28 AY30:AZ30 BA29:BJ30 BA4:BA28">
-    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
+  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 A4:G27 AA18:AA29 W4:AB13 AB14:AB30 BK4:BO30 BF4:BJ16 BD4 AY4:AY29 BC4:BC16 BC17:BJ28 AY30:AZ30 BA29:BJ30 BA4:BA28 AC4:AX30">
+    <cfRule type="expression" dxfId="44" priority="35" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="36" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28">
-    <cfRule type="expression" dxfId="30" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="33" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="34" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA16:AA17">
-    <cfRule type="expression" dxfId="28" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="47" stopIfTrue="1">
       <formula>$A15="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="48" stopIfTrue="1">
       <formula>$A15="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA15">
-    <cfRule type="expression" dxfId="26" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="19" stopIfTrue="1">
       <formula>$A14="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="20" stopIfTrue="1">
       <formula>$A14="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD5:BD16">
-    <cfRule type="expression" dxfId="24" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="17" stopIfTrue="1">
       <formula>$A5="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="18" stopIfTrue="1">
       <formula>$A5="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE4:BE16">
-    <cfRule type="expression" dxfId="22" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="15" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="16" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ4:AZ29">
-    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="3" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="4" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB4:BB28">
-    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="1" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="2" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10687,74 +10829,74 @@
   <sheetData>
     <row r="1" spans="1:55" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:55" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="166" t="s">
+      <c r="B2" s="172" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="167"/>
-      <c r="H2" s="168"/>
-      <c r="I2" s="160" t="s">
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="173"/>
+      <c r="G2" s="173"/>
+      <c r="H2" s="174"/>
+      <c r="I2" s="166" t="s">
         <v>1062</v>
       </c>
-      <c r="J2" s="161"/>
-      <c r="K2" s="169"/>
-      <c r="L2" s="169"/>
-      <c r="M2" s="169"/>
-      <c r="N2" s="169"/>
-      <c r="O2" s="169"/>
-      <c r="P2" s="169"/>
-      <c r="Q2" s="169"/>
-      <c r="R2" s="169"/>
-      <c r="S2" s="169"/>
-      <c r="T2" s="170"/>
-      <c r="U2" s="171" t="s">
+      <c r="J2" s="167"/>
+      <c r="K2" s="175"/>
+      <c r="L2" s="175"/>
+      <c r="M2" s="175"/>
+      <c r="N2" s="175"/>
+      <c r="O2" s="175"/>
+      <c r="P2" s="175"/>
+      <c r="Q2" s="175"/>
+      <c r="R2" s="175"/>
+      <c r="S2" s="175"/>
+      <c r="T2" s="176"/>
+      <c r="U2" s="177" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="172"/>
-      <c r="W2" s="172"/>
-      <c r="X2" s="172"/>
-      <c r="Y2" s="172"/>
-      <c r="Z2" s="172"/>
-      <c r="AA2" s="172"/>
-      <c r="AB2" s="172"/>
-      <c r="AC2" s="172"/>
-      <c r="AD2" s="172"/>
-      <c r="AE2" s="172"/>
-      <c r="AF2" s="172"/>
-      <c r="AG2" s="172"/>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="173"/>
-      <c r="AK2" s="183" t="s">
+      <c r="V2" s="178"/>
+      <c r="W2" s="178"/>
+      <c r="X2" s="178"/>
+      <c r="Y2" s="178"/>
+      <c r="Z2" s="178"/>
+      <c r="AA2" s="178"/>
+      <c r="AB2" s="178"/>
+      <c r="AC2" s="178"/>
+      <c r="AD2" s="178"/>
+      <c r="AE2" s="178"/>
+      <c r="AF2" s="178"/>
+      <c r="AG2" s="178"/>
+      <c r="AH2" s="178"/>
+      <c r="AI2" s="178"/>
+      <c r="AJ2" s="179"/>
+      <c r="AK2" s="189" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="175"/>
-      <c r="AM2" s="175"/>
-      <c r="AN2" s="175"/>
-      <c r="AO2" s="175"/>
-      <c r="AP2" s="176"/>
-      <c r="AQ2" s="183" t="s">
+      <c r="AL2" s="181"/>
+      <c r="AM2" s="181"/>
+      <c r="AN2" s="181"/>
+      <c r="AO2" s="181"/>
+      <c r="AP2" s="182"/>
+      <c r="AQ2" s="189" t="s">
         <v>1061</v>
       </c>
-      <c r="AR2" s="174"/>
-      <c r="AS2" s="174"/>
-      <c r="AT2" s="184"/>
-      <c r="AU2" s="180" t="s">
+      <c r="AR2" s="180"/>
+      <c r="AS2" s="180"/>
+      <c r="AT2" s="190"/>
+      <c r="AU2" s="186" t="s">
         <v>18</v>
       </c>
-      <c r="AV2" s="181"/>
-      <c r="AW2" s="181"/>
-      <c r="AX2" s="182"/>
-      <c r="AY2" s="160" t="s">
+      <c r="AV2" s="187"/>
+      <c r="AW2" s="187"/>
+      <c r="AX2" s="188"/>
+      <c r="AY2" s="166" t="s">
         <v>1047</v>
       </c>
-      <c r="AZ2" s="161"/>
-      <c r="BA2" s="161"/>
-      <c r="BB2" s="161"/>
-      <c r="BC2" s="162"/>
+      <c r="AZ2" s="167"/>
+      <c r="BA2" s="167"/>
+      <c r="BB2" s="167"/>
+      <c r="BC2" s="168"/>
     </row>
     <row r="3" spans="1:55" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -14641,42 +14783,42 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A4:BC21 C29:F32 A29:B33 G29:BC31 I33:BC33 I32:K32 M32:BC32 J22:AI27 AK22:BC27 A22:G27 H20:H28">
-    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="15" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="16" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28 J28:AI28 AK28:BC28">
-    <cfRule type="expression" dxfId="14" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="5" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="6" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="12" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="19" stopIfTrue="1">
       <formula>$A32="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="20" stopIfTrue="1">
       <formula>$A32="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I28">
-    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="3" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="4" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ22:AJ28">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="1" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="2" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46122,31 +46264,31 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="C782:C787 C844:C855 C789:C842">
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
       <formula>$A782=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
       <formula>$A782=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B336:C353 B764:C769 B301:C303 B4:C10 B297:C299 B38:C49 B25:C36 B496:C528 B12:C23 B844:B855 B315:C326 B530:C539 B541:C550 B728:C743 B745:C748 B750:C758 B332:C334 B771:C780 B328:C330 B760:C760 B762:C762 B305:C313 B355:C358 B782:B787 B552:C561 B51:C131 B133:C213 B215:C295 B360:C494 B563:C616 B673:C726 B618:C671 B789:B842">
-    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
       <formula>$A4=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="4" stopIfTrue="1">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2 D2:Z2">
-    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A10 A12:A23 A25:A36 A38:A49 A297:A299 A301:A303 A305:A313 A315:A326 A328:A330 A332:A334 A336:A353 A355:A358 A496:A528 A530:A539 A541:A550 A552:A561 A745:A748 A750:A758 A760 A762 A764:A769 A771:A780 A782:A787 A844:A855 A51:A131 A133:A213 A215:A295 A360:A494 A563:A616 A673:A726 A618:A671 A728:A743 A789:A842">
-    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="6" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated dependencies. added conditional compilation for beamdyn debugging and changed ReadFASTInputMeshes.m so it can read the BD meshes, too. fixed an issue with AFAeroMod in conversion script. added comments from rrd on airfoil UA parameters.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1048 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -36,7 +36,7 @@
     <definedName name="_Toc46290869" localSheetId="2">Variables!$B$770</definedName>
     <definedName name="_Toc46290870" localSheetId="2">Variables!$B$781</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">TestMatrix!$B$2:$AX$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'TestMatrix (new)'!$B$2:$BC$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'TestMatrix (new)'!$B$2:$BE$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Variables!$B$1:$P$855</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2954" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="1143">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3472,6 +3472,12 @@
   </si>
   <si>
     <t>Mean Wind Speed (m/s)</t>
+  </si>
+  <si>
+    <t>Tower Potential Flow</t>
+  </si>
+  <si>
+    <t>Tower Aero</t>
   </si>
 </sst>
 </file>
@@ -4178,7 +4184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4704,12 +4710,113 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="61">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -4862,6 +4969,20 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -5345,13 +5466,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO61"/>
+  <dimension ref="A1:BQ61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="AM16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="AM4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AS22" sqref="AS22:AT28"/>
+      <selection pane="bottomRight" activeCell="AW5" sqref="AW5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5383,26 +5504,26 @@
     <col min="35" max="35" width="4.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="36" max="42" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="43" max="47" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="4.33203125" style="2" customWidth="1"/>
-    <col min="50" max="51" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="5.33203125" style="45" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="5.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="3.33203125" style="160" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="4.88671875" style="2" customWidth="1"/>
-    <col min="57" max="57" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="4.88671875" style="2" customWidth="1"/>
-    <col min="60" max="62" width="1.88671875" style="2" customWidth="1"/>
-    <col min="63" max="63" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="64" max="65" width="3.33203125" style="45" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="5.6640625" style="45" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="4.44140625" customWidth="1"/>
-    <col min="69" max="69" width="4.33203125" customWidth="1"/>
+    <col min="48" max="51" width="4.33203125" style="2" customWidth="1"/>
+    <col min="52" max="53" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="5.33203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="5.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="3.33203125" style="160" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="4.88671875" style="2" customWidth="1"/>
+    <col min="59" max="59" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="4.88671875" style="2" customWidth="1"/>
+    <col min="62" max="64" width="1.88671875" style="2" customWidth="1"/>
+    <col min="65" max="65" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="3.33203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="5.6640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="4.44140625" customWidth="1"/>
+    <col min="71" max="71" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:67" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="172" t="s">
         <v>27</v>
       </c>
@@ -5461,32 +5582,34 @@
       <c r="AU2" s="181"/>
       <c r="AV2" s="181"/>
       <c r="AW2" s="181"/>
-      <c r="AX2" s="182"/>
-      <c r="AY2" s="186" t="s">
+      <c r="AX2" s="181"/>
+      <c r="AY2" s="181"/>
+      <c r="AZ2" s="182"/>
+      <c r="BA2" s="186" t="s">
         <v>1138</v>
       </c>
-      <c r="AZ2" s="187"/>
-      <c r="BA2" s="187"/>
       <c r="BB2" s="187"/>
-      <c r="BC2" s="188"/>
-      <c r="BD2" s="183" t="s">
+      <c r="BC2" s="187"/>
+      <c r="BD2" s="187"/>
+      <c r="BE2" s="188"/>
+      <c r="BF2" s="183" t="s">
         <v>1129</v>
       </c>
-      <c r="BE2" s="184"/>
-      <c r="BF2" s="184"/>
       <c r="BG2" s="184"/>
       <c r="BH2" s="184"/>
       <c r="BI2" s="184"/>
-      <c r="BJ2" s="185"/>
-      <c r="BK2" s="166" t="s">
+      <c r="BJ2" s="184"/>
+      <c r="BK2" s="184"/>
+      <c r="BL2" s="185"/>
+      <c r="BM2" s="166" t="s">
         <v>1047</v>
       </c>
-      <c r="BL2" s="167"/>
-      <c r="BM2" s="167"/>
       <c r="BN2" s="167"/>
-      <c r="BO2" s="168"/>
-    </row>
-    <row r="3" spans="1:67" s="1" customFormat="1" ht="88.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BO2" s="167"/>
+      <c r="BP2" s="167"/>
+      <c r="BQ2" s="168"/>
+    </row>
+    <row r="3" spans="1:69" s="1" customFormat="1" ht="114.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
       <c r="B3" s="79" t="s">
         <v>287</v>
@@ -5629,59 +5752,65 @@
       <c r="AV3" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="AW3" s="73" t="s">
+      <c r="AW3" s="191" t="s">
+        <v>1141</v>
+      </c>
+      <c r="AX3" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="AX3" s="74" t="s">
+      <c r="AY3" s="191" t="s">
+        <v>1142</v>
+      </c>
+      <c r="AZ3" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="AY3" s="75" t="s">
+      <c r="BA3" s="75" t="s">
         <v>1139</v>
       </c>
-      <c r="AZ3" s="164" t="s">
+      <c r="BB3" s="164" t="s">
         <v>1132</v>
       </c>
-      <c r="BA3" s="165" t="s">
+      <c r="BC3" s="165" t="s">
         <v>1140</v>
       </c>
-      <c r="BB3" s="77" t="s">
+      <c r="BD3" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="BC3" s="76" t="s">
+      <c r="BE3" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="BD3" s="157" t="s">
+      <c r="BF3" s="157" t="s">
         <v>1121</v>
       </c>
-      <c r="BE3" s="158" t="s">
+      <c r="BG3" s="158" t="s">
         <v>1122</v>
       </c>
-      <c r="BF3" s="158" t="s">
+      <c r="BH3" s="158" t="s">
         <v>1123</v>
       </c>
-      <c r="BG3" s="158" t="s">
+      <c r="BI3" s="158" t="s">
         <v>1124</v>
       </c>
-      <c r="BH3" s="158"/>
-      <c r="BI3" s="158"/>
-      <c r="BJ3" s="159"/>
-      <c r="BK3" s="66" t="s">
+      <c r="BJ3" s="158"/>
+      <c r="BK3" s="158"/>
+      <c r="BL3" s="159"/>
+      <c r="BM3" s="66" t="s">
         <v>1045</v>
       </c>
-      <c r="BL3" s="69" t="s">
+      <c r="BN3" s="69" t="s">
         <v>1046</v>
       </c>
-      <c r="BM3" s="70" t="s">
+      <c r="BO3" s="70" t="s">
         <v>1051</v>
       </c>
-      <c r="BN3" s="70" t="s">
+      <c r="BP3" s="70" t="s">
         <v>1054</v>
       </c>
-      <c r="BO3" s="68" t="s">
+      <c r="BQ3" s="68" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="85" t="s">
         <v>20</v>
@@ -5822,60 +5951,66 @@
       <c r="AV4" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="AW4" s="35" t="s">
+      <c r="AW4" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX4" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="AX4" s="33">
+      <c r="AY4" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ4" s="33">
         <v>15</v>
       </c>
-      <c r="AY4" s="36">
+      <c r="BA4" s="36">
         <v>2</v>
       </c>
-      <c r="AZ4" s="150">
+      <c r="BB4" s="150">
         <v>30</v>
       </c>
-      <c r="BA4" s="150">
+      <c r="BC4" s="150">
         <v>12</v>
       </c>
-      <c r="BB4" s="37">
+      <c r="BD4" s="37">
         <v>0.2</v>
       </c>
-      <c r="BC4" s="38" t="s">
+      <c r="BE4" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="BD4" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE4" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF4" s="41" t="s">
+      <c r="BF4" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG4" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH4" s="35"/>
-      <c r="BI4" s="35"/>
-      <c r="BJ4" s="33"/>
-      <c r="BK4" s="59">
-        <v>0</v>
-      </c>
-      <c r="BL4" s="55">
+      <c r="BH4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ4" s="35"/>
+      <c r="BK4" s="35"/>
+      <c r="BL4" s="33"/>
+      <c r="BM4" s="59">
+        <v>0</v>
+      </c>
+      <c r="BN4" s="55">
         <v>3</v>
       </c>
-      <c r="BM4" s="62">
+      <c r="BO4" s="62">
         <f>Variables!D2</f>
         <v>23</v>
       </c>
-      <c r="BN4" s="62" t="s">
+      <c r="BP4" s="62" t="s">
         <v>1048</v>
       </c>
-      <c r="BO4" s="38" t="s">
+      <c r="BQ4" s="38" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="27"/>
       <c r="B5" s="85" t="s">
         <v>33</v>
@@ -6019,57 +6154,63 @@
       <c r="AW5" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX5" s="42">
-        <v>0</v>
-      </c>
-      <c r="AY5" s="43">
+      <c r="AX5" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY5" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ5" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="43">
         <v>1</v>
       </c>
-      <c r="AZ5" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA5" s="151">
+      <c r="BB5" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="151">
         <v>12</v>
       </c>
-      <c r="BB5" s="44">
-        <v>0</v>
-      </c>
-      <c r="BC5" s="42" t="s">
+      <c r="BD5" s="44">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD5" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE5" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF5" s="41" t="s">
+      <c r="BF5" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG5" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH5" s="41"/>
-      <c r="BI5" s="41"/>
-      <c r="BJ5" s="42"/>
-      <c r="BK5" s="60">
-        <v>0</v>
-      </c>
-      <c r="BL5" s="56">
+      <c r="BH5" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI5" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ5" s="41"/>
+      <c r="BK5" s="41"/>
+      <c r="BL5" s="42"/>
+      <c r="BM5" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN5" s="56">
         <v>1</v>
       </c>
-      <c r="BM5" s="63">
+      <c r="BO5" s="63">
         <f>Variables!E2</f>
         <v>22</v>
       </c>
-      <c r="BN5" s="63" t="s">
+      <c r="BP5" s="63" t="s">
         <v>1049</v>
       </c>
-      <c r="BO5" s="42" t="s">
+      <c r="BQ5" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
       <c r="B6" s="85" t="s">
         <v>34</v>
@@ -6211,59 +6352,65 @@
         <v>22</v>
       </c>
       <c r="AW6" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX6" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX6" s="42" t="s">
+      <c r="AY6" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ6" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY6" s="43">
+      <c r="BA6" s="43">
         <v>2</v>
       </c>
-      <c r="AZ6" s="151">
+      <c r="BB6" s="151">
         <v>30</v>
       </c>
-      <c r="BA6" s="151">
+      <c r="BC6" s="151">
         <v>12</v>
       </c>
-      <c r="BB6" s="44">
+      <c r="BD6" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC6" s="42" t="s">
+      <c r="BE6" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD6" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE6" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF6" s="41" t="s">
+      <c r="BF6" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG6" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH6" s="41"/>
-      <c r="BI6" s="41"/>
-      <c r="BJ6" s="42"/>
-      <c r="BK6" s="60">
-        <v>0</v>
-      </c>
-      <c r="BL6" s="56">
+      <c r="BH6" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI6" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ6" s="41"/>
+      <c r="BK6" s="41"/>
+      <c r="BL6" s="42"/>
+      <c r="BM6" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN6" s="56">
         <v>3</v>
       </c>
-      <c r="BM6" s="63">
+      <c r="BO6" s="63">
         <f>Variables!F$2</f>
         <v>23</v>
       </c>
-      <c r="BN6" s="63" t="s">
+      <c r="BP6" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO6" s="42" t="s">
+      <c r="BQ6" s="42" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="7" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
       <c r="B7" s="85" t="s">
         <v>35</v>
@@ -6405,59 +6552,65 @@
         <v>22</v>
       </c>
       <c r="AW7" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX7" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX7" s="42" t="s">
+      <c r="AY7" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ7" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY7" s="43">
+      <c r="BA7" s="43">
         <v>4</v>
       </c>
-      <c r="AZ7" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA7" s="151">
+      <c r="BB7" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="151">
         <v>12</v>
       </c>
-      <c r="BB7" s="44">
+      <c r="BD7" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC7" s="42" t="s">
+      <c r="BE7" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD7" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE7" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF7" s="41" t="s">
+      <c r="BF7" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG7" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH7" s="41"/>
-      <c r="BI7" s="41"/>
-      <c r="BJ7" s="42"/>
-      <c r="BK7" s="60">
-        <v>0</v>
-      </c>
-      <c r="BL7" s="56">
+      <c r="BH7" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI7" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ7" s="41"/>
+      <c r="BK7" s="41"/>
+      <c r="BL7" s="42"/>
+      <c r="BM7" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN7" s="56">
         <v>5</v>
       </c>
-      <c r="BM7" s="63">
+      <c r="BO7" s="63">
         <f>Variables!F$2</f>
         <v>23</v>
       </c>
-      <c r="BN7" s="63" t="s">
+      <c r="BP7" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BO7" s="42" t="s">
+      <c r="BQ7" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="85" t="s">
         <v>36</v>
@@ -6601,57 +6754,63 @@
       <c r="AW8" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX8" s="42">
-        <v>0</v>
-      </c>
-      <c r="AY8" s="43">
+      <c r="AX8" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY8" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ8" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="43">
         <v>2</v>
       </c>
-      <c r="AZ8" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA8" s="151">
+      <c r="BB8" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="151">
         <v>12</v>
       </c>
-      <c r="BB8" s="44">
-        <v>0</v>
-      </c>
-      <c r="BC8" s="42" t="s">
+      <c r="BD8" s="44">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD8" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE8" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF8" s="41" t="s">
+      <c r="BF8" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG8" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH8" s="41"/>
-      <c r="BI8" s="41"/>
-      <c r="BJ8" s="42"/>
-      <c r="BK8" s="60">
-        <v>0</v>
-      </c>
-      <c r="BL8" s="56">
+      <c r="BH8" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI8" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ8" s="41"/>
+      <c r="BK8" s="41"/>
+      <c r="BL8" s="42"/>
+      <c r="BM8" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN8" s="56">
         <v>3</v>
       </c>
-      <c r="BM8" s="63">
+      <c r="BO8" s="63">
         <f>Variables!G$2</f>
         <v>24</v>
       </c>
-      <c r="BN8" s="63" t="s">
+      <c r="BP8" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO8" s="42" t="s">
+      <c r="BQ8" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="85" t="s">
         <v>37</v>
@@ -6794,59 +6953,65 @@
         <v>22</v>
       </c>
       <c r="AW9" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX9" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX9" s="42">
-        <v>0</v>
-      </c>
-      <c r="AY9" s="43">
+      <c r="AY9" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ9" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="43">
         <v>2</v>
       </c>
-      <c r="AZ9" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA9" s="151">
+      <c r="BB9" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="151">
         <v>12</v>
       </c>
-      <c r="BB9" s="44">
-        <v>0</v>
-      </c>
-      <c r="BC9" s="42" t="s">
+      <c r="BD9" s="44">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD9" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE9" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF9" s="41" t="s">
+      <c r="BF9" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG9" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH9" s="41"/>
-      <c r="BI9" s="41"/>
-      <c r="BJ9" s="42"/>
-      <c r="BK9" s="60">
-        <v>0</v>
-      </c>
-      <c r="BL9" s="56">
+      <c r="BH9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ9" s="41"/>
+      <c r="BK9" s="41"/>
+      <c r="BL9" s="42"/>
+      <c r="BM9" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN9" s="56">
         <v>5</v>
       </c>
-      <c r="BM9" s="63">
+      <c r="BO9" s="63">
         <f>Variables!H$2</f>
         <v>22</v>
       </c>
-      <c r="BN9" s="63" t="s">
+      <c r="BP9" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO9" s="42" t="s">
+      <c r="BQ9" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="85" t="s">
         <v>38</v>
@@ -6989,59 +7154,65 @@
         <v>22</v>
       </c>
       <c r="AW10" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX10" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX10" s="42">
-        <v>0</v>
-      </c>
-      <c r="AY10" s="43">
+      <c r="AY10" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ10" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="43">
         <v>4</v>
       </c>
-      <c r="AZ10" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA10" s="151">
+      <c r="BB10" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC10" s="151">
         <v>12</v>
       </c>
-      <c r="BB10" s="44">
+      <c r="BD10" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC10" s="42" t="s">
+      <c r="BE10" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD10" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE10" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF10" s="41" t="s">
+      <c r="BF10" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG10" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH10" s="41"/>
-      <c r="BI10" s="41"/>
-      <c r="BJ10" s="42"/>
-      <c r="BK10" s="60">
-        <v>0</v>
-      </c>
-      <c r="BL10" s="56">
+      <c r="BH10" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI10" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ10" s="41"/>
+      <c r="BK10" s="41"/>
+      <c r="BL10" s="42"/>
+      <c r="BM10" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN10" s="56">
         <v>3</v>
       </c>
-      <c r="BM10" s="63">
+      <c r="BO10" s="63">
         <f>Variables!I$2</f>
         <v>24</v>
       </c>
-      <c r="BN10" s="63" t="s">
+      <c r="BP10" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO10" s="42" t="s">
+      <c r="BQ10" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
       <c r="B11" s="85" t="s">
         <v>39</v>
@@ -7184,59 +7355,65 @@
         <v>22</v>
       </c>
       <c r="AW11" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX11" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX11" s="42">
+      <c r="AY11" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ11" s="42">
         <v>15</v>
       </c>
-      <c r="AY11" s="43">
+      <c r="BA11" s="43">
         <v>1</v>
       </c>
-      <c r="AZ11" s="151">
+      <c r="BB11" s="151">
         <v>30</v>
       </c>
-      <c r="BA11" s="151">
+      <c r="BC11" s="151">
         <v>11</v>
       </c>
-      <c r="BB11" s="44">
+      <c r="BD11" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC11" s="42" t="s">
+      <c r="BE11" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD11" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE11" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF11" s="41" t="s">
+      <c r="BF11" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG11" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH11" s="41"/>
-      <c r="BI11" s="41"/>
-      <c r="BJ11" s="42"/>
-      <c r="BK11" s="60">
-        <v>0</v>
-      </c>
-      <c r="BL11" s="56">
+      <c r="BH11" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI11" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ11" s="41"/>
+      <c r="BK11" s="41"/>
+      <c r="BL11" s="42"/>
+      <c r="BM11" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN11" s="56">
         <v>2</v>
       </c>
-      <c r="BM11" s="63">
+      <c r="BO11" s="63">
         <f>Variables!J$2</f>
         <v>27</v>
       </c>
-      <c r="BN11" s="63" t="s">
+      <c r="BP11" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO11" s="42" t="s">
+      <c r="BQ11" s="42" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="12" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
       <c r="B12" s="85" t="s">
         <v>40</v>
@@ -7378,59 +7555,65 @@
         <v>32</v>
       </c>
       <c r="AW12" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX12" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AX12" s="42" t="s">
+      <c r="AY12" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ12" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY12" s="43">
+      <c r="BA12" s="43">
         <v>2</v>
       </c>
-      <c r="AZ12" s="151">
+      <c r="BB12" s="151">
         <v>30</v>
       </c>
-      <c r="BA12" s="151">
+      <c r="BC12" s="151">
         <v>11</v>
       </c>
-      <c r="BB12" s="44">
+      <c r="BD12" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC12" s="42" t="s">
+      <c r="BE12" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD12" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE12" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF12" s="41" t="s">
+      <c r="BF12" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG12" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH12" s="41"/>
-      <c r="BI12" s="41"/>
-      <c r="BJ12" s="42"/>
-      <c r="BK12" s="60">
-        <v>0</v>
-      </c>
-      <c r="BL12" s="56">
+      <c r="BH12" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI12" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ12" s="41"/>
+      <c r="BK12" s="41"/>
+      <c r="BL12" s="42"/>
+      <c r="BM12" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN12" s="56">
         <v>5</v>
       </c>
-      <c r="BM12" s="63">
+      <c r="BO12" s="63">
         <f>Variables!K$2</f>
         <v>26</v>
       </c>
-      <c r="BN12" s="63" t="s">
+      <c r="BP12" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO12" s="42" t="s">
+      <c r="BQ12" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27"/>
       <c r="B13" s="85" t="s">
         <v>41</v>
@@ -7574,57 +7757,63 @@
       <c r="AW13" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX13" s="42">
-        <v>0</v>
-      </c>
-      <c r="AY13" s="43">
+      <c r="AX13" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY13" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ13" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA13" s="43">
         <v>2</v>
       </c>
-      <c r="AZ13" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA13" s="163" t="s">
+      <c r="BB13" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC13" s="163" t="s">
         <v>1133</v>
       </c>
-      <c r="BB13" s="44">
-        <v>0</v>
-      </c>
-      <c r="BC13" s="42" t="s">
+      <c r="BD13" s="44">
+        <v>0</v>
+      </c>
+      <c r="BE13" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD13" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE13" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF13" s="41" t="s">
+      <c r="BF13" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG13" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH13" s="41"/>
-      <c r="BI13" s="41"/>
-      <c r="BJ13" s="42"/>
-      <c r="BK13" s="60">
-        <v>0</v>
-      </c>
-      <c r="BL13" s="56">
-        <v>0</v>
-      </c>
-      <c r="BM13" s="63">
+      <c r="BH13" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI13" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ13" s="41"/>
+      <c r="BK13" s="41"/>
+      <c r="BL13" s="42"/>
+      <c r="BM13" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN13" s="56">
+        <v>0</v>
+      </c>
+      <c r="BO13" s="63">
         <f>Variables!L$2</f>
         <v>24</v>
       </c>
-      <c r="BN13" s="63" t="s">
+      <c r="BP13" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO13" s="42" t="s">
+      <c r="BQ13" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="85" t="s">
         <v>51</v>
@@ -7768,57 +7957,63 @@
       <c r="AW14" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX14" s="42">
-        <v>0</v>
-      </c>
-      <c r="AY14" s="43">
+      <c r="AX14" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY14" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ14" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA14" s="43">
         <v>4</v>
       </c>
-      <c r="AZ14" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA14" s="151">
+      <c r="BB14" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC14" s="151">
         <v>12</v>
       </c>
-      <c r="BB14" s="44">
+      <c r="BD14" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC14" s="42" t="s">
+      <c r="BE14" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD14" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE14" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF14" s="41" t="s">
+      <c r="BF14" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG14" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH14" s="41"/>
-      <c r="BI14" s="41"/>
-      <c r="BJ14" s="42"/>
-      <c r="BK14" s="60">
+      <c r="BH14" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI14" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ14" s="41"/>
+      <c r="BK14" s="41"/>
+      <c r="BL14" s="42"/>
+      <c r="BM14" s="60">
         <v>2</v>
       </c>
-      <c r="BL14" s="56">
-        <v>0</v>
-      </c>
-      <c r="BM14" s="63">
+      <c r="BN14" s="56">
+        <v>0</v>
+      </c>
+      <c r="BO14" s="63">
         <f>Variables!M$2</f>
         <v>21</v>
       </c>
-      <c r="BN14" s="63" t="s">
+      <c r="BP14" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO14" s="42" t="s">
+      <c r="BQ14" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27"/>
       <c r="B15" s="85" t="s">
         <v>52</v>
@@ -7962,57 +8157,63 @@
       <c r="AW15" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX15" s="42" t="s">
+      <c r="AX15" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY15" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ15" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY15" s="43">
+      <c r="BA15" s="43">
         <v>2</v>
       </c>
-      <c r="AZ15" s="163" t="s">
+      <c r="BB15" s="163" t="s">
         <v>1134</v>
       </c>
-      <c r="BA15" s="163" t="s">
+      <c r="BC15" s="163" t="s">
         <v>1135</v>
       </c>
-      <c r="BB15" s="44">
+      <c r="BD15" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC15" s="42" t="s">
+      <c r="BE15" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD15" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE15" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF15" s="41" t="s">
+      <c r="BF15" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG15" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH15" s="41"/>
-      <c r="BI15" s="41"/>
-      <c r="BJ15" s="42"/>
-      <c r="BK15" s="60">
+      <c r="BH15" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI15" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ15" s="41"/>
+      <c r="BK15" s="41"/>
+      <c r="BL15" s="42"/>
+      <c r="BM15" s="60">
         <v>2</v>
       </c>
-      <c r="BL15" s="56">
+      <c r="BN15" s="56">
         <v>4</v>
       </c>
-      <c r="BM15" s="63">
+      <c r="BO15" s="63">
         <f>Variables!N$2</f>
         <v>21</v>
       </c>
-      <c r="BN15" s="63" t="s">
+      <c r="BP15" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO15" s="42" t="s">
+      <c r="BQ15" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27"/>
       <c r="B16" s="85" t="s">
         <v>53</v>
@@ -8156,57 +8357,63 @@
       <c r="AW16" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX16" s="42">
-        <v>0</v>
-      </c>
-      <c r="AY16" s="43">
+      <c r="AX16" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY16" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ16" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA16" s="43">
         <v>4</v>
       </c>
-      <c r="AZ16" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA16" s="151">
+      <c r="BB16" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC16" s="151">
         <v>12</v>
       </c>
-      <c r="BB16" s="44">
+      <c r="BD16" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC16" s="42" t="s">
+      <c r="BE16" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD16" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE16" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF16" s="41" t="s">
+      <c r="BF16" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG16" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH16" s="41"/>
-      <c r="BI16" s="41"/>
-      <c r="BJ16" s="42"/>
-      <c r="BK16" s="60">
+      <c r="BH16" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI16" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ16" s="41"/>
+      <c r="BK16" s="41"/>
+      <c r="BL16" s="42"/>
+      <c r="BM16" s="60">
         <v>2</v>
       </c>
-      <c r="BL16" s="56">
-        <v>0</v>
-      </c>
-      <c r="BM16" s="63">
+      <c r="BN16" s="56">
+        <v>0</v>
+      </c>
+      <c r="BO16" s="63">
         <f>Variables!O$2</f>
         <v>23</v>
       </c>
-      <c r="BN16" s="63" t="s">
+      <c r="BP16" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO16" s="42" t="s">
+      <c r="BQ16" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="17" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="125"/>
       <c r="C17" s="148"/>
@@ -8256,26 +8463,28 @@
       <c r="AU17" s="129"/>
       <c r="AV17" s="129"/>
       <c r="AW17" s="129"/>
-      <c r="AX17" s="130"/>
-      <c r="AY17" s="128"/>
-      <c r="AZ17" s="152"/>
-      <c r="BA17" s="152"/>
-      <c r="BB17" s="132"/>
-      <c r="BC17" s="130"/>
-      <c r="BD17" s="131"/>
-      <c r="BE17" s="129"/>
-      <c r="BF17" s="129"/>
+      <c r="AX17" s="129"/>
+      <c r="AY17" s="129"/>
+      <c r="AZ17" s="130"/>
+      <c r="BA17" s="128"/>
+      <c r="BB17" s="152"/>
+      <c r="BC17" s="152"/>
+      <c r="BD17" s="132"/>
+      <c r="BE17" s="130"/>
+      <c r="BF17" s="131"/>
       <c r="BG17" s="129"/>
       <c r="BH17" s="129"/>
       <c r="BI17" s="129"/>
-      <c r="BJ17" s="130"/>
-      <c r="BK17" s="133"/>
-      <c r="BL17" s="134"/>
-      <c r="BM17" s="135"/>
-      <c r="BN17" s="135"/>
-      <c r="BO17" s="130"/>
-    </row>
-    <row r="18" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="BJ17" s="129"/>
+      <c r="BK17" s="129"/>
+      <c r="BL17" s="130"/>
+      <c r="BM17" s="133"/>
+      <c r="BN17" s="134"/>
+      <c r="BO17" s="135"/>
+      <c r="BP17" s="135"/>
+      <c r="BQ17" s="130"/>
+    </row>
+    <row r="18" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="27"/>
       <c r="B18" s="85" t="s">
         <v>289</v>
@@ -8419,57 +8628,63 @@
       <c r="AW18" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX18" s="42" t="s">
+      <c r="AX18" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY18" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ18" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY18" s="43">
+      <c r="BA18" s="43">
         <v>2</v>
       </c>
-      <c r="AZ18" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA18" s="163" t="s">
+      <c r="BB18" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC18" s="163" t="s">
         <v>1136</v>
       </c>
-      <c r="BB18" s="44">
+      <c r="BD18" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC18" s="42" t="s">
+      <c r="BE18" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD18" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE18" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF18" s="41" t="s">
+      <c r="BF18" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG18" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH18" s="41"/>
-      <c r="BI18" s="41"/>
-      <c r="BJ18" s="42"/>
-      <c r="BK18" s="60">
-        <v>0</v>
-      </c>
-      <c r="BL18" s="61">
-        <v>0</v>
-      </c>
-      <c r="BM18" s="63">
+      <c r="BH18" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI18" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ18" s="41"/>
+      <c r="BK18" s="41"/>
+      <c r="BL18" s="42"/>
+      <c r="BM18" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN18" s="61">
+        <v>0</v>
+      </c>
+      <c r="BO18" s="63">
         <f>Variables!Q$2</f>
         <v>0</v>
       </c>
-      <c r="BN18" s="63" t="s">
+      <c r="BP18" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO18" s="42" t="s">
+      <c r="BQ18" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="27"/>
       <c r="B19" s="85" t="s">
         <v>309</v>
@@ -8613,57 +8828,63 @@
       <c r="AW19" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX19" s="42" t="s">
+      <c r="AX19" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY19" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ19" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY19" s="43">
+      <c r="BA19" s="43">
         <v>2</v>
       </c>
-      <c r="AZ19" s="163" t="s">
+      <c r="BB19" s="163" t="s">
         <v>1137</v>
       </c>
-      <c r="BA19" s="151">
+      <c r="BC19" s="151">
         <v>11.9</v>
       </c>
-      <c r="BB19" s="44">
+      <c r="BD19" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC19" s="42" t="s">
+      <c r="BE19" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD19" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE19" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF19" s="41" t="s">
+      <c r="BF19" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG19" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH19" s="41"/>
-      <c r="BI19" s="41"/>
-      <c r="BJ19" s="42"/>
-      <c r="BK19" s="60">
-        <v>0</v>
-      </c>
-      <c r="BL19" s="56">
-        <v>0</v>
-      </c>
-      <c r="BM19" s="63">
+      <c r="BH19" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI19" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ19" s="41"/>
+      <c r="BK19" s="41"/>
+      <c r="BL19" s="42"/>
+      <c r="BM19" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN19" s="56">
+        <v>0</v>
+      </c>
+      <c r="BO19" s="63">
         <f>Variables!R$2</f>
         <v>25</v>
       </c>
-      <c r="BN19" s="63" t="s">
+      <c r="BP19" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO19" s="42" t="s">
+      <c r="BQ19" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="27"/>
       <c r="B20" s="85" t="s">
         <v>336</v>
@@ -8807,57 +9028,63 @@
       <c r="AW20" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX20" s="42" t="s">
+      <c r="AX20" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY20" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ20" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="AY20" s="43">
+      <c r="BA20" s="43">
         <v>4</v>
       </c>
-      <c r="AZ20" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA20" s="151">
+      <c r="BB20" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC20" s="151">
         <v>16</v>
       </c>
-      <c r="BB20" s="44">
+      <c r="BD20" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC20" s="42" t="s">
+      <c r="BE20" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD20" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE20" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF20" s="41" t="s">
+      <c r="BF20" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG20" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH20" s="41"/>
-      <c r="BI20" s="41"/>
-      <c r="BJ20" s="42"/>
-      <c r="BK20" s="60">
-        <v>0</v>
-      </c>
-      <c r="BL20" s="61">
-        <v>0</v>
-      </c>
-      <c r="BM20" s="63">
+      <c r="BH20" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI20" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ20" s="41"/>
+      <c r="BK20" s="41"/>
+      <c r="BL20" s="42"/>
+      <c r="BM20" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN20" s="61">
+        <v>0</v>
+      </c>
+      <c r="BO20" s="63">
         <f>Variables!S$2</f>
         <v>25</v>
       </c>
-      <c r="BN20" s="63" t="s">
+      <c r="BP20" s="63" t="s">
         <v>1048</v>
       </c>
-      <c r="BO20" s="42" t="s">
+      <c r="BQ20" s="42" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="85" t="s">
         <v>1060</v>
@@ -8999,48 +9226,54 @@
         <v>32</v>
       </c>
       <c r="AW21" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AX21" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX21" s="42"/>
-      <c r="AY21" s="43">
+      <c r="AY21" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AZ21" s="42"/>
+      <c r="BA21" s="43">
         <v>3</v>
       </c>
-      <c r="AZ21" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA21" s="151">
+      <c r="BB21" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC21" s="151">
         <v>12</v>
       </c>
-      <c r="BB21" s="44">
+      <c r="BD21" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC21" s="42" t="s">
+      <c r="BE21" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD21" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE21" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF21" s="41" t="s">
+      <c r="BF21" s="98" t="s">
         <v>42</v>
       </c>
       <c r="BG21" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH21" s="41"/>
-      <c r="BI21" s="41"/>
-      <c r="BJ21" s="42"/>
-      <c r="BK21" s="60"/>
-      <c r="BL21" s="61"/>
-      <c r="BM21" s="63"/>
-      <c r="BN21" s="63" t="s">
+      <c r="BH21" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI21" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ21" s="41"/>
+      <c r="BK21" s="41"/>
+      <c r="BL21" s="42"/>
+      <c r="BM21" s="60"/>
+      <c r="BN21" s="61"/>
+      <c r="BO21" s="63"/>
+      <c r="BP21" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BO21" s="42"/>
-    </row>
-    <row r="22" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="BQ21" s="42"/>
+    </row>
+    <row r="22" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
       <c r="B22" s="85" t="s">
         <v>1065</v>
@@ -9176,48 +9409,54 @@
       </c>
       <c r="AV22" s="41"/>
       <c r="AW22" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AX22" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX22" s="42"/>
-      <c r="AY22" s="43">
+      <c r="AY22" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ22" s="42"/>
+      <c r="BA22" s="43">
         <v>3</v>
       </c>
-      <c r="AZ22" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA22" s="151">
+      <c r="BB22" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC22" s="151">
         <v>12</v>
       </c>
-      <c r="BB22" s="44">
+      <c r="BD22" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC22" s="42" t="s">
+      <c r="BE22" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD22" s="99">
+      <c r="BF22" s="99">
         <v>20</v>
       </c>
-      <c r="BE22" s="41">
+      <c r="BG22" s="41">
         <v>2</v>
       </c>
-      <c r="BF22" s="41">
+      <c r="BH22" s="41">
         <v>6</v>
       </c>
-      <c r="BG22" s="41">
+      <c r="BI22" s="41">
         <v>10</v>
       </c>
-      <c r="BH22" s="41"/>
-      <c r="BI22" s="41"/>
-      <c r="BJ22" s="42"/>
-      <c r="BK22" s="60"/>
-      <c r="BL22" s="61"/>
-      <c r="BM22" s="63"/>
-      <c r="BN22" s="63" t="s">
+      <c r="BJ22" s="41"/>
+      <c r="BK22" s="41"/>
+      <c r="BL22" s="42"/>
+      <c r="BM22" s="60"/>
+      <c r="BN22" s="61"/>
+      <c r="BO22" s="63"/>
+      <c r="BP22" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BO22" s="42"/>
-    </row>
-    <row r="23" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="BQ22" s="42"/>
+    </row>
+    <row r="23" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="85" t="s">
         <v>1070</v>
@@ -9353,48 +9592,54 @@
       </c>
       <c r="AV23" s="41"/>
       <c r="AW23" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AX23" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX23" s="42"/>
-      <c r="AY23" s="43">
+      <c r="AY23" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ23" s="42"/>
+      <c r="BA23" s="43">
         <v>1</v>
       </c>
-      <c r="AZ23" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA23" s="151">
+      <c r="BB23" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC23" s="151">
         <v>8</v>
       </c>
-      <c r="BB23" s="44">
-        <v>0</v>
-      </c>
-      <c r="BC23" s="42" t="s">
+      <c r="BD23" s="44">
+        <v>0</v>
+      </c>
+      <c r="BE23" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD23" s="99">
+      <c r="BF23" s="99">
         <v>45</v>
       </c>
-      <c r="BE23" s="41" t="s">
+      <c r="BG23" s="41" t="s">
         <v>1125</v>
       </c>
-      <c r="BF23" s="41" t="s">
+      <c r="BH23" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BG23" s="41" t="s">
+      <c r="BI23" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH23" s="41"/>
-      <c r="BI23" s="41"/>
-      <c r="BJ23" s="42"/>
-      <c r="BK23" s="60"/>
-      <c r="BL23" s="61"/>
-      <c r="BM23" s="63"/>
-      <c r="BN23" s="63" t="s">
+      <c r="BJ23" s="41"/>
+      <c r="BK23" s="41"/>
+      <c r="BL23" s="42"/>
+      <c r="BM23" s="60"/>
+      <c r="BN23" s="61"/>
+      <c r="BO23" s="63"/>
+      <c r="BP23" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BO23" s="42"/>
-    </row>
-    <row r="24" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="BQ23" s="42"/>
+    </row>
+    <row r="24" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="27"/>
       <c r="B24" s="85" t="s">
         <v>1071</v>
@@ -9530,48 +9775,54 @@
       </c>
       <c r="AV24" s="41"/>
       <c r="AW24" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AX24" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX24" s="42"/>
-      <c r="AY24" s="43">
+      <c r="AY24" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ24" s="42"/>
+      <c r="BA24" s="43">
         <v>3</v>
       </c>
-      <c r="AZ24" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA24" s="151">
+      <c r="BB24" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC24" s="151">
         <v>12</v>
       </c>
-      <c r="BB24" s="44">
+      <c r="BD24" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC24" s="42" t="s">
+      <c r="BE24" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD24" s="99">
+      <c r="BF24" s="99">
         <v>50</v>
       </c>
-      <c r="BE24" s="41">
+      <c r="BG24" s="41">
         <v>2</v>
       </c>
-      <c r="BF24" s="41">
+      <c r="BH24" s="41">
         <v>8</v>
       </c>
-      <c r="BG24" s="41">
+      <c r="BI24" s="41">
         <v>10</v>
       </c>
-      <c r="BH24" s="41"/>
-      <c r="BI24" s="41"/>
-      <c r="BJ24" s="42"/>
-      <c r="BK24" s="60"/>
-      <c r="BL24" s="61"/>
-      <c r="BM24" s="63"/>
-      <c r="BN24" s="63" t="s">
+      <c r="BJ24" s="41"/>
+      <c r="BK24" s="41"/>
+      <c r="BL24" s="42"/>
+      <c r="BM24" s="60"/>
+      <c r="BN24" s="61"/>
+      <c r="BO24" s="63"/>
+      <c r="BP24" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BO24" s="42"/>
-    </row>
-    <row r="25" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="BQ24" s="42"/>
+    </row>
+    <row r="25" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
       <c r="B25" s="85" t="s">
         <v>1120</v>
@@ -9709,46 +9960,52 @@
       <c r="AW25" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX25" s="42"/>
-      <c r="AY25" s="43">
+      <c r="AX25" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY25" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ25" s="42"/>
+      <c r="BA25" s="43">
         <v>3</v>
       </c>
-      <c r="AZ25" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA25" s="151">
+      <c r="BB25" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC25" s="151">
         <v>12</v>
       </c>
-      <c r="BB25" s="44">
+      <c r="BD25" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC25" s="42" t="s">
+      <c r="BE25" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD25" s="99">
+      <c r="BF25" s="99">
         <v>150</v>
       </c>
-      <c r="BE25" s="41">
+      <c r="BG25" s="41">
         <v>2</v>
       </c>
-      <c r="BF25" s="41">
+      <c r="BH25" s="41">
         <v>5</v>
       </c>
-      <c r="BG25" s="41">
+      <c r="BI25" s="41">
         <v>12.4</v>
       </c>
-      <c r="BH25" s="41"/>
-      <c r="BI25" s="41"/>
-      <c r="BJ25" s="42"/>
-      <c r="BK25" s="60"/>
-      <c r="BL25" s="61"/>
-      <c r="BM25" s="63"/>
-      <c r="BN25" s="63" t="s">
+      <c r="BJ25" s="41"/>
+      <c r="BK25" s="41"/>
+      <c r="BL25" s="42"/>
+      <c r="BM25" s="60"/>
+      <c r="BN25" s="61"/>
+      <c r="BO25" s="63"/>
+      <c r="BP25" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BO25" s="42"/>
-    </row>
-    <row r="26" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BQ25" s="42"/>
+    </row>
+    <row r="26" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="85" t="s">
         <v>1119</v>
@@ -9886,46 +10143,52 @@
       <c r="AW26" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX26" s="42"/>
-      <c r="AY26" s="43">
+      <c r="AX26" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY26" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ26" s="42"/>
+      <c r="BA26" s="43">
         <v>3</v>
       </c>
-      <c r="AZ26" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA26" s="151">
+      <c r="BB26" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC26" s="151">
         <v>12</v>
       </c>
-      <c r="BB26" s="44">
+      <c r="BD26" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC26" s="42" t="s">
+      <c r="BE26" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD26" s="99">
+      <c r="BF26" s="99">
         <v>200</v>
       </c>
-      <c r="BE26" s="41">
+      <c r="BG26" s="41">
         <v>2</v>
       </c>
-      <c r="BF26" s="41">
+      <c r="BH26" s="41">
         <v>6</v>
       </c>
-      <c r="BG26" s="41">
+      <c r="BI26" s="41">
         <v>10</v>
       </c>
-      <c r="BH26" s="41"/>
-      <c r="BI26" s="41"/>
-      <c r="BJ26" s="42"/>
-      <c r="BK26" s="60"/>
-      <c r="BL26" s="61"/>
-      <c r="BM26" s="63"/>
-      <c r="BN26" s="63" t="s">
+      <c r="BJ26" s="41"/>
+      <c r="BK26" s="41"/>
+      <c r="BL26" s="42"/>
+      <c r="BM26" s="60"/>
+      <c r="BN26" s="61"/>
+      <c r="BO26" s="63"/>
+      <c r="BP26" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BO26" s="42"/>
-    </row>
-    <row r="27" spans="1:67" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BQ26" s="42"/>
+    </row>
+    <row r="27" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
       <c r="B27" s="85" t="s">
         <v>1118</v>
@@ -10063,46 +10326,52 @@
       <c r="AW27" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX27" s="42"/>
-      <c r="AY27" s="43">
+      <c r="AX27" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY27" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ27" s="42"/>
+      <c r="BA27" s="43">
         <v>3</v>
       </c>
-      <c r="AZ27" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA27" s="151">
+      <c r="BB27" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC27" s="151">
         <v>12</v>
       </c>
-      <c r="BB27" s="44">
+      <c r="BD27" s="44">
         <v>0.2</v>
       </c>
-      <c r="BC27" s="42" t="s">
+      <c r="BE27" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="BD27" s="99">
+      <c r="BF27" s="99">
         <v>320</v>
       </c>
-      <c r="BE27" s="41">
+      <c r="BG27" s="41">
         <v>2</v>
       </c>
-      <c r="BF27" s="41">
+      <c r="BH27" s="41">
         <v>6</v>
       </c>
-      <c r="BG27" s="41">
+      <c r="BI27" s="41">
         <v>10</v>
       </c>
-      <c r="BH27" s="41"/>
-      <c r="BI27" s="41"/>
-      <c r="BJ27" s="42"/>
-      <c r="BK27" s="60"/>
-      <c r="BL27" s="61"/>
-      <c r="BM27" s="63"/>
-      <c r="BN27" s="63" t="s">
+      <c r="BJ27" s="41"/>
+      <c r="BK27" s="41"/>
+      <c r="BL27" s="42"/>
+      <c r="BM27" s="60"/>
+      <c r="BN27" s="61"/>
+      <c r="BO27" s="63"/>
+      <c r="BP27" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BO27" s="42"/>
-    </row>
-    <row r="28" spans="1:67" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="BQ27" s="42"/>
+    </row>
+    <row r="28" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="27"/>
       <c r="B28" s="85" t="s">
         <v>1117</v>
@@ -10240,46 +10509,52 @@
       <c r="AW28" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AX28" s="42"/>
-      <c r="AY28" s="43">
+      <c r="AX28" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY28" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ28" s="42"/>
+      <c r="BA28" s="43">
         <v>1</v>
       </c>
-      <c r="AZ28" s="151">
-        <v>0</v>
-      </c>
-      <c r="BA28" s="151">
+      <c r="BB28" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC28" s="151">
         <v>8</v>
       </c>
-      <c r="BB28" s="44">
-        <v>0</v>
-      </c>
-      <c r="BC28" s="42" t="s">
+      <c r="BD28" s="44">
+        <v>0</v>
+      </c>
+      <c r="BE28" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BD28" s="99">
+      <c r="BF28" s="99">
         <v>200</v>
       </c>
-      <c r="BE28" s="41">
+      <c r="BG28" s="41">
         <v>3</v>
       </c>
-      <c r="BF28" s="41">
+      <c r="BH28" s="41">
         <v>1.2645999999999999</v>
       </c>
-      <c r="BG28" s="41" t="s">
+      <c r="BI28" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BH28" s="41"/>
-      <c r="BI28" s="41"/>
-      <c r="BJ28" s="42"/>
-      <c r="BK28" s="60"/>
-      <c r="BL28" s="61"/>
-      <c r="BM28" s="63"/>
-      <c r="BN28" s="63" t="s">
+      <c r="BJ28" s="41"/>
+      <c r="BK28" s="41"/>
+      <c r="BL28" s="42"/>
+      <c r="BM28" s="60"/>
+      <c r="BN28" s="61"/>
+      <c r="BO28" s="63"/>
+      <c r="BP28" s="63" t="s">
         <v>1050</v>
       </c>
-      <c r="BO28" s="42"/>
-    </row>
-    <row r="29" spans="1:67" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BQ28" s="42"/>
+    </row>
+    <row r="29" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="149"/>
       <c r="D29" s="3"/>
@@ -10330,445 +10605,447 @@
       <c r="AU29" s="8"/>
       <c r="AV29" s="8"/>
       <c r="AW29" s="8"/>
-      <c r="AX29" s="6"/>
-      <c r="AY29" s="7"/>
-      <c r="AZ29" s="153"/>
-      <c r="BA29" s="153"/>
-      <c r="BB29" s="161"/>
-      <c r="BC29" s="6"/>
-      <c r="BD29" s="100"/>
-      <c r="BE29" s="8"/>
-      <c r="BF29" s="8"/>
+      <c r="AX29" s="8"/>
+      <c r="AY29" s="8"/>
+      <c r="AZ29" s="6"/>
+      <c r="BA29" s="7"/>
+      <c r="BB29" s="153"/>
+      <c r="BC29" s="153"/>
+      <c r="BD29" s="161"/>
+      <c r="BE29" s="6"/>
+      <c r="BF29" s="100"/>
       <c r="BG29" s="8"/>
       <c r="BH29" s="8"/>
       <c r="BI29" s="8"/>
-      <c r="BJ29" s="6"/>
-      <c r="BK29" s="7"/>
-      <c r="BL29" s="48"/>
-      <c r="BM29" s="64"/>
-      <c r="BN29" s="64"/>
-      <c r="BO29" s="6"/>
-    </row>
-    <row r="33" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY33" s="9"/>
-      <c r="AZ33" s="2"/>
-      <c r="BA33" s="2"/>
-      <c r="BB33" s="162"/>
-      <c r="BC33" s="45"/>
-      <c r="BJ33" s="45"/>
-      <c r="BK33" s="45"/>
-      <c r="BM33" s="2"/>
-      <c r="BN33"/>
-      <c r="BO33"/>
-    </row>
-    <row r="34" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY34" s="9"/>
-      <c r="AZ34" s="2"/>
-      <c r="BA34" s="2"/>
-      <c r="BB34" s="162"/>
-      <c r="BC34" s="45"/>
-      <c r="BJ34" s="45"/>
-      <c r="BK34" s="45"/>
-      <c r="BM34" s="2"/>
-      <c r="BN34"/>
-      <c r="BO34"/>
-    </row>
-    <row r="35" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY35" s="9"/>
-      <c r="AZ35" s="2"/>
-      <c r="BA35" s="2"/>
-      <c r="BB35" s="162"/>
-      <c r="BC35" s="45"/>
-      <c r="BJ35" s="45"/>
-      <c r="BK35" s="45"/>
-      <c r="BM35" s="2"/>
-      <c r="BN35"/>
-      <c r="BO35"/>
-    </row>
-    <row r="36" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY36" s="9"/>
-      <c r="AZ36" s="2"/>
-      <c r="BA36" s="2"/>
-      <c r="BB36" s="162"/>
-      <c r="BC36" s="45"/>
-      <c r="BJ36" s="45"/>
-      <c r="BK36" s="45"/>
-      <c r="BM36" s="2"/>
-      <c r="BN36"/>
-      <c r="BO36"/>
-    </row>
-    <row r="37" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY37" s="9"/>
-      <c r="AZ37" s="2"/>
-      <c r="BA37" s="2"/>
-      <c r="BB37" s="162"/>
-      <c r="BC37" s="45"/>
-      <c r="BJ37" s="45"/>
-      <c r="BK37" s="45"/>
-      <c r="BM37" s="2"/>
-      <c r="BN37"/>
-      <c r="BO37"/>
-    </row>
-    <row r="38" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY38" s="9"/>
-      <c r="AZ38" s="2"/>
-      <c r="BA38" s="2"/>
-      <c r="BB38" s="162"/>
-      <c r="BC38" s="45"/>
-      <c r="BJ38" s="45"/>
-      <c r="BK38" s="45"/>
-      <c r="BM38" s="2"/>
-      <c r="BN38"/>
-      <c r="BO38"/>
-    </row>
-    <row r="39" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY39" s="9"/>
-      <c r="AZ39" s="2"/>
-      <c r="BA39" s="2"/>
-      <c r="BB39" s="162"/>
-      <c r="BC39" s="45"/>
-      <c r="BJ39" s="45"/>
-      <c r="BK39" s="45"/>
-      <c r="BM39" s="2"/>
-      <c r="BN39"/>
-      <c r="BO39"/>
-    </row>
-    <row r="40" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY40" s="9"/>
-      <c r="AZ40" s="2"/>
-      <c r="BA40" s="2"/>
-      <c r="BB40" s="162"/>
-      <c r="BC40" s="45"/>
-      <c r="BJ40" s="45"/>
-      <c r="BK40" s="45"/>
-      <c r="BM40" s="2"/>
-      <c r="BN40"/>
-      <c r="BO40"/>
-    </row>
-    <row r="41" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY41" s="9"/>
-      <c r="AZ41" s="2"/>
-      <c r="BA41" s="2"/>
-      <c r="BB41" s="162"/>
-      <c r="BC41" s="45"/>
-      <c r="BJ41" s="45"/>
-      <c r="BK41" s="45"/>
-      <c r="BM41" s="2"/>
-      <c r="BN41"/>
-      <c r="BO41"/>
-    </row>
-    <row r="42" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY42" s="9"/>
-      <c r="AZ42" s="2"/>
-      <c r="BA42" s="2"/>
-      <c r="BB42" s="162"/>
-      <c r="BC42" s="45"/>
-      <c r="BJ42" s="45"/>
-      <c r="BK42" s="45"/>
-      <c r="BM42" s="2"/>
-      <c r="BN42"/>
-      <c r="BO42"/>
-    </row>
-    <row r="43" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY43" s="9"/>
-      <c r="AZ43" s="2"/>
-      <c r="BA43" s="2"/>
-      <c r="BB43" s="162"/>
-      <c r="BC43" s="45"/>
-      <c r="BJ43" s="45"/>
-      <c r="BK43" s="45"/>
-      <c r="BM43" s="2"/>
-      <c r="BN43"/>
-      <c r="BO43"/>
-    </row>
-    <row r="44" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY44" s="9"/>
-      <c r="AZ44" s="2"/>
-      <c r="BA44" s="2"/>
-      <c r="BB44" s="162"/>
-      <c r="BC44" s="45"/>
-      <c r="BJ44" s="45"/>
-      <c r="BK44" s="45"/>
-      <c r="BM44" s="2"/>
-      <c r="BN44"/>
-      <c r="BO44"/>
-    </row>
-    <row r="45" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY45" s="9"/>
-      <c r="AZ45" s="2"/>
-      <c r="BA45" s="2"/>
-      <c r="BB45" s="162"/>
-      <c r="BC45" s="45"/>
-      <c r="BJ45" s="45"/>
-      <c r="BK45" s="45"/>
-      <c r="BM45" s="2"/>
-      <c r="BN45"/>
-      <c r="BO45"/>
-    </row>
-    <row r="46" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY46" s="9"/>
-      <c r="AZ46" s="2"/>
-      <c r="BA46" s="2"/>
-      <c r="BB46" s="162"/>
-      <c r="BC46" s="45"/>
-      <c r="BJ46" s="45"/>
-      <c r="BK46" s="45"/>
-      <c r="BM46" s="2"/>
-      <c r="BN46"/>
-      <c r="BO46"/>
-    </row>
-    <row r="47" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY47" s="9"/>
-      <c r="AZ47" s="2"/>
-      <c r="BA47" s="2"/>
-      <c r="BB47" s="162"/>
-      <c r="BC47" s="45"/>
-      <c r="BJ47" s="45"/>
-      <c r="BK47" s="45"/>
-      <c r="BM47" s="2"/>
-      <c r="BN47"/>
-      <c r="BO47"/>
-    </row>
-    <row r="48" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY48" s="9"/>
-      <c r="AZ48" s="2"/>
-      <c r="BA48" s="2"/>
-      <c r="BB48" s="162"/>
-      <c r="BC48" s="45"/>
-      <c r="BJ48" s="45"/>
-      <c r="BK48" s="45"/>
-      <c r="BM48" s="2"/>
-      <c r="BN48"/>
-      <c r="BO48"/>
-    </row>
-    <row r="49" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY49" s="9"/>
-      <c r="AZ49" s="2"/>
-      <c r="BA49" s="2"/>
-      <c r="BB49" s="162"/>
-      <c r="BC49" s="45"/>
-      <c r="BJ49" s="45"/>
-      <c r="BK49" s="45"/>
-      <c r="BM49" s="2"/>
-      <c r="BN49"/>
-      <c r="BO49"/>
-    </row>
-    <row r="50" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY50" s="9"/>
-      <c r="AZ50" s="2"/>
-      <c r="BA50" s="2"/>
-      <c r="BB50" s="162"/>
-      <c r="BC50" s="45"/>
-      <c r="BJ50" s="45"/>
-      <c r="BK50" s="45"/>
-      <c r="BM50" s="2"/>
-      <c r="BN50"/>
-      <c r="BO50"/>
-    </row>
-    <row r="51" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY51" s="9"/>
-      <c r="AZ51" s="2"/>
-      <c r="BA51" s="2"/>
-      <c r="BB51" s="162"/>
-      <c r="BC51" s="45"/>
-      <c r="BJ51" s="45"/>
-      <c r="BK51" s="45"/>
-      <c r="BM51" s="2"/>
-      <c r="BN51"/>
-      <c r="BO51"/>
-    </row>
-    <row r="52" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY52" s="9"/>
-      <c r="AZ52" s="2"/>
-      <c r="BA52" s="2"/>
-      <c r="BB52" s="162"/>
-      <c r="BC52" s="45"/>
-      <c r="BJ52" s="45"/>
-      <c r="BK52" s="45"/>
-      <c r="BM52" s="2"/>
-      <c r="BN52"/>
-      <c r="BO52"/>
-    </row>
-    <row r="53" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY53" s="9"/>
-      <c r="AZ53" s="2"/>
-      <c r="BA53" s="2"/>
-      <c r="BB53" s="162"/>
-      <c r="BC53" s="45"/>
-      <c r="BJ53" s="45"/>
-      <c r="BK53" s="45"/>
-      <c r="BM53" s="2"/>
-      <c r="BN53"/>
-      <c r="BO53"/>
-    </row>
-    <row r="54" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY54" s="9"/>
-      <c r="AZ54" s="2"/>
-      <c r="BA54" s="2"/>
-      <c r="BB54" s="162"/>
-      <c r="BC54" s="45"/>
-      <c r="BJ54" s="45"/>
-      <c r="BK54" s="45"/>
-      <c r="BM54" s="2"/>
-      <c r="BN54"/>
-      <c r="BO54"/>
-    </row>
-    <row r="55" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY55" s="9"/>
-      <c r="AZ55" s="2"/>
-      <c r="BA55" s="2"/>
-      <c r="BB55" s="162"/>
-      <c r="BC55" s="45"/>
-      <c r="BJ55" s="45"/>
-      <c r="BK55" s="45"/>
-      <c r="BM55" s="2"/>
-      <c r="BN55"/>
-      <c r="BO55"/>
-    </row>
-    <row r="56" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY56" s="9"/>
-      <c r="AZ56" s="2"/>
-      <c r="BA56" s="2"/>
-      <c r="BB56" s="162"/>
-      <c r="BC56" s="45"/>
-      <c r="BJ56" s="45"/>
-      <c r="BK56" s="45"/>
-      <c r="BM56" s="2"/>
-      <c r="BN56"/>
-      <c r="BO56"/>
-    </row>
-    <row r="57" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY57" s="9"/>
-      <c r="AZ57" s="2"/>
-      <c r="BA57" s="2"/>
-      <c r="BB57" s="162"/>
-      <c r="BC57" s="45"/>
-      <c r="BJ57" s="45"/>
-      <c r="BK57" s="45"/>
-      <c r="BM57" s="2"/>
-      <c r="BN57"/>
-      <c r="BO57"/>
-    </row>
-    <row r="58" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY58" s="9"/>
-      <c r="AZ58" s="2"/>
-      <c r="BA58" s="2"/>
-      <c r="BB58" s="162"/>
-      <c r="BC58" s="45"/>
-      <c r="BJ58" s="45"/>
-      <c r="BK58" s="45"/>
-      <c r="BM58" s="2"/>
-      <c r="BN58"/>
-      <c r="BO58"/>
-    </row>
-    <row r="59" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY59" s="9"/>
-      <c r="AZ59" s="2"/>
-      <c r="BA59" s="2"/>
-      <c r="BB59" s="162"/>
-      <c r="BC59" s="45"/>
-      <c r="BJ59" s="45"/>
-      <c r="BK59" s="45"/>
-      <c r="BM59" s="2"/>
-      <c r="BN59"/>
-      <c r="BO59"/>
-    </row>
-    <row r="60" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY60" s="9"/>
-      <c r="AZ60" s="2"/>
-      <c r="BA60" s="2"/>
-      <c r="BB60" s="162"/>
-      <c r="BC60" s="45"/>
-      <c r="BJ60" s="45"/>
-      <c r="BK60" s="45"/>
-      <c r="BM60" s="2"/>
-      <c r="BN60"/>
-      <c r="BO60"/>
-    </row>
-    <row r="61" spans="51:67" x14ac:dyDescent="0.25">
-      <c r="AY61" s="9"/>
-      <c r="AZ61" s="2"/>
-      <c r="BA61" s="2"/>
-      <c r="BB61" s="162"/>
-      <c r="BC61" s="45"/>
-      <c r="BJ61" s="45"/>
-      <c r="BK61" s="45"/>
-      <c r="BM61" s="2"/>
-      <c r="BN61"/>
-      <c r="BO61"/>
+      <c r="BJ29" s="8"/>
+      <c r="BK29" s="8"/>
+      <c r="BL29" s="6"/>
+      <c r="BM29" s="7"/>
+      <c r="BN29" s="48"/>
+      <c r="BO29" s="64"/>
+      <c r="BP29" s="64"/>
+      <c r="BQ29" s="6"/>
+    </row>
+    <row r="33" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA33" s="9"/>
+      <c r="BB33" s="2"/>
+      <c r="BC33" s="2"/>
+      <c r="BD33" s="162"/>
+      <c r="BE33" s="45"/>
+      <c r="BL33" s="45"/>
+      <c r="BM33" s="45"/>
+      <c r="BO33" s="2"/>
+      <c r="BP33"/>
+      <c r="BQ33"/>
+    </row>
+    <row r="34" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA34" s="9"/>
+      <c r="BB34" s="2"/>
+      <c r="BC34" s="2"/>
+      <c r="BD34" s="162"/>
+      <c r="BE34" s="45"/>
+      <c r="BL34" s="45"/>
+      <c r="BM34" s="45"/>
+      <c r="BO34" s="2"/>
+      <c r="BP34"/>
+      <c r="BQ34"/>
+    </row>
+    <row r="35" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA35" s="9"/>
+      <c r="BB35" s="2"/>
+      <c r="BC35" s="2"/>
+      <c r="BD35" s="162"/>
+      <c r="BE35" s="45"/>
+      <c r="BL35" s="45"/>
+      <c r="BM35" s="45"/>
+      <c r="BO35" s="2"/>
+      <c r="BP35"/>
+      <c r="BQ35"/>
+    </row>
+    <row r="36" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA36" s="9"/>
+      <c r="BB36" s="2"/>
+      <c r="BC36" s="2"/>
+      <c r="BD36" s="162"/>
+      <c r="BE36" s="45"/>
+      <c r="BL36" s="45"/>
+      <c r="BM36" s="45"/>
+      <c r="BO36" s="2"/>
+      <c r="BP36"/>
+      <c r="BQ36"/>
+    </row>
+    <row r="37" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA37" s="9"/>
+      <c r="BB37" s="2"/>
+      <c r="BC37" s="2"/>
+      <c r="BD37" s="162"/>
+      <c r="BE37" s="45"/>
+      <c r="BL37" s="45"/>
+      <c r="BM37" s="45"/>
+      <c r="BO37" s="2"/>
+      <c r="BP37"/>
+      <c r="BQ37"/>
+    </row>
+    <row r="38" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA38" s="9"/>
+      <c r="BB38" s="2"/>
+      <c r="BC38" s="2"/>
+      <c r="BD38" s="162"/>
+      <c r="BE38" s="45"/>
+      <c r="BL38" s="45"/>
+      <c r="BM38" s="45"/>
+      <c r="BO38" s="2"/>
+      <c r="BP38"/>
+      <c r="BQ38"/>
+    </row>
+    <row r="39" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA39" s="9"/>
+      <c r="BB39" s="2"/>
+      <c r="BC39" s="2"/>
+      <c r="BD39" s="162"/>
+      <c r="BE39" s="45"/>
+      <c r="BL39" s="45"/>
+      <c r="BM39" s="45"/>
+      <c r="BO39" s="2"/>
+      <c r="BP39"/>
+      <c r="BQ39"/>
+    </row>
+    <row r="40" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA40" s="9"/>
+      <c r="BB40" s="2"/>
+      <c r="BC40" s="2"/>
+      <c r="BD40" s="162"/>
+      <c r="BE40" s="45"/>
+      <c r="BL40" s="45"/>
+      <c r="BM40" s="45"/>
+      <c r="BO40" s="2"/>
+      <c r="BP40"/>
+      <c r="BQ40"/>
+    </row>
+    <row r="41" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA41" s="9"/>
+      <c r="BB41" s="2"/>
+      <c r="BC41" s="2"/>
+      <c r="BD41" s="162"/>
+      <c r="BE41" s="45"/>
+      <c r="BL41" s="45"/>
+      <c r="BM41" s="45"/>
+      <c r="BO41" s="2"/>
+      <c r="BP41"/>
+      <c r="BQ41"/>
+    </row>
+    <row r="42" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA42" s="9"/>
+      <c r="BB42" s="2"/>
+      <c r="BC42" s="2"/>
+      <c r="BD42" s="162"/>
+      <c r="BE42" s="45"/>
+      <c r="BL42" s="45"/>
+      <c r="BM42" s="45"/>
+      <c r="BO42" s="2"/>
+      <c r="BP42"/>
+      <c r="BQ42"/>
+    </row>
+    <row r="43" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA43" s="9"/>
+      <c r="BB43" s="2"/>
+      <c r="BC43" s="2"/>
+      <c r="BD43" s="162"/>
+      <c r="BE43" s="45"/>
+      <c r="BL43" s="45"/>
+      <c r="BM43" s="45"/>
+      <c r="BO43" s="2"/>
+      <c r="BP43"/>
+      <c r="BQ43"/>
+    </row>
+    <row r="44" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA44" s="9"/>
+      <c r="BB44" s="2"/>
+      <c r="BC44" s="2"/>
+      <c r="BD44" s="162"/>
+      <c r="BE44" s="45"/>
+      <c r="BL44" s="45"/>
+      <c r="BM44" s="45"/>
+      <c r="BO44" s="2"/>
+      <c r="BP44"/>
+      <c r="BQ44"/>
+    </row>
+    <row r="45" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA45" s="9"/>
+      <c r="BB45" s="2"/>
+      <c r="BC45" s="2"/>
+      <c r="BD45" s="162"/>
+      <c r="BE45" s="45"/>
+      <c r="BL45" s="45"/>
+      <c r="BM45" s="45"/>
+      <c r="BO45" s="2"/>
+      <c r="BP45"/>
+      <c r="BQ45"/>
+    </row>
+    <row r="46" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA46" s="9"/>
+      <c r="BB46" s="2"/>
+      <c r="BC46" s="2"/>
+      <c r="BD46" s="162"/>
+      <c r="BE46" s="45"/>
+      <c r="BL46" s="45"/>
+      <c r="BM46" s="45"/>
+      <c r="BO46" s="2"/>
+      <c r="BP46"/>
+      <c r="BQ46"/>
+    </row>
+    <row r="47" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA47" s="9"/>
+      <c r="BB47" s="2"/>
+      <c r="BC47" s="2"/>
+      <c r="BD47" s="162"/>
+      <c r="BE47" s="45"/>
+      <c r="BL47" s="45"/>
+      <c r="BM47" s="45"/>
+      <c r="BO47" s="2"/>
+      <c r="BP47"/>
+      <c r="BQ47"/>
+    </row>
+    <row r="48" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA48" s="9"/>
+      <c r="BB48" s="2"/>
+      <c r="BC48" s="2"/>
+      <c r="BD48" s="162"/>
+      <c r="BE48" s="45"/>
+      <c r="BL48" s="45"/>
+      <c r="BM48" s="45"/>
+      <c r="BO48" s="2"/>
+      <c r="BP48"/>
+      <c r="BQ48"/>
+    </row>
+    <row r="49" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA49" s="9"/>
+      <c r="BB49" s="2"/>
+      <c r="BC49" s="2"/>
+      <c r="BD49" s="162"/>
+      <c r="BE49" s="45"/>
+      <c r="BL49" s="45"/>
+      <c r="BM49" s="45"/>
+      <c r="BO49" s="2"/>
+      <c r="BP49"/>
+      <c r="BQ49"/>
+    </row>
+    <row r="50" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA50" s="9"/>
+      <c r="BB50" s="2"/>
+      <c r="BC50" s="2"/>
+      <c r="BD50" s="162"/>
+      <c r="BE50" s="45"/>
+      <c r="BL50" s="45"/>
+      <c r="BM50" s="45"/>
+      <c r="BO50" s="2"/>
+      <c r="BP50"/>
+      <c r="BQ50"/>
+    </row>
+    <row r="51" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA51" s="9"/>
+      <c r="BB51" s="2"/>
+      <c r="BC51" s="2"/>
+      <c r="BD51" s="162"/>
+      <c r="BE51" s="45"/>
+      <c r="BL51" s="45"/>
+      <c r="BM51" s="45"/>
+      <c r="BO51" s="2"/>
+      <c r="BP51"/>
+      <c r="BQ51"/>
+    </row>
+    <row r="52" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA52" s="9"/>
+      <c r="BB52" s="2"/>
+      <c r="BC52" s="2"/>
+      <c r="BD52" s="162"/>
+      <c r="BE52" s="45"/>
+      <c r="BL52" s="45"/>
+      <c r="BM52" s="45"/>
+      <c r="BO52" s="2"/>
+      <c r="BP52"/>
+      <c r="BQ52"/>
+    </row>
+    <row r="53" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA53" s="9"/>
+      <c r="BB53" s="2"/>
+      <c r="BC53" s="2"/>
+      <c r="BD53" s="162"/>
+      <c r="BE53" s="45"/>
+      <c r="BL53" s="45"/>
+      <c r="BM53" s="45"/>
+      <c r="BO53" s="2"/>
+      <c r="BP53"/>
+      <c r="BQ53"/>
+    </row>
+    <row r="54" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA54" s="9"/>
+      <c r="BB54" s="2"/>
+      <c r="BC54" s="2"/>
+      <c r="BD54" s="162"/>
+      <c r="BE54" s="45"/>
+      <c r="BL54" s="45"/>
+      <c r="BM54" s="45"/>
+      <c r="BO54" s="2"/>
+      <c r="BP54"/>
+      <c r="BQ54"/>
+    </row>
+    <row r="55" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA55" s="9"/>
+      <c r="BB55" s="2"/>
+      <c r="BC55" s="2"/>
+      <c r="BD55" s="162"/>
+      <c r="BE55" s="45"/>
+      <c r="BL55" s="45"/>
+      <c r="BM55" s="45"/>
+      <c r="BO55" s="2"/>
+      <c r="BP55"/>
+      <c r="BQ55"/>
+    </row>
+    <row r="56" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA56" s="9"/>
+      <c r="BB56" s="2"/>
+      <c r="BC56" s="2"/>
+      <c r="BD56" s="162"/>
+      <c r="BE56" s="45"/>
+      <c r="BL56" s="45"/>
+      <c r="BM56" s="45"/>
+      <c r="BO56" s="2"/>
+      <c r="BP56"/>
+      <c r="BQ56"/>
+    </row>
+    <row r="57" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA57" s="9"/>
+      <c r="BB57" s="2"/>
+      <c r="BC57" s="2"/>
+      <c r="BD57" s="162"/>
+      <c r="BE57" s="45"/>
+      <c r="BL57" s="45"/>
+      <c r="BM57" s="45"/>
+      <c r="BO57" s="2"/>
+      <c r="BP57"/>
+      <c r="BQ57"/>
+    </row>
+    <row r="58" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA58" s="9"/>
+      <c r="BB58" s="2"/>
+      <c r="BC58" s="2"/>
+      <c r="BD58" s="162"/>
+      <c r="BE58" s="45"/>
+      <c r="BL58" s="45"/>
+      <c r="BM58" s="45"/>
+      <c r="BO58" s="2"/>
+      <c r="BP58"/>
+      <c r="BQ58"/>
+    </row>
+    <row r="59" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA59" s="9"/>
+      <c r="BB59" s="2"/>
+      <c r="BC59" s="2"/>
+      <c r="BD59" s="162"/>
+      <c r="BE59" s="45"/>
+      <c r="BL59" s="45"/>
+      <c r="BM59" s="45"/>
+      <c r="BO59" s="2"/>
+      <c r="BP59"/>
+      <c r="BQ59"/>
+    </row>
+    <row r="60" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA60" s="9"/>
+      <c r="BB60" s="2"/>
+      <c r="BC60" s="2"/>
+      <c r="BD60" s="162"/>
+      <c r="BE60" s="45"/>
+      <c r="BL60" s="45"/>
+      <c r="BM60" s="45"/>
+      <c r="BO60" s="2"/>
+      <c r="BP60"/>
+      <c r="BQ60"/>
+    </row>
+    <row r="61" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA61" s="9"/>
+      <c r="BB61" s="2"/>
+      <c r="BC61" s="2"/>
+      <c r="BD61" s="162"/>
+      <c r="BE61" s="45"/>
+      <c r="BL61" s="45"/>
+      <c r="BM61" s="45"/>
+      <c r="BO61" s="2"/>
+      <c r="BP61"/>
+      <c r="BQ61"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="BK2:BO2"/>
+    <mergeCell ref="BM2:BQ2"/>
     <mergeCell ref="H2:V2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="W2:AD2"/>
     <mergeCell ref="AE2:AP2"/>
-    <mergeCell ref="AQ2:AX2"/>
-    <mergeCell ref="BD2:BJ2"/>
-    <mergeCell ref="AY2:BC2"/>
+    <mergeCell ref="AQ2:AZ2"/>
+    <mergeCell ref="BF2:BL2"/>
+    <mergeCell ref="BA2:BE2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 A4:G27 AA18:AA29 W4:AB13 AB14:AB30 BK4:BO30 BF4:BJ16 BD4 AY4:AY29 BC4:BC16 BC17:BJ28 AY30:AZ30 BA29:BJ30 BA4:BA28 AC4:AX30">
-    <cfRule type="expression" dxfId="44" priority="35" stopIfTrue="1">
+  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 A4:G27 AA18:AA29 W4:AB13 AB14:AB30 BM4:BQ30 BH4:BL16 BF4 BA4:BA29 BE4:BE16 BE17:BL28 BA30:BB30 BC29:BL30 BC4:BC28 AC4:AZ30">
+    <cfRule type="expression" dxfId="58" priority="35" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="36" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28">
-    <cfRule type="expression" dxfId="42" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="33" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="34" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA16:AA17">
-    <cfRule type="expression" dxfId="40" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="47" stopIfTrue="1">
       <formula>$A15="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="48" stopIfTrue="1">
       <formula>$A15="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA15">
-    <cfRule type="expression" dxfId="38" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="19" stopIfTrue="1">
       <formula>$A14="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="20" stopIfTrue="1">
       <formula>$A14="p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BD5:BD16">
-    <cfRule type="expression" dxfId="36" priority="17" stopIfTrue="1">
+  <conditionalFormatting sqref="BF5:BF16">
+    <cfRule type="expression" dxfId="50" priority="17" stopIfTrue="1">
       <formula>$A5="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="18" stopIfTrue="1">
       <formula>$A5="p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE4:BE16">
-    <cfRule type="expression" dxfId="34" priority="15" stopIfTrue="1">
+  <conditionalFormatting sqref="BG4:BG16">
+    <cfRule type="expression" dxfId="48" priority="15" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="16" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AZ4:AZ29">
-    <cfRule type="expression" dxfId="32" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="BB4:BB29">
+    <cfRule type="expression" dxfId="46" priority="3" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="4" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BB4:BB28">
-    <cfRule type="expression" dxfId="30" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="BD4:BD28">
+    <cfRule type="expression" dxfId="44" priority="1" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="2" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14783,42 +15060,42 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A4:BC21 C29:F32 A29:B33 G29:BC31 I33:BC33 I32:K32 M32:BC32 J22:AI27 AK22:BC27 A22:G27 H20:H28">
-    <cfRule type="expression" dxfId="28" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="15" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="16" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28 J28:AI28 AK28:BC28">
-    <cfRule type="expression" dxfId="26" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="5" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="6" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="24" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="19" stopIfTrue="1">
       <formula>$A32="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="20" stopIfTrue="1">
       <formula>$A32="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I28">
-    <cfRule type="expression" dxfId="22" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="3" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="4" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ22:AJ28">
-    <cfRule type="expression" dxfId="20" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="1" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="2" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46264,31 +46541,31 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="C782:C787 C844:C855 C789:C842">
-    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="1" stopIfTrue="1">
       <formula>$A782=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="2" stopIfTrue="1">
       <formula>$A782=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B336:C353 B764:C769 B301:C303 B4:C10 B297:C299 B38:C49 B25:C36 B496:C528 B12:C23 B844:B855 B315:C326 B530:C539 B541:C550 B728:C743 B745:C748 B750:C758 B332:C334 B771:C780 B328:C330 B760:C760 B762:C762 B305:C313 B355:C358 B782:B787 B552:C561 B51:C131 B133:C213 B215:C295 B360:C494 B563:C616 B673:C726 B618:C671 B789:B842">
-    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="3" stopIfTrue="1">
       <formula>$A4=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="4" stopIfTrue="1">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2 D2:Z2">
-    <cfRule type="cellIs" dxfId="14" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A10 A12:A23 A25:A36 A38:A49 A297:A299 A301:A303 A305:A313 A315:A326 A328:A330 A332:A334 A336:A353 A355:A358 A496:A528 A530:A539 A541:A550 A552:A561 A745:A748 A750:A758 A760 A762 A764:A769 A771:A780 A782:A787 A844:A855 A51:A131 A133:A213 A215:A295 A360:A494 A563:A616 A673:A726 A618:A671 A728:A743 A789:A842">
-    <cfRule type="cellIs" dxfId="13" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="6" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="7" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
+ added integration for OrcaFlex interface + updated primary FAST input file: removed CompUserPtfmLd and CompUserTwrLd because they aren't used, and updated comment on CompMooring line re: OrcaFlex interface. + added Test 26 to CertTest.bat + removed UserPtfmLd and UserTwrLd from UserSubs.f90 (were never called anyway)
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1120 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -36,7 +36,7 @@
     <definedName name="_Toc46290869" localSheetId="2">Variables!$B$770</definedName>
     <definedName name="_Toc46290870" localSheetId="2">Variables!$B$781</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">TestMatrix!$B$2:$AX$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'TestMatrix (new)'!$B$2:$BE$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'TestMatrix (new)'!$B$2:$BE$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Variables!$B$1:$P$855</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="1145">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3478,6 +3478,12 @@
   </si>
   <si>
     <t>Tower Aero</t>
+  </si>
+  <si>
+    <t>Test26</t>
+  </si>
+  <si>
+    <t>Flexible, DLL control, tower potential flow and drag, turbulence - using BeamDyn</t>
   </si>
 </sst>
 </file>
@@ -3588,7 +3594,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -4179,12 +4185,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4713,12 +4780,252 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="47" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="63">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -5270,13 +5577,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BQ61"/>
+  <dimension ref="A1:BQ62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="AE7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="AU13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AU12" sqref="AU12"/>
+      <selection pane="bottomRight" activeCell="BQ29" sqref="BQ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5303,8 +5610,7 @@
     <col min="28" max="28" width="3.33203125" style="2" customWidth="1"/>
     <col min="29" max="30" width="5.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="3.33203125" style="2" customWidth="1"/>
-    <col min="33" max="34" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="4" style="2" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="4.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="36" max="42" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="43" max="47" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -10358,89 +10664,267 @@
       </c>
       <c r="BQ28" s="42"/>
     </row>
-    <row r="29" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="5"/>
-      <c r="C29" s="149"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="139"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4" t="s">
+    <row r="29" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="27"/>
+      <c r="B29" s="192" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C29" s="193" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D29" s="194">
+        <v>3</v>
+      </c>
+      <c r="E29" s="25">
+        <v>126</v>
+      </c>
+      <c r="F29" s="25">
+        <v>5000</v>
+      </c>
+      <c r="G29" s="143" t="s">
+        <v>1144</v>
+      </c>
+      <c r="H29" s="195">
+        <v>20</v>
+      </c>
+      <c r="I29" s="196">
+        <v>1E-3</v>
+      </c>
+      <c r="J29" s="194">
+        <v>2</v>
+      </c>
+      <c r="K29" s="194">
+        <v>0</v>
+      </c>
+      <c r="L29" s="25">
+        <v>99999</v>
+      </c>
+      <c r="M29" s="194">
+        <v>2</v>
+      </c>
+      <c r="N29" s="194">
+        <v>2</v>
+      </c>
+      <c r="O29" s="194">
+        <v>1</v>
+      </c>
+      <c r="P29" s="194">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="194">
+        <v>0</v>
+      </c>
+      <c r="R29" s="194">
+        <v>0</v>
+      </c>
+      <c r="S29" s="194">
+        <v>0</v>
+      </c>
+      <c r="T29" s="196">
+        <f>I29</f>
+        <v>1E-3</v>
+      </c>
+      <c r="U29" s="194">
+        <v>0</v>
+      </c>
+      <c r="V29" s="197">
+        <v>2</v>
+      </c>
+      <c r="W29" s="43">
+        <v>0</v>
+      </c>
+      <c r="X29" s="25">
+        <v>5</v>
+      </c>
+      <c r="Y29" s="25">
+        <v>5</v>
+      </c>
+      <c r="Z29" s="25">
+        <v>2</v>
+      </c>
+      <c r="AA29" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB29" s="25">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD29" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE29" s="40"/>
+      <c r="AF29" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG29" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH29" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI29" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP29" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ29" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR29" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS29" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT29" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU29" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV29" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AW29" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AX29" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY29" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AZ29" s="197"/>
+      <c r="BA29" s="43">
+        <v>3</v>
+      </c>
+      <c r="BB29" s="151">
+        <v>0</v>
+      </c>
+      <c r="BC29" s="151">
+        <v>12</v>
+      </c>
+      <c r="BD29" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="BE29" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="BF29" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG29" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH29" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI29" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ29" s="198"/>
+      <c r="BK29" s="198"/>
+      <c r="BL29" s="197"/>
+      <c r="BM29" s="199"/>
+      <c r="BN29" s="200"/>
+      <c r="BO29" s="201"/>
+      <c r="BP29" s="201" t="s">
+        <v>1050</v>
+      </c>
+      <c r="BQ29" s="197"/>
+    </row>
+    <row r="30" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="5"/>
+      <c r="C30" s="149"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="139"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4" t="s">
         <v>1102</v>
       </c>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="6"/>
-      <c r="W29" s="7"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
-      <c r="AA29" s="4"/>
-      <c r="AB29" s="4"/>
-      <c r="AC29" s="8"/>
-      <c r="AD29" s="8"/>
-      <c r="AE29" s="5"/>
-      <c r="AF29" s="7"/>
-      <c r="AG29" s="4"/>
-      <c r="AH29" s="4"/>
-      <c r="AI29" s="4"/>
-      <c r="AJ29" s="4"/>
-      <c r="AK29" s="4"/>
-      <c r="AL29" s="4"/>
-      <c r="AM29" s="4"/>
-      <c r="AN29" s="4"/>
-      <c r="AO29" s="4"/>
-      <c r="AP29" s="6"/>
-      <c r="AQ29" s="7"/>
-      <c r="AR29" s="4"/>
-      <c r="AS29" s="8"/>
-      <c r="AT29" s="8"/>
-      <c r="AU29" s="8"/>
-      <c r="AV29" s="8"/>
-      <c r="AW29" s="8"/>
-      <c r="AX29" s="8"/>
-      <c r="AY29" s="8"/>
-      <c r="AZ29" s="6"/>
-      <c r="BA29" s="7"/>
-      <c r="BB29" s="153"/>
-      <c r="BC29" s="153"/>
-      <c r="BD29" s="161"/>
-      <c r="BE29" s="6"/>
-      <c r="BF29" s="100"/>
-      <c r="BG29" s="8"/>
-      <c r="BH29" s="8"/>
-      <c r="BI29" s="8"/>
-      <c r="BJ29" s="8"/>
-      <c r="BK29" s="8"/>
-      <c r="BL29" s="6"/>
-      <c r="BM29" s="7"/>
-      <c r="BN29" s="48"/>
-      <c r="BO29" s="64"/>
-      <c r="BP29" s="64"/>
-      <c r="BQ29" s="6"/>
-    </row>
-    <row r="33" spans="53:69" x14ac:dyDescent="0.25">
-      <c r="BA33" s="9"/>
-      <c r="BB33" s="2"/>
-      <c r="BC33" s="2"/>
-      <c r="BD33" s="162"/>
-      <c r="BE33" s="45"/>
-      <c r="BL33" s="45"/>
-      <c r="BM33" s="45"/>
-      <c r="BO33" s="2"/>
-      <c r="BP33"/>
-      <c r="BQ33"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="8"/>
+      <c r="AD30" s="8"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="7"/>
+      <c r="AG30" s="4"/>
+      <c r="AH30" s="4"/>
+      <c r="AI30" s="4"/>
+      <c r="AJ30" s="4"/>
+      <c r="AK30" s="4"/>
+      <c r="AL30" s="4"/>
+      <c r="AM30" s="4"/>
+      <c r="AN30" s="4"/>
+      <c r="AO30" s="4"/>
+      <c r="AP30" s="6"/>
+      <c r="AQ30" s="7"/>
+      <c r="AR30" s="4"/>
+      <c r="AS30" s="8"/>
+      <c r="AT30" s="8"/>
+      <c r="AU30" s="8"/>
+      <c r="AV30" s="8"/>
+      <c r="AW30" s="8"/>
+      <c r="AX30" s="8"/>
+      <c r="AY30" s="8"/>
+      <c r="AZ30" s="6"/>
+      <c r="BA30" s="7"/>
+      <c r="BB30" s="153"/>
+      <c r="BC30" s="153"/>
+      <c r="BD30" s="161"/>
+      <c r="BE30" s="6"/>
+      <c r="BF30" s="100"/>
+      <c r="BG30" s="8"/>
+      <c r="BH30" s="8"/>
+      <c r="BI30" s="8"/>
+      <c r="BJ30" s="8"/>
+      <c r="BK30" s="8"/>
+      <c r="BL30" s="6"/>
+      <c r="BM30" s="7"/>
+      <c r="BN30" s="48"/>
+      <c r="BO30" s="64"/>
+      <c r="BP30" s="64"/>
+      <c r="BQ30" s="6"/>
     </row>
     <row r="34" spans="53:69" x14ac:dyDescent="0.25">
       <c r="BA34" s="9"/>
@@ -10778,6 +11262,18 @@
       <c r="BP61"/>
       <c r="BQ61"/>
     </row>
+    <row r="62" spans="53:69" x14ac:dyDescent="0.25">
+      <c r="BA62" s="9"/>
+      <c r="BB62" s="2"/>
+      <c r="BC62" s="2"/>
+      <c r="BD62" s="162"/>
+      <c r="BE62" s="45"/>
+      <c r="BL62" s="45"/>
+      <c r="BM62" s="45"/>
+      <c r="BO62" s="2"/>
+      <c r="BP62"/>
+      <c r="BQ62"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="BM2:BQ2"/>
@@ -10789,68 +11285,108 @@
     <mergeCell ref="BF2:BL2"/>
     <mergeCell ref="BA2:BE2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A29:G30 W14:Z30 H4:V30 AA14 A4:G27 AA18:AA29 W4:AB13 AB14:AB30 BM4:BQ30 BH4:BL16 BF4 BA4:BA29 BE4:BE16 BE17:BL28 BA30:BB30 BC29:BL30 BC4:BC28 AC4:AZ30">
-    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
+  <conditionalFormatting sqref="A30:G31 W14:Z28 AA14 A4:G27 AA18:AA28 W4:AB13 AB14:AB28 BM4:BQ31 BH4:BL16 BF4 BE4:BE16 BE17:BL28 BA31:BB31 BC30:BL31 BC4:BC28 AC4:BA28 H4:V31 AB30:AZ31 AA30 W30:Z31 AE29:AZ29 BA30 BF29:BL29">
+    <cfRule type="expression" dxfId="62" priority="45" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="46" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A28:G28">
-    <cfRule type="expression" dxfId="30" priority="33" stopIfTrue="1">
+  <conditionalFormatting sqref="A28:G28 A29:F29">
+    <cfRule type="expression" dxfId="60" priority="43" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="44" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA16:AA17">
-    <cfRule type="expression" dxfId="28" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="57" stopIfTrue="1">
       <formula>$A15="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="58" stopIfTrue="1">
       <formula>$A15="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA15">
-    <cfRule type="expression" dxfId="26" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="29" stopIfTrue="1">
       <formula>$A14="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="30" stopIfTrue="1">
       <formula>$A14="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF5:BF16">
-    <cfRule type="expression" dxfId="24" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="27" stopIfTrue="1">
       <formula>$A5="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="28" stopIfTrue="1">
       <formula>$A5="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG4:BG16">
-    <cfRule type="expression" dxfId="22" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="25" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="26" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BB4:BB29">
-    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="BB4:BB28 BB30">
+    <cfRule type="expression" dxfId="50" priority="13" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="14" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD4:BD28">
-    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="11" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="12" stopIfTrue="1">
       <formula>$A4="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G29">
+    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
+      <formula>$A29="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="10" stopIfTrue="1">
+      <formula>$A29="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W29:AD29">
+    <cfRule type="expression" dxfId="21" priority="7" stopIfTrue="1">
+      <formula>$A29="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="8" stopIfTrue="1">
+      <formula>$A29="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BE29 BC29 BA29">
+    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+      <formula>$A29="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+      <formula>$A29="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB29">
+    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
+      <formula>$A29="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
+      <formula>$A29="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BD29">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+      <formula>$A29="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+      <formula>$A29="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>
@@ -14864,42 +15400,42 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A4:BC21 C29:F32 A29:B33 G29:BC31 I33:BC33 I32:K32 M32:BC32 J22:AI27 AK22:BC27 A22:G27 H20:H28">
-    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="15" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="16" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28 J28:AI28 AK28:BC28">
-    <cfRule type="expression" dxfId="14" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="5" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="6" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="12" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="19" stopIfTrue="1">
       <formula>$A32="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="20" stopIfTrue="1">
       <formula>$A32="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I28">
-    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="3" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="4" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ22:AJ28">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="1" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="2" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46345,31 +46881,31 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="C782:C787 C844:C855 C789:C842">
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="1" stopIfTrue="1">
       <formula>$A782=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="2" stopIfTrue="1">
       <formula>$A782=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B336:C353 B764:C769 B301:C303 B4:C10 B297:C299 B38:C49 B25:C36 B496:C528 B12:C23 B844:B855 B315:C326 B530:C539 B541:C550 B728:C743 B745:C748 B750:C758 B332:C334 B771:C780 B328:C330 B760:C760 B762:C762 B305:C313 B355:C358 B782:B787 B552:C561 B51:C131 B133:C213 B215:C295 B360:C494 B563:C616 B673:C726 B618:C671 B789:B842">
-    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="3" stopIfTrue="1">
       <formula>$A4=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="4" stopIfTrue="1">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2 D2:Z2">
-    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A10 A12:A23 A25:A36 A38:A49 A297:A299 A301:A303 A305:A313 A315:A326 A328:A330 A332:A334 A336:A353 A355:A358 A496:A528 A530:A539 A541:A550 A552:A561 A745:A748 A750:A758 A760 A762 A764:A769 A771:A780 A782:A787 A844:A855 A51:A131 A133:A213 A215:A295 A360:A494 A563:A616 A673:A726 A618:A671 A728:A743 A789:A842">
-    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="6" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="7" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added MoorDyn to test 25 and FEAMooring to test 23.
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1156 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -4705,6 +4705,36 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="47" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4780,42 +4810,43 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="47" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="43">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="12"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -4829,6 +4860,30 @@
         <extend val="0"/>
         <color indexed="10"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="53"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4899,201 +4954,6 @@
         <extend val="0"/>
         <color indexed="10"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="12"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="53"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5580,10 +5440,10 @@
   <dimension ref="A1:BQ62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="AU13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="H19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BQ29" sqref="BQ29"/>
+      <selection pane="bottomRight" activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5634,90 +5494,90 @@
   <sheetData>
     <row r="1" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="183" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="170" t="s">
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="180" t="s">
         <v>1104</v>
       </c>
-      <c r="I2" s="171"/>
-      <c r="J2" s="171"/>
-      <c r="K2" s="171"/>
-      <c r="L2" s="171"/>
-      <c r="M2" s="171"/>
-      <c r="N2" s="171"/>
-      <c r="O2" s="171"/>
-      <c r="P2" s="171"/>
-      <c r="Q2" s="171"/>
-      <c r="R2" s="171"/>
-      <c r="S2" s="171"/>
-      <c r="T2" s="171"/>
-      <c r="U2" s="171"/>
-      <c r="V2" s="172"/>
-      <c r="W2" s="168" t="s">
+      <c r="I2" s="181"/>
+      <c r="J2" s="181"/>
+      <c r="K2" s="181"/>
+      <c r="L2" s="181"/>
+      <c r="M2" s="181"/>
+      <c r="N2" s="181"/>
+      <c r="O2" s="181"/>
+      <c r="P2" s="181"/>
+      <c r="Q2" s="181"/>
+      <c r="R2" s="181"/>
+      <c r="S2" s="181"/>
+      <c r="T2" s="181"/>
+      <c r="U2" s="181"/>
+      <c r="V2" s="182"/>
+      <c r="W2" s="178" t="s">
         <v>1110</v>
       </c>
-      <c r="X2" s="176"/>
-      <c r="Y2" s="176"/>
-      <c r="Z2" s="176"/>
-      <c r="AA2" s="176"/>
-      <c r="AB2" s="176"/>
-      <c r="AC2" s="176"/>
-      <c r="AD2" s="177"/>
-      <c r="AE2" s="178" t="s">
+      <c r="X2" s="186"/>
+      <c r="Y2" s="186"/>
+      <c r="Z2" s="186"/>
+      <c r="AA2" s="186"/>
+      <c r="AB2" s="186"/>
+      <c r="AC2" s="186"/>
+      <c r="AD2" s="187"/>
+      <c r="AE2" s="188" t="s">
         <v>1126</v>
       </c>
-      <c r="AF2" s="179"/>
-      <c r="AG2" s="179"/>
-      <c r="AH2" s="179"/>
-      <c r="AI2" s="179"/>
-      <c r="AJ2" s="179"/>
-      <c r="AK2" s="179"/>
-      <c r="AL2" s="179"/>
-      <c r="AM2" s="179"/>
-      <c r="AN2" s="179"/>
-      <c r="AO2" s="179"/>
-      <c r="AP2" s="180"/>
-      <c r="AQ2" s="181" t="s">
+      <c r="AF2" s="189"/>
+      <c r="AG2" s="189"/>
+      <c r="AH2" s="189"/>
+      <c r="AI2" s="189"/>
+      <c r="AJ2" s="189"/>
+      <c r="AK2" s="189"/>
+      <c r="AL2" s="189"/>
+      <c r="AM2" s="189"/>
+      <c r="AN2" s="189"/>
+      <c r="AO2" s="189"/>
+      <c r="AP2" s="190"/>
+      <c r="AQ2" s="191" t="s">
         <v>1130</v>
       </c>
-      <c r="AR2" s="182"/>
-      <c r="AS2" s="182"/>
-      <c r="AT2" s="182"/>
-      <c r="AU2" s="182"/>
-      <c r="AV2" s="182"/>
-      <c r="AW2" s="182"/>
-      <c r="AX2" s="182"/>
-      <c r="AY2" s="182"/>
-      <c r="AZ2" s="183"/>
-      <c r="BA2" s="187" t="s">
+      <c r="AR2" s="192"/>
+      <c r="AS2" s="192"/>
+      <c r="AT2" s="192"/>
+      <c r="AU2" s="192"/>
+      <c r="AV2" s="192"/>
+      <c r="AW2" s="192"/>
+      <c r="AX2" s="192"/>
+      <c r="AY2" s="192"/>
+      <c r="AZ2" s="193"/>
+      <c r="BA2" s="197" t="s">
         <v>1138</v>
       </c>
-      <c r="BB2" s="188"/>
-      <c r="BC2" s="188"/>
-      <c r="BD2" s="188"/>
-      <c r="BE2" s="189"/>
-      <c r="BF2" s="184" t="s">
+      <c r="BB2" s="198"/>
+      <c r="BC2" s="198"/>
+      <c r="BD2" s="198"/>
+      <c r="BE2" s="199"/>
+      <c r="BF2" s="194" t="s">
         <v>1129</v>
       </c>
-      <c r="BG2" s="185"/>
-      <c r="BH2" s="185"/>
-      <c r="BI2" s="185"/>
-      <c r="BJ2" s="185"/>
-      <c r="BK2" s="185"/>
-      <c r="BL2" s="186"/>
-      <c r="BM2" s="167" t="s">
+      <c r="BG2" s="195"/>
+      <c r="BH2" s="195"/>
+      <c r="BI2" s="195"/>
+      <c r="BJ2" s="195"/>
+      <c r="BK2" s="195"/>
+      <c r="BL2" s="196"/>
+      <c r="BM2" s="177" t="s">
         <v>1047</v>
       </c>
-      <c r="BN2" s="168"/>
-      <c r="BO2" s="168"/>
-      <c r="BP2" s="168"/>
-      <c r="BQ2" s="169"/>
+      <c r="BN2" s="178"/>
+      <c r="BO2" s="178"/>
+      <c r="BP2" s="178"/>
+      <c r="BQ2" s="179"/>
     </row>
     <row r="3" spans="1:69" s="1" customFormat="1" ht="114.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
@@ -10166,7 +10026,7 @@
         <v>0</v>
       </c>
       <c r="R26" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S26" s="25">
         <v>0</v>
@@ -10532,7 +10392,7 @@
         <v>0</v>
       </c>
       <c r="R28" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S28" s="25">
         <v>0</v>
@@ -10666,13 +10526,13 @@
     </row>
     <row r="29" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
-      <c r="B29" s="192" t="s">
+      <c r="B29" s="167" t="s">
         <v>1143</v>
       </c>
-      <c r="C29" s="193" t="s">
+      <c r="C29" s="168" t="s">
         <v>1089</v>
       </c>
-      <c r="D29" s="194">
+      <c r="D29" s="169">
         <v>3</v>
       </c>
       <c r="E29" s="25">
@@ -10684,50 +10544,50 @@
       <c r="G29" s="143" t="s">
         <v>1144</v>
       </c>
-      <c r="H29" s="195">
+      <c r="H29" s="170">
         <v>20</v>
       </c>
-      <c r="I29" s="196">
+      <c r="I29" s="171">
         <v>1E-3</v>
       </c>
-      <c r="J29" s="194">
+      <c r="J29" s="169">
         <v>2</v>
       </c>
-      <c r="K29" s="194">
+      <c r="K29" s="169">
         <v>0</v>
       </c>
       <c r="L29" s="25">
         <v>99999</v>
       </c>
-      <c r="M29" s="194">
+      <c r="M29" s="169">
         <v>2</v>
       </c>
-      <c r="N29" s="194">
+      <c r="N29" s="169">
         <v>2</v>
       </c>
-      <c r="O29" s="194">
+      <c r="O29" s="169">
         <v>1</v>
       </c>
-      <c r="P29" s="194">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="194">
-        <v>0</v>
-      </c>
-      <c r="R29" s="194">
-        <v>0</v>
-      </c>
-      <c r="S29" s="194">
-        <v>0</v>
-      </c>
-      <c r="T29" s="196">
+      <c r="P29" s="169">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="169">
+        <v>0</v>
+      </c>
+      <c r="R29" s="169">
+        <v>0</v>
+      </c>
+      <c r="S29" s="169">
+        <v>0</v>
+      </c>
+      <c r="T29" s="171">
         <f>I29</f>
         <v>1E-3</v>
       </c>
-      <c r="U29" s="194">
-        <v>0</v>
-      </c>
-      <c r="V29" s="197">
+      <c r="U29" s="169">
+        <v>0</v>
+      </c>
+      <c r="V29" s="172">
         <v>2</v>
       </c>
       <c r="W29" s="43">
@@ -10815,7 +10675,7 @@
       <c r="AY29" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AZ29" s="197"/>
+      <c r="AZ29" s="172"/>
       <c r="BA29" s="43">
         <v>3</v>
       </c>
@@ -10843,16 +10703,16 @@
       <c r="BI29" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BJ29" s="198"/>
-      <c r="BK29" s="198"/>
-      <c r="BL29" s="197"/>
-      <c r="BM29" s="199"/>
-      <c r="BN29" s="200"/>
-      <c r="BO29" s="201"/>
-      <c r="BP29" s="201" t="s">
+      <c r="BJ29" s="173"/>
+      <c r="BK29" s="173"/>
+      <c r="BL29" s="172"/>
+      <c r="BM29" s="174"/>
+      <c r="BN29" s="175"/>
+      <c r="BO29" s="176"/>
+      <c r="BP29" s="176" t="s">
         <v>1050</v>
       </c>
-      <c r="BQ29" s="197"/>
+      <c r="BQ29" s="172"/>
     </row>
     <row r="30" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
@@ -11286,106 +11146,106 @@
     <mergeCell ref="BA2:BE2"/>
   </mergeCells>
   <conditionalFormatting sqref="A30:G31 W14:Z28 AA14 A4:G27 AA18:AA28 W4:AB13 AB14:AB28 BM4:BQ31 BH4:BL16 BF4 BE4:BE16 BE17:BL28 BA31:BB31 BC30:BL31 BC4:BC28 AC4:BA28 H4:V31 AB30:AZ31 AA30 W30:Z31 AE29:AZ29 BA30 BF29:BL29">
-    <cfRule type="expression" dxfId="62" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="45" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="46" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28 A29:F29">
-    <cfRule type="expression" dxfId="60" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="43" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="44" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA16:AA17">
-    <cfRule type="expression" dxfId="58" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="57" stopIfTrue="1">
       <formula>$A15="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="58" stopIfTrue="1">
       <formula>$A15="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA15">
-    <cfRule type="expression" dxfId="56" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="29" stopIfTrue="1">
       <formula>$A14="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="30" stopIfTrue="1">
       <formula>$A14="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF5:BF16">
-    <cfRule type="expression" dxfId="54" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="27" stopIfTrue="1">
       <formula>$A5="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="28" stopIfTrue="1">
       <formula>$A5="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG4:BG16">
-    <cfRule type="expression" dxfId="52" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="25" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="26" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB4:BB28 BB30">
-    <cfRule type="expression" dxfId="50" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="13" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="14" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD4:BD28">
-    <cfRule type="expression" dxfId="48" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="11" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="12" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="9" stopIfTrue="1">
       <formula>$A29="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="10" stopIfTrue="1">
       <formula>$A29="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W29:AD29">
-    <cfRule type="expression" dxfId="21" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="7" stopIfTrue="1">
       <formula>$A29="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="8" stopIfTrue="1">
       <formula>$A29="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE29 BC29 BA29">
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="5" stopIfTrue="1">
       <formula>$A29="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="6" stopIfTrue="1">
       <formula>$A29="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB29">
-    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
       <formula>$A29="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="4" stopIfTrue="1">
       <formula>$A29="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD29">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
       <formula>$A29="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
       <formula>$A29="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11446,74 +11306,74 @@
   <sheetData>
     <row r="1" spans="1:55" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:55" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="173" t="s">
+      <c r="B2" s="183" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="167" t="s">
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="177" t="s">
         <v>1062</v>
       </c>
-      <c r="J2" s="168"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
-      <c r="N2" s="176"/>
-      <c r="O2" s="176"/>
-      <c r="P2" s="176"/>
-      <c r="Q2" s="176"/>
-      <c r="R2" s="176"/>
-      <c r="S2" s="176"/>
-      <c r="T2" s="177"/>
-      <c r="U2" s="178" t="s">
+      <c r="J2" s="178"/>
+      <c r="K2" s="186"/>
+      <c r="L2" s="186"/>
+      <c r="M2" s="186"/>
+      <c r="N2" s="186"/>
+      <c r="O2" s="186"/>
+      <c r="P2" s="186"/>
+      <c r="Q2" s="186"/>
+      <c r="R2" s="186"/>
+      <c r="S2" s="186"/>
+      <c r="T2" s="187"/>
+      <c r="U2" s="188" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="179"/>
-      <c r="W2" s="179"/>
-      <c r="X2" s="179"/>
-      <c r="Y2" s="179"/>
-      <c r="Z2" s="179"/>
-      <c r="AA2" s="179"/>
-      <c r="AB2" s="179"/>
-      <c r="AC2" s="179"/>
-      <c r="AD2" s="179"/>
-      <c r="AE2" s="179"/>
-      <c r="AF2" s="179"/>
-      <c r="AG2" s="179"/>
-      <c r="AH2" s="179"/>
-      <c r="AI2" s="179"/>
-      <c r="AJ2" s="180"/>
-      <c r="AK2" s="190" t="s">
+      <c r="V2" s="189"/>
+      <c r="W2" s="189"/>
+      <c r="X2" s="189"/>
+      <c r="Y2" s="189"/>
+      <c r="Z2" s="189"/>
+      <c r="AA2" s="189"/>
+      <c r="AB2" s="189"/>
+      <c r="AC2" s="189"/>
+      <c r="AD2" s="189"/>
+      <c r="AE2" s="189"/>
+      <c r="AF2" s="189"/>
+      <c r="AG2" s="189"/>
+      <c r="AH2" s="189"/>
+      <c r="AI2" s="189"/>
+      <c r="AJ2" s="190"/>
+      <c r="AK2" s="200" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="182"/>
-      <c r="AM2" s="182"/>
-      <c r="AN2" s="182"/>
-      <c r="AO2" s="182"/>
-      <c r="AP2" s="183"/>
-      <c r="AQ2" s="190" t="s">
+      <c r="AL2" s="192"/>
+      <c r="AM2" s="192"/>
+      <c r="AN2" s="192"/>
+      <c r="AO2" s="192"/>
+      <c r="AP2" s="193"/>
+      <c r="AQ2" s="200" t="s">
         <v>1061</v>
       </c>
-      <c r="AR2" s="181"/>
-      <c r="AS2" s="181"/>
-      <c r="AT2" s="191"/>
-      <c r="AU2" s="187" t="s">
+      <c r="AR2" s="191"/>
+      <c r="AS2" s="191"/>
+      <c r="AT2" s="201"/>
+      <c r="AU2" s="197" t="s">
         <v>18</v>
       </c>
-      <c r="AV2" s="188"/>
-      <c r="AW2" s="188"/>
-      <c r="AX2" s="189"/>
-      <c r="AY2" s="167" t="s">
+      <c r="AV2" s="198"/>
+      <c r="AW2" s="198"/>
+      <c r="AX2" s="199"/>
+      <c r="AY2" s="177" t="s">
         <v>1047</v>
       </c>
-      <c r="AZ2" s="168"/>
-      <c r="BA2" s="168"/>
-      <c r="BB2" s="168"/>
-      <c r="BC2" s="169"/>
+      <c r="AZ2" s="178"/>
+      <c r="BA2" s="178"/>
+      <c r="BB2" s="178"/>
+      <c r="BC2" s="179"/>
     </row>
     <row r="3" spans="1:55" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -15400,42 +15260,42 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A4:BC21 C29:F32 A29:B33 G29:BC31 I33:BC33 I32:K32 M32:BC32 J22:AI27 AK22:BC27 A22:G27 H20:H28">
-    <cfRule type="expression" dxfId="46" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28 J28:AI28 AK28:BC28">
-    <cfRule type="expression" dxfId="44" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="5" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="42" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="19" stopIfTrue="1">
       <formula>$A32="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
       <formula>$A32="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I28">
-    <cfRule type="expression" dxfId="40" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ22:AJ28">
-    <cfRule type="expression" dxfId="38" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46881,31 +46741,31 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="C782:C787 C844:C855 C789:C842">
-    <cfRule type="expression" dxfId="36" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>$A782=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
       <formula>$A782=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B336:C353 B764:C769 B301:C303 B4:C10 B297:C299 B38:C49 B25:C36 B496:C528 B12:C23 B844:B855 B315:C326 B530:C539 B541:C550 B728:C743 B745:C748 B750:C758 B332:C334 B771:C780 B328:C330 B760:C760 B762:C762 B305:C313 B355:C358 B782:B787 B552:C561 B51:C131 B133:C213 B215:C295 B360:C494 B563:C616 B673:C726 B618:C671 B789:B842">
-    <cfRule type="expression" dxfId="34" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>$A4=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2 D2:Z2">
-    <cfRule type="cellIs" dxfId="32" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A10 A12:A23 A25:A36 A38:A49 A297:A299 A301:A303 A305:A313 A315:A326 A328:A330 A332:A334 A336:A353 A355:A358 A496:A528 A530:A539 A541:A550 A552:A561 A745:A748 A750:A758 A760 A762 A764:A769 A771:A780 A782:A787 A844:A855 A51:A131 A133:A213 A215:A295 A360:A494 A563:A616 A673:A726 A618:A671 A728:A743 A789:A842">
-    <cfRule type="cellIs" dxfId="31" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
- added wave surface visualization - modified scripts to update to latest FAST version - updated ReadMe document
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1230 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -5440,10 +5440,10 @@
   <dimension ref="A1:BQ62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="H19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R29" sqref="R29"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5819,7 +5819,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O4" s="25">
         <v>1</v>
@@ -6219,7 +6219,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6" s="25">
         <v>1</v>
@@ -6419,7 +6419,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7" s="25">
         <v>1</v>
@@ -7021,7 +7021,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10" s="25">
         <v>1</v>
@@ -7222,7 +7222,7 @@
         <v>1</v>
       </c>
       <c r="N11" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11" s="25">
         <v>1</v>
@@ -7622,7 +7622,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" s="25">
         <v>1</v>
@@ -7822,7 +7822,7 @@
         <v>1</v>
       </c>
       <c r="N14" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" s="25">
         <v>1</v>
@@ -8222,7 +8222,7 @@
         <v>1</v>
       </c>
       <c r="N16" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O16" s="25">
         <v>1</v>
@@ -8493,7 +8493,7 @@
         <v>1</v>
       </c>
       <c r="N18" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O18" s="25">
         <v>1</v>
@@ -8693,7 +8693,7 @@
         <v>1</v>
       </c>
       <c r="N19" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O19" s="25">
         <v>1</v>
@@ -9093,7 +9093,7 @@
         <v>1</v>
       </c>
       <c r="N21" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O21" s="25">
         <v>1</v>
@@ -9282,7 +9282,7 @@
         <v>1</v>
       </c>
       <c r="N22" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O22" s="25">
         <v>1</v>
@@ -9465,7 +9465,7 @@
         <v>1</v>
       </c>
       <c r="N23" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O23" s="25">
         <v>1</v>
@@ -9648,7 +9648,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O24" s="25">
         <v>1</v>
@@ -10014,7 +10014,7 @@
         <v>1</v>
       </c>
       <c r="N26" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O26" s="25">
         <v>1</v>
@@ -10197,7 +10197,7 @@
         <v>1</v>
       </c>
       <c r="N27" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O27" s="25">
         <v>1</v>
@@ -10380,7 +10380,7 @@
         <v>1</v>
       </c>
       <c r="N28" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O28" s="25">
         <v>1</v>

</xml_diff>

<commit_message>
- modified AD15 airfoild tables for changes to AFI - updated dependencies - set ParseFASTInputLine.m to recognize special character "@" in AFI files
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1238 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -40,11 +40,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">Variables!$B$1:$P$855</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="1145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="1146">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3393,9 +3394,6 @@
     <t>Flexible, DLL control, tower potential flow, turbulence, irregular waves, marine growth</t>
   </si>
   <si>
-    <t>Flexible, DLL control, irregular &amp; multidirectional waves, turbulence</t>
-  </si>
-  <si>
     <t>Flexible, DLL control, turbulence, irregular waves</t>
   </si>
   <si>
@@ -3484,6 +3482,12 @@
   </si>
   <si>
     <t>Flexible, DLL control, tower potential flow and drag, turbulence - using BeamDyn</t>
+  </si>
+  <si>
+    <t>Flexible, DLL control, turbulence, irregular &amp; multidirectional waves</t>
+  </si>
+  <si>
+    <t>Flexible, DLL control, irregular waves, turbulence</t>
   </si>
 </sst>
 </file>
@@ -4251,7 +4255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4733,6 +4737,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5443,7 +5450,7 @@
       <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5494,90 +5501,90 @@
   <sheetData>
     <row r="1" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="183" t="s">
+      <c r="B2" s="184" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="185"/>
-      <c r="H2" s="180" t="s">
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="181" t="s">
         <v>1104</v>
       </c>
-      <c r="I2" s="181"/>
-      <c r="J2" s="181"/>
-      <c r="K2" s="181"/>
-      <c r="L2" s="181"/>
-      <c r="M2" s="181"/>
-      <c r="N2" s="181"/>
-      <c r="O2" s="181"/>
-      <c r="P2" s="181"/>
-      <c r="Q2" s="181"/>
-      <c r="R2" s="181"/>
-      <c r="S2" s="181"/>
-      <c r="T2" s="181"/>
-      <c r="U2" s="181"/>
-      <c r="V2" s="182"/>
-      <c r="W2" s="178" t="s">
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182"/>
+      <c r="M2" s="182"/>
+      <c r="N2" s="182"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182"/>
+      <c r="R2" s="182"/>
+      <c r="S2" s="182"/>
+      <c r="T2" s="182"/>
+      <c r="U2" s="182"/>
+      <c r="V2" s="183"/>
+      <c r="W2" s="179" t="s">
         <v>1110</v>
       </c>
-      <c r="X2" s="186"/>
-      <c r="Y2" s="186"/>
-      <c r="Z2" s="186"/>
-      <c r="AA2" s="186"/>
-      <c r="AB2" s="186"/>
-      <c r="AC2" s="186"/>
-      <c r="AD2" s="187"/>
-      <c r="AE2" s="188" t="s">
-        <v>1126</v>
-      </c>
-      <c r="AF2" s="189"/>
-      <c r="AG2" s="189"/>
-      <c r="AH2" s="189"/>
-      <c r="AI2" s="189"/>
-      <c r="AJ2" s="189"/>
-      <c r="AK2" s="189"/>
-      <c r="AL2" s="189"/>
-      <c r="AM2" s="189"/>
-      <c r="AN2" s="189"/>
-      <c r="AO2" s="189"/>
-      <c r="AP2" s="190"/>
-      <c r="AQ2" s="191" t="s">
-        <v>1130</v>
-      </c>
-      <c r="AR2" s="192"/>
-      <c r="AS2" s="192"/>
-      <c r="AT2" s="192"/>
-      <c r="AU2" s="192"/>
-      <c r="AV2" s="192"/>
-      <c r="AW2" s="192"/>
-      <c r="AX2" s="192"/>
-      <c r="AY2" s="192"/>
-      <c r="AZ2" s="193"/>
-      <c r="BA2" s="197" t="s">
-        <v>1138</v>
-      </c>
-      <c r="BB2" s="198"/>
-      <c r="BC2" s="198"/>
-      <c r="BD2" s="198"/>
-      <c r="BE2" s="199"/>
-      <c r="BF2" s="194" t="s">
+      <c r="X2" s="187"/>
+      <c r="Y2" s="187"/>
+      <c r="Z2" s="187"/>
+      <c r="AA2" s="187"/>
+      <c r="AB2" s="187"/>
+      <c r="AC2" s="187"/>
+      <c r="AD2" s="188"/>
+      <c r="AE2" s="189" t="s">
+        <v>1125</v>
+      </c>
+      <c r="AF2" s="190"/>
+      <c r="AG2" s="190"/>
+      <c r="AH2" s="190"/>
+      <c r="AI2" s="190"/>
+      <c r="AJ2" s="190"/>
+      <c r="AK2" s="190"/>
+      <c r="AL2" s="190"/>
+      <c r="AM2" s="190"/>
+      <c r="AN2" s="190"/>
+      <c r="AO2" s="190"/>
+      <c r="AP2" s="191"/>
+      <c r="AQ2" s="192" t="s">
         <v>1129</v>
       </c>
-      <c r="BG2" s="195"/>
-      <c r="BH2" s="195"/>
-      <c r="BI2" s="195"/>
-      <c r="BJ2" s="195"/>
-      <c r="BK2" s="195"/>
-      <c r="BL2" s="196"/>
-      <c r="BM2" s="177" t="s">
+      <c r="AR2" s="193"/>
+      <c r="AS2" s="193"/>
+      <c r="AT2" s="193"/>
+      <c r="AU2" s="193"/>
+      <c r="AV2" s="193"/>
+      <c r="AW2" s="193"/>
+      <c r="AX2" s="193"/>
+      <c r="AY2" s="193"/>
+      <c r="AZ2" s="194"/>
+      <c r="BA2" s="198" t="s">
+        <v>1137</v>
+      </c>
+      <c r="BB2" s="199"/>
+      <c r="BC2" s="199"/>
+      <c r="BD2" s="199"/>
+      <c r="BE2" s="200"/>
+      <c r="BF2" s="195" t="s">
+        <v>1128</v>
+      </c>
+      <c r="BG2" s="196"/>
+      <c r="BH2" s="196"/>
+      <c r="BI2" s="196"/>
+      <c r="BJ2" s="196"/>
+      <c r="BK2" s="196"/>
+      <c r="BL2" s="197"/>
+      <c r="BM2" s="178" t="s">
         <v>1047</v>
       </c>
-      <c r="BN2" s="178"/>
-      <c r="BO2" s="178"/>
-      <c r="BP2" s="178"/>
-      <c r="BQ2" s="179"/>
+      <c r="BN2" s="179"/>
+      <c r="BO2" s="179"/>
+      <c r="BP2" s="179"/>
+      <c r="BQ2" s="180"/>
     </row>
     <row r="3" spans="1:69" s="1" customFormat="1" ht="114.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
@@ -5669,7 +5676,7 @@
         <v>1056</v>
       </c>
       <c r="AE3" s="82" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="AF3" s="154" t="s">
         <v>5</v>
@@ -5723,25 +5730,25 @@
         <v>46</v>
       </c>
       <c r="AW3" s="166" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="AX3" s="73" t="s">
         <v>31</v>
       </c>
       <c r="AY3" s="166" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="AZ3" s="74" t="s">
         <v>26</v>
       </c>
       <c r="BA3" s="75" t="s">
+        <v>1138</v>
+      </c>
+      <c r="BB3" s="164" t="s">
+        <v>1131</v>
+      </c>
+      <c r="BC3" s="165" t="s">
         <v>1139</v>
-      </c>
-      <c r="BB3" s="164" t="s">
-        <v>1132</v>
-      </c>
-      <c r="BC3" s="165" t="s">
-        <v>1140</v>
       </c>
       <c r="BD3" s="77" t="s">
         <v>23</v>
@@ -5750,16 +5757,16 @@
         <v>17</v>
       </c>
       <c r="BF3" s="157" t="s">
+        <v>1120</v>
+      </c>
+      <c r="BG3" s="158" t="s">
         <v>1121</v>
       </c>
-      <c r="BG3" s="158" t="s">
+      <c r="BH3" s="158" t="s">
         <v>1122</v>
       </c>
-      <c r="BH3" s="158" t="s">
+      <c r="BI3" s="158" t="s">
         <v>1123</v>
-      </c>
-      <c r="BI3" s="158" t="s">
-        <v>1124</v>
       </c>
       <c r="BJ3" s="158"/>
       <c r="BK3" s="158"/>
@@ -5818,7 +5825,7 @@
       <c r="M4" s="25">
         <v>1</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4" s="107">
         <v>2</v>
       </c>
       <c r="O4" s="25">
@@ -5998,7 +6005,7 @@
         <v>175</v>
       </c>
       <c r="G5" s="143" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="H5" s="40">
         <v>20</v>
@@ -6218,7 +6225,7 @@
       <c r="M6" s="25">
         <v>1</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6" s="107">
         <v>2</v>
       </c>
       <c r="O6" s="25">
@@ -6418,7 +6425,7 @@
       <c r="M7" s="25">
         <v>1</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="107">
         <v>2</v>
       </c>
       <c r="O7" s="25">
@@ -7020,7 +7027,7 @@
       <c r="M10" s="25">
         <v>1</v>
       </c>
-      <c r="N10" s="25">
+      <c r="N10" s="107">
         <v>2</v>
       </c>
       <c r="O10" s="25">
@@ -7221,7 +7228,7 @@
       <c r="M11" s="25">
         <v>1</v>
       </c>
-      <c r="N11" s="25">
+      <c r="N11" s="107">
         <v>2</v>
       </c>
       <c r="O11" s="25">
@@ -7621,7 +7628,7 @@
       <c r="M13" s="25">
         <v>1</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13" s="107">
         <v>2</v>
       </c>
       <c r="O13" s="25">
@@ -7743,7 +7750,7 @@
         <v>0</v>
       </c>
       <c r="BC13" s="163" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="BD13" s="44">
         <v>0</v>
@@ -7821,7 +7828,7 @@
       <c r="M14" s="25">
         <v>1</v>
       </c>
-      <c r="N14" s="25">
+      <c r="N14" s="107">
         <v>2</v>
       </c>
       <c r="O14" s="25">
@@ -8140,10 +8147,10 @@
         <v>2</v>
       </c>
       <c r="BB15" s="163" t="s">
+        <v>1133</v>
+      </c>
+      <c r="BC15" s="163" t="s">
         <v>1134</v>
-      </c>
-      <c r="BC15" s="163" t="s">
-        <v>1135</v>
       </c>
       <c r="BD15" s="44">
         <v>0.2</v>
@@ -8221,7 +8228,7 @@
       <c r="M16" s="25">
         <v>1</v>
       </c>
-      <c r="N16" s="25">
+      <c r="N16" s="107">
         <v>2</v>
       </c>
       <c r="O16" s="25">
@@ -8492,7 +8499,7 @@
       <c r="M18" s="25">
         <v>1</v>
       </c>
-      <c r="N18" s="25">
+      <c r="N18" s="107">
         <v>2</v>
       </c>
       <c r="O18" s="25">
@@ -8614,7 +8621,7 @@
         <v>0</v>
       </c>
       <c r="BC18" s="163" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="BD18" s="44">
         <v>0.2</v>
@@ -8692,7 +8699,7 @@
       <c r="M19" s="25">
         <v>1</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19" s="107">
         <v>2</v>
       </c>
       <c r="O19" s="25">
@@ -8811,7 +8818,7 @@
         <v>2</v>
       </c>
       <c r="BB19" s="163" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="BC19" s="151">
         <v>11.9</v>
@@ -8892,7 +8899,7 @@
       <c r="M20" s="25">
         <v>1</v>
       </c>
-      <c r="N20" s="25">
+      <c r="N20" s="107">
         <v>1</v>
       </c>
       <c r="O20" s="25">
@@ -9092,7 +9099,7 @@
       <c r="M21" s="25">
         <v>1</v>
       </c>
-      <c r="N21" s="25">
+      <c r="N21" s="107">
         <v>2</v>
       </c>
       <c r="O21" s="25">
@@ -9281,7 +9288,7 @@
       <c r="M22" s="25">
         <v>1</v>
       </c>
-      <c r="N22" s="25">
+      <c r="N22" s="107">
         <v>2</v>
       </c>
       <c r="O22" s="25">
@@ -9444,7 +9451,7 @@
         <v>5000</v>
       </c>
       <c r="G23" s="143" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="H23" s="40">
         <v>60</v>
@@ -9464,7 +9471,7 @@
       <c r="M23" s="25">
         <v>1</v>
       </c>
-      <c r="N23" s="25">
+      <c r="N23" s="107">
         <v>2</v>
       </c>
       <c r="O23" s="25">
@@ -9590,7 +9597,7 @@
         <v>45</v>
       </c>
       <c r="BG23" s="41" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="BH23" s="41" t="s">
         <v>42</v>
@@ -9647,7 +9654,7 @@
       <c r="M24" s="25">
         <v>1</v>
       </c>
-      <c r="N24" s="25">
+      <c r="N24" s="107">
         <v>2</v>
       </c>
       <c r="O24" s="25">
@@ -9792,10 +9799,10 @@
       </c>
       <c r="BQ24" s="42"/>
     </row>
-    <row r="25" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
       <c r="B25" s="85" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C25" s="147" t="s">
         <v>1085</v>
@@ -9810,7 +9817,7 @@
         <v>5000</v>
       </c>
       <c r="G25" s="143" t="s">
-        <v>1114</v>
+        <v>1145</v>
       </c>
       <c r="H25" s="40">
         <v>60</v>
@@ -9975,10 +9982,10 @@
       </c>
       <c r="BQ25" s="42"/>
     </row>
-    <row r="26" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="85" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C26" s="147" t="s">
         <v>1086</v>
@@ -9993,7 +10000,7 @@
         <v>5000</v>
       </c>
       <c r="G26" s="143" t="s">
-        <v>1115</v>
+        <v>1144</v>
       </c>
       <c r="H26" s="40">
         <v>60</v>
@@ -10013,7 +10020,7 @@
       <c r="M26" s="25">
         <v>1</v>
       </c>
-      <c r="N26" s="25">
+      <c r="N26" s="107">
         <v>2</v>
       </c>
       <c r="O26" s="25">
@@ -10161,7 +10168,7 @@
     <row r="27" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
       <c r="B27" s="85" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C27" s="147" t="s">
         <v>1087</v>
@@ -10176,7 +10183,7 @@
         <v>5000</v>
       </c>
       <c r="G27" s="143" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="H27" s="40">
         <v>60</v>
@@ -10196,7 +10203,7 @@
       <c r="M27" s="25">
         <v>1</v>
       </c>
-      <c r="N27" s="25">
+      <c r="N27" s="107">
         <v>2</v>
       </c>
       <c r="O27" s="25">
@@ -10344,7 +10351,7 @@
     <row r="28" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="27"/>
       <c r="B28" s="85" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C28" s="147" t="s">
         <v>1105</v>
@@ -10359,7 +10366,7 @@
         <v>5000</v>
       </c>
       <c r="G28" s="143" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="H28" s="40">
         <v>60</v>
@@ -10379,7 +10386,7 @@
       <c r="M28" s="25">
         <v>1</v>
       </c>
-      <c r="N28" s="25">
+      <c r="N28" s="107">
         <v>2</v>
       </c>
       <c r="O28" s="25">
@@ -10527,7 +10534,7 @@
     <row r="29" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="167" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C29" s="168" t="s">
         <v>1089</v>
@@ -10542,7 +10549,7 @@
         <v>5000</v>
       </c>
       <c r="G29" s="143" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="H29" s="170">
         <v>20</v>
@@ -10562,7 +10569,7 @@
       <c r="M29" s="169">
         <v>2</v>
       </c>
-      <c r="N29" s="169">
+      <c r="N29" s="177">
         <v>2</v>
       </c>
       <c r="O29" s="169">
@@ -11306,74 +11313,74 @@
   <sheetData>
     <row r="1" spans="1:55" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:55" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="183" t="s">
+      <c r="B2" s="184" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="185"/>
-      <c r="I2" s="177" t="s">
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="178" t="s">
         <v>1062</v>
       </c>
-      <c r="J2" s="178"/>
-      <c r="K2" s="186"/>
-      <c r="L2" s="186"/>
-      <c r="M2" s="186"/>
-      <c r="N2" s="186"/>
-      <c r="O2" s="186"/>
-      <c r="P2" s="186"/>
-      <c r="Q2" s="186"/>
-      <c r="R2" s="186"/>
-      <c r="S2" s="186"/>
-      <c r="T2" s="187"/>
-      <c r="U2" s="188" t="s">
+      <c r="J2" s="179"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="187"/>
+      <c r="M2" s="187"/>
+      <c r="N2" s="187"/>
+      <c r="O2" s="187"/>
+      <c r="P2" s="187"/>
+      <c r="Q2" s="187"/>
+      <c r="R2" s="187"/>
+      <c r="S2" s="187"/>
+      <c r="T2" s="188"/>
+      <c r="U2" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="189"/>
-      <c r="W2" s="189"/>
-      <c r="X2" s="189"/>
-      <c r="Y2" s="189"/>
-      <c r="Z2" s="189"/>
-      <c r="AA2" s="189"/>
-      <c r="AB2" s="189"/>
-      <c r="AC2" s="189"/>
-      <c r="AD2" s="189"/>
-      <c r="AE2" s="189"/>
-      <c r="AF2" s="189"/>
-      <c r="AG2" s="189"/>
-      <c r="AH2" s="189"/>
-      <c r="AI2" s="189"/>
-      <c r="AJ2" s="190"/>
-      <c r="AK2" s="200" t="s">
+      <c r="V2" s="190"/>
+      <c r="W2" s="190"/>
+      <c r="X2" s="190"/>
+      <c r="Y2" s="190"/>
+      <c r="Z2" s="190"/>
+      <c r="AA2" s="190"/>
+      <c r="AB2" s="190"/>
+      <c r="AC2" s="190"/>
+      <c r="AD2" s="190"/>
+      <c r="AE2" s="190"/>
+      <c r="AF2" s="190"/>
+      <c r="AG2" s="190"/>
+      <c r="AH2" s="190"/>
+      <c r="AI2" s="190"/>
+      <c r="AJ2" s="191"/>
+      <c r="AK2" s="201" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="192"/>
-      <c r="AM2" s="192"/>
-      <c r="AN2" s="192"/>
-      <c r="AO2" s="192"/>
-      <c r="AP2" s="193"/>
-      <c r="AQ2" s="200" t="s">
+      <c r="AL2" s="193"/>
+      <c r="AM2" s="193"/>
+      <c r="AN2" s="193"/>
+      <c r="AO2" s="193"/>
+      <c r="AP2" s="194"/>
+      <c r="AQ2" s="201" t="s">
         <v>1061</v>
       </c>
-      <c r="AR2" s="191"/>
-      <c r="AS2" s="191"/>
-      <c r="AT2" s="201"/>
-      <c r="AU2" s="197" t="s">
+      <c r="AR2" s="192"/>
+      <c r="AS2" s="192"/>
+      <c r="AT2" s="202"/>
+      <c r="AU2" s="198" t="s">
         <v>18</v>
       </c>
-      <c r="AV2" s="198"/>
-      <c r="AW2" s="198"/>
-      <c r="AX2" s="199"/>
-      <c r="AY2" s="177" t="s">
+      <c r="AV2" s="199"/>
+      <c r="AW2" s="199"/>
+      <c r="AX2" s="200"/>
+      <c r="AY2" s="178" t="s">
         <v>1047</v>
       </c>
-      <c r="AZ2" s="178"/>
-      <c r="BA2" s="178"/>
-      <c r="BB2" s="178"/>
-      <c r="BC2" s="179"/>
+      <c r="AZ2" s="179"/>
+      <c r="BA2" s="179"/>
+      <c r="BB2" s="179"/>
+      <c r="BC2" s="180"/>
     </row>
     <row r="3" spans="1:55" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">

</xml_diff>

<commit_message>
* fixed propagation direction in tests 1 and 8, which were broken in last commits * added test14 to certtest
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman@1301 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/CertTest/FASTCertTestCases.xlsx
+++ b/CertTest/FASTCertTestCases.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3043" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3082" uniqueCount="1148">
   <si>
     <t>Turbine Name</t>
   </si>
@@ -3524,6 +3524,9 @@
   </si>
   <si>
     <t>Flexible, steady wind, startup, high-speed shaft brake shutdown</t>
+  </si>
+  <si>
+    <t>Flexible, stationary, linearization in vacuum</t>
   </si>
 </sst>
 </file>
@@ -4310,7 +4313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4654,35 +4657,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="12" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="12" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4707,9 +4688,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4719,9 +4697,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4729,7 +4704,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
@@ -4880,7 +4854,889 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="169">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -4949,20 +5805,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -5519,17 +6361,17 @@
   <dimension ref="A1:BQ62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="AK19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="Y4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="AF17" sqref="AF17:AP17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" style="145" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" style="136" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.109375" style="2" bestFit="1" customWidth="1"/>
@@ -5543,11 +6385,11 @@
     <col min="19" max="19" width="3.33203125" style="2" customWidth="1"/>
     <col min="20" max="20" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="3.33203125" style="2" customWidth="1"/>
-    <col min="26" max="26" width="4.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.33203125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="3.33203125" style="2" customWidth="1"/>
-    <col min="29" max="30" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="4" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="32" max="34" width="4" style="2" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="4.109375" style="2" bestFit="1" customWidth="1"/>
@@ -5557,7 +6399,7 @@
     <col min="52" max="53" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="5.33203125" style="45" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="5.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="3.33203125" style="160" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="3.33203125" style="149" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="4.88671875" style="2" customWidth="1"/>
     <col min="59" max="59" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
@@ -5573,90 +6415,90 @@
   <sheetData>
     <row r="1" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="174" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="187"/>
-      <c r="H2" s="182" t="s">
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="171" t="s">
         <v>1104</v>
       </c>
-      <c r="I2" s="183"/>
-      <c r="J2" s="183"/>
-      <c r="K2" s="183"/>
-      <c r="L2" s="183"/>
-      <c r="M2" s="183"/>
-      <c r="N2" s="183"/>
-      <c r="O2" s="183"/>
-      <c r="P2" s="183"/>
-      <c r="Q2" s="183"/>
-      <c r="R2" s="183"/>
-      <c r="S2" s="183"/>
-      <c r="T2" s="183"/>
-      <c r="U2" s="183"/>
-      <c r="V2" s="184"/>
-      <c r="W2" s="180" t="s">
+      <c r="I2" s="172"/>
+      <c r="J2" s="172"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="172"/>
+      <c r="M2" s="172"/>
+      <c r="N2" s="172"/>
+      <c r="O2" s="172"/>
+      <c r="P2" s="172"/>
+      <c r="Q2" s="172"/>
+      <c r="R2" s="172"/>
+      <c r="S2" s="172"/>
+      <c r="T2" s="172"/>
+      <c r="U2" s="172"/>
+      <c r="V2" s="173"/>
+      <c r="W2" s="169" t="s">
         <v>1110</v>
       </c>
-      <c r="X2" s="188"/>
-      <c r="Y2" s="188"/>
-      <c r="Z2" s="188"/>
-      <c r="AA2" s="188"/>
-      <c r="AB2" s="188"/>
-      <c r="AC2" s="188"/>
-      <c r="AD2" s="189"/>
-      <c r="AE2" s="190" t="s">
+      <c r="X2" s="177"/>
+      <c r="Y2" s="177"/>
+      <c r="Z2" s="177"/>
+      <c r="AA2" s="177"/>
+      <c r="AB2" s="177"/>
+      <c r="AC2" s="177"/>
+      <c r="AD2" s="178"/>
+      <c r="AE2" s="179" t="s">
         <v>1125</v>
       </c>
-      <c r="AF2" s="191"/>
-      <c r="AG2" s="191"/>
-      <c r="AH2" s="191"/>
-      <c r="AI2" s="191"/>
-      <c r="AJ2" s="191"/>
-      <c r="AK2" s="191"/>
-      <c r="AL2" s="191"/>
-      <c r="AM2" s="191"/>
-      <c r="AN2" s="191"/>
-      <c r="AO2" s="191"/>
-      <c r="AP2" s="192"/>
-      <c r="AQ2" s="193" t="s">
+      <c r="AF2" s="180"/>
+      <c r="AG2" s="180"/>
+      <c r="AH2" s="180"/>
+      <c r="AI2" s="180"/>
+      <c r="AJ2" s="180"/>
+      <c r="AK2" s="180"/>
+      <c r="AL2" s="180"/>
+      <c r="AM2" s="180"/>
+      <c r="AN2" s="180"/>
+      <c r="AO2" s="180"/>
+      <c r="AP2" s="181"/>
+      <c r="AQ2" s="182" t="s">
         <v>1128</v>
       </c>
-      <c r="AR2" s="194"/>
-      <c r="AS2" s="194"/>
-      <c r="AT2" s="194"/>
-      <c r="AU2" s="194"/>
-      <c r="AV2" s="194"/>
-      <c r="AW2" s="194"/>
-      <c r="AX2" s="194"/>
-      <c r="AY2" s="194"/>
-      <c r="AZ2" s="195"/>
-      <c r="BA2" s="199" t="s">
+      <c r="AR2" s="183"/>
+      <c r="AS2" s="183"/>
+      <c r="AT2" s="183"/>
+      <c r="AU2" s="183"/>
+      <c r="AV2" s="183"/>
+      <c r="AW2" s="183"/>
+      <c r="AX2" s="183"/>
+      <c r="AY2" s="183"/>
+      <c r="AZ2" s="184"/>
+      <c r="BA2" s="188" t="s">
         <v>1136</v>
       </c>
-      <c r="BB2" s="200"/>
-      <c r="BC2" s="200"/>
-      <c r="BD2" s="200"/>
-      <c r="BE2" s="201"/>
-      <c r="BF2" s="196" t="s">
+      <c r="BB2" s="189"/>
+      <c r="BC2" s="189"/>
+      <c r="BD2" s="189"/>
+      <c r="BE2" s="190"/>
+      <c r="BF2" s="185" t="s">
         <v>1127</v>
       </c>
-      <c r="BG2" s="197"/>
-      <c r="BH2" s="197"/>
-      <c r="BI2" s="197"/>
-      <c r="BJ2" s="197"/>
-      <c r="BK2" s="197"/>
-      <c r="BL2" s="198"/>
-      <c r="BM2" s="179" t="s">
+      <c r="BG2" s="186"/>
+      <c r="BH2" s="186"/>
+      <c r="BI2" s="186"/>
+      <c r="BJ2" s="186"/>
+      <c r="BK2" s="186"/>
+      <c r="BL2" s="187"/>
+      <c r="BM2" s="168" t="s">
         <v>1047</v>
       </c>
-      <c r="BN2" s="180"/>
-      <c r="BO2" s="180"/>
-      <c r="BP2" s="180"/>
-      <c r="BQ2" s="181"/>
+      <c r="BN2" s="169"/>
+      <c r="BO2" s="169"/>
+      <c r="BP2" s="169"/>
+      <c r="BQ2" s="170"/>
     </row>
     <row r="3" spans="1:69" s="1" customFormat="1" ht="114.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
@@ -5675,10 +6517,10 @@
       <c r="F3" s="80" t="s">
         <v>488</v>
       </c>
-      <c r="G3" s="138" t="s">
+      <c r="G3" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="136" t="s">
+      <c r="H3" s="128" t="s">
         <v>1090</v>
       </c>
       <c r="I3" s="121" t="s">
@@ -5750,7 +6592,7 @@
       <c r="AE3" s="82" t="s">
         <v>1126</v>
       </c>
-      <c r="AF3" s="154" t="s">
+      <c r="AF3" s="143" t="s">
         <v>5</v>
       </c>
       <c r="AG3" s="83" t="s">
@@ -5780,10 +6622,10 @@
       <c r="AO3" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="AP3" s="141" t="s">
+      <c r="AP3" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="AQ3" s="140" t="s">
+      <c r="AQ3" s="132" t="s">
         <v>44</v>
       </c>
       <c r="AR3" s="72" t="s">
@@ -5801,13 +6643,13 @@
       <c r="AV3" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="AW3" s="166" t="s">
+      <c r="AW3" s="155" t="s">
         <v>1139</v>
       </c>
       <c r="AX3" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="AY3" s="166" t="s">
+      <c r="AY3" s="155" t="s">
         <v>1140</v>
       </c>
       <c r="AZ3" s="74" t="s">
@@ -5816,10 +6658,10 @@
       <c r="BA3" s="75" t="s">
         <v>1137</v>
       </c>
-      <c r="BB3" s="164" t="s">
+      <c r="BB3" s="153" t="s">
         <v>1130</v>
       </c>
-      <c r="BC3" s="165" t="s">
+      <c r="BC3" s="154" t="s">
         <v>1138</v>
       </c>
       <c r="BD3" s="77" t="s">
@@ -5828,21 +6670,21 @@
       <c r="BE3" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="BF3" s="157" t="s">
+      <c r="BF3" s="146" t="s">
         <v>1120</v>
       </c>
-      <c r="BG3" s="158" t="s">
+      <c r="BG3" s="147" t="s">
         <v>1121</v>
       </c>
-      <c r="BH3" s="158" t="s">
+      <c r="BH3" s="147" t="s">
         <v>1122</v>
       </c>
-      <c r="BI3" s="158" t="s">
+      <c r="BI3" s="147" t="s">
         <v>1123</v>
       </c>
-      <c r="BJ3" s="158"/>
-      <c r="BK3" s="158"/>
-      <c r="BL3" s="159"/>
+      <c r="BJ3" s="147"/>
+      <c r="BK3" s="147"/>
+      <c r="BL3" s="148"/>
       <c r="BM3" s="66" t="s">
         <v>1045</v>
       </c>
@@ -5864,7 +6706,7 @@
       <c r="B4" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="146" t="s">
+      <c r="C4" s="137" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="29">
@@ -5876,10 +6718,10 @@
       <c r="F4" s="55">
         <v>175</v>
       </c>
-      <c r="G4" s="142" t="s">
+      <c r="G4" s="134" t="s">
         <v>497</v>
       </c>
-      <c r="H4" s="137">
+      <c r="H4" s="129">
         <v>20</v>
       </c>
       <c r="I4" s="117">
@@ -5897,7 +6739,7 @@
       <c r="M4" s="25">
         <v>1</v>
       </c>
-      <c r="N4" s="177">
+      <c r="N4" s="166">
         <v>1</v>
       </c>
       <c r="O4" s="25">
@@ -6015,10 +6857,10 @@
       <c r="BA4" s="36">
         <v>2</v>
       </c>
-      <c r="BB4" s="150">
+      <c r="BB4" s="140">
         <v>30</v>
       </c>
-      <c r="BC4" s="150">
+      <c r="BC4" s="140">
         <v>12</v>
       </c>
       <c r="BD4" s="37">
@@ -6064,7 +6906,7 @@
       <c r="B5" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="146" t="s">
+      <c r="C5" s="137" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="29">
@@ -6076,7 +6918,7 @@
       <c r="F5" s="55">
         <v>175</v>
       </c>
-      <c r="G5" s="143" t="s">
+      <c r="G5" s="135" t="s">
         <v>1146</v>
       </c>
       <c r="H5" s="40">
@@ -6097,7 +6939,7 @@
       <c r="M5" s="25">
         <v>1</v>
       </c>
-      <c r="N5" s="177">
+      <c r="N5" s="166">
         <v>2</v>
       </c>
       <c r="O5" s="25">
@@ -6215,10 +7057,10 @@
       <c r="BA5" s="43">
         <v>1</v>
       </c>
-      <c r="BB5" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC5" s="151">
+      <c r="BB5" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="141">
         <v>12</v>
       </c>
       <c r="BD5" s="44">
@@ -6264,7 +7106,7 @@
       <c r="B6" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="146" t="s">
+      <c r="C6" s="137" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="29">
@@ -6276,7 +7118,7 @@
       <c r="F6" s="55">
         <v>175</v>
       </c>
-      <c r="G6" s="143" t="s">
+      <c r="G6" s="135" t="s">
         <v>491</v>
       </c>
       <c r="H6" s="40">
@@ -6297,7 +7139,7 @@
       <c r="M6" s="25">
         <v>1</v>
       </c>
-      <c r="N6" s="177">
+      <c r="N6" s="166">
         <v>2</v>
       </c>
       <c r="O6" s="25">
@@ -6415,10 +7257,10 @@
       <c r="BA6" s="43">
         <v>2</v>
       </c>
-      <c r="BB6" s="151">
+      <c r="BB6" s="141">
         <v>30</v>
       </c>
-      <c r="BC6" s="151">
+      <c r="BC6" s="141">
         <v>12</v>
       </c>
       <c r="BD6" s="44">
@@ -6464,7 +7306,7 @@
       <c r="B7" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="146" t="s">
+      <c r="C7" s="137" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="29">
@@ -6476,7 +7318,7 @@
       <c r="F7" s="55">
         <v>175</v>
       </c>
-      <c r="G7" s="143" t="s">
+      <c r="G7" s="135" t="s">
         <v>492</v>
       </c>
       <c r="H7" s="40">
@@ -6497,7 +7339,7 @@
       <c r="M7" s="25">
         <v>1</v>
       </c>
-      <c r="N7" s="177">
+      <c r="N7" s="166">
         <v>1</v>
       </c>
       <c r="O7" s="25">
@@ -6615,10 +7457,10 @@
       <c r="BA7" s="43">
         <v>4</v>
       </c>
-      <c r="BB7" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC7" s="151">
+      <c r="BB7" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="141">
         <v>12</v>
       </c>
       <c r="BD7" s="44">
@@ -6664,7 +7506,7 @@
       <c r="B8" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="146" t="s">
+      <c r="C8" s="137" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="29">
@@ -6676,7 +7518,7 @@
       <c r="F8" s="55">
         <v>175</v>
       </c>
-      <c r="G8" s="143" t="s">
+      <c r="G8" s="135" t="s">
         <v>1145</v>
       </c>
       <c r="H8" s="40">
@@ -6697,7 +7539,7 @@
       <c r="M8" s="25">
         <v>1</v>
       </c>
-      <c r="N8" s="177">
+      <c r="N8" s="166">
         <v>2</v>
       </c>
       <c r="O8" s="25">
@@ -6815,10 +7657,10 @@
       <c r="BA8" s="43">
         <v>2</v>
       </c>
-      <c r="BB8" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC8" s="151">
+      <c r="BB8" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="141">
         <v>12</v>
       </c>
       <c r="BD8" s="44">
@@ -6864,7 +7706,7 @@
       <c r="B9" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="147" t="s">
+      <c r="C9" s="138" t="s">
         <v>279</v>
       </c>
       <c r="D9" s="25">
@@ -6877,7 +7719,7 @@
       <c r="F9" s="25">
         <v>50</v>
       </c>
-      <c r="G9" s="143" t="s">
+      <c r="G9" s="135" t="s">
         <v>1106</v>
       </c>
       <c r="H9" s="40">
@@ -7016,10 +7858,10 @@
       <c r="BA9" s="43">
         <v>2</v>
       </c>
-      <c r="BB9" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC9" s="151">
+      <c r="BB9" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="141">
         <v>12</v>
       </c>
       <c r="BD9" s="44">
@@ -7065,7 +7907,7 @@
       <c r="B10" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="147" t="s">
+      <c r="C10" s="138" t="s">
         <v>279</v>
       </c>
       <c r="D10" s="25">
@@ -7078,7 +7920,7 @@
       <c r="F10" s="25">
         <v>50</v>
       </c>
-      <c r="G10" s="143" t="s">
+      <c r="G10" s="135" t="s">
         <v>492</v>
       </c>
       <c r="H10" s="40">
@@ -7099,7 +7941,7 @@
       <c r="M10" s="25">
         <v>1</v>
       </c>
-      <c r="N10" s="177">
+      <c r="N10" s="166">
         <v>2</v>
       </c>
       <c r="O10" s="25">
@@ -7217,10 +8059,10 @@
       <c r="BA10" s="43">
         <v>4</v>
       </c>
-      <c r="BB10" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC10" s="151">
+      <c r="BB10" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC10" s="141">
         <v>12</v>
       </c>
       <c r="BD10" s="44">
@@ -7266,7 +8108,7 @@
       <c r="B11" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="147" t="s">
+      <c r="C11" s="138" t="s">
         <v>279</v>
       </c>
       <c r="D11" s="25">
@@ -7279,7 +8121,7 @@
       <c r="F11" s="25">
         <v>50</v>
       </c>
-      <c r="G11" s="142" t="s">
+      <c r="G11" s="134" t="s">
         <v>497</v>
       </c>
       <c r="H11" s="40">
@@ -7300,7 +8142,7 @@
       <c r="M11" s="25">
         <v>1</v>
       </c>
-      <c r="N11" s="177">
+      <c r="N11" s="166">
         <v>2</v>
       </c>
       <c r="O11" s="25">
@@ -7418,10 +8260,10 @@
       <c r="BA11" s="43">
         <v>1</v>
       </c>
-      <c r="BB11" s="151">
+      <c r="BB11" s="141">
         <v>30</v>
       </c>
-      <c r="BC11" s="151">
+      <c r="BC11" s="141">
         <v>11</v>
       </c>
       <c r="BD11" s="44">
@@ -7467,7 +8309,7 @@
       <c r="B12" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="147" t="s">
+      <c r="C12" s="138" t="s">
         <v>489</v>
       </c>
       <c r="D12" s="25">
@@ -7479,7 +8321,7 @@
       <c r="F12" s="25">
         <v>20</v>
       </c>
-      <c r="G12" s="143" t="s">
+      <c r="G12" s="135" t="s">
         <v>493</v>
       </c>
       <c r="H12" s="40">
@@ -7618,10 +8460,10 @@
       <c r="BA12" s="43">
         <v>2</v>
       </c>
-      <c r="BB12" s="151">
+      <c r="BB12" s="141">
         <v>30</v>
       </c>
-      <c r="BC12" s="151">
+      <c r="BC12" s="141">
         <v>11</v>
       </c>
       <c r="BD12" s="44">
@@ -7667,7 +8509,7 @@
       <c r="B13" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="147" t="s">
+      <c r="C13" s="138" t="s">
         <v>490</v>
       </c>
       <c r="D13" s="25">
@@ -7679,7 +8521,7 @@
       <c r="F13" s="25">
         <v>20</v>
       </c>
-      <c r="G13" s="143" t="s">
+      <c r="G13" s="135" t="s">
         <v>496</v>
       </c>
       <c r="H13" s="40">
@@ -7700,7 +8542,7 @@
       <c r="M13" s="25">
         <v>1</v>
       </c>
-      <c r="N13" s="177">
+      <c r="N13" s="166">
         <v>2</v>
       </c>
       <c r="O13" s="25">
@@ -7818,10 +8660,10 @@
       <c r="BA13" s="43">
         <v>2</v>
       </c>
-      <c r="BB13" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC13" s="163" t="s">
+      <c r="BB13" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC13" s="152" t="s">
         <v>1131</v>
       </c>
       <c r="BD13" s="44">
@@ -7867,7 +8709,7 @@
       <c r="B14" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="147" t="s">
+      <c r="C14" s="138" t="s">
         <v>286</v>
       </c>
       <c r="D14" s="25">
@@ -7879,7 +8721,7 @@
       <c r="F14" s="25">
         <v>1500</v>
       </c>
-      <c r="G14" s="143" t="s">
+      <c r="G14" s="135" t="s">
         <v>500</v>
       </c>
       <c r="H14" s="40">
@@ -7900,7 +8742,7 @@
       <c r="M14" s="25">
         <v>1</v>
       </c>
-      <c r="N14" s="177">
+      <c r="N14" s="166">
         <v>1</v>
       </c>
       <c r="O14" s="25">
@@ -8018,10 +8860,10 @@
       <c r="BA14" s="43">
         <v>4</v>
       </c>
-      <c r="BB14" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC14" s="151">
+      <c r="BB14" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC14" s="141">
         <v>12</v>
       </c>
       <c r="BD14" s="44">
@@ -8067,7 +8909,7 @@
       <c r="B15" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="147" t="s">
+      <c r="C15" s="138" t="s">
         <v>286</v>
       </c>
       <c r="D15" s="25">
@@ -8079,7 +8921,7 @@
       <c r="F15" s="25">
         <v>1500</v>
       </c>
-      <c r="G15" s="143" t="s">
+      <c r="G15" s="135" t="s">
         <v>494</v>
       </c>
       <c r="H15" s="40">
@@ -8100,7 +8942,7 @@
       <c r="M15" s="25">
         <v>1</v>
       </c>
-      <c r="N15" s="177">
+      <c r="N15" s="166">
         <v>2</v>
       </c>
       <c r="O15" s="25">
@@ -8218,10 +9060,10 @@
       <c r="BA15" s="43">
         <v>2</v>
       </c>
-      <c r="BB15" s="163" t="s">
+      <c r="BB15" s="152" t="s">
         <v>1132</v>
       </c>
-      <c r="BC15" s="163" t="s">
+      <c r="BC15" s="152" t="s">
         <v>1133</v>
       </c>
       <c r="BD15" s="44">
@@ -8267,7 +9109,7 @@
       <c r="B16" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="147" t="s">
+      <c r="C16" s="138" t="s">
         <v>286</v>
       </c>
       <c r="D16" s="25">
@@ -8279,7 +9121,7 @@
       <c r="F16" s="25">
         <v>1500</v>
       </c>
-      <c r="G16" s="143" t="s">
+      <c r="G16" s="135" t="s">
         <v>495</v>
       </c>
       <c r="H16" s="40">
@@ -8300,7 +9142,7 @@
       <c r="M16" s="25">
         <v>1</v>
       </c>
-      <c r="N16" s="177">
+      <c r="N16" s="166">
         <v>2</v>
       </c>
       <c r="O16" s="25">
@@ -8418,10 +9260,10 @@
       <c r="BA16" s="43">
         <v>4</v>
       </c>
-      <c r="BB16" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC16" s="151">
+      <c r="BB16" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC16" s="141">
         <v>12</v>
       </c>
       <c r="BD16" s="44">
@@ -8464,81 +9306,202 @@
     </row>
     <row r="17" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
-      <c r="B17" s="125"/>
-      <c r="C17" s="148"/>
-      <c r="D17" s="127"/>
-      <c r="E17" s="127"/>
-      <c r="F17" s="127"/>
-      <c r="G17" s="144"/>
-      <c r="H17" s="125"/>
-      <c r="I17" s="126"/>
-      <c r="J17" s="127"/>
-      <c r="K17" s="127"/>
-      <c r="L17" s="127"/>
-      <c r="M17" s="127"/>
-      <c r="N17" s="127"/>
-      <c r="O17" s="127"/>
-      <c r="P17" s="127"/>
-      <c r="Q17" s="127"/>
-      <c r="R17" s="127"/>
-      <c r="S17" s="127"/>
-      <c r="T17" s="126"/>
-      <c r="U17" s="127"/>
-      <c r="V17" s="130"/>
-      <c r="W17" s="128"/>
-      <c r="X17" s="127"/>
-      <c r="Y17" s="127"/>
-      <c r="Z17" s="127"/>
-      <c r="AA17" s="127"/>
-      <c r="AB17" s="127"/>
-      <c r="AC17" s="129"/>
-      <c r="AD17" s="129"/>
-      <c r="AE17" s="125"/>
-      <c r="AF17" s="128"/>
-      <c r="AG17" s="127"/>
-      <c r="AH17" s="127"/>
-      <c r="AI17" s="127"/>
-      <c r="AJ17" s="127"/>
-      <c r="AK17" s="127"/>
-      <c r="AL17" s="127"/>
-      <c r="AM17" s="127"/>
-      <c r="AN17" s="127"/>
-      <c r="AO17" s="127"/>
-      <c r="AP17" s="130"/>
-      <c r="AQ17" s="128"/>
-      <c r="AR17" s="127"/>
-      <c r="AS17" s="129"/>
-      <c r="AT17" s="129"/>
-      <c r="AU17" s="129"/>
-      <c r="AV17" s="129"/>
-      <c r="AW17" s="129"/>
-      <c r="AX17" s="129"/>
-      <c r="AY17" s="129"/>
-      <c r="AZ17" s="130"/>
-      <c r="BA17" s="128"/>
-      <c r="BB17" s="152"/>
-      <c r="BC17" s="152"/>
-      <c r="BD17" s="132"/>
-      <c r="BE17" s="130"/>
-      <c r="BF17" s="131"/>
-      <c r="BG17" s="129"/>
-      <c r="BH17" s="129"/>
-      <c r="BI17" s="129"/>
-      <c r="BJ17" s="129"/>
-      <c r="BK17" s="129"/>
-      <c r="BL17" s="130"/>
-      <c r="BM17" s="133"/>
-      <c r="BN17" s="134"/>
-      <c r="BO17" s="135"/>
-      <c r="BP17" s="135"/>
-      <c r="BQ17" s="130"/>
+      <c r="B17" s="85" t="s">
+        <v>288</v>
+      </c>
+      <c r="C17" s="138" t="s">
+        <v>286</v>
+      </c>
+      <c r="D17" s="25">
+        <v>3</v>
+      </c>
+      <c r="E17" s="25">
+        <v>70</v>
+      </c>
+      <c r="F17" s="25">
+        <v>1500</v>
+      </c>
+      <c r="G17" s="135" t="s">
+        <v>1147</v>
+      </c>
+      <c r="H17" s="40">
+        <v>0</v>
+      </c>
+      <c r="I17" s="118">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J17" s="125"/>
+      <c r="K17" s="125"/>
+      <c r="L17" s="125"/>
+      <c r="M17" s="25">
+        <v>1</v>
+      </c>
+      <c r="N17" s="166">
+        <v>0</v>
+      </c>
+      <c r="O17" s="166">
+        <v>0</v>
+      </c>
+      <c r="P17" s="166">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="166">
+        <v>0</v>
+      </c>
+      <c r="R17" s="166">
+        <v>0</v>
+      </c>
+      <c r="S17" s="166">
+        <v>0</v>
+      </c>
+      <c r="T17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="U17" s="166">
+        <v>0</v>
+      </c>
+      <c r="V17" s="42">
+        <v>1</v>
+      </c>
+      <c r="W17" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="X17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE17" s="40"/>
+      <c r="AF17" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG17" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH17" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI17" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ17" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK17" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL17" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM17" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN17" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO17" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP17" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ17" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AW17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AX17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AY17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="AZ17" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="BA17" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BC17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BD17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BE17" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="BF17" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI17" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ17" s="41"/>
+      <c r="BK17" s="41"/>
+      <c r="BL17" s="42"/>
+      <c r="BM17" s="60">
+        <v>0</v>
+      </c>
+      <c r="BN17" s="56">
+        <v>0</v>
+      </c>
+      <c r="BO17" s="63">
+        <f>Variables!Q$2</f>
+        <v>0</v>
+      </c>
+      <c r="BP17" s="63" t="s">
+        <v>1048</v>
+      </c>
+      <c r="BQ17" s="42"/>
     </row>
     <row r="18" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="27"/>
       <c r="B18" s="85" t="s">
         <v>289</v>
       </c>
-      <c r="C18" s="147" t="s">
+      <c r="C18" s="138" t="s">
         <v>310</v>
       </c>
       <c r="D18" s="25">
@@ -8550,7 +9513,7 @@
       <c r="F18" s="25">
         <v>10</v>
       </c>
-      <c r="G18" s="143" t="s">
+      <c r="G18" s="135" t="s">
         <v>1107</v>
       </c>
       <c r="H18" s="40">
@@ -8571,7 +9534,7 @@
       <c r="M18" s="25">
         <v>1</v>
       </c>
-      <c r="N18" s="177">
+      <c r="N18" s="166">
         <v>2</v>
       </c>
       <c r="O18" s="25">
@@ -8689,10 +9652,10 @@
       <c r="BA18" s="43">
         <v>2</v>
       </c>
-      <c r="BB18" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC18" s="163" t="s">
+      <c r="BB18" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC18" s="152" t="s">
         <v>1134</v>
       </c>
       <c r="BD18" s="44">
@@ -8701,18 +9664,10 @@
       <c r="BE18" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BF18" s="98" t="s">
-        <v>42</v>
-      </c>
-      <c r="BG18" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BH18" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="BI18" s="41" t="s">
-        <v>42</v>
-      </c>
+      <c r="BF18" s="127"/>
+      <c r="BG18" s="126"/>
+      <c r="BH18" s="126"/>
+      <c r="BI18" s="126"/>
       <c r="BJ18" s="41"/>
       <c r="BK18" s="41"/>
       <c r="BL18" s="42"/>
@@ -8738,7 +9693,7 @@
       <c r="B19" s="85" t="s">
         <v>309</v>
       </c>
-      <c r="C19" s="147" t="s">
+      <c r="C19" s="138" t="s">
         <v>310</v>
       </c>
       <c r="D19" s="25">
@@ -8750,7 +9705,7 @@
       <c r="F19" s="25">
         <v>10</v>
       </c>
-      <c r="G19" s="143" t="s">
+      <c r="G19" s="135" t="s">
         <v>1108</v>
       </c>
       <c r="H19" s="40">
@@ -8771,7 +9726,7 @@
       <c r="M19" s="25">
         <v>1</v>
       </c>
-      <c r="N19" s="177">
+      <c r="N19" s="166">
         <v>2</v>
       </c>
       <c r="O19" s="25">
@@ -8889,10 +9844,10 @@
       <c r="BA19" s="43">
         <v>2</v>
       </c>
-      <c r="BB19" s="163" t="s">
+      <c r="BB19" s="152" t="s">
         <v>1135</v>
       </c>
-      <c r="BC19" s="151">
+      <c r="BC19" s="141">
         <v>11.9</v>
       </c>
       <c r="BD19" s="44">
@@ -8938,7 +9893,7 @@
       <c r="B20" s="85" t="s">
         <v>336</v>
       </c>
-      <c r="C20" s="147" t="s">
+      <c r="C20" s="138" t="s">
         <v>310</v>
       </c>
       <c r="D20" s="25">
@@ -8950,7 +9905,7 @@
       <c r="F20" s="25">
         <v>10</v>
       </c>
-      <c r="G20" s="143" t="s">
+      <c r="G20" s="135" t="s">
         <v>1109</v>
       </c>
       <c r="H20" s="40">
@@ -8971,7 +9926,7 @@
       <c r="M20" s="25">
         <v>1</v>
       </c>
-      <c r="N20" s="177">
+      <c r="N20" s="166">
         <v>1</v>
       </c>
       <c r="O20" s="25">
@@ -9089,10 +10044,10 @@
       <c r="BA20" s="43">
         <v>4</v>
       </c>
-      <c r="BB20" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC20" s="151">
+      <c r="BB20" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC20" s="141">
         <v>16</v>
       </c>
       <c r="BD20" s="44">
@@ -9138,7 +10093,7 @@
       <c r="B21" s="85" t="s">
         <v>1060</v>
       </c>
-      <c r="C21" s="147" t="s">
+      <c r="C21" s="138" t="s">
         <v>1089</v>
       </c>
       <c r="D21" s="25">
@@ -9150,7 +10105,7 @@
       <c r="F21" s="25">
         <v>5000</v>
       </c>
-      <c r="G21" s="143" t="s">
+      <c r="G21" s="135" t="s">
         <v>1111</v>
       </c>
       <c r="H21" s="40">
@@ -9171,7 +10126,7 @@
       <c r="M21" s="25">
         <v>1</v>
       </c>
-      <c r="N21" s="177">
+      <c r="N21" s="166">
         <v>2</v>
       </c>
       <c r="O21" s="25">
@@ -9287,10 +10242,10 @@
       <c r="BA21" s="43">
         <v>3</v>
       </c>
-      <c r="BB21" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC21" s="151">
+      <c r="BB21" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC21" s="141">
         <v>12</v>
       </c>
       <c r="BD21" s="44">
@@ -9327,7 +10282,7 @@
       <c r="B22" s="85" t="s">
         <v>1065</v>
       </c>
-      <c r="C22" s="147" t="s">
+      <c r="C22" s="138" t="s">
         <v>1082</v>
       </c>
       <c r="D22" s="25">
@@ -9339,7 +10294,7 @@
       <c r="F22" s="25">
         <v>5000</v>
       </c>
-      <c r="G22" s="143" t="s">
+      <c r="G22" s="135" t="s">
         <v>1112</v>
       </c>
       <c r="H22" s="40">
@@ -9360,7 +10315,7 @@
       <c r="M22" s="25">
         <v>1</v>
       </c>
-      <c r="N22" s="177">
+      <c r="N22" s="166">
         <v>2</v>
       </c>
       <c r="O22" s="25">
@@ -9472,10 +10427,10 @@
       <c r="BA22" s="43">
         <v>3</v>
       </c>
-      <c r="BB22" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC22" s="151">
+      <c r="BB22" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC22" s="141">
         <v>12</v>
       </c>
       <c r="BD22" s="44">
@@ -9512,7 +10467,7 @@
       <c r="B23" s="85" t="s">
         <v>1070</v>
       </c>
-      <c r="C23" s="147" t="s">
+      <c r="C23" s="138" t="s">
         <v>1083</v>
       </c>
       <c r="D23" s="25">
@@ -9524,7 +10479,7 @@
       <c r="F23" s="25">
         <v>5000</v>
       </c>
-      <c r="G23" s="143" t="s">
+      <c r="G23" s="135" t="s">
         <v>1115</v>
       </c>
       <c r="H23" s="40">
@@ -9545,7 +10500,7 @@
       <c r="M23" s="25">
         <v>1</v>
       </c>
-      <c r="N23" s="177">
+      <c r="N23" s="166">
         <v>2</v>
       </c>
       <c r="O23" s="25">
@@ -9657,10 +10612,10 @@
       <c r="BA23" s="43">
         <v>1</v>
       </c>
-      <c r="BB23" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC23" s="151">
+      <c r="BB23" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC23" s="141">
         <v>8</v>
       </c>
       <c r="BD23" s="44">
@@ -9697,7 +10652,7 @@
       <c r="B24" s="85" t="s">
         <v>1071</v>
       </c>
-      <c r="C24" s="147" t="s">
+      <c r="C24" s="138" t="s">
         <v>1084</v>
       </c>
       <c r="D24" s="25">
@@ -9709,7 +10664,7 @@
       <c r="F24" s="25">
         <v>5000</v>
       </c>
-      <c r="G24" s="143" t="s">
+      <c r="G24" s="135" t="s">
         <v>1113</v>
       </c>
       <c r="H24" s="40">
@@ -9730,7 +10685,7 @@
       <c r="M24" s="25">
         <v>1</v>
       </c>
-      <c r="N24" s="177">
+      <c r="N24" s="166">
         <v>2</v>
       </c>
       <c r="O24" s="25">
@@ -9842,10 +10797,10 @@
       <c r="BA24" s="43">
         <v>3</v>
       </c>
-      <c r="BB24" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC24" s="151">
+      <c r="BB24" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC24" s="141">
         <v>12</v>
       </c>
       <c r="BD24" s="44">
@@ -9882,7 +10837,7 @@
       <c r="B25" s="85" t="s">
         <v>1119</v>
       </c>
-      <c r="C25" s="147" t="s">
+      <c r="C25" s="138" t="s">
         <v>1085</v>
       </c>
       <c r="D25" s="25">
@@ -9894,7 +10849,7 @@
       <c r="F25" s="25">
         <v>5000</v>
       </c>
-      <c r="G25" s="143" t="s">
+      <c r="G25" s="135" t="s">
         <v>1144</v>
       </c>
       <c r="H25" s="40">
@@ -9915,7 +10870,7 @@
       <c r="M25" s="25">
         <v>1</v>
       </c>
-      <c r="N25" s="177">
+      <c r="N25" s="166">
         <v>1</v>
       </c>
       <c r="O25" s="25">
@@ -10027,10 +10982,10 @@
       <c r="BA25" s="43">
         <v>3</v>
       </c>
-      <c r="BB25" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC25" s="151">
+      <c r="BB25" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC25" s="141">
         <v>12</v>
       </c>
       <c r="BD25" s="44">
@@ -10067,7 +11022,7 @@
       <c r="B26" s="85" t="s">
         <v>1118</v>
       </c>
-      <c r="C26" s="147" t="s">
+      <c r="C26" s="138" t="s">
         <v>1086</v>
       </c>
       <c r="D26" s="25">
@@ -10079,7 +11034,7 @@
       <c r="F26" s="25">
         <v>5000</v>
       </c>
-      <c r="G26" s="143" t="s">
+      <c r="G26" s="135" t="s">
         <v>1143</v>
       </c>
       <c r="H26" s="40">
@@ -10100,7 +11055,7 @@
       <c r="M26" s="25">
         <v>1</v>
       </c>
-      <c r="N26" s="177">
+      <c r="N26" s="166">
         <v>2</v>
       </c>
       <c r="O26" s="25">
@@ -10212,10 +11167,10 @@
       <c r="BA26" s="43">
         <v>3</v>
       </c>
-      <c r="BB26" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC26" s="151">
+      <c r="BB26" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC26" s="141">
         <v>12</v>
       </c>
       <c r="BD26" s="44">
@@ -10252,7 +11207,7 @@
       <c r="B27" s="85" t="s">
         <v>1117</v>
       </c>
-      <c r="C27" s="147" t="s">
+      <c r="C27" s="138" t="s">
         <v>1087</v>
       </c>
       <c r="D27" s="25">
@@ -10264,7 +11219,7 @@
       <c r="F27" s="25">
         <v>5000</v>
       </c>
-      <c r="G27" s="143" t="s">
+      <c r="G27" s="135" t="s">
         <v>1114</v>
       </c>
       <c r="H27" s="40">
@@ -10285,7 +11240,7 @@
       <c r="M27" s="25">
         <v>1</v>
       </c>
-      <c r="N27" s="177">
+      <c r="N27" s="166">
         <v>2</v>
       </c>
       <c r="O27" s="25">
@@ -10397,10 +11352,10 @@
       <c r="BA27" s="43">
         <v>3</v>
       </c>
-      <c r="BB27" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC27" s="151">
+      <c r="BB27" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC27" s="141">
         <v>12</v>
       </c>
       <c r="BD27" s="44">
@@ -10437,7 +11392,7 @@
       <c r="B28" s="85" t="s">
         <v>1116</v>
       </c>
-      <c r="C28" s="147" t="s">
+      <c r="C28" s="138" t="s">
         <v>1105</v>
       </c>
       <c r="D28" s="25">
@@ -10449,7 +11404,7 @@
       <c r="F28" s="25">
         <v>5000</v>
       </c>
-      <c r="G28" s="143" t="s">
+      <c r="G28" s="135" t="s">
         <v>1129</v>
       </c>
       <c r="H28" s="40">
@@ -10470,7 +11425,7 @@
       <c r="M28" s="25">
         <v>1</v>
       </c>
-      <c r="N28" s="177">
+      <c r="N28" s="166">
         <v>2</v>
       </c>
       <c r="O28" s="25">
@@ -10582,10 +11537,10 @@
       <c r="BA28" s="43">
         <v>1</v>
       </c>
-      <c r="BB28" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC28" s="151">
+      <c r="BB28" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC28" s="141">
         <v>8</v>
       </c>
       <c r="BD28" s="44">
@@ -10619,13 +11574,13 @@
     </row>
     <row r="29" spans="1:69" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
-      <c r="B29" s="167" t="s">
+      <c r="B29" s="156" t="s">
         <v>1141</v>
       </c>
-      <c r="C29" s="168" t="s">
+      <c r="C29" s="157" t="s">
         <v>1089</v>
       </c>
-      <c r="D29" s="169">
+      <c r="D29" s="158">
         <v>3</v>
       </c>
       <c r="E29" s="25">
@@ -10634,53 +11589,53 @@
       <c r="F29" s="25">
         <v>5000</v>
       </c>
-      <c r="G29" s="143" t="s">
+      <c r="G29" s="135" t="s">
         <v>1142</v>
       </c>
-      <c r="H29" s="170">
+      <c r="H29" s="159">
         <v>20</v>
       </c>
-      <c r="I29" s="171">
+      <c r="I29" s="160">
         <v>1E-3</v>
       </c>
-      <c r="J29" s="169">
+      <c r="J29" s="158">
         <v>2</v>
       </c>
-      <c r="K29" s="169">
+      <c r="K29" s="158">
         <v>0</v>
       </c>
       <c r="L29" s="25">
         <v>99999</v>
       </c>
-      <c r="M29" s="169">
+      <c r="M29" s="158">
         <v>2</v>
       </c>
-      <c r="N29" s="178">
+      <c r="N29" s="167">
         <v>2</v>
       </c>
-      <c r="O29" s="169">
+      <c r="O29" s="158">
         <v>1</v>
       </c>
-      <c r="P29" s="169">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="169">
-        <v>0</v>
-      </c>
-      <c r="R29" s="169">
-        <v>0</v>
-      </c>
-      <c r="S29" s="169">
-        <v>0</v>
-      </c>
-      <c r="T29" s="171">
+      <c r="P29" s="158">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="158">
+        <v>0</v>
+      </c>
+      <c r="R29" s="158">
+        <v>0</v>
+      </c>
+      <c r="S29" s="158">
+        <v>0</v>
+      </c>
+      <c r="T29" s="160">
         <f>I29</f>
         <v>1E-3</v>
       </c>
-      <c r="U29" s="169">
-        <v>0</v>
-      </c>
-      <c r="V29" s="172">
+      <c r="U29" s="158">
+        <v>0</v>
+      </c>
+      <c r="V29" s="161">
         <v>2</v>
       </c>
       <c r="W29" s="43">
@@ -10768,14 +11723,14 @@
       <c r="AY29" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AZ29" s="172"/>
+      <c r="AZ29" s="161"/>
       <c r="BA29" s="43">
         <v>3</v>
       </c>
-      <c r="BB29" s="151">
-        <v>0</v>
-      </c>
-      <c r="BC29" s="151">
+      <c r="BB29" s="141">
+        <v>0</v>
+      </c>
+      <c r="BC29" s="141">
         <v>12</v>
       </c>
       <c r="BD29" s="44">
@@ -10796,24 +11751,24 @@
       <c r="BI29" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="BJ29" s="173"/>
-      <c r="BK29" s="173"/>
-      <c r="BL29" s="172"/>
-      <c r="BM29" s="174"/>
-      <c r="BN29" s="175"/>
-      <c r="BO29" s="176"/>
-      <c r="BP29" s="176" t="s">
+      <c r="BJ29" s="162"/>
+      <c r="BK29" s="162"/>
+      <c r="BL29" s="161"/>
+      <c r="BM29" s="163"/>
+      <c r="BN29" s="164"/>
+      <c r="BO29" s="165"/>
+      <c r="BP29" s="165" t="s">
         <v>1050</v>
       </c>
-      <c r="BQ29" s="172"/>
+      <c r="BQ29" s="161"/>
     </row>
     <row r="30" spans="1:69" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
-      <c r="C30" s="149"/>
+      <c r="C30" s="139"/>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="139"/>
+      <c r="G30" s="131"/>
       <c r="H30" s="5"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -10862,9 +11817,9 @@
       <c r="AY30" s="8"/>
       <c r="AZ30" s="6"/>
       <c r="BA30" s="7"/>
-      <c r="BB30" s="153"/>
-      <c r="BC30" s="153"/>
-      <c r="BD30" s="161"/>
+      <c r="BB30" s="142"/>
+      <c r="BC30" s="142"/>
+      <c r="BD30" s="150"/>
       <c r="BE30" s="6"/>
       <c r="BF30" s="100"/>
       <c r="BG30" s="8"/>
@@ -10883,7 +11838,7 @@
       <c r="BA34" s="9"/>
       <c r="BB34" s="2"/>
       <c r="BC34" s="2"/>
-      <c r="BD34" s="162"/>
+      <c r="BD34" s="151"/>
       <c r="BE34" s="45"/>
       <c r="BL34" s="45"/>
       <c r="BM34" s="45"/>
@@ -10895,7 +11850,7 @@
       <c r="BA35" s="9"/>
       <c r="BB35" s="2"/>
       <c r="BC35" s="2"/>
-      <c r="BD35" s="162"/>
+      <c r="BD35" s="151"/>
       <c r="BE35" s="45"/>
       <c r="BL35" s="45"/>
       <c r="BM35" s="45"/>
@@ -10907,7 +11862,7 @@
       <c r="BA36" s="9"/>
       <c r="BB36" s="2"/>
       <c r="BC36" s="2"/>
-      <c r="BD36" s="162"/>
+      <c r="BD36" s="151"/>
       <c r="BE36" s="45"/>
       <c r="BL36" s="45"/>
       <c r="BM36" s="45"/>
@@ -10919,7 +11874,7 @@
       <c r="BA37" s="9"/>
       <c r="BB37" s="2"/>
       <c r="BC37" s="2"/>
-      <c r="BD37" s="162"/>
+      <c r="BD37" s="151"/>
       <c r="BE37" s="45"/>
       <c r="BL37" s="45"/>
       <c r="BM37" s="45"/>
@@ -10931,7 +11886,7 @@
       <c r="BA38" s="9"/>
       <c r="BB38" s="2"/>
       <c r="BC38" s="2"/>
-      <c r="BD38" s="162"/>
+      <c r="BD38" s="151"/>
       <c r="BE38" s="45"/>
       <c r="BL38" s="45"/>
       <c r="BM38" s="45"/>
@@ -10943,7 +11898,7 @@
       <c r="BA39" s="9"/>
       <c r="BB39" s="2"/>
       <c r="BC39" s="2"/>
-      <c r="BD39" s="162"/>
+      <c r="BD39" s="151"/>
       <c r="BE39" s="45"/>
       <c r="BL39" s="45"/>
       <c r="BM39" s="45"/>
@@ -10955,7 +11910,7 @@
       <c r="BA40" s="9"/>
       <c r="BB40" s="2"/>
       <c r="BC40" s="2"/>
-      <c r="BD40" s="162"/>
+      <c r="BD40" s="151"/>
       <c r="BE40" s="45"/>
       <c r="BL40" s="45"/>
       <c r="BM40" s="45"/>
@@ -10967,7 +11922,7 @@
       <c r="BA41" s="9"/>
       <c r="BB41" s="2"/>
       <c r="BC41" s="2"/>
-      <c r="BD41" s="162"/>
+      <c r="BD41" s="151"/>
       <c r="BE41" s="45"/>
       <c r="BL41" s="45"/>
       <c r="BM41" s="45"/>
@@ -10979,7 +11934,7 @@
       <c r="BA42" s="9"/>
       <c r="BB42" s="2"/>
       <c r="BC42" s="2"/>
-      <c r="BD42" s="162"/>
+      <c r="BD42" s="151"/>
       <c r="BE42" s="45"/>
       <c r="BL42" s="45"/>
       <c r="BM42" s="45"/>
@@ -10991,7 +11946,7 @@
       <c r="BA43" s="9"/>
       <c r="BB43" s="2"/>
       <c r="BC43" s="2"/>
-      <c r="BD43" s="162"/>
+      <c r="BD43" s="151"/>
       <c r="BE43" s="45"/>
       <c r="BL43" s="45"/>
       <c r="BM43" s="45"/>
@@ -11003,7 +11958,7 @@
       <c r="BA44" s="9"/>
       <c r="BB44" s="2"/>
       <c r="BC44" s="2"/>
-      <c r="BD44" s="162"/>
+      <c r="BD44" s="151"/>
       <c r="BE44" s="45"/>
       <c r="BL44" s="45"/>
       <c r="BM44" s="45"/>
@@ -11015,7 +11970,7 @@
       <c r="BA45" s="9"/>
       <c r="BB45" s="2"/>
       <c r="BC45" s="2"/>
-      <c r="BD45" s="162"/>
+      <c r="BD45" s="151"/>
       <c r="BE45" s="45"/>
       <c r="BL45" s="45"/>
       <c r="BM45" s="45"/>
@@ -11027,7 +11982,7 @@
       <c r="BA46" s="9"/>
       <c r="BB46" s="2"/>
       <c r="BC46" s="2"/>
-      <c r="BD46" s="162"/>
+      <c r="BD46" s="151"/>
       <c r="BE46" s="45"/>
       <c r="BL46" s="45"/>
       <c r="BM46" s="45"/>
@@ -11039,7 +11994,7 @@
       <c r="BA47" s="9"/>
       <c r="BB47" s="2"/>
       <c r="BC47" s="2"/>
-      <c r="BD47" s="162"/>
+      <c r="BD47" s="151"/>
       <c r="BE47" s="45"/>
       <c r="BL47" s="45"/>
       <c r="BM47" s="45"/>
@@ -11051,7 +12006,7 @@
       <c r="BA48" s="9"/>
       <c r="BB48" s="2"/>
       <c r="BC48" s="2"/>
-      <c r="BD48" s="162"/>
+      <c r="BD48" s="151"/>
       <c r="BE48" s="45"/>
       <c r="BL48" s="45"/>
       <c r="BM48" s="45"/>
@@ -11063,7 +12018,7 @@
       <c r="BA49" s="9"/>
       <c r="BB49" s="2"/>
       <c r="BC49" s="2"/>
-      <c r="BD49" s="162"/>
+      <c r="BD49" s="151"/>
       <c r="BE49" s="45"/>
       <c r="BL49" s="45"/>
       <c r="BM49" s="45"/>
@@ -11075,7 +12030,7 @@
       <c r="BA50" s="9"/>
       <c r="BB50" s="2"/>
       <c r="BC50" s="2"/>
-      <c r="BD50" s="162"/>
+      <c r="BD50" s="151"/>
       <c r="BE50" s="45"/>
       <c r="BL50" s="45"/>
       <c r="BM50" s="45"/>
@@ -11087,7 +12042,7 @@
       <c r="BA51" s="9"/>
       <c r="BB51" s="2"/>
       <c r="BC51" s="2"/>
-      <c r="BD51" s="162"/>
+      <c r="BD51" s="151"/>
       <c r="BE51" s="45"/>
       <c r="BL51" s="45"/>
       <c r="BM51" s="45"/>
@@ -11099,7 +12054,7 @@
       <c r="BA52" s="9"/>
       <c r="BB52" s="2"/>
       <c r="BC52" s="2"/>
-      <c r="BD52" s="162"/>
+      <c r="BD52" s="151"/>
       <c r="BE52" s="45"/>
       <c r="BL52" s="45"/>
       <c r="BM52" s="45"/>
@@ -11111,7 +12066,7 @@
       <c r="BA53" s="9"/>
       <c r="BB53" s="2"/>
       <c r="BC53" s="2"/>
-      <c r="BD53" s="162"/>
+      <c r="BD53" s="151"/>
       <c r="BE53" s="45"/>
       <c r="BL53" s="45"/>
       <c r="BM53" s="45"/>
@@ -11123,7 +12078,7 @@
       <c r="BA54" s="9"/>
       <c r="BB54" s="2"/>
       <c r="BC54" s="2"/>
-      <c r="BD54" s="162"/>
+      <c r="BD54" s="151"/>
       <c r="BE54" s="45"/>
       <c r="BL54" s="45"/>
       <c r="BM54" s="45"/>
@@ -11135,7 +12090,7 @@
       <c r="BA55" s="9"/>
       <c r="BB55" s="2"/>
       <c r="BC55" s="2"/>
-      <c r="BD55" s="162"/>
+      <c r="BD55" s="151"/>
       <c r="BE55" s="45"/>
       <c r="BL55" s="45"/>
       <c r="BM55" s="45"/>
@@ -11147,7 +12102,7 @@
       <c r="BA56" s="9"/>
       <c r="BB56" s="2"/>
       <c r="BC56" s="2"/>
-      <c r="BD56" s="162"/>
+      <c r="BD56" s="151"/>
       <c r="BE56" s="45"/>
       <c r="BL56" s="45"/>
       <c r="BM56" s="45"/>
@@ -11159,7 +12114,7 @@
       <c r="BA57" s="9"/>
       <c r="BB57" s="2"/>
       <c r="BC57" s="2"/>
-      <c r="BD57" s="162"/>
+      <c r="BD57" s="151"/>
       <c r="BE57" s="45"/>
       <c r="BL57" s="45"/>
       <c r="BM57" s="45"/>
@@ -11171,7 +12126,7 @@
       <c r="BA58" s="9"/>
       <c r="BB58" s="2"/>
       <c r="BC58" s="2"/>
-      <c r="BD58" s="162"/>
+      <c r="BD58" s="151"/>
       <c r="BE58" s="45"/>
       <c r="BL58" s="45"/>
       <c r="BM58" s="45"/>
@@ -11183,7 +12138,7 @@
       <c r="BA59" s="9"/>
       <c r="BB59" s="2"/>
       <c r="BC59" s="2"/>
-      <c r="BD59" s="162"/>
+      <c r="BD59" s="151"/>
       <c r="BE59" s="45"/>
       <c r="BL59" s="45"/>
       <c r="BM59" s="45"/>
@@ -11195,7 +12150,7 @@
       <c r="BA60" s="9"/>
       <c r="BB60" s="2"/>
       <c r="BC60" s="2"/>
-      <c r="BD60" s="162"/>
+      <c r="BD60" s="151"/>
       <c r="BE60" s="45"/>
       <c r="BL60" s="45"/>
       <c r="BM60" s="45"/>
@@ -11207,7 +12162,7 @@
       <c r="BA61" s="9"/>
       <c r="BB61" s="2"/>
       <c r="BC61" s="2"/>
-      <c r="BD61" s="162"/>
+      <c r="BD61" s="151"/>
       <c r="BE61" s="45"/>
       <c r="BL61" s="45"/>
       <c r="BM61" s="45"/>
@@ -11219,7 +12174,7 @@
       <c r="BA62" s="9"/>
       <c r="BB62" s="2"/>
       <c r="BC62" s="2"/>
-      <c r="BD62" s="162"/>
+      <c r="BD62" s="151"/>
       <c r="BE62" s="45"/>
       <c r="BL62" s="45"/>
       <c r="BM62" s="45"/>
@@ -11238,116 +12193,236 @@
     <mergeCell ref="BF2:BL2"/>
     <mergeCell ref="BA2:BE2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A30:G31 W14:Z28 AA14 A4:G27 AA18:AA28 W4:AB13 AB14:AB28 BM4:BQ31 BH4:BL16 BF4 BE4:BE16 BE17:BL28 BA31:BB31 BC30:BL31 BC4:BC28 H4:V31 AB30:AZ31 AA30 W30:Z31 AE29:AQ29 BA30 BF29:BL29 AC4:BA25 AC26:AQ28 AS26:BA28 AS29:AZ29">
-    <cfRule type="expression" dxfId="44" priority="47" stopIfTrue="1">
+  <conditionalFormatting sqref="A30:G31 AA14 W4:AB13 AB14:AB16 BH4:BL16 BF4 BE4:BE16 BA31:BB31 BC30:BL31 BC4:BC16 AB30:AZ31 AA30 W30:Z31 AE29:AQ29 BA30 BF29:BL29 AC26:AQ28 AS26:BA28 AS29:AZ29 A4:G27 BM4:BQ31 BE18:BL28 AC4:BA16 BC18:BC28 BF17:BL17 AC18:BA25 BA17 W14:Z16 W18:AB28 H4:V16 H18:V31 H17:S17 U17:W17 AD17:AQ17">
+    <cfRule type="expression" dxfId="95" priority="81" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="82" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28 A29:F29">
-    <cfRule type="expression" dxfId="42" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="168" priority="79" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="167" priority="80" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA16:AA17">
-    <cfRule type="expression" dxfId="40" priority="59" stopIfTrue="1">
+  <conditionalFormatting sqref="AA16">
+    <cfRule type="expression" dxfId="166" priority="93" stopIfTrue="1">
       <formula>$A15="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="165" priority="94" stopIfTrue="1">
       <formula>$A15="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA15">
-    <cfRule type="expression" dxfId="38" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="65" stopIfTrue="1">
       <formula>$A14="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="66" stopIfTrue="1">
       <formula>$A14="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF5:BF16">
-    <cfRule type="expression" dxfId="36" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="63" stopIfTrue="1">
       <formula>$A5="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="64" stopIfTrue="1">
       <formula>$A5="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG4:BG16">
-    <cfRule type="expression" dxfId="34" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="61" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="62" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BB4:BB28 BB30">
-    <cfRule type="expression" dxfId="32" priority="15" stopIfTrue="1">
+  <conditionalFormatting sqref="BB4:BB16 BB30 BB18:BB28">
+    <cfRule type="expression" dxfId="158" priority="49" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="50" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BD4:BD28">
-    <cfRule type="expression" dxfId="30" priority="13" stopIfTrue="1">
+  <conditionalFormatting sqref="BD4:BD16 BD18:BD28">
+    <cfRule type="expression" dxfId="156" priority="47" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="48" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="expression" dxfId="28" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="45" stopIfTrue="1">
       <formula>$A29="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="46" stopIfTrue="1">
       <formula>$A29="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W29:AD29">
-    <cfRule type="expression" dxfId="26" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="43" stopIfTrue="1">
       <formula>$A29="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="44" stopIfTrue="1">
       <formula>$A29="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE29 BC29 BA29">
-    <cfRule type="expression" dxfId="24" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="41" stopIfTrue="1">
       <formula>$A29="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="42" stopIfTrue="1">
       <formula>$A29="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB29">
-    <cfRule type="expression" dxfId="22" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="39" stopIfTrue="1">
       <formula>$A29="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="40" stopIfTrue="1">
       <formula>$A29="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD29">
-    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="37" stopIfTrue="1">
       <formula>$A29="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="38" stopIfTrue="1">
       <formula>$A29="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR26:AR29">
-    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="35" stopIfTrue="1">
       <formula>$A26="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="36" stopIfTrue="1">
       <formula>$A26="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BF17">
+    <cfRule type="expression" dxfId="81" priority="33" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="34" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BG17">
+    <cfRule type="expression" dxfId="77" priority="31" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="32" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BA17">
+    <cfRule type="expression" dxfId="71" priority="29" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="30" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB17:BD17">
+    <cfRule type="expression" dxfId="67" priority="27" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="28" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB17:BD17">
+    <cfRule type="expression" dxfId="63" priority="25" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="26" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BE17">
+    <cfRule type="expression" dxfId="51" priority="19" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="20" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AZ17">
+    <cfRule type="expression" dxfId="47" priority="17" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="18" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ17">
+    <cfRule type="expression" dxfId="41" priority="15" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="16" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR17:AY17">
+    <cfRule type="expression" dxfId="37" priority="13" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="14" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR17:AY17">
+    <cfRule type="expression" dxfId="33" priority="11" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="12" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W17">
+    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="10" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X17:AC17">
+    <cfRule type="expression" dxfId="21" priority="7" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="8" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X17:AC17">
+    <cfRule type="expression" dxfId="17" priority="5" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T17">
+    <cfRule type="expression" dxfId="11" priority="3" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="4" stopIfTrue="1">
+      <formula>$A17="p"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T17">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
+      <formula>$A17="n"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+      <formula>$A17="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>
@@ -11408,74 +12483,74 @@
   <sheetData>
     <row r="1" spans="1:55" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:55" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="174" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="187"/>
-      <c r="I2" s="179" t="s">
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="168" t="s">
         <v>1062</v>
       </c>
-      <c r="J2" s="180"/>
-      <c r="K2" s="188"/>
-      <c r="L2" s="188"/>
-      <c r="M2" s="188"/>
-      <c r="N2" s="188"/>
-      <c r="O2" s="188"/>
-      <c r="P2" s="188"/>
-      <c r="Q2" s="188"/>
-      <c r="R2" s="188"/>
-      <c r="S2" s="188"/>
-      <c r="T2" s="189"/>
-      <c r="U2" s="190" t="s">
+      <c r="J2" s="169"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
+      <c r="P2" s="177"/>
+      <c r="Q2" s="177"/>
+      <c r="R2" s="177"/>
+      <c r="S2" s="177"/>
+      <c r="T2" s="178"/>
+      <c r="U2" s="179" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="191"/>
-      <c r="W2" s="191"/>
-      <c r="X2" s="191"/>
-      <c r="Y2" s="191"/>
-      <c r="Z2" s="191"/>
-      <c r="AA2" s="191"/>
-      <c r="AB2" s="191"/>
-      <c r="AC2" s="191"/>
-      <c r="AD2" s="191"/>
-      <c r="AE2" s="191"/>
-      <c r="AF2" s="191"/>
-      <c r="AG2" s="191"/>
-      <c r="AH2" s="191"/>
-      <c r="AI2" s="191"/>
-      <c r="AJ2" s="192"/>
-      <c r="AK2" s="202" t="s">
+      <c r="V2" s="180"/>
+      <c r="W2" s="180"/>
+      <c r="X2" s="180"/>
+      <c r="Y2" s="180"/>
+      <c r="Z2" s="180"/>
+      <c r="AA2" s="180"/>
+      <c r="AB2" s="180"/>
+      <c r="AC2" s="180"/>
+      <c r="AD2" s="180"/>
+      <c r="AE2" s="180"/>
+      <c r="AF2" s="180"/>
+      <c r="AG2" s="180"/>
+      <c r="AH2" s="180"/>
+      <c r="AI2" s="180"/>
+      <c r="AJ2" s="181"/>
+      <c r="AK2" s="191" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="194"/>
-      <c r="AM2" s="194"/>
-      <c r="AN2" s="194"/>
-      <c r="AO2" s="194"/>
-      <c r="AP2" s="195"/>
-      <c r="AQ2" s="202" t="s">
+      <c r="AL2" s="183"/>
+      <c r="AM2" s="183"/>
+      <c r="AN2" s="183"/>
+      <c r="AO2" s="183"/>
+      <c r="AP2" s="184"/>
+      <c r="AQ2" s="191" t="s">
         <v>1061</v>
       </c>
-      <c r="AR2" s="193"/>
-      <c r="AS2" s="193"/>
-      <c r="AT2" s="203"/>
-      <c r="AU2" s="199" t="s">
+      <c r="AR2" s="182"/>
+      <c r="AS2" s="182"/>
+      <c r="AT2" s="192"/>
+      <c r="AU2" s="188" t="s">
         <v>18</v>
       </c>
-      <c r="AV2" s="200"/>
-      <c r="AW2" s="200"/>
-      <c r="AX2" s="201"/>
-      <c r="AY2" s="179" t="s">
+      <c r="AV2" s="189"/>
+      <c r="AW2" s="189"/>
+      <c r="AX2" s="190"/>
+      <c r="AY2" s="168" t="s">
         <v>1047</v>
       </c>
-      <c r="AZ2" s="180"/>
-      <c r="BA2" s="180"/>
-      <c r="BB2" s="180"/>
-      <c r="BC2" s="181"/>
+      <c r="AZ2" s="169"/>
+      <c r="BA2" s="169"/>
+      <c r="BB2" s="169"/>
+      <c r="BC2" s="170"/>
     </row>
     <row r="3" spans="1:55" s="1" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -11658,7 +12733,7 @@
       <c r="G4" s="28" t="s">
         <v>497</v>
       </c>
-      <c r="H4" s="155" t="s">
+      <c r="H4" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I4" s="109" t="s">
@@ -11818,7 +12893,7 @@
       <c r="G5" s="39" t="s">
         <v>498</v>
       </c>
-      <c r="H5" s="156" t="s">
+      <c r="H5" s="145" t="s">
         <v>32</v>
       </c>
       <c r="I5" s="110" t="s">
@@ -11978,7 +13053,7 @@
       <c r="G6" s="39" t="s">
         <v>491</v>
       </c>
-      <c r="H6" s="155" t="s">
+      <c r="H6" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I6" s="110" t="s">
@@ -12138,7 +13213,7 @@
       <c r="G7" s="39" t="s">
         <v>492</v>
       </c>
-      <c r="H7" s="155" t="s">
+      <c r="H7" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I7" s="110" t="s">
@@ -12298,7 +13373,7 @@
       <c r="G8" s="39" t="s">
         <v>499</v>
       </c>
-      <c r="H8" s="155" t="s">
+      <c r="H8" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I8" s="110" t="s">
@@ -12459,7 +13534,7 @@
       <c r="G9" s="39" t="s">
         <v>499</v>
       </c>
-      <c r="H9" s="155" t="s">
+      <c r="H9" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I9" s="110" t="s">
@@ -12620,7 +13695,7 @@
       <c r="G10" s="39" t="s">
         <v>492</v>
       </c>
-      <c r="H10" s="155" t="s">
+      <c r="H10" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I10" s="110" t="s">
@@ -12781,7 +13856,7 @@
       <c r="G11" s="28" t="s">
         <v>497</v>
       </c>
-      <c r="H11" s="155" t="s">
+      <c r="H11" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I11" s="110" t="s">
@@ -12941,7 +14016,7 @@
       <c r="G12" s="39" t="s">
         <v>493</v>
       </c>
-      <c r="H12" s="155" t="s">
+      <c r="H12" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I12" s="110" t="s">
@@ -13101,7 +14176,7 @@
       <c r="G13" s="39" t="s">
         <v>496</v>
       </c>
-      <c r="H13" s="155" t="s">
+      <c r="H13" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I13" s="110" t="s">
@@ -13261,7 +14336,7 @@
       <c r="G14" s="39" t="s">
         <v>500</v>
       </c>
-      <c r="H14" s="155" t="s">
+      <c r="H14" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I14" s="110" t="s">
@@ -13421,7 +14496,7 @@
       <c r="G15" s="39" t="s">
         <v>494</v>
       </c>
-      <c r="H15" s="155" t="s">
+      <c r="H15" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I15" s="110" t="s">
@@ -13581,7 +14656,7 @@
       <c r="G16" s="39" t="s">
         <v>495</v>
       </c>
-      <c r="H16" s="155" t="s">
+      <c r="H16" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I16" s="110" t="s">
@@ -13741,7 +14816,7 @@
       <c r="G17" s="108" t="s">
         <v>501</v>
       </c>
-      <c r="H17" s="156" t="s">
+      <c r="H17" s="145" t="s">
         <v>22</v>
       </c>
       <c r="I17" s="110" t="s">
@@ -13901,7 +14976,7 @@
       <c r="G18" s="39" t="s">
         <v>502</v>
       </c>
-      <c r="H18" s="155" t="s">
+      <c r="H18" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I18" s="110" t="s">
@@ -14061,7 +15136,7 @@
       <c r="G19" s="39" t="s">
         <v>503</v>
       </c>
-      <c r="H19" s="155" t="s">
+      <c r="H19" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I19" s="110" t="s">
@@ -14221,7 +15296,7 @@
       <c r="G20" s="39" t="s">
         <v>504</v>
       </c>
-      <c r="H20" s="155" t="s">
+      <c r="H20" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I20" s="110" t="s">
@@ -14379,7 +15454,7 @@
       <c r="G21" s="39" t="s">
         <v>1074</v>
       </c>
-      <c r="H21" s="155" t="s">
+      <c r="H21" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I21" s="110" t="s">
@@ -14522,7 +15597,7 @@
       <c r="G22" s="39" t="s">
         <v>1076</v>
       </c>
-      <c r="H22" s="155" t="s">
+      <c r="H22" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I22" s="110" t="s">
@@ -14607,7 +15682,7 @@
       <c r="G23" s="39" t="s">
         <v>1075</v>
       </c>
-      <c r="H23" s="155" t="s">
+      <c r="H23" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I23" s="110" t="s">
@@ -14688,7 +15763,7 @@
       <c r="G24" s="39" t="s">
         <v>1072</v>
       </c>
-      <c r="H24" s="155" t="s">
+      <c r="H24" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I24" s="110" t="s">
@@ -14769,7 +15844,7 @@
       <c r="G25" s="39" t="s">
         <v>1066</v>
       </c>
-      <c r="H25" s="155" t="s">
+      <c r="H25" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I25" s="110" t="s">
@@ -14854,7 +15929,7 @@
       <c r="G26" s="39" t="s">
         <v>1080</v>
       </c>
-      <c r="H26" s="155" t="s">
+      <c r="H26" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I26" s="110" t="s">
@@ -14939,7 +16014,7 @@
       <c r="G27" s="39" t="s">
         <v>1077</v>
       </c>
-      <c r="H27" s="155" t="s">
+      <c r="H27" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I27" s="110" t="s">
@@ -15024,7 +16099,7 @@
       <c r="G28" s="39" t="s">
         <v>1079</v>
       </c>
-      <c r="H28" s="155" t="s">
+      <c r="H28" s="144" t="s">
         <v>32</v>
       </c>
       <c r="I28" s="110" t="s">
@@ -15362,42 +16437,42 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A4:BC21 C29:F32 A29:B33 G29:BC31 I33:BC33 I32:K32 M32:BC32 J22:AI27 AK22:BC27 A22:G27 H20:H28">
-    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="15" stopIfTrue="1">
       <formula>$A4="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="16" stopIfTrue="1">
       <formula>$A4="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:G28 J28:AI28 AK28:BC28">
-    <cfRule type="expression" dxfId="14" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="5" stopIfTrue="1">
       <formula>$A28="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="6" stopIfTrue="1">
       <formula>$A28="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="12" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="19" stopIfTrue="1">
       <formula>$A32="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="20" stopIfTrue="1">
       <formula>$A32="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I28">
-    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="3" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="4" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ22:AJ28">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="1" stopIfTrue="1">
       <formula>$A22="n"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="2" stopIfTrue="1">
       <formula>$A22="p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46843,31 +47918,31 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="C782:C787 C844:C855 C789:C842">
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="1" stopIfTrue="1">
       <formula>$A782=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="2" stopIfTrue="1">
       <formula>$A782=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B336:C353 B764:C769 B301:C303 B4:C10 B297:C299 B38:C49 B25:C36 B496:C528 B12:C23 B844:B855 B315:C326 B530:C539 B541:C550 B728:C743 B745:C748 B750:C758 B332:C334 B771:C780 B328:C330 B760:C760 B762:C762 B305:C313 B355:C358 B782:B787 B552:C561 B51:C131 B133:C213 B215:C295 B360:C494 B563:C616 B673:C726 B618:C671 B789:B842">
-    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="3" stopIfTrue="1">
       <formula>$A4=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="4" stopIfTrue="1">
       <formula>$A4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2 D2:Z2">
-    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A10 A12:A23 A25:A36 A38:A49 A297:A299 A301:A303 A305:A313 A315:A326 A328:A330 A332:A334 A336:A353 A355:A358 A496:A528 A530:A539 A541:A550 A552:A561 A745:A748 A750:A758 A760 A762 A764:A769 A771:A780 A782:A787 A844:A855 A51:A131 A133:A213 A215:A295 A360:A494 A563:A616 A673:A726 A618:A671 A728:A743 A789:A842">
-    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="6" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="7" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>